<commit_message>
Add Grove of Patriarchs, Silver Falls, and Owyhigh Lakes
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B8114C6-78BE-4F4E-B932-622D9204F283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B054C20A-976D-4DA7-98F5-F3AC6AFC42FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Owyhigh Lakes from White River Road</t>
+  </si>
+  <si>
+    <t>Grove of the Patriarchs and Silver Falls Loop</t>
   </si>
 </sst>
 </file>
@@ -256,7 +262,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A134A1B-3AE7-4DD5-9B5E-851CC31C35DF}" type="CELLRANGE">
+                    <a:fld id="{0EEBA64E-F695-4F74-902C-EB7B5C80F0DE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -290,7 +296,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F198E97F-5693-4082-BDE2-ED7820D1BD37}" type="CELLRANGE">
+                    <a:fld id="{9AD81F53-2DEB-4B1F-9E8D-7FDC05858FB1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -324,7 +330,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{99CEB3F6-5B0E-4B30-97D8-57343589DC7C}" type="CELLRANGE">
+                    <a:fld id="{7F6A3B08-50E5-4E1D-A6B4-0CC4CC94A3F9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -358,7 +364,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{965840A8-A096-4B6A-BD95-BBD6AE5B102C}" type="CELLRANGE">
+                    <a:fld id="{3BA769D1-4810-4B4F-98A3-6BC14CEEECD2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -392,7 +398,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{652A61CE-8289-4E42-9643-3AC653C9A226}" type="CELLRANGE">
+                    <a:fld id="{A6AE6FCB-BA5C-46A2-B416-B4185077D102}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -426,7 +432,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B8F6BD2-EA5A-4C73-BF1D-9766654FCABB}" type="CELLRANGE">
+                    <a:fld id="{6022959C-D42A-475E-B1D5-72AAED30A519}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -460,7 +466,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CDB3B623-A061-417A-B0A1-2455FFB5EB0D}" type="CELLRANGE">
+                    <a:fld id="{0E72380F-E7F5-44D9-B6E6-C37A3381B743}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -494,7 +500,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A368882-55D7-46DC-9063-B4BE26014C3A}" type="CELLRANGE">
+                    <a:fld id="{417E9F32-D23C-4DED-B72D-3411E7A72025}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -528,7 +534,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0BE51AF1-36CB-456A-8EC1-F57365FCD06A}" type="CELLRANGE">
+                    <a:fld id="{2632DD0A-EC54-435F-ADF5-2AEA5505C50F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -562,7 +568,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70E9F3F4-ABF7-4577-894A-3E46333E32DA}" type="CELLRANGE">
+                    <a:fld id="{35B46D2F-AD96-4BB1-9802-E7CABD8AE321}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -596,7 +602,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7FE10551-3840-430E-BC09-94CF64F39B83}" type="CELLRANGE">
+                    <a:fld id="{6D577B93-074F-4AAA-900C-5E0F27F04F19}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -630,7 +636,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9AFDA6FA-5B40-493D-B1B1-D2ECA7B11885}" type="CELLRANGE">
+                    <a:fld id="{9D403827-CF6B-4924-B1B3-83124AD3E4D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -664,7 +670,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C9A1827A-67CE-45BF-8E04-84A3542C3302}" type="CELLRANGE">
+                    <a:fld id="{12DC1285-2C28-48D7-A9CB-25D0F49FFA3D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -698,7 +704,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA722924-44C3-4B26-814C-57384D48BD71}" type="CELLRANGE">
+                    <a:fld id="{0C5BE4F1-E92E-4767-B4D7-FD9A9CC5F6E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -732,7 +738,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E526659F-6177-4613-B96A-D97A2A53D802}" type="CELLRANGE">
+                    <a:fld id="{364212BA-E147-4086-A724-FC21F4C910DC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -766,7 +772,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BD638A2E-A868-48E7-A964-DEFDCDDE8249}" type="CELLRANGE">
+                    <a:fld id="{3397760A-25AE-4EF0-A42F-AC05BA9AA645}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -800,7 +806,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B4595637-B5F9-44AC-BC6B-8890FDE2DAE0}" type="CELLRANGE">
+                    <a:fld id="{2DCE4002-9009-4C6A-A061-F612E9E3FCD0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -834,7 +840,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A648464-456C-40D4-AB2C-5E4AEEB03AE3}" type="CELLRANGE">
+                    <a:fld id="{35314757-5425-49C6-9888-4546220FEDE1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -868,7 +874,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{328FE9EB-46A6-4F31-8E26-2D50A59B3AD8}" type="CELLRANGE">
+                    <a:fld id="{AAADE927-BAE6-4739-A5A4-749BF1FA89A2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -902,7 +908,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD12E66E-ADF5-4861-AC8A-037D55543EAA}" type="CELLRANGE">
+                    <a:fld id="{460C6CFC-7016-44C1-A93F-37F9CAF0E811}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -936,7 +942,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34938EDD-F7EC-46D5-8C15-ADB14524755F}" type="CELLRANGE">
+                    <a:fld id="{97CBE7C7-5854-48CF-A080-35C90F6CDDD0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -970,7 +976,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{77FD823E-8FA3-4916-B1D8-C2F4D7B7D27F}" type="CELLRANGE">
+                    <a:fld id="{1A773C9F-4DD9-4997-B24A-FA3196F0AD1B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1004,7 +1010,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E6D3B7F7-6C2A-4398-858B-426DED52D174}" type="CELLRANGE">
+                    <a:fld id="{E376D8CE-965C-4826-B20A-3D562B816A64}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1038,7 +1044,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56418730-8D84-4840-8662-38E60FF850F5}" type="CELLRANGE">
+                    <a:fld id="{9B21E14D-9A9B-4417-8D75-2D51535815EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1072,7 +1078,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1EB8B98A-856C-4337-B98F-1413BB4C7EB0}" type="CELLRANGE">
+                    <a:fld id="{A5FEAAC9-E79F-4D05-97D3-AF6AF559FD8D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1106,7 +1112,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5AFA2311-54FC-4D8C-A075-81D5A9ABD78B}" type="CELLRANGE">
+                    <a:fld id="{DDDF9627-BD65-41C9-B389-22909B04C947}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1130,6 +1136,74 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000001A-CCFE-43AC-B5D6-A892358F6818}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="26"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{67B12179-BD26-4721-A2DD-24913AB7B368}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-5540-4AF6-8C95-CDB15D52B94B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="27"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{F25E5DAB-6AEF-4410-9FE4-6ADCAA1C6A03}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-5540-4AF6-8C95-CDB15D52B94B}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1179,10 +1253,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$27</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
@@ -1260,16 +1334,22 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$27</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>2840</c:v>
                 </c:pt>
@@ -1347,6 +1427,12 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>2180</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1670</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1435,6 +1521,12 @@
                   </c:pt>
                   <c:pt idx="25">
                     <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>easy</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -2440,8 +2532,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D27" totalsRowShown="0">
-  <autoFilter ref="A1:D27" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D29" totalsRowShown="0">
+  <autoFilter ref="A1:D29" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{462E7F18-8F43-4DC9-9F61-009B88773B23}" name="Distance"/>
@@ -2749,10 +2841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3144,6 +3236,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>1670</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <v>5.2</v>
+      </c>
+      <c r="C29">
+        <v>1000</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Crystal Lakes hike
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B054C20A-976D-4DA7-98F5-F3AC6AFC42FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5783993-5A66-455E-8EE9-305C7596F5DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Grove of the Patriarchs and Silver Falls Loop</t>
+  </si>
+  <si>
+    <t>Crystal Lakes and Sourdough Gap</t>
   </si>
 </sst>
 </file>
@@ -262,7 +265,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0EEBA64E-F695-4F74-902C-EB7B5C80F0DE}" type="CELLRANGE">
+                    <a:fld id="{24A23C4C-E604-45E8-81FE-BD600911C7E7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -296,7 +299,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9AD81F53-2DEB-4B1F-9E8D-7FDC05858FB1}" type="CELLRANGE">
+                    <a:fld id="{3F1AE220-CC39-4939-8DE1-29943FEED284}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -330,7 +333,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F6A3B08-50E5-4E1D-A6B4-0CC4CC94A3F9}" type="CELLRANGE">
+                    <a:fld id="{95A6F342-9B82-4BAF-92EB-C150B973067B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -364,7 +367,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3BA769D1-4810-4B4F-98A3-6BC14CEEECD2}" type="CELLRANGE">
+                    <a:fld id="{B7AA74AD-2546-4946-9344-ECEA1B1EBFB6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -398,7 +401,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A6AE6FCB-BA5C-46A2-B416-B4185077D102}" type="CELLRANGE">
+                    <a:fld id="{D2829E61-625B-4006-BD59-A9DF8C32878C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -432,7 +435,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6022959C-D42A-475E-B1D5-72AAED30A519}" type="CELLRANGE">
+                    <a:fld id="{E8303493-B63A-4C70-ADD7-0EA295BEFBBE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -466,7 +469,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E72380F-E7F5-44D9-B6E6-C37A3381B743}" type="CELLRANGE">
+                    <a:fld id="{D70BD4A8-0FA5-4719-911B-DF8049ABDA1B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -500,7 +503,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{417E9F32-D23C-4DED-B72D-3411E7A72025}" type="CELLRANGE">
+                    <a:fld id="{DE155453-2641-4D1B-AA79-18219B25BB14}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -534,7 +537,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2632DD0A-EC54-435F-ADF5-2AEA5505C50F}" type="CELLRANGE">
+                    <a:fld id="{F5230F1C-CE27-4A8A-9C20-57547B6D5BBD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -568,7 +571,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35B46D2F-AD96-4BB1-9802-E7CABD8AE321}" type="CELLRANGE">
+                    <a:fld id="{39B0DCB0-A18F-42EB-8257-28DA34313653}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -602,7 +605,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D577B93-074F-4AAA-900C-5E0F27F04F19}" type="CELLRANGE">
+                    <a:fld id="{0BDC9FED-B2B2-43C5-8F44-21DFADB7A936}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -636,7 +639,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D403827-CF6B-4924-B1B3-83124AD3E4D8}" type="CELLRANGE">
+                    <a:fld id="{00F59BC8-6F67-439B-A928-9ADAB727C9CD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -670,7 +673,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12DC1285-2C28-48D7-A9CB-25D0F49FFA3D}" type="CELLRANGE">
+                    <a:fld id="{54F32DF5-E93C-4162-9C09-610C20D3B310}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -704,7 +707,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C5BE4F1-E92E-4767-B4D7-FD9A9CC5F6E4}" type="CELLRANGE">
+                    <a:fld id="{901327EF-B31A-48B0-905F-4B7235610934}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -738,7 +741,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{364212BA-E147-4086-A724-FC21F4C910DC}" type="CELLRANGE">
+                    <a:fld id="{94CF9DBE-60DF-4CFF-AF5D-C62E595D84D2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -772,7 +775,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3397760A-25AE-4EF0-A42F-AC05BA9AA645}" type="CELLRANGE">
+                    <a:fld id="{3D08F95E-5CCA-4D23-9041-09868F021831}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -806,7 +809,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2DCE4002-9009-4C6A-A061-F612E9E3FCD0}" type="CELLRANGE">
+                    <a:fld id="{E46E7706-9642-458B-B6E5-8C9C474A3909}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -840,7 +843,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35314757-5425-49C6-9888-4546220FEDE1}" type="CELLRANGE">
+                    <a:fld id="{53C4B43F-2165-43DD-867B-FC8E9D5942F1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -874,7 +877,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AAADE927-BAE6-4739-A5A4-749BF1FA89A2}" type="CELLRANGE">
+                    <a:fld id="{7B28458C-3ED5-4BAA-89E4-F00E05A8C752}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -908,7 +911,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{460C6CFC-7016-44C1-A93F-37F9CAF0E811}" type="CELLRANGE">
+                    <a:fld id="{E8F67E08-01EB-4B78-921C-06EEC956DDC0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -942,7 +945,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97CBE7C7-5854-48CF-A080-35C90F6CDDD0}" type="CELLRANGE">
+                    <a:fld id="{766FF3C8-621A-4889-B944-3C8EFE84634F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -976,7 +979,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A773C9F-4DD9-4997-B24A-FA3196F0AD1B}" type="CELLRANGE">
+                    <a:fld id="{57AFFEDF-78EA-4146-8544-1C3F849EACCD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1010,7 +1013,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E376D8CE-965C-4826-B20A-3D562B816A64}" type="CELLRANGE">
+                    <a:fld id="{AE931269-4756-4A72-953B-B0FAA00DCD9F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1044,7 +1047,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B21E14D-9A9B-4417-8D75-2D51535815EE}" type="CELLRANGE">
+                    <a:fld id="{22EA8430-2B4B-4DBD-A552-7789FE046937}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1078,7 +1081,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5FEAAC9-E79F-4D05-97D3-AF6AF559FD8D}" type="CELLRANGE">
+                    <a:fld id="{07C71AFA-0115-4C50-8905-FFC9AAF7D665}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1112,7 +1115,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DDDF9627-BD65-41C9-B389-22909B04C947}" type="CELLRANGE">
+                    <a:fld id="{0679A9ED-E9F7-4EB9-9F88-F6149E4BBF21}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1146,7 +1149,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67B12179-BD26-4721-A2DD-24913AB7B368}" type="CELLRANGE">
+                    <a:fld id="{BCB6CD2C-FBE2-4618-8B54-6CA5B35DBE34}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1180,7 +1183,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F25E5DAB-6AEF-4410-9FE4-6ADCAA1C6A03}" type="CELLRANGE">
+                    <a:fld id="{4FB8D52E-E8D2-43B4-BE96-79071AE3EA52}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1204,6 +1207,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-5540-4AF6-8C95-CDB15D52B94B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="28"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{BBB2F61C-3E24-4DEF-9820-9756530C8889}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-DF82-44F8-8CA5-5DBD7A001CB3}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1253,10 +1290,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$29</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
@@ -1340,16 +1377,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$29</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>2840</c:v>
                 </c:pt>
@@ -1433,6 +1473,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2970</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1527,6 +1570,9 @@
                   </c:pt>
                   <c:pt idx="27">
                     <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -2532,8 +2578,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D29" totalsRowShown="0">
-  <autoFilter ref="A1:D29" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D30" totalsRowShown="0">
+  <autoFilter ref="A1:D30" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{462E7F18-8F43-4DC9-9F61-009B88773B23}" name="Distance"/>
@@ -2841,10 +2887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3264,6 +3310,20 @@
         <v>8</v>
       </c>
     </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>7.5</v>
+      </c>
+      <c r="C30">
+        <v>2970</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Snow Lake trail
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B8958E-C6ED-42CB-8D17-0FD84A7A05CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD53990-782F-4D97-A8B3-17B51D4FDD4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>South Puyallup Pipe Organ</t>
+  </si>
+  <si>
+    <t>Eagle Peak</t>
+  </si>
+  <si>
+    <t>Snow Lake</t>
   </si>
 </sst>
 </file>
@@ -271,7 +277,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{683F8EA6-1B13-4F73-8BA7-0179D7AE7AF1}" type="CELLRANGE">
+                    <a:fld id="{3F8502BF-350C-4191-BC40-5E55B120067F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -305,7 +311,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD8A8C57-EADA-4E6D-89DE-328B388D7AB0}" type="CELLRANGE">
+                    <a:fld id="{51C07408-2689-44EF-BAB4-6BECAED68159}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -339,7 +345,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{574E8921-A9B0-4E4C-BE8A-75EFB2B53C9D}" type="CELLRANGE">
+                    <a:fld id="{BB4E95DE-E93C-443B-81E4-F3C81D06706B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -373,7 +379,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BC5D9215-0A5D-41F7-9454-70D2F6567690}" type="CELLRANGE">
+                    <a:fld id="{9F2C5256-0A55-4BB4-9E6A-AB7A6816C13C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -407,7 +413,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5CA3A9F5-82DD-44F5-A873-4B5317ED9E4C}" type="CELLRANGE">
+                    <a:fld id="{775BC8C4-C54D-44C9-A84B-536EB9BC4812}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -441,7 +447,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{54D988CC-26B5-4046-A149-7C31F1434D24}" type="CELLRANGE">
+                    <a:fld id="{A2CC2FC4-F140-4533-A044-D277193607A4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -475,7 +481,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A6A095EA-8A97-48F5-AF6A-D9550B2644DB}" type="CELLRANGE">
+                    <a:fld id="{3559DCC4-E521-42DD-B20C-B77D0B05760E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -509,7 +515,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95319BCA-9EA6-4EB3-A256-AB430C6667A2}" type="CELLRANGE">
+                    <a:fld id="{4F20573E-0609-4131-8C7C-389CE5E8CDCD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -543,7 +549,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F2EF2B5-E8CB-446D-828D-FAA6367B2F72}" type="CELLRANGE">
+                    <a:fld id="{178B5E76-6A06-4EE5-8273-B3268596F8EC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -577,7 +583,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C2D887A6-9775-474E-B8ED-749198D97396}" type="CELLRANGE">
+                    <a:fld id="{3784C741-216C-419D-ABEF-F7A759DE23E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -611,7 +617,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{980FD1B4-67A1-4A3D-8AB5-2262055BFD10}" type="CELLRANGE">
+                    <a:fld id="{CAD77D56-3018-4AA0-B9EA-12D4623919A2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -645,7 +651,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7766388A-6F58-438B-867D-C3C470C96079}" type="CELLRANGE">
+                    <a:fld id="{6F1CA893-1957-4F80-9187-C658AF013D5A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -679,7 +685,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D373D76D-46B1-4107-BBFF-D05C904D05A9}" type="CELLRANGE">
+                    <a:fld id="{3E71E0DE-B441-4B4E-93FC-0D96F97679D6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -713,7 +719,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7CB854E6-65CD-4C29-881C-0A1C398C585E}" type="CELLRANGE">
+                    <a:fld id="{0BD409A5-AEC8-4DF4-BBBE-427D48990AD9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -747,7 +753,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{074BBCBE-B4CC-4DBA-A495-57ED6A98EE0F}" type="CELLRANGE">
+                    <a:fld id="{D0C61470-C985-4161-931A-DE4CA8E9E216}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -781,7 +787,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3128763-73DD-4A17-83AC-35D3C1E53070}" type="CELLRANGE">
+                    <a:fld id="{5EA9FD9C-58F2-40F9-887A-8840BB889E3F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -815,7 +821,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D066AABC-6044-4DE9-8A66-A21B7E3E26A0}" type="CELLRANGE">
+                    <a:fld id="{6122EFF2-7B5E-4E08-9E43-F3D271FDEE54}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -849,7 +855,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F01F9D6B-CE65-45A2-A11E-9C75E75B9797}" type="CELLRANGE">
+                    <a:fld id="{CE6E7033-2FD9-4A35-9CFB-B82BE7C3FFA3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -883,7 +889,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79641355-C15E-4AF4-8821-E909546327ED}" type="CELLRANGE">
+                    <a:fld id="{6A40E867-D73B-4738-987B-55165FEF8102}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -917,7 +923,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A794E0ED-12F2-4E0C-BE14-A15020EE3C43}" type="CELLRANGE">
+                    <a:fld id="{29B20C99-E0A1-400F-8C00-120C674BAB48}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -951,7 +957,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AA72E951-36C4-49DA-9FB7-72237A7B8F25}" type="CELLRANGE">
+                    <a:fld id="{3E38855A-68F3-4EF8-A0A3-66B652045F89}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -985,7 +991,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C76A34AE-7628-4592-A289-7CC893586C06}" type="CELLRANGE">
+                    <a:fld id="{6B9DF212-E1D7-48EB-86A3-3A4DF0EE8B4D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1019,7 +1025,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8A8B3FB-5B3B-46F7-BC60-F2EE2B1DF397}" type="CELLRANGE">
+                    <a:fld id="{31FF868B-295F-4264-91AF-D2539D248BC6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1053,7 +1059,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D4FADC0-EA24-4E23-910B-4FD97E992424}" type="CELLRANGE">
+                    <a:fld id="{DE486E87-68BA-4F9A-BDDE-C85CD364B44C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1087,7 +1093,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DDE0051F-7843-4C2B-9AA8-0338427E4A5F}" type="CELLRANGE">
+                    <a:fld id="{80A4C3FB-7FAA-4792-B793-9FCFFF54199E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1121,7 +1127,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{847AF180-102F-4E9C-981A-D912A22337C8}" type="CELLRANGE">
+                    <a:fld id="{55815BA7-AA31-4D03-9DAD-9771782771F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1155,7 +1161,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C886D2E-4B2A-4BE9-A1B0-4373B5D75F1F}" type="CELLRANGE">
+                    <a:fld id="{5D35AECA-3494-4F4A-B36F-6EA922CDB633}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1189,7 +1195,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3EDD7CAD-75C1-4AE4-8E08-91293B3F6150}" type="CELLRANGE">
+                    <a:fld id="{19910BAE-2C54-4B1B-B746-A27F57560013}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1223,7 +1229,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8DA961AE-BCE8-4390-9101-4362B20AF9FB}" type="CELLRANGE">
+                    <a:fld id="{E33A5DC6-22D9-468F-9A02-E416B3180D0F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1257,7 +1263,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C5E0EF7-6962-4754-B57B-0D24C33490FE}" type="CELLRANGE">
+                    <a:fld id="{072F3239-327B-40D7-85F9-352FAB951C57}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1291,7 +1297,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A524EF5-8929-4D45-9F34-81B740FF40D7}" type="CELLRANGE">
+                    <a:fld id="{1A744067-D188-4BA2-AE53-3ED784483093}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1315,6 +1321,74 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-F59E-4694-B0D3-DE0C2E6817EB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="31"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{1C605926-8558-4A04-9665-DC927937546F}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-D32D-4B88-BB47-9917441C7F35}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="32"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FC4C48AD-1CC1-4D85-8C33-73BE861E0A35}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-D32D-4B88-BB47-9917441C7F35}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1364,10 +1438,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$32</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
@@ -1387,78 +1461,84 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>9.8000000000000007</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>9.6</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>9.1</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>12.2</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>9.75</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>5.4</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1466,10 +1546,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$32</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>2840</c:v>
                 </c:pt>
@@ -1489,78 +1569,84 @@
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>3030</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2880</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>3290</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>2780</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>4800</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>4120</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>3420</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>1450</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -1595,19 +1681,19 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>strenuous</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="8">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="11">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>strenuous</c:v>
@@ -1619,16 +1705,16 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="15">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="17">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="18">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="19">
                     <c:v>moderate</c:v>
@@ -1637,33 +1723,39 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="21">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="22">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="24">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="25">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="26">
-                    <c:v>strenuous</c:v>
-                  </c:pt>
                   <c:pt idx="27">
-                    <c:v>strenuous</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="28">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="29">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="30">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="32">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -2670,10 +2762,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D32" totalsRowShown="0">
-  <autoFilter ref="A1:D32" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D32">
-    <sortCondition ref="A1:A32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D34" totalsRowShown="0">
+  <autoFilter ref="A1:D34" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D34">
+    <sortCondition ref="A1:A34"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -2982,10 +3074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3097,13 +3189,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B8">
-        <v>9.8000000000000007</v>
+        <v>7.1</v>
       </c>
       <c r="C8">
-        <v>2880</v>
+        <v>3030</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
@@ -3111,27 +3203,27 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>9.6</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C9">
-        <v>3290</v>
+        <v>2880</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>14</v>
+        <v>9.6</v>
       </c>
       <c r="C10">
-        <v>2780</v>
+        <v>3290</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -3139,55 +3231,55 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>9.1</v>
+        <v>14</v>
       </c>
       <c r="C11">
-        <v>1580</v>
+        <v>2780</v>
       </c>
       <c r="D11" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>5.2</v>
+        <v>9.1</v>
       </c>
       <c r="C12">
-        <v>1000</v>
+        <v>1580</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B13">
-        <v>14</v>
+        <v>5.2</v>
       </c>
       <c r="C13">
-        <v>4800</v>
+        <v>1000</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>12.2</v>
+        <v>14</v>
       </c>
       <c r="C14">
-        <v>4120</v>
+        <v>4800</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -3195,13 +3287,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>12.2</v>
       </c>
       <c r="C15">
-        <v>3420</v>
+        <v>4120</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -3209,15 +3301,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <f>19.5/2</f>
-        <v>9.75</v>
+        <v>12</v>
       </c>
       <c r="C16">
-        <f>4400*7/8</f>
-        <v>3850</v>
+        <v>3420</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -3225,69 +3315,71 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B17">
-        <v>5.4</v>
+        <f>19.5/2</f>
+        <v>9.75</v>
       </c>
       <c r="C17">
-        <v>1450</v>
+        <f>4400*7/8</f>
+        <v>3850</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>11.4</v>
+        <v>5.4</v>
       </c>
       <c r="C18">
-        <v>2550</v>
+        <v>1450</v>
       </c>
       <c r="D18" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>8.5</v>
+        <v>11.4</v>
       </c>
       <c r="C19">
-        <v>3350</v>
+        <v>2550</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>10.4</v>
+        <v>8.5</v>
       </c>
       <c r="C20">
-        <v>1420</v>
+        <v>3350</v>
       </c>
       <c r="D20" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>7</v>
+        <v>10.4</v>
       </c>
       <c r="C21">
-        <v>1670</v>
+        <v>1420</v>
       </c>
       <c r="D21" t="s">
         <v>1</v>
@@ -3295,13 +3387,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B22">
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="C22">
-        <v>1850</v>
+        <v>1670</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
@@ -3309,27 +3401,27 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C23">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>4.8</v>
       </c>
       <c r="C24">
-        <v>1470</v>
+        <v>1300</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
@@ -3337,27 +3429,27 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C25">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D25" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>11</v>
+        <v>6.9</v>
       </c>
       <c r="C26">
-        <v>2170</v>
+        <v>2000</v>
       </c>
       <c r="D26" t="s">
         <v>1</v>
@@ -3365,71 +3457,71 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B27">
-        <v>7.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C27">
-        <v>2250</v>
+        <v>750</v>
       </c>
       <c r="D27" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B28">
-        <f>16*2/3</f>
-        <v>10.666666666666666</v>
+        <v>11</v>
       </c>
       <c r="C28">
-        <f>4910*2/3</f>
-        <v>3273.3333333333335</v>
+        <v>2170</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B29">
-        <v>11</v>
+        <v>7.3</v>
       </c>
       <c r="C29">
-        <v>3060</v>
+        <v>2250</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B30">
-        <v>6.2</v>
+        <f>16*2/3</f>
+        <v>10.666666666666666</v>
       </c>
       <c r="C30">
-        <v>1890</v>
+        <f>4910*2/3</f>
+        <v>3273.3333333333335</v>
       </c>
       <c r="D30" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C31">
-        <v>3550</v>
+        <v>3060</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -3437,15 +3529,43 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <v>6.2</v>
+      </c>
+      <c r="C32">
+        <v>1890</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>7.3</v>
+      </c>
+      <c r="C33">
+        <v>3550</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
         <v>30</v>
       </c>
-      <c r="B32">
+      <c r="B34">
         <v>6</v>
       </c>
-      <c r="C32">
+      <c r="C34">
         <v>2180</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D34" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Palisades Lakes, Dege Peak from Sunrise Point, and ability for photos to be formatted as panoramas (spanning 2 columns)
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87315C3D-90F9-4BD7-8F5D-3E7BE89B1E86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C799C9-073E-4FF8-AAD4-ACB6F8D13C61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -56,9 +56,6 @@
     <t>easy (but long)</t>
   </si>
   <si>
-    <t>Dege Peak</t>
-  </si>
-  <si>
     <t>easy</t>
   </si>
   <si>
@@ -162,6 +159,15 @@
   </si>
   <si>
     <t>Laughingwater Creek</t>
+  </si>
+  <si>
+    <t>Dege Peak from Sunrise</t>
+  </si>
+  <si>
+    <t>Dege Peak from Sunrise Point</t>
+  </si>
+  <si>
+    <t>Palisades Lakes</t>
   </si>
 </sst>
 </file>
@@ -280,7 +286,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3DA6C52F-0FBF-4F09-A035-A8AE5B2B3209}" type="CELLRANGE">
+                    <a:fld id="{00AE4784-A6DB-4D2D-B16A-30208AC1028A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -314,7 +320,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EED617C4-A2FE-4AC7-B7D6-BD2F585D0481}" type="CELLRANGE">
+                    <a:fld id="{B6C75FF2-ED58-4440-AEA5-9D30C6327469}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -348,7 +354,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{240F9D97-656E-4098-B32B-4F4E6DB36F88}" type="CELLRANGE">
+                    <a:fld id="{71867DC4-A4BA-4F53-99C7-1668A6147944}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -382,7 +388,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{573D7A73-F4D4-436E-BBAB-4DF2480ECF7B}" type="CELLRANGE">
+                    <a:fld id="{81331FA5-E855-498C-92B5-1A2A87E9FFCB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -416,7 +422,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{495CAF82-B345-4682-A40C-3B6B34234098}" type="CELLRANGE">
+                    <a:fld id="{F835D06A-C77B-4A3B-BCAF-D83C9EEBC1DE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -450,7 +456,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42D15F54-7A1B-43A0-8844-97B3D7D71805}" type="CELLRANGE">
+                    <a:fld id="{C7D7C246-C1A7-4FAC-89BE-3EDF2889003A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -484,7 +490,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{80FDA851-178B-4AFA-B56B-67400CD519A0}" type="CELLRANGE">
+                    <a:fld id="{B19A72E9-1F93-4FA4-ADE8-0FD34EBAB0E2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -518,7 +524,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{093B5836-B4DF-42BC-87BE-C58AB3807BC9}" type="CELLRANGE">
+                    <a:fld id="{1C0C80BD-F3AB-4EC1-95E3-F7EF764A1B2C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -552,7 +558,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7AD3330A-7523-43FF-8856-3D5441D222F5}" type="CELLRANGE">
+                    <a:fld id="{BCE27744-A018-4D0C-9130-7867961A2D9D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -586,7 +592,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{72C12DD0-64A6-4387-8A85-1601F0C34DEE}" type="CELLRANGE">
+                    <a:fld id="{DA1CC337-9790-4D9A-95F9-FCBEFA75645A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -620,7 +626,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C678890-ED5F-4BD8-9F9B-A5D3B87E1F76}" type="CELLRANGE">
+                    <a:fld id="{0BF3EFF7-B062-4D86-8DBE-B9DFA2788C8C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -654,7 +660,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5E467967-8036-41BF-A424-B5B142174AB8}" type="CELLRANGE">
+                    <a:fld id="{F4CB5679-E8A5-440F-A8A6-9522904B4A9D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -688,7 +694,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4781FEAD-1DAE-453F-A1E4-42C4C3C91275}" type="CELLRANGE">
+                    <a:fld id="{93F92925-19AC-497B-8ED3-099FB7B0978C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -722,7 +728,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{16C2F8A8-A8CD-4D96-A21B-D58D97E5C9DE}" type="CELLRANGE">
+                    <a:fld id="{876413F7-129B-40AC-BC85-1141DBD0B25B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -756,7 +762,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A1A2318A-6B7A-4435-B282-A9D9711E8C10}" type="CELLRANGE">
+                    <a:fld id="{FFD3C5D1-EBA7-4053-9618-3182BAAF764B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -790,7 +796,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17493855-819C-4B5E-90DD-DFA88236DC6A}" type="CELLRANGE">
+                    <a:fld id="{E509600E-9D80-4C2B-BCDA-341F2E5BECDD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -824,7 +830,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6BF8AA55-1A04-41AB-9622-00DF13A1C3B0}" type="CELLRANGE">
+                    <a:fld id="{429B2F49-1089-43D5-963E-D85FA2512887}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -858,7 +864,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E9C87C1-866E-488D-B4C1-58D452F28DDD}" type="CELLRANGE">
+                    <a:fld id="{5348A3D8-3D19-4060-B038-88CB0432F391}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -892,7 +898,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17FA9EB5-59E3-40D2-A339-BFEB7F2EF335}" type="CELLRANGE">
+                    <a:fld id="{99C111C9-51FA-4461-ABB2-C8CAA05E534C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -926,7 +932,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{563800A8-1CF0-45EE-AD93-2ABF396F6CBB}" type="CELLRANGE">
+                    <a:fld id="{E4550BFE-E3FD-409A-91DB-9BDB9C0EE88E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -960,7 +966,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E37DDA2-EDCD-45E2-9C76-C8769656F6B3}" type="CELLRANGE">
+                    <a:fld id="{31C832E3-1F8E-462F-89CE-F3BA79A5896F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -994,7 +1000,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4166B05D-AEB2-4FBF-8241-E22A91098AA4}" type="CELLRANGE">
+                    <a:fld id="{3E0DE975-952A-43C4-B562-4D52F5A84C94}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1028,7 +1034,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4FCEF040-7EA3-45B2-8700-7FB3951C8B72}" type="CELLRANGE">
+                    <a:fld id="{74DFAFCB-E0D7-4175-97B2-005DA28BADD7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1062,7 +1068,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FCF9F975-67AC-4244-BB48-E0332DBEA8C1}" type="CELLRANGE">
+                    <a:fld id="{34F29501-F3A5-422E-BF55-E775CA8386D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1096,7 +1102,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DBD21376-B8AF-4683-9FFC-4020BC4CCF50}" type="CELLRANGE">
+                    <a:fld id="{1B3B0D87-D90D-421A-9944-FE44B24BA45E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1130,7 +1136,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9A12C44-E431-4673-BDE2-D7137C4478FC}" type="CELLRANGE">
+                    <a:fld id="{F555825B-4451-469B-8DC5-C5CB0A9CB6D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1164,7 +1170,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2EAD3B8C-A403-40E4-B6D6-DB7E35EBCBD6}" type="CELLRANGE">
+                    <a:fld id="{CEFF0B21-53E8-4D80-B751-F39EC45705DC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1198,7 +1204,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{851ECB91-6737-4D43-84AB-CFD22539DD2E}" type="CELLRANGE">
+                    <a:fld id="{137B39C7-E19C-48C1-B329-C5D3E2FAA414}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1232,7 +1238,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40FC86A0-0699-458A-AE9C-4CAFE5CF2CCC}" type="CELLRANGE">
+                    <a:fld id="{2BD43716-4C35-4DFE-BC83-9B8BEFE19D1A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1266,7 +1272,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ACBA423E-0A6C-4816-89EF-3675F14854ED}" type="CELLRANGE">
+                    <a:fld id="{8970C37F-F732-45F9-9CB9-283964B733C7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1300,7 +1306,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6DA7EDE1-078C-4C86-812C-9C694CB3B83D}" type="CELLRANGE">
+                    <a:fld id="{35247972-FD5F-4A09-A4D0-4E93181EEB7D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1334,7 +1340,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{817FA6B5-E02D-4913-AD05-135663CA9DDA}" type="CELLRANGE">
+                    <a:fld id="{29738F20-E26D-48A3-AAFF-4EE6A4002EAA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1368,7 +1374,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{37CA43D6-7FA3-4A6E-A7D2-8ED15932AA1F}" type="CELLRANGE">
+                    <a:fld id="{81F757FE-58CD-487F-8AA4-5B85591600C7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1402,7 +1408,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BA10BD34-9B58-4564-B17C-C13418C733DD}" type="CELLRANGE">
+                    <a:fld id="{326FFD9D-E8A7-4349-98AE-002890CC91F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1426,6 +1432,74 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-0411-4483-8A5E-4A2C7E846C06}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="34"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FBD9927C-D367-4C4B-9451-8B7AF5F92C7C}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-483D-4790-BCFB-31A3BB924CC8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="35"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{E7A2FDCA-FEB6-4654-AAB5-1097288B9558}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-483D-4790-BCFB-31A3BB924CC8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1475,10 +1549,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$35</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
@@ -1498,87 +1572,93 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>7.1</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>9.8000000000000007</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9.6</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>9.1</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>12.2</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>9.75</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>5.4</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>11.9</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1586,10 +1666,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$35</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>2840</c:v>
                 </c:pt>
@@ -1609,87 +1689,93 @@
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>1090</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>3030</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>2880</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>3290</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>2780</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>4800</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>4120</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>3420</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>1450</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>3160</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -1721,25 +1807,25 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>strenuous</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="10">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="12">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="13">
                     <c:v>strenuous</c:v>
@@ -1751,19 +1837,19 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="16">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="18">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="19">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="20">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="21">
                     <c:v>moderate</c:v>
@@ -1772,13 +1858,13 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="26">
                     <c:v>easy</c:v>
@@ -1787,21 +1873,27 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="28">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="29">
-                    <c:v>strenuous</c:v>
-                  </c:pt>
                   <c:pt idx="30">
-                    <c:v>strenuous</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="31">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="32">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="33">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="34">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -2808,10 +2900,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D35" totalsRowShown="0">
-  <autoFilter ref="A1:D35" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D35">
-    <sortCondition ref="A1:A35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D37" totalsRowShown="0">
+  <autoFilter ref="A1:D37" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D37">
+    <sortCondition ref="A1:A37"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -3120,10 +3212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3136,16 +3228,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -3207,7 +3299,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>7.5</v>
@@ -3221,7 +3313,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -3230,32 +3322,32 @@
         <v>1000</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B8">
-        <v>7.1</v>
+        <v>2.9</v>
       </c>
       <c r="C8">
-        <v>3030</v>
+        <v>1090</v>
       </c>
       <c r="D8" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B9">
-        <v>9.8000000000000007</v>
+        <v>7.1</v>
       </c>
       <c r="C9">
-        <v>2880</v>
+        <v>3030</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
@@ -3263,197 +3355,197 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>9.6</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C10">
-        <v>3290</v>
+        <v>2880</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>14</v>
+        <v>9.6</v>
       </c>
       <c r="C11">
-        <v>2780</v>
+        <v>3290</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>9.1</v>
+        <v>14</v>
       </c>
       <c r="C12">
-        <v>1580</v>
+        <v>2780</v>
       </c>
       <c r="D12" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>5.2</v>
+        <v>9.1</v>
       </c>
       <c r="C13">
-        <v>1000</v>
+        <v>1580</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>5.2</v>
       </c>
       <c r="C14">
-        <v>4800</v>
+        <v>1000</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>12.2</v>
+        <v>14</v>
       </c>
       <c r="C15">
-        <v>4120</v>
+        <v>4800</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>12</v>
+        <v>12.2</v>
       </c>
       <c r="C16">
-        <v>3420</v>
+        <v>4120</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <f>19.5/2</f>
-        <v>9.75</v>
+        <v>12</v>
       </c>
       <c r="C17">
-        <f>4400*7/8</f>
-        <v>3850</v>
+        <v>3420</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B18">
-        <v>5.4</v>
+        <f>19.5/2</f>
+        <v>9.75</v>
       </c>
       <c r="C18">
-        <v>1450</v>
+        <f>4400*7/8</f>
+        <v>3850</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="B19">
-        <v>11.9</v>
+        <v>5.4</v>
       </c>
       <c r="C19">
-        <v>3160</v>
+        <v>1450</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B20">
-        <v>11.4</v>
+        <v>11.9</v>
       </c>
       <c r="C20">
-        <v>2550</v>
+        <v>3160</v>
       </c>
       <c r="D20" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21">
-        <v>8.5</v>
+        <v>11.4</v>
       </c>
       <c r="C21">
-        <v>3350</v>
+        <v>2550</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B22">
-        <v>10.4</v>
+        <v>8.5</v>
       </c>
       <c r="C22">
-        <v>1420</v>
+        <v>3350</v>
       </c>
       <c r="D22" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B23">
-        <v>7</v>
+        <v>10.4</v>
       </c>
       <c r="C23">
-        <v>1670</v>
+        <v>1420</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
@@ -3461,13 +3553,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B24">
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="C24">
-        <v>1850</v>
+        <v>1670</v>
       </c>
       <c r="D24" t="s">
         <v>1</v>
@@ -3475,69 +3567,69 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B25">
-        <v>4.8</v>
+        <v>8.1</v>
       </c>
       <c r="C25">
-        <v>1300</v>
+        <v>2400</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B26">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C26">
-        <v>1470</v>
+        <v>1850</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B27">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C27">
-        <v>2000</v>
+        <v>1300</v>
       </c>
       <c r="D27" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B28">
-        <v>2.2000000000000002</v>
+        <v>4.8</v>
       </c>
       <c r="C28">
-        <v>750</v>
+        <v>1470</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B29">
-        <v>11</v>
+        <v>6.9</v>
       </c>
       <c r="C29">
-        <v>2170</v>
+        <v>2000</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
@@ -3545,87 +3637,115 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B30">
-        <v>7.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C30">
-        <v>2250</v>
+        <v>750</v>
       </c>
       <c r="D30" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B31">
-        <f>16*2/3</f>
-        <v>10.666666666666666</v>
+        <v>11</v>
       </c>
       <c r="C31">
-        <f>4910*2/3</f>
-        <v>3273.3333333333335</v>
+        <v>2170</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B32">
-        <v>11</v>
+        <v>7.3</v>
       </c>
       <c r="C32">
-        <v>3060</v>
+        <v>2250</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B33">
-        <v>6.2</v>
+        <f>16*2/3</f>
+        <v>10.666666666666666</v>
       </c>
       <c r="C33">
-        <v>1890</v>
+        <f>4910*2/3</f>
+        <v>3273.3333333333335</v>
       </c>
       <c r="D33" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B34">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C34">
-        <v>3550</v>
+        <v>3060</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B35">
+        <v>6.2</v>
+      </c>
+      <c r="C35">
+        <v>1890</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36">
+        <v>7.3</v>
+      </c>
+      <c r="C36">
+        <v>3550</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37">
         <v>6</v>
       </c>
-      <c r="C35">
+      <c r="C37">
         <v>2180</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D37" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Twin Firs Loop
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E22DD4-F71E-4D2D-9518-C0FF1FED6AF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4826D6BD-E463-4615-85B6-92C6E6165F7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="49">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Northern Loop</t>
+  </si>
+  <si>
+    <t>Twin Firs Loop</t>
   </si>
 </sst>
 </file>
@@ -295,7 +298,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2631CFB6-2D50-48BE-A69F-5A14B18D3E3C}" type="CELLRANGE">
+                    <a:fld id="{4F800E49-4A1A-48B6-BDEC-C55D93C8F46E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -329,7 +332,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9ED3D3B-D3E3-4D25-ACD3-BC40EE4B3C31}" type="CELLRANGE">
+                    <a:fld id="{A97B2886-8405-4822-9989-5610FFBE9328}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -363,7 +366,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E008F73-CEDB-4691-93EB-041358C709A5}" type="CELLRANGE">
+                    <a:fld id="{6C271EC6-BF04-4DF5-9D48-56067B91175B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -397,7 +400,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7348A1D6-E1D4-4EF7-8C59-2E85B7881637}" type="CELLRANGE">
+                    <a:fld id="{7B654CA7-95F5-4CAB-AB18-709076F8EC31}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -431,7 +434,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E657664B-7C5B-470A-869A-29EB37D5E216}" type="CELLRANGE">
+                    <a:fld id="{6AEC647A-28BA-43D9-AE14-DF20337C72C7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -465,7 +468,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{09102301-7FFE-499F-83DA-DF4332AC3C0B}" type="CELLRANGE">
+                    <a:fld id="{E3769732-4AE6-4DF3-89E5-86B7700FF907}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -499,7 +502,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{07D9D0B9-3B69-4198-AB39-DD07E55AF99E}" type="CELLRANGE">
+                    <a:fld id="{A43F16DB-5F29-41AE-B970-9AE7EFBEC564}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -533,7 +536,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{635D1FA6-CA52-4595-B1D5-FC39D464D3FD}" type="CELLRANGE">
+                    <a:fld id="{FFE3A353-4016-481F-ACB9-00BC4AACA01C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -567,7 +570,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C92E9075-ADD6-419E-93EE-EBDAB1089648}" type="CELLRANGE">
+                    <a:fld id="{13D2976B-2B8A-4F39-BCEE-750D8EE9ABDA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -601,7 +604,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B3EBC1F8-9A1A-4C2B-B221-4F70C754508D}" type="CELLRANGE">
+                    <a:fld id="{B868EEEF-83BC-46BF-AD08-D74A84141E9A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -635,7 +638,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97DDF3D8-6F65-4E58-82F3-61883331262B}" type="CELLRANGE">
+                    <a:fld id="{AAB46494-90E5-4846-9D45-C964242EE839}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -669,7 +672,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4532615D-BD39-43FD-98C5-AF1AC99376CE}" type="CELLRANGE">
+                    <a:fld id="{9B40FEB3-A7E3-42C3-ACEB-F50A1C62D7D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -703,7 +706,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B8C1955-4DC8-4BB5-9A27-2A00E48350AB}" type="CELLRANGE">
+                    <a:fld id="{0D77063D-1E3B-4A1D-86C3-F55B260F8055}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -737,7 +740,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{55FF509E-0806-407F-BF83-06E9B2B1D873}" type="CELLRANGE">
+                    <a:fld id="{9B465284-A161-4F62-A9B3-6A6DA20C21A5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -771,7 +774,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F1B6ED4A-CC1F-4425-8DDC-142E2C53EDDA}" type="CELLRANGE">
+                    <a:fld id="{2AD051D1-F18E-420F-B018-A8AA5ED2CFDD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -805,7 +808,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ACCF7F90-6127-4675-9BE4-DCC21D2F8C9B}" type="CELLRANGE">
+                    <a:fld id="{778F39A3-0C85-418B-9FA1-B4D91E85FA74}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -839,7 +842,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A571BE2-1F7B-4E8D-8EBA-949C46BD00D6}" type="CELLRANGE">
+                    <a:fld id="{C60E6525-3C8B-450D-BB7C-27D655BAFBFE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -873,7 +876,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD926859-56B7-4E71-B2BF-28D55CB968C6}" type="CELLRANGE">
+                    <a:fld id="{16D0314B-4367-46BA-8CF2-883D23AE98C0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -907,7 +910,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73EF7E63-6CF2-41FD-81D1-B90AFA40ED87}" type="CELLRANGE">
+                    <a:fld id="{FAC2E5DE-91D6-4508-9FF3-58CA08D2A7E9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -941,7 +944,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{735095E3-68DF-4363-8609-3E9118CF9AEF}" type="CELLRANGE">
+                    <a:fld id="{01DB661A-EE0C-4AEE-BE40-49D2EE1BBB12}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -975,7 +978,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19BFF811-480F-4C73-B42C-AE0E16AC732A}" type="CELLRANGE">
+                    <a:fld id="{048AB159-A95B-4444-8390-5596629B8622}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1009,7 +1012,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C832204-54AD-4DE0-88E6-E228AD1DF598}" type="CELLRANGE">
+                    <a:fld id="{B98156F9-D49D-444F-A2D5-E0D4871C98E5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1043,7 +1046,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AB55AFB6-8389-4111-8ACD-D39DEB5F6DEF}" type="CELLRANGE">
+                    <a:fld id="{BB5CEB4E-747F-4280-B15F-3068083AD5EA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1077,7 +1080,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED681432-7DC8-4BD1-8BEA-BC2D4F693664}" type="CELLRANGE">
+                    <a:fld id="{FF139F4B-1490-4F92-8522-65B4923442B9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1111,7 +1114,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E338DED-26C4-487E-B86E-8B61332E4708}" type="CELLRANGE">
+                    <a:fld id="{F2E5599E-8431-42E7-A79C-FDB1C552DE9A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1145,7 +1148,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0647DF8-DDE4-4CA2-A859-F4244FB57329}" type="CELLRANGE">
+                    <a:fld id="{3C82300E-8FE1-4711-9B3E-C409C8393461}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1179,7 +1182,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD24C022-F8C4-4A07-AE5B-FE8D7B469D25}" type="CELLRANGE">
+                    <a:fld id="{1726B677-52A0-40FE-93A1-F60EA9874069}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1213,7 +1216,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C739A60-7C64-4516-8D0B-A81A2E60B285}" type="CELLRANGE">
+                    <a:fld id="{79F1D2EE-A3F7-43E7-BE4E-3A3B43900A78}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1247,7 +1250,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D990057D-F389-401E-AB85-A2D38164230B}" type="CELLRANGE">
+                    <a:fld id="{EF3B5976-DF93-4673-9FCA-BFC3AB2F49FE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1281,7 +1284,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95EE0751-A4E1-4DDD-A3A0-9ADDF4616635}" type="CELLRANGE">
+                    <a:fld id="{15ADBFA0-35C6-4376-B5AD-7B3246C1CA8A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1315,7 +1318,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0BD9B39E-0659-4160-9884-C4987D01146A}" type="CELLRANGE">
+                    <a:fld id="{02E9D6E0-AAE4-44F1-8F20-2CF7B2E0A2FC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1349,7 +1352,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B7FEA02D-DE53-4203-80BC-6D410E4A8777}" type="CELLRANGE">
+                    <a:fld id="{B9D04058-9B5C-404B-A654-C6618D68539F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1383,7 +1386,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ECC2627C-06E3-4F77-89F1-7D312F63DFC7}" type="CELLRANGE">
+                    <a:fld id="{FE7EDCC6-E9DC-433D-9CF4-67CA8F253504}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1417,7 +1420,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{923919B8-C684-4442-B2BF-5CC00609B31F}" type="CELLRANGE">
+                    <a:fld id="{726154F4-1E50-4500-92CA-DC54EE5E7BE6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1451,7 +1454,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A950E643-78FE-4EF0-8916-BB591836D05F}" type="CELLRANGE">
+                    <a:fld id="{914DFCFD-8DA9-4D72-96C3-18615A3C492F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1485,7 +1488,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{428C800A-FACC-476F-B4E5-B45D3AFE05D8}" type="CELLRANGE">
+                    <a:fld id="{959B42FD-A953-494B-AC3B-530ABCC8D41C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1519,7 +1522,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4400C457-811C-4BCB-9BC2-C9C8BD901B7F}" type="CELLRANGE">
+                    <a:fld id="{51FF5FE9-C6E1-42FB-A712-874183341EDC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1553,7 +1556,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{487F58D1-57F5-47BB-89B9-97BB8E687A5D}" type="CELLRANGE">
+                    <a:fld id="{FE0AAD35-7341-43B9-8714-19FF0AA870BD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1587,7 +1590,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{61348E15-AB73-4883-B9A9-42A483D518A7}" type="CELLRANGE">
+                    <a:fld id="{D1E6A440-0B5A-4AFD-8CDB-1B1CBD3E1133}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1611,6 +1614,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-1245-4918-BD35-DEEB15AD6DC2}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="39"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{F1D13691-C5E9-4C10-BADD-76E910DA2657}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-79A6-46B5-8B68-531C343FA2C7}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1660,10 +1697,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$40</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
@@ -1776,9 +1813,12 @@
                   <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="37">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1786,10 +1826,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$40</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>2840</c:v>
                 </c:pt>
@@ -1902,9 +1942,12 @@
                   <c:v>1890</c:v>
                 </c:pt>
                 <c:pt idx="37">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2029,9 +2072,12 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="37">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="38">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="38">
+                  <c:pt idx="39">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3038,10 +3084,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D40" totalsRowShown="0">
-  <autoFilter ref="A1:D40" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D40">
-    <sortCondition ref="A1:A40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D41" totalsRowShown="0">
+  <autoFilter ref="A1:D41" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D41">
+    <sortCondition ref="A1:A41"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -3350,10 +3396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3903,29 +3949,43 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B39">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C39">
-        <v>3550</v>
+        <v>180</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40">
+        <v>7.3</v>
+      </c>
+      <c r="C40">
+        <v>3550</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>29</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>6</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <v>2180</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Stevens Creek Trail
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4826D6BD-E463-4615-85B6-92C6E6165F7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0132AC15-4EC7-4288-9151-622638E2400C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Twin Firs Loop</t>
+  </si>
+  <si>
+    <t>Stevens Creek Trail</t>
   </si>
 </sst>
 </file>
@@ -298,7 +301,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F800E49-4A1A-48B6-BDEC-C55D93C8F46E}" type="CELLRANGE">
+                    <a:fld id="{49261E61-DD06-425D-8D4E-361543869884}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -332,7 +335,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A97B2886-8405-4822-9989-5610FFBE9328}" type="CELLRANGE">
+                    <a:fld id="{E6205EDF-F063-470A-A6FF-241F23A46908}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -366,7 +369,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C271EC6-BF04-4DF5-9D48-56067B91175B}" type="CELLRANGE">
+                    <a:fld id="{610A363A-29CF-41E3-9452-501E1E25F618}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -400,7 +403,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7B654CA7-95F5-4CAB-AB18-709076F8EC31}" type="CELLRANGE">
+                    <a:fld id="{C6969C19-4B08-4EC4-9479-CD6D8A634434}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -434,7 +437,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6AEC647A-28BA-43D9-AE14-DF20337C72C7}" type="CELLRANGE">
+                    <a:fld id="{4081BE36-8BC3-4FC8-93C4-2C29B5E1627D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -468,7 +471,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E3769732-4AE6-4DF3-89E5-86B7700FF907}" type="CELLRANGE">
+                    <a:fld id="{BB166B83-8093-4596-A7B5-57FFC5BE6670}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -502,7 +505,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A43F16DB-5F29-41AE-B970-9AE7EFBEC564}" type="CELLRANGE">
+                    <a:fld id="{877D1025-DB93-46DF-9942-C5ABDD588FC2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -536,7 +539,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FFE3A353-4016-481F-ACB9-00BC4AACA01C}" type="CELLRANGE">
+                    <a:fld id="{E2BD4D47-8AD9-42C3-9739-2D31916FB1A4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -570,7 +573,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{13D2976B-2B8A-4F39-BCEE-750D8EE9ABDA}" type="CELLRANGE">
+                    <a:fld id="{359B35F6-077D-4E7C-BFDF-F6CCC54F413A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -604,7 +607,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B868EEEF-83BC-46BF-AD08-D74A84141E9A}" type="CELLRANGE">
+                    <a:fld id="{3D04850A-77DA-4B83-9068-98EFA2C5CA81}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -638,7 +641,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AAB46494-90E5-4846-9D45-C964242EE839}" type="CELLRANGE">
+                    <a:fld id="{D963F6EF-CE8A-4141-8C7A-C088C49ECF7D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -672,7 +675,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B40FEB3-A7E3-42C3-ACEB-F50A1C62D7D7}" type="CELLRANGE">
+                    <a:fld id="{7DF74EF8-6F7B-47D7-B16F-54B6410D53B3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -706,7 +709,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D77063D-1E3B-4A1D-86C3-F55B260F8055}" type="CELLRANGE">
+                    <a:fld id="{E2CF8E9E-E3D4-4E90-9125-97949464175F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -740,7 +743,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B465284-A161-4F62-A9B3-6A6DA20C21A5}" type="CELLRANGE">
+                    <a:fld id="{A44B5F3D-2E00-414F-8169-58035CD39EF2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -774,7 +777,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2AD051D1-F18E-420F-B018-A8AA5ED2CFDD}" type="CELLRANGE">
+                    <a:fld id="{507469D2-88BB-4B24-B07E-C1445FF3D868}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -808,7 +811,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{778F39A3-0C85-418B-9FA1-B4D91E85FA74}" type="CELLRANGE">
+                    <a:fld id="{A26849F0-7E0C-43F2-B1C4-3EC520CBD81E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -842,7 +845,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C60E6525-3C8B-450D-BB7C-27D655BAFBFE}" type="CELLRANGE">
+                    <a:fld id="{66613EEC-2EAF-4B46-9793-16B111EE9D85}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -876,7 +879,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{16D0314B-4367-46BA-8CF2-883D23AE98C0}" type="CELLRANGE">
+                    <a:fld id="{1E8F37C3-59C1-45F6-9775-0234699E2284}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -910,7 +913,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FAC2E5DE-91D6-4508-9FF3-58CA08D2A7E9}" type="CELLRANGE">
+                    <a:fld id="{8D23BCDB-997E-468E-8809-8E48F5D35D0F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -944,7 +947,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{01DB661A-EE0C-4AEE-BE40-49D2EE1BBB12}" type="CELLRANGE">
+                    <a:fld id="{ECCFA6E0-F1DC-4B39-B385-2362A2B30B17}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -978,7 +981,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{048AB159-A95B-4444-8390-5596629B8622}" type="CELLRANGE">
+                    <a:fld id="{EA48E336-5A55-45BA-925F-ED3BF72EC2C9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1012,7 +1015,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B98156F9-D49D-444F-A2D5-E0D4871C98E5}" type="CELLRANGE">
+                    <a:fld id="{2C07D5F6-C07F-457A-8BB1-29987788271F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1046,7 +1049,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB5CEB4E-747F-4280-B15F-3068083AD5EA}" type="CELLRANGE">
+                    <a:fld id="{8C3166EA-8566-4EEB-B69C-3D8DA71E902E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1080,7 +1083,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF139F4B-1490-4F92-8522-65B4923442B9}" type="CELLRANGE">
+                    <a:fld id="{A952C7E0-435D-47AD-9AB6-F0E452FA7E5E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1114,7 +1117,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F2E5599E-8431-42E7-A79C-FDB1C552DE9A}" type="CELLRANGE">
+                    <a:fld id="{2BD7A6F1-13B7-475E-B604-6B716966C746}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1148,7 +1151,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C82300E-8FE1-4711-9B3E-C409C8393461}" type="CELLRANGE">
+                    <a:fld id="{45E66FCA-2445-48C2-86FB-4C8B5C9D5207}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1182,7 +1185,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1726B677-52A0-40FE-93A1-F60EA9874069}" type="CELLRANGE">
+                    <a:fld id="{279064C6-D271-42BC-9E08-97238F679D2C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1216,7 +1219,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79F1D2EE-A3F7-43E7-BE4E-3A3B43900A78}" type="CELLRANGE">
+                    <a:fld id="{514BED04-F1AC-4E3A-B156-DC949A5B50D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1250,7 +1253,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EF3B5976-DF93-4673-9FCA-BFC3AB2F49FE}" type="CELLRANGE">
+                    <a:fld id="{2FF7599C-9874-42C3-A5A4-487D3E104834}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1284,7 +1287,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{15ADBFA0-35C6-4376-B5AD-7B3246C1CA8A}" type="CELLRANGE">
+                    <a:fld id="{360C6483-3DE9-4C58-B87E-3AA72BEA8A06}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1318,7 +1321,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02E9D6E0-AAE4-44F1-8F20-2CF7B2E0A2FC}" type="CELLRANGE">
+                    <a:fld id="{13D4AB98-B78E-41F5-8332-6B58D76594FC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1352,7 +1355,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B9D04058-9B5C-404B-A654-C6618D68539F}" type="CELLRANGE">
+                    <a:fld id="{E0E92445-F412-4D23-93F9-006D61B7ACA8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1386,7 +1389,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FE7EDCC6-E9DC-433D-9CF4-67CA8F253504}" type="CELLRANGE">
+                    <a:fld id="{AC6CFB3C-07F5-4CB7-BFF5-EDC6B0A64F88}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1420,7 +1423,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{726154F4-1E50-4500-92CA-DC54EE5E7BE6}" type="CELLRANGE">
+                    <a:fld id="{7C6FC564-BB14-432B-BAE3-D19D1263E77A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1454,7 +1457,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{914DFCFD-8DA9-4D72-96C3-18615A3C492F}" type="CELLRANGE">
+                    <a:fld id="{94461FA1-8775-49AA-8FF6-90476933F89E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1488,7 +1491,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{959B42FD-A953-494B-AC3B-530ABCC8D41C}" type="CELLRANGE">
+                    <a:fld id="{3C434FEB-C216-4F15-8C43-CBF7710BB89F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1522,7 +1525,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{51FF5FE9-C6E1-42FB-A712-874183341EDC}" type="CELLRANGE">
+                    <a:fld id="{EBF6FD96-F692-4962-838E-9026518DAE8C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1556,7 +1559,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FE0AAD35-7341-43B9-8714-19FF0AA870BD}" type="CELLRANGE">
+                    <a:fld id="{BB827584-A829-4CE3-83F4-4A6B5100AE5A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1590,7 +1593,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1E6A440-0B5A-4AFD-8CDB-1B1CBD3E1133}" type="CELLRANGE">
+                    <a:fld id="{CD713143-6361-475F-B526-D873A6A6C76C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1624,7 +1627,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F1D13691-C5E9-4C10-BADD-76E910DA2657}" type="CELLRANGE">
+                    <a:fld id="{D5979947-10D7-456F-B57E-B6CC999C3501}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1648,6 +1651,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-79A6-46B5-8B68-531C343FA2C7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="40"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{09A74C92-4BA8-43FE-BA1E-953A90090176}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-6D6C-4C05-9E73-4F8D75C24EF1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1697,10 +1734,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$41</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
@@ -1807,18 +1844,21 @@
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="35">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1826,10 +1866,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$41</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>2840</c:v>
                 </c:pt>
@@ -1936,18 +1976,21 @@
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
                 <c:pt idx="35">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2066,18 +2109,21 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="35">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="36">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="36">
+                  <c:pt idx="37">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="37">
+                  <c:pt idx="38">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="38">
+                  <c:pt idx="39">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="39">
+                  <c:pt idx="40">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3084,10 +3130,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D41" totalsRowShown="0">
-  <autoFilter ref="A1:D41" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D41">
-    <sortCondition ref="A1:A41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D42" totalsRowShown="0">
+  <autoFilter ref="A1:D42" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D42">
+    <sortCondition ref="A1:A42"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -3396,10 +3442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3921,71 +3967,85 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B37">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C37">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D37" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B38">
-        <v>6.2</v>
+        <v>11</v>
       </c>
       <c r="C38">
-        <v>1890</v>
+        <v>3060</v>
       </c>
       <c r="D38" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B39">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C39">
-        <v>180</v>
+        <v>1890</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B40">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C40">
-        <v>3550</v>
+        <v>180</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41">
+        <v>7.3</v>
+      </c>
+      <c r="C41">
+        <v>3550</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
         <v>29</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>6</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>2180</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
In-progress Fremont Lookout entry
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0132AC15-4EC7-4288-9151-622638E2400C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1D99FE-639E-4696-B360-F4ACA0A26FCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>Stevens Creek Trail</t>
+  </si>
+  <si>
+    <t>Fremont Lookout</t>
   </si>
 </sst>
 </file>
@@ -301,7 +304,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{49261E61-DD06-425D-8D4E-361543869884}" type="CELLRANGE">
+                    <a:fld id="{AE438C3D-7BCC-43D4-A26A-BEC1A71419FF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -335,7 +338,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E6205EDF-F063-470A-A6FF-241F23A46908}" type="CELLRANGE">
+                    <a:fld id="{1CAF5EF8-5F00-4083-8D8C-50CCDEC110E2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -369,7 +372,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{610A363A-29CF-41E3-9452-501E1E25F618}" type="CELLRANGE">
+                    <a:fld id="{15CE121E-0B6E-4A47-A24C-B4E42CB8463F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -403,7 +406,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C6969C19-4B08-4EC4-9479-CD6D8A634434}" type="CELLRANGE">
+                    <a:fld id="{F851D60D-EBA3-483E-BA2E-EAC690655A67}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -437,7 +440,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4081BE36-8BC3-4FC8-93C4-2C29B5E1627D}" type="CELLRANGE">
+                    <a:fld id="{87EC9BAD-65A8-42C8-9F89-8B18D4DC25A3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -471,7 +474,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB166B83-8093-4596-A7B5-57FFC5BE6670}" type="CELLRANGE">
+                    <a:fld id="{BB6EC943-A315-4714-8E60-9FBFAF663C28}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -505,7 +508,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{877D1025-DB93-46DF-9942-C5ABDD588FC2}" type="CELLRANGE">
+                    <a:fld id="{197C760C-DE78-4059-9C78-4EF7AC00B078}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -539,7 +542,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E2BD4D47-8AD9-42C3-9739-2D31916FB1A4}" type="CELLRANGE">
+                    <a:fld id="{59147674-1A7A-42EB-BB9D-97EABA95AB6B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -573,7 +576,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{359B35F6-077D-4E7C-BFDF-F6CCC54F413A}" type="CELLRANGE">
+                    <a:fld id="{56454CD5-2088-4776-B21B-38235C00E1F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -607,7 +610,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D04850A-77DA-4B83-9068-98EFA2C5CA81}" type="CELLRANGE">
+                    <a:fld id="{3AA9FB8A-B918-4970-8BC0-FB08F1FE62C6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -641,7 +644,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D963F6EF-CE8A-4141-8C7A-C088C49ECF7D}" type="CELLRANGE">
+                    <a:fld id="{883CD8C6-6CE9-4872-A9EB-F05FF4F451A6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -675,7 +678,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7DF74EF8-6F7B-47D7-B16F-54B6410D53B3}" type="CELLRANGE">
+                    <a:fld id="{507A93DF-CE09-498E-82D5-C8F290EA4BE0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -709,7 +712,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E2CF8E9E-E3D4-4E90-9125-97949464175F}" type="CELLRANGE">
+                    <a:fld id="{CFCCD554-7B6D-43D4-947F-05B86BCFD748}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -743,7 +746,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A44B5F3D-2E00-414F-8169-58035CD39EF2}" type="CELLRANGE">
+                    <a:fld id="{635E47CB-44DF-4871-B7E1-3EE51382CD5F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -777,7 +780,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{507469D2-88BB-4B24-B07E-C1445FF3D868}" type="CELLRANGE">
+                    <a:fld id="{CE3E41F0-4552-4F0A-A954-DB408930E69C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -811,7 +814,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A26849F0-7E0C-43F2-B1C4-3EC520CBD81E}" type="CELLRANGE">
+                    <a:fld id="{C1003110-5629-48D5-A833-EE39568E2A0C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -845,7 +848,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{66613EEC-2EAF-4B46-9793-16B111EE9D85}" type="CELLRANGE">
+                    <a:fld id="{8EB3F62E-7E29-4985-9912-2789348CAC54}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -879,7 +882,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1E8F37C3-59C1-45F6-9775-0234699E2284}" type="CELLRANGE">
+                    <a:fld id="{426624FE-0CC1-4761-822A-3C6A50FCE12C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -913,7 +916,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8D23BCDB-997E-468E-8809-8E48F5D35D0F}" type="CELLRANGE">
+                    <a:fld id="{84015CE6-637C-49B3-9572-D6376EC749C4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -947,7 +950,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ECCFA6E0-F1DC-4B39-B385-2362A2B30B17}" type="CELLRANGE">
+                    <a:fld id="{69A95B73-A0C0-4BF6-96AC-07E8627B7DAE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -981,7 +984,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA48E336-5A55-45BA-925F-ED3BF72EC2C9}" type="CELLRANGE">
+                    <a:fld id="{99C72DB6-7475-4348-B78C-632365E7C4AF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1015,7 +1018,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C07D5F6-C07F-457A-8BB1-29987788271F}" type="CELLRANGE">
+                    <a:fld id="{0F5497B0-1E9A-4128-8143-AF0150AD66E6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1049,7 +1052,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C3166EA-8566-4EEB-B69C-3D8DA71E902E}" type="CELLRANGE">
+                    <a:fld id="{CAC7A1E8-39DA-4991-B16E-36699E395A86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1083,7 +1086,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A952C7E0-435D-47AD-9AB6-F0E452FA7E5E}" type="CELLRANGE">
+                    <a:fld id="{36FD799E-BB1B-4FAA-A581-CAAF40AEE2CE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1117,7 +1120,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2BD7A6F1-13B7-475E-B604-6B716966C746}" type="CELLRANGE">
+                    <a:fld id="{47F11B6A-8E37-475C-9B5B-BDE6FAA52B7F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1151,7 +1154,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{45E66FCA-2445-48C2-86FB-4C8B5C9D5207}" type="CELLRANGE">
+                    <a:fld id="{D7AE58E8-7542-4561-8FFB-CB8D595C9832}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1185,7 +1188,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{279064C6-D271-42BC-9E08-97238F679D2C}" type="CELLRANGE">
+                    <a:fld id="{07D5ACAA-05A7-4692-AC7C-0C0C137A4279}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1219,7 +1222,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{514BED04-F1AC-4E3A-B156-DC949A5B50D8}" type="CELLRANGE">
+                    <a:fld id="{A4AD331E-1F60-47AD-A4C1-B27D556DD206}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1253,7 +1256,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2FF7599C-9874-42C3-A5A4-487D3E104834}" type="CELLRANGE">
+                    <a:fld id="{F5C51CCE-4138-4978-AF9D-C06822BBD5AA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1287,7 +1290,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{360C6483-3DE9-4C58-B87E-3AA72BEA8A06}" type="CELLRANGE">
+                    <a:fld id="{FD386BE5-95F7-42D3-B0AD-1AE054DF9102}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1321,7 +1324,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{13D4AB98-B78E-41F5-8332-6B58D76594FC}" type="CELLRANGE">
+                    <a:fld id="{3F426E1D-65DA-4D42-B54F-6B98F19EC8EF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1355,7 +1358,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E0E92445-F412-4D23-93F9-006D61B7ACA8}" type="CELLRANGE">
+                    <a:fld id="{D1281689-DFE2-4820-9133-75DA673AE9B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1389,7 +1392,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AC6CFB3C-07F5-4CB7-BFF5-EDC6B0A64F88}" type="CELLRANGE">
+                    <a:fld id="{E70C52C3-6D38-46CD-A239-CA91371EC27C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1423,7 +1426,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7C6FC564-BB14-432B-BAE3-D19D1263E77A}" type="CELLRANGE">
+                    <a:fld id="{DF290658-69E3-4852-A605-1A2A0891B2BC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1457,7 +1460,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{94461FA1-8775-49AA-8FF6-90476933F89E}" type="CELLRANGE">
+                    <a:fld id="{BE3BE9BC-1F82-43B8-8E6B-2A0206F244C8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1491,7 +1494,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C434FEB-C216-4F15-8C43-CBF7710BB89F}" type="CELLRANGE">
+                    <a:fld id="{B61D6244-F9C2-4742-A3F3-F061B87DD5A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1525,7 +1528,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EBF6FD96-F692-4962-838E-9026518DAE8C}" type="CELLRANGE">
+                    <a:fld id="{AA1E2FFD-6BF7-4AAE-AB10-F9126CC11A95}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1559,7 +1562,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB827584-A829-4CE3-83F4-4A6B5100AE5A}" type="CELLRANGE">
+                    <a:fld id="{BFED981D-A165-4A94-AAD1-5DFFE455D4D1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1593,7 +1596,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD713143-6361-475F-B526-D873A6A6C76C}" type="CELLRANGE">
+                    <a:fld id="{1DF90154-5B86-455E-942B-7C7A36BB6C94}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1627,7 +1630,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D5979947-10D7-456F-B57E-B6CC999C3501}" type="CELLRANGE">
+                    <a:fld id="{E68A6A86-B79B-4E82-8DB8-734443DDA4BB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1661,7 +1664,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{09A74C92-4BA8-43FE-BA1E-953A90090176}" type="CELLRANGE">
+                    <a:fld id="{1F580175-D418-4C6C-914E-5793176B876A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1685,6 +1688,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-6D6C-4C05-9E73-4F8D75C24EF1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="41"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B64E9F71-D753-4E44-94DD-3C22AF62BC6C}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-C3D7-430F-BB2C-382742E5871A}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1734,10 +1771,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$42</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
@@ -1763,102 +1800,105 @@
                   <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>9.8000000000000007</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>9.6</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11.6</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>9.1</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>12.2</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>9.75</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>5.4</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>11.9</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1866,10 +1906,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$42</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>2840</c:v>
                 </c:pt>
@@ -1895,102 +1935,105 @@
                   <c:v>3030</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>1540</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2880</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>3290</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>2660</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>2780</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>4800</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>4120</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>3420</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>1450</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>3160</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2031,22 +2074,22 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="11">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="12">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="13">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="14">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="15">
                     <c:v>strenuous</c:v>
@@ -2058,25 +2101,25 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="18">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="20">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="21">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="22">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="23">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="23">
+                  <c:pt idx="24">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="25">
                     <c:v>moderate</c:v>
@@ -2085,45 +2128,48 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="27">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="28">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="29">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="30">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="30">
+                  <c:pt idx="31">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="31">
+                  <c:pt idx="32">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="32">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="33">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="34">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="36">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="36">
+                  <c:pt idx="37">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="37">
+                  <c:pt idx="38">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="38">
+                  <c:pt idx="39">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="39">
+                  <c:pt idx="40">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="40">
+                  <c:pt idx="41">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3031,13 +3077,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>114310</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>42863</xdr:rowOff>
+      <xdr:rowOff>138123</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3052,7 +3098,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6238875" y="3819525"/>
+          <a:off x="6238875" y="3914785"/>
           <a:ext cx="5686425" cy="1652588"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3130,10 +3176,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D42" totalsRowShown="0">
-  <autoFilter ref="A1:D42" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D42">
-    <sortCondition ref="A1:A42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D43" totalsRowShown="0">
+  <autoFilter ref="A1:D43" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D43">
+    <sortCondition ref="A1:A43"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -3442,10 +3488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3585,13 +3631,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B10">
-        <v>9.8000000000000007</v>
+        <v>6.5</v>
       </c>
       <c r="C10">
-        <v>2880</v>
+        <v>1540</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
@@ -3599,97 +3645,97 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <v>9.6</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C11">
-        <v>3290</v>
+        <v>2880</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="B12">
-        <v>11.6</v>
+        <v>9.6</v>
       </c>
       <c r="C12">
-        <v>2660</v>
+        <v>3290</v>
       </c>
       <c r="D12" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B13">
-        <v>14</v>
+        <v>11.6</v>
       </c>
       <c r="C13">
-        <v>2780</v>
+        <v>2660</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>9.1</v>
+        <v>14</v>
       </c>
       <c r="C14">
-        <v>1580</v>
+        <v>2780</v>
       </c>
       <c r="D14" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>5.2</v>
+        <v>9.1</v>
       </c>
       <c r="C15">
-        <v>1000</v>
+        <v>1580</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>5.2</v>
       </c>
       <c r="C16">
-        <v>4800</v>
+        <v>1000</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
         <v>14</v>
       </c>
-      <c r="B17">
-        <v>12.2</v>
-      </c>
       <c r="C17">
-        <v>4120</v>
+        <v>4800</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
@@ -3697,13 +3743,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18">
-        <v>12</v>
+        <v>12.2</v>
       </c>
       <c r="C18">
-        <v>3420</v>
+        <v>4120</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
@@ -3711,127 +3757,127 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>3420</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <f>19.5/2</f>
         <v>9.75</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <f>4400*7/8</f>
         <v>3850</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20">
-        <v>5.4</v>
-      </c>
-      <c r="C20">
-        <v>1450</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B21">
-        <v>11.9</v>
+        <v>5.4</v>
       </c>
       <c r="C21">
-        <v>3160</v>
+        <v>1450</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B22">
-        <v>11.4</v>
+        <v>11.9</v>
       </c>
       <c r="C22">
-        <v>2550</v>
+        <v>3160</v>
       </c>
       <c r="D22" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23">
-        <v>8.5</v>
+        <v>11.4</v>
       </c>
       <c r="C23">
-        <v>3350</v>
+        <v>2550</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24">
-        <v>10.4</v>
+        <v>8.5</v>
       </c>
       <c r="C24">
-        <v>1420</v>
+        <v>3350</v>
       </c>
       <c r="D24" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B25">
-        <v>13.6</v>
+        <v>10.4</v>
       </c>
       <c r="C25">
-        <v>3930</v>
+        <v>1420</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>13.6</v>
       </c>
       <c r="C26">
-        <v>1670</v>
+        <v>3930</v>
       </c>
       <c r="D26" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B27">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="C27">
-        <v>2400</v>
+        <v>1670</v>
       </c>
       <c r="D27" t="s">
         <v>1</v>
@@ -3839,13 +3885,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B28">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C28">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D28" t="s">
         <v>1</v>
@@ -3853,27 +3899,27 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B29">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C29">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B30">
         <v>4.8</v>
       </c>
       <c r="C30">
-        <v>1470</v>
+        <v>1300</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -3881,69 +3927,69 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C31">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D31" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B32">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C32">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B33">
-        <v>2.2000000000000002</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C33">
-        <v>750</v>
+        <v>3490</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B34">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C34">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D34" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B35">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C35">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D35" t="s">
         <v>1</v>
@@ -3951,101 +3997,115 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36">
+        <v>7.3</v>
+      </c>
+      <c r="C36">
+        <v>2250</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>25</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37">
-        <v>1.2</v>
-      </c>
-      <c r="C37">
-        <v>500</v>
-      </c>
-      <c r="D37" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B38">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C38">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D38" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B39">
-        <v>6.2</v>
+        <v>11</v>
       </c>
       <c r="C39">
-        <v>1890</v>
+        <v>3060</v>
       </c>
       <c r="D39" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B40">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C40">
-        <v>180</v>
+        <v>1890</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B41">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C41">
-        <v>3550</v>
+        <v>180</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42">
+        <v>7.3</v>
+      </c>
+      <c r="C42">
+        <v>3550</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>29</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <v>6</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <v>2180</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add a separate entry for Myrtle Falls
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1D99FE-639E-4696-B360-F4ACA0A26FCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C934E4F0-6505-4626-892F-D2F5E335C424}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Fremont Lookout</t>
+  </si>
+  <si>
+    <t>Myrtle Falls</t>
   </si>
 </sst>
 </file>
@@ -304,7 +307,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE438C3D-7BCC-43D4-A26A-BEC1A71419FF}" type="CELLRANGE">
+                    <a:fld id="{DE468E81-039D-40CF-8D01-3EC1EF05CE2A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -338,7 +341,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1CAF5EF8-5F00-4083-8D8C-50CCDEC110E2}" type="CELLRANGE">
+                    <a:fld id="{88315B4D-C813-4C96-A1A7-E2CF2EECCE51}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -372,7 +375,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{15CE121E-0B6E-4A47-A24C-B4E42CB8463F}" type="CELLRANGE">
+                    <a:fld id="{F61C5A35-0ED2-4526-8909-B8F87E8A9AF5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -406,7 +409,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F851D60D-EBA3-483E-BA2E-EAC690655A67}" type="CELLRANGE">
+                    <a:fld id="{293D2272-BFA2-48E6-9B38-F601F57B29AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -440,7 +443,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{87EC9BAD-65A8-42C8-9F89-8B18D4DC25A3}" type="CELLRANGE">
+                    <a:fld id="{99FA28A5-22CA-4239-B757-9FB48F207E68}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -474,7 +477,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB6EC943-A315-4714-8E60-9FBFAF663C28}" type="CELLRANGE">
+                    <a:fld id="{9940006B-C455-4177-B562-358DA5D18D0E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -508,7 +511,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{197C760C-DE78-4059-9C78-4EF7AC00B078}" type="CELLRANGE">
+                    <a:fld id="{422B67CC-5FFA-4FA0-A3BD-46C5189EEFBD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -542,7 +545,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{59147674-1A7A-42EB-BB9D-97EABA95AB6B}" type="CELLRANGE">
+                    <a:fld id="{66E8E31D-7F3E-4D8B-8A6F-ADB617B6343C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -576,7 +579,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56454CD5-2088-4776-B21B-38235C00E1F8}" type="CELLRANGE">
+                    <a:fld id="{9D46333D-54F4-47AA-BF08-97300074354D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -610,7 +613,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3AA9FB8A-B918-4970-8BC0-FB08F1FE62C6}" type="CELLRANGE">
+                    <a:fld id="{7F35FC87-C942-4A6C-BB24-BE3EFBCCEA01}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -644,7 +647,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{883CD8C6-6CE9-4872-A9EB-F05FF4F451A6}" type="CELLRANGE">
+                    <a:fld id="{C84C8D42-FA65-49E0-8E7D-337326A998D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -678,7 +681,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{507A93DF-CE09-498E-82D5-C8F290EA4BE0}" type="CELLRANGE">
+                    <a:fld id="{99B9321F-4EA7-47A0-BEDE-BDD786C082A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -712,7 +715,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CFCCD554-7B6D-43D4-947F-05B86BCFD748}" type="CELLRANGE">
+                    <a:fld id="{AFC83C5A-155D-4C24-91F5-F9B069ED8EE9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -746,7 +749,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{635E47CB-44DF-4871-B7E1-3EE51382CD5F}" type="CELLRANGE">
+                    <a:fld id="{68B7234E-1CDD-4B56-B31D-B9D23F8AF44E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -780,7 +783,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE3E41F0-4552-4F0A-A954-DB408930E69C}" type="CELLRANGE">
+                    <a:fld id="{E08D717D-7415-4571-9949-93F817004507}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -814,7 +817,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C1003110-5629-48D5-A833-EE39568E2A0C}" type="CELLRANGE">
+                    <a:fld id="{0F4ED99D-D674-4C90-9B54-3A60FD842E1C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -848,7 +851,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8EB3F62E-7E29-4985-9912-2789348CAC54}" type="CELLRANGE">
+                    <a:fld id="{02E2BA11-98E2-4B9E-96C3-07303E746482}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -882,7 +885,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{426624FE-0CC1-4761-822A-3C6A50FCE12C}" type="CELLRANGE">
+                    <a:fld id="{3445D921-C215-4C10-8E59-AA15E38A0737}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -916,7 +919,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{84015CE6-637C-49B3-9572-D6376EC749C4}" type="CELLRANGE">
+                    <a:fld id="{20066F60-737C-4B64-BBE3-E0A10B37B7C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -950,7 +953,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69A95B73-A0C0-4BF6-96AC-07E8627B7DAE}" type="CELLRANGE">
+                    <a:fld id="{6EC1BF55-79E7-4795-8AF5-D2962295C315}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -984,7 +987,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{99C72DB6-7475-4348-B78C-632365E7C4AF}" type="CELLRANGE">
+                    <a:fld id="{63E13A7D-998C-4038-9456-431CE755FFCB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1018,7 +1021,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F5497B0-1E9A-4128-8143-AF0150AD66E6}" type="CELLRANGE">
+                    <a:fld id="{8F693580-FC0D-4B7D-8D88-266734C6DE46}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1052,7 +1055,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CAC7A1E8-39DA-4991-B16E-36699E395A86}" type="CELLRANGE">
+                    <a:fld id="{22D89AAA-BF01-4C4D-A2D1-F6CB340E49F3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1086,7 +1089,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36FD799E-BB1B-4FAA-A581-CAAF40AEE2CE}" type="CELLRANGE">
+                    <a:fld id="{1E6E09B0-805A-4641-8515-852B1245D244}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1120,7 +1123,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47F11B6A-8E37-475C-9B5B-BDE6FAA52B7F}" type="CELLRANGE">
+                    <a:fld id="{DB339E7B-42BC-45F5-91AB-3365CFD33C73}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1154,7 +1157,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D7AE58E8-7542-4561-8FFB-CB8D595C9832}" type="CELLRANGE">
+                    <a:fld id="{88B80F5A-216B-45FC-BAB6-E1FDE601B45F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1188,7 +1191,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{07D5ACAA-05A7-4692-AC7C-0C0C137A4279}" type="CELLRANGE">
+                    <a:fld id="{916A27ED-B2E4-447A-8B3E-4A665D78E43F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1222,7 +1225,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A4AD331E-1F60-47AD-A4C1-B27D556DD206}" type="CELLRANGE">
+                    <a:fld id="{E1BDF8ED-EBA1-4304-A7FD-EFCC56B7A4A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1256,7 +1259,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5C51CCE-4138-4978-AF9D-C06822BBD5AA}" type="CELLRANGE">
+                    <a:fld id="{C9D2F329-E90B-4582-94F3-F9EBA67D7FDD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1290,7 +1293,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD386BE5-95F7-42D3-B0AD-1AE054DF9102}" type="CELLRANGE">
+                    <a:fld id="{156D7F3A-6988-4072-BB91-2A846530D3DA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1324,7 +1327,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F426E1D-65DA-4D42-B54F-6B98F19EC8EF}" type="CELLRANGE">
+                    <a:fld id="{2A9DAD3B-59B4-4939-BB14-6E5B98057470}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1358,7 +1361,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1281689-DFE2-4820-9133-75DA673AE9B2}" type="CELLRANGE">
+                    <a:fld id="{3F37B00B-8D50-43AE-BDB8-3D92DA3D0D2C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1392,7 +1395,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E70C52C3-6D38-46CD-A239-CA91371EC27C}" type="CELLRANGE">
+                    <a:fld id="{684C6435-CB1B-424A-B257-5B099DF3B61E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1426,7 +1429,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF290658-69E3-4852-A605-1A2A0891B2BC}" type="CELLRANGE">
+                    <a:fld id="{DB956C56-1DAE-4559-A9C3-8063DEBC6CF8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1460,7 +1463,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BE3BE9BC-1F82-43B8-8E6B-2A0206F244C8}" type="CELLRANGE">
+                    <a:fld id="{8A68B26B-B66F-45B1-AEC6-7850D9C468C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1494,7 +1497,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B61D6244-F9C2-4742-A3F3-F061B87DD5A7}" type="CELLRANGE">
+                    <a:fld id="{295CE7BF-49BD-4F9D-A479-0CF1BA5D9306}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1528,7 +1531,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AA1E2FFD-6BF7-4AAE-AB10-F9126CC11A95}" type="CELLRANGE">
+                    <a:fld id="{822E1F09-FC81-4B80-9784-C6F88BDB04E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1562,7 +1565,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BFED981D-A165-4A94-AAD1-5DFFE455D4D1}" type="CELLRANGE">
+                    <a:fld id="{5FA66BB6-82C5-454F-9FF2-710CE74F2718}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1596,7 +1599,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1DF90154-5B86-455E-942B-7C7A36BB6C94}" type="CELLRANGE">
+                    <a:fld id="{E1B0160C-0711-4A59-B1DF-CDA8981B1A11}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1630,7 +1633,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E68A6A86-B79B-4E82-8DB8-734443DDA4BB}" type="CELLRANGE">
+                    <a:fld id="{E1E8C7B3-4484-4F18-807D-5809D940D6D5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1664,7 +1667,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1F580175-D418-4C6C-914E-5793176B876A}" type="CELLRANGE">
+                    <a:fld id="{DD6F69BF-901F-4FFB-BA5A-F466E1E0042C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1698,7 +1701,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B64E9F71-D753-4E44-94DD-3C22AF62BC6C}" type="CELLRANGE">
+                    <a:fld id="{730AF1C7-081B-414F-8652-42A8EA41FCBF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1722,6 +1725,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-C3D7-430F-BB2C-382742E5871A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="42"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{BB28578C-D9D9-4E50-A5AD-D7BB49AC2113}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-37EF-46BA-9580-BC03701ED96F}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1771,10 +1808,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$43</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
@@ -1848,57 +1885,60 @@
                   <c:v>10.4</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1906,10 +1946,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$43</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>2840</c:v>
                 </c:pt>
@@ -1983,57 +2023,60 @@
                   <c:v>1420</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2119,10 +2162,10 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="24">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="26">
                     <c:v>moderate</c:v>
@@ -2131,45 +2174,48 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="28">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="29">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="30">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="31">
+                  <c:pt idx="32">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="32">
+                  <c:pt idx="33">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="33">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="34">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="35">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="36">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="36">
+                  <c:pt idx="37">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="37">
+                  <c:pt idx="38">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="38">
+                  <c:pt idx="39">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="39">
+                  <c:pt idx="40">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="40">
+                  <c:pt idx="41">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="41">
+                  <c:pt idx="42">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3176,10 +3222,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D43" totalsRowShown="0">
-  <autoFilter ref="A1:D43" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D43">
-    <sortCondition ref="A1:A43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D44" totalsRowShown="0">
+  <autoFilter ref="A1:D44" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D44">
+    <sortCondition ref="A1:A44"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -3488,10 +3534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3857,41 +3903,41 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B26">
-        <v>13.6</v>
+        <v>0.9</v>
       </c>
       <c r="C26">
-        <v>3930</v>
+        <v>200</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B27">
-        <v>7</v>
+        <v>13.6</v>
       </c>
       <c r="C27">
-        <v>1670</v>
+        <v>3930</v>
       </c>
       <c r="D27" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B28">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="C28">
-        <v>2400</v>
+        <v>1670</v>
       </c>
       <c r="D28" t="s">
         <v>1</v>
@@ -3899,13 +3945,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B29">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C29">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
@@ -3913,27 +3959,27 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C30">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31">
         <v>4.8</v>
       </c>
       <c r="C31">
-        <v>1470</v>
+        <v>1300</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -3941,69 +3987,69 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C32">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D32" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B33">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C33">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B34">
-        <v>2.2000000000000002</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C34">
-        <v>750</v>
+        <v>3490</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B35">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C35">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D35" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B36">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C36">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D36" t="s">
         <v>1</v>
@@ -4011,101 +4057,115 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37">
+        <v>7.3</v>
+      </c>
+      <c r="C37">
+        <v>2250</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
         <v>25</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>49</v>
-      </c>
-      <c r="B38">
-        <v>1.2</v>
-      </c>
-      <c r="C38">
-        <v>500</v>
-      </c>
-      <c r="D38" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B39">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C39">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B40">
-        <v>6.2</v>
+        <v>11</v>
       </c>
       <c r="C40">
-        <v>1890</v>
+        <v>3060</v>
       </c>
       <c r="D40" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B41">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C41">
-        <v>180</v>
+        <v>1890</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B42">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C42">
-        <v>3550</v>
+        <v>180</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43">
+        <v>7.3</v>
+      </c>
+      <c r="C43">
+        <v>3550</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
         <v>29</v>
       </c>
-      <c r="B43">
+      <c r="B44">
         <v>6</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <v>2180</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Narada Falls Loop
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C624BF0-C9FC-4193-8475-461AF81BBBB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BBAB76-6831-40E1-ADAA-2D0F632A9865}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>Moraine Trail</t>
+  </si>
+  <si>
+    <t>Narada Falls Loop</t>
   </si>
 </sst>
 </file>
@@ -313,7 +316,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F38C2118-3340-4318-9BB4-44FB9BCF37CF}" type="CELLRANGE">
+                    <a:fld id="{407F6F11-A865-46E3-9862-6F4C1B0C55B1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -347,7 +350,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A19D1C36-2281-4383-8ACD-64184C16D70D}" type="CELLRANGE">
+                    <a:fld id="{EAF0634F-DBDC-400D-BF98-537918347B21}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -381,7 +384,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{94779537-F974-4504-8C93-8499EB29EE4D}" type="CELLRANGE">
+                    <a:fld id="{802D65AC-30FF-4525-BB10-F9295BE122CE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -415,7 +418,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA85A19A-A6B5-4A2B-B8A5-587BF2A6A23B}" type="CELLRANGE">
+                    <a:fld id="{AD3CFE76-0CEC-4B13-972F-40FA17DCF896}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -449,7 +452,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F343DD2E-B613-4681-85FE-FC8D8796D22A}" type="CELLRANGE">
+                    <a:fld id="{8BD6D477-EAC9-48AA-A782-87BC16B67C85}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -483,7 +486,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{020F5D38-4D17-42CE-8C26-3DE1B066CAFA}" type="CELLRANGE">
+                    <a:fld id="{61C59047-4695-4204-AD91-3D101454BBDD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -517,7 +520,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E4CD6E4-DEC7-4B21-8BF0-26E8A1029411}" type="CELLRANGE">
+                    <a:fld id="{4F4B9167-9F99-4C90-BA10-1DFC603ABA68}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -551,7 +554,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{963C12AC-38FB-42E5-B788-BF1DD7A14640}" type="CELLRANGE">
+                    <a:fld id="{ADA32F91-471D-4865-97A7-89C6F8440F32}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -585,7 +588,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{09BB59E5-2B1E-4278-8A55-39F805A4F561}" type="CELLRANGE">
+                    <a:fld id="{4D1A7621-718F-46C5-9D0B-060119A82F45}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -619,7 +622,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79C559D4-0192-46B4-991D-814E49F6E52A}" type="CELLRANGE">
+                    <a:fld id="{93CF7C01-7B01-4C98-8A44-4CB59B61C28E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -653,7 +656,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD81C256-D964-4227-AFA8-FB322EB2FD1C}" type="CELLRANGE">
+                    <a:fld id="{9E8BDC7B-E91C-4317-918F-BBA55980B513}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -687,7 +690,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C7BA8A3-877D-4C10-A6A7-917B21CFE529}" type="CELLRANGE">
+                    <a:fld id="{6A7187EE-E545-4152-9955-B6E024781544}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -721,7 +724,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D6E2A48-FAAF-424C-9D3C-6F554C221C7C}" type="CELLRANGE">
+                    <a:fld id="{EDC10205-4460-4AA7-8F66-4D49F3423D8F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -755,7 +758,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{84256984-AAE6-46D2-A278-D7F18BC63A05}" type="CELLRANGE">
+                    <a:fld id="{1E5A7F68-9D8E-4AC5-9654-18A44E0E2F1D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -789,7 +792,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{01CE9A5A-84A9-4F01-AD3F-E850B3E2D3FC}" type="CELLRANGE">
+                    <a:fld id="{B4DDD1C5-B16E-4743-8187-22BBB11A1F7A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -823,7 +826,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97BBF09B-ED6F-4B72-9015-B4464D14A7AD}" type="CELLRANGE">
+                    <a:fld id="{B749E4CC-525D-4862-9EF9-486A510190BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -857,7 +860,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{651496DE-D651-4014-ABDA-B96D1AB02024}" type="CELLRANGE">
+                    <a:fld id="{039748DD-ABA4-4D5A-B757-27B8C50773AF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -891,7 +894,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{902F8861-FC4F-48D0-AB32-554EABF44C9F}" type="CELLRANGE">
+                    <a:fld id="{7577AFFD-5E7A-49B8-81D0-C9E8642FB111}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -925,7 +928,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06A78EEB-D70E-468D-B744-6A5E075E87ED}" type="CELLRANGE">
+                    <a:fld id="{F3C7BFB3-DAB1-4F64-844E-C9E399ED35E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -959,7 +962,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36C924CD-6230-4DD4-9B92-66D9F27FBB3A}" type="CELLRANGE">
+                    <a:fld id="{02BEFC15-7C7D-4179-9EA3-3C6B61522A20}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -993,7 +996,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE38E89F-9424-4764-8BA6-C108F44BD709}" type="CELLRANGE">
+                    <a:fld id="{0471C185-5D40-44BA-A726-4C2EE813DEDC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1027,7 +1030,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C4CC10BE-9FB1-4AD7-A014-82D4A6CF2829}" type="CELLRANGE">
+                    <a:fld id="{9C5541EA-E946-4075-9932-9C0B7B845FD9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1061,7 +1064,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{98D8D890-1758-46F7-B7EE-47C92C98B046}" type="CELLRANGE">
+                    <a:fld id="{2EFF1D19-F324-428E-B6F7-9ACF6787D721}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1095,7 +1098,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D38E440-3017-4420-A386-D99BC4A83C42}" type="CELLRANGE">
+                    <a:fld id="{BE1112C0-9AEB-40D8-B1F3-BBA8251B70D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1129,7 +1132,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A5754BC-34D3-4FD4-86DA-6ACEEF4922C0}" type="CELLRANGE">
+                    <a:fld id="{DD9C43D3-2403-44A9-99F5-498A18117D0F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1163,7 +1166,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4B47072F-415E-460C-A610-E9E50D911D37}" type="CELLRANGE">
+                    <a:fld id="{0F3FB0EE-E8DD-464B-8E0A-D54DF6AA9E2C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1197,7 +1200,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F4394C6-65CA-46D2-87B3-83DEA90A3912}" type="CELLRANGE">
+                    <a:fld id="{C9BF6460-7F15-4642-B01C-67B017B31C1F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1231,7 +1234,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D051464-C7A3-4A6E-8051-9FAF3E07B418}" type="CELLRANGE">
+                    <a:fld id="{B1851EC6-5D53-4E86-8D9F-20B8AEFC04B9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1265,7 +1268,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B354CB48-37C0-4711-84FD-31506C745707}" type="CELLRANGE">
+                    <a:fld id="{532AAB65-DD51-4F4F-9C60-CA896A155BE7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1299,7 +1302,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9505E4C9-ABC8-49E3-A98C-2BB0DBCD169D}" type="CELLRANGE">
+                    <a:fld id="{96A062EC-7F5F-40C2-A521-B67D5DC16DAA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1333,7 +1336,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97026E00-6407-46C9-895B-3CAA5AEB79D4}" type="CELLRANGE">
+                    <a:fld id="{E66C8CCA-E7A1-44E3-AFE5-D507187E23F2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1367,7 +1370,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E048427-121D-4373-A2D5-F38491AC4C4B}" type="CELLRANGE">
+                    <a:fld id="{030227F9-AD6B-4A22-A8FE-2A2D799D4FD9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1401,7 +1404,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5022A05C-CF5D-4023-8970-F7D62C977931}" type="CELLRANGE">
+                    <a:fld id="{8EB5C38D-2187-4F6D-BE7F-E2BA033ED757}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1435,7 +1438,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73C29E93-D7B5-4C17-8182-A361A7DC85BC}" type="CELLRANGE">
+                    <a:fld id="{A8727C2E-D054-4E4A-8C4D-3F3D4FBA313C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1469,7 +1472,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B1716CF-766B-43BB-BBDB-525695FA78B8}" type="CELLRANGE">
+                    <a:fld id="{DD5BE07C-3152-41CD-8D7B-720D6911094D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1503,7 +1506,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{74FE8E5A-9C0D-409D-A45F-1541ECD20CCD}" type="CELLRANGE">
+                    <a:fld id="{9F9DB7E6-5445-4A20-ABDA-8A7AA6E508EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1537,7 +1540,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D059D71C-9688-467A-9576-B328D93448E1}" type="CELLRANGE">
+                    <a:fld id="{C51C551E-09C5-4F3D-9BEF-7111F06215A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1571,7 +1574,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B587C73-4FB4-4B77-AEEA-321C88228541}" type="CELLRANGE">
+                    <a:fld id="{5906254F-3817-4ED5-A647-F5B001B5596C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1605,7 +1608,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56430DC0-5AA6-44E6-9C7B-D5862A6706BF}" type="CELLRANGE">
+                    <a:fld id="{E128B0D2-1E27-493E-AD5D-A90A20E99182}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1639,7 +1642,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{49C03E70-60FE-49E8-9F97-DD0CA9162849}" type="CELLRANGE">
+                    <a:fld id="{08F51735-227F-415D-A723-8A74A28F1266}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1673,7 +1676,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60BED1E4-2437-4E5B-A0A6-D75DA5009D23}" type="CELLRANGE">
+                    <a:fld id="{29835523-99F6-4F4C-A7C5-84E2BEAD6DCC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1707,7 +1710,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC39B36B-732E-48EB-B5E9-357173A3A827}" type="CELLRANGE">
+                    <a:fld id="{B1F51EAC-EB2E-4F46-A2D9-F3CFED8ACAE9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1741,7 +1744,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B03038D5-A651-4C74-B955-CC52AF7D9292}" type="CELLRANGE">
+                    <a:fld id="{A577F68F-B584-416D-94C6-BC2B3F3FC2E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1775,7 +1778,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{843C30C1-A81B-4713-B9F2-311C91BFF45C}" type="CELLRANGE">
+                    <a:fld id="{ACAAF75B-47DF-4629-BE01-2165D57980AE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1809,7 +1812,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{199FDDC9-13A8-4965-9B98-99C5B19B4694}" type="CELLRANGE">
+                    <a:fld id="{96B8A2A4-0E6E-4347-ADF8-8FA131F4FE2E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1833,6 +1836,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-57F0-4FD3-B511-197259A54F0E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="45"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7FA522A7-03FA-4DD2-BB22-4F7B4C75BF87}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-2FB8-4950-B2D1-FCD2790725B3}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1882,10 +1919,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$46</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
@@ -1965,60 +2002,63 @@
                   <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="33">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2026,10 +2066,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$46</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>2840</c:v>
                 </c:pt>
@@ -2109,60 +2149,63 @@
                   <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>1260</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2257,10 +2300,10 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="27">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="29">
                     <c:v>moderate</c:v>
@@ -2269,45 +2312,48 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="31">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="32">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="33">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="34">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="34">
+                  <c:pt idx="35">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="36">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="36">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="37">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="38">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="39">
+                  <c:pt idx="40">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="40">
+                  <c:pt idx="41">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="41">
+                  <c:pt idx="42">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="42">
+                  <c:pt idx="43">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="43">
+                  <c:pt idx="44">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="44">
+                  <c:pt idx="45">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3314,10 +3360,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D46" totalsRowShown="0">
-  <autoFilter ref="A1:D46" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D46">
-    <sortCondition ref="A1:A46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D47" totalsRowShown="0">
+  <autoFilter ref="A1:D47" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D47">
+    <sortCondition ref="A1:A47"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -3626,10 +3672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4023,13 +4069,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B28">
-        <v>1.4</v>
+        <v>4.8</v>
       </c>
       <c r="C28">
-        <v>375</v>
+        <v>1260</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -4037,41 +4083,41 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B29">
-        <v>13.6</v>
+        <v>1.4</v>
       </c>
       <c r="C29">
-        <v>3930</v>
+        <v>375</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B30">
-        <v>7</v>
+        <v>13.6</v>
       </c>
       <c r="C30">
-        <v>1670</v>
+        <v>3930</v>
       </c>
       <c r="D30" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B31">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="C31">
-        <v>2400</v>
+        <v>1670</v>
       </c>
       <c r="D31" t="s">
         <v>1</v>
@@ -4079,13 +4125,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B32">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C32">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D32" t="s">
         <v>1</v>
@@ -4093,27 +4139,27 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C33">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34">
         <v>4.8</v>
       </c>
       <c r="C34">
-        <v>1470</v>
+        <v>1300</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
@@ -4121,69 +4167,69 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C35">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D35" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B36">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C36">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B37">
-        <v>2.2000000000000002</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C37">
-        <v>750</v>
+        <v>3490</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B38">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C38">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D38" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B39">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C39">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D39" t="s">
         <v>1</v>
@@ -4191,101 +4237,115 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40">
+        <v>7.3</v>
+      </c>
+      <c r="C40">
+        <v>2250</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>25</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>49</v>
-      </c>
-      <c r="B41">
-        <v>1.2</v>
-      </c>
-      <c r="C41">
-        <v>500</v>
-      </c>
-      <c r="D41" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B42">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C42">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B43">
-        <v>6.2</v>
+        <v>11</v>
       </c>
       <c r="C43">
-        <v>1890</v>
+        <v>3060</v>
       </c>
       <c r="D43" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B44">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C44">
-        <v>180</v>
+        <v>1890</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B45">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C45">
-        <v>3550</v>
+        <v>180</v>
       </c>
       <c r="D45" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46">
+        <v>7.3</v>
+      </c>
+      <c r="C46">
+        <v>3550</v>
+      </c>
+      <c r="D46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
         <v>29</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <v>6</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <v>2180</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add North Puyallup River
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BBAB76-6831-40E1-ADAA-2D0F632A9865}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58430F7B-76B5-41B7-8506-3D3D7258FA55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Narada Falls Loop</t>
+  </si>
+  <si>
+    <t>Westside Road to North Puyallup</t>
   </si>
 </sst>
 </file>
@@ -316,7 +319,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{407F6F11-A865-46E3-9862-6F4C1B0C55B1}" type="CELLRANGE">
+                    <a:fld id="{5C75E656-154C-4561-A21F-E00DCD1EFF80}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -350,7 +353,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EAF0634F-DBDC-400D-BF98-537918347B21}" type="CELLRANGE">
+                    <a:fld id="{7368B84E-5CA2-4D18-9DEE-40F2BB5A9E26}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -384,7 +387,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{802D65AC-30FF-4525-BB10-F9295BE122CE}" type="CELLRANGE">
+                    <a:fld id="{577D542A-D522-4411-AC1F-A683F04B1034}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -418,7 +421,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD3CFE76-0CEC-4B13-972F-40FA17DCF896}" type="CELLRANGE">
+                    <a:fld id="{EC4A2F2C-848F-47F1-A7ED-AD8AA1446AF4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -452,7 +455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8BD6D477-EAC9-48AA-A782-87BC16B67C85}" type="CELLRANGE">
+                    <a:fld id="{1DE00B65-B614-4AC7-A7BE-536CADA668D9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -486,7 +489,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{61C59047-4695-4204-AD91-3D101454BBDD}" type="CELLRANGE">
+                    <a:fld id="{F15982A1-EEFF-4348-90C8-16AA6CEBDFC3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -520,7 +523,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F4B9167-9F99-4C90-BA10-1DFC603ABA68}" type="CELLRANGE">
+                    <a:fld id="{273E9638-6C1F-4DA4-A2D4-B18BEBD9E610}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -554,7 +557,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ADA32F91-471D-4865-97A7-89C6F8440F32}" type="CELLRANGE">
+                    <a:fld id="{D2F7F8FE-F582-4F1F-BD63-786FA0F9F3F3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -588,7 +591,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D1A7621-718F-46C5-9D0B-060119A82F45}" type="CELLRANGE">
+                    <a:fld id="{D00CBC90-5309-416D-9B6B-DDD15CB3B105}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -622,7 +625,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{93CF7C01-7B01-4C98-8A44-4CB59B61C28E}" type="CELLRANGE">
+                    <a:fld id="{32F63458-67F6-4DC2-8966-40DA51E07E82}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -656,7 +659,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E8BDC7B-E91C-4317-918F-BBA55980B513}" type="CELLRANGE">
+                    <a:fld id="{E9181B82-3275-42D9-AD5A-88451EDB0871}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -690,7 +693,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6A7187EE-E545-4152-9955-B6E024781544}" type="CELLRANGE">
+                    <a:fld id="{E81CE2ED-53E2-431F-8829-3662E1EE2EA6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -724,7 +727,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EDC10205-4460-4AA7-8F66-4D49F3423D8F}" type="CELLRANGE">
+                    <a:fld id="{86693298-E020-488F-BFB1-9C71E60FD9C0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -758,7 +761,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1E5A7F68-9D8E-4AC5-9654-18A44E0E2F1D}" type="CELLRANGE">
+                    <a:fld id="{3D8A69CE-5198-4F2E-96D0-A8CDEDE6DC51}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -792,7 +795,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B4DDD1C5-B16E-4743-8187-22BBB11A1F7A}" type="CELLRANGE">
+                    <a:fld id="{2E333CFE-8E9C-4DF6-82C3-0257A6053543}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -826,7 +829,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B749E4CC-525D-4862-9EF9-486A510190BA}" type="CELLRANGE">
+                    <a:fld id="{C454DAA8-DACE-48E5-A316-33E645E1EA87}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -860,7 +863,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{039748DD-ABA4-4D5A-B757-27B8C50773AF}" type="CELLRANGE">
+                    <a:fld id="{39CA3282-CA02-458B-84A9-FD47C89CC125}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -894,7 +897,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7577AFFD-5E7A-49B8-81D0-C9E8642FB111}" type="CELLRANGE">
+                    <a:fld id="{006731DF-5CCB-482B-9801-DBEACD49234F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -928,7 +931,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3C7BFB3-DAB1-4F64-844E-C9E399ED35E8}" type="CELLRANGE">
+                    <a:fld id="{32A3DD83-9E86-4FD8-B78E-FC39878ACD73}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -962,7 +965,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02BEFC15-7C7D-4179-9EA3-3C6B61522A20}" type="CELLRANGE">
+                    <a:fld id="{CB176E0F-8FEC-4DFD-BE23-4FE89AFAF9F0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -996,7 +999,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0471C185-5D40-44BA-A726-4C2EE813DEDC}" type="CELLRANGE">
+                    <a:fld id="{79671C4B-FC74-4435-B719-CD2C90777837}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1030,7 +1033,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C5541EA-E946-4075-9932-9C0B7B845FD9}" type="CELLRANGE">
+                    <a:fld id="{514BBCD7-DB80-42E5-97AD-2E5884ABCC72}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1064,7 +1067,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2EFF1D19-F324-428E-B6F7-9ACF6787D721}" type="CELLRANGE">
+                    <a:fld id="{2AF2C81E-6276-4682-8A20-32133C48907A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1098,7 +1101,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BE1112C0-9AEB-40D8-B1F3-BBA8251B70D0}" type="CELLRANGE">
+                    <a:fld id="{7E3245BE-106D-4517-A5BE-3C9BBAB57595}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1132,7 +1135,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD9C43D3-2403-44A9-99F5-498A18117D0F}" type="CELLRANGE">
+                    <a:fld id="{6B992660-7A43-41C4-A3AF-D1D27441D972}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1166,7 +1169,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F3FB0EE-E8DD-464B-8E0A-D54DF6AA9E2C}" type="CELLRANGE">
+                    <a:fld id="{6DB5FBE0-7AAC-4A50-8939-91DB52BBD5C9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1200,7 +1203,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C9BF6460-7F15-4642-B01C-67B017B31C1F}" type="CELLRANGE">
+                    <a:fld id="{75977432-C09A-40D5-B92F-08ECDFE0FEEC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1234,7 +1237,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B1851EC6-5D53-4E86-8D9F-20B8AEFC04B9}" type="CELLRANGE">
+                    <a:fld id="{B3589E52-70DA-4B89-96E8-D04A3864E4FE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1268,7 +1271,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{532AAB65-DD51-4F4F-9C60-CA896A155BE7}" type="CELLRANGE">
+                    <a:fld id="{89EF1700-1EC6-4ED2-AADF-3CC910768305}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1302,7 +1305,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96A062EC-7F5F-40C2-A521-B67D5DC16DAA}" type="CELLRANGE">
+                    <a:fld id="{451C6A2E-7DAA-45F7-8DB6-5F7CBF72DC5C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1336,7 +1339,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E66C8CCA-E7A1-44E3-AFE5-D507187E23F2}" type="CELLRANGE">
+                    <a:fld id="{F6120E8C-84F1-4731-B278-19F05352DF27}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1370,7 +1373,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{030227F9-AD6B-4A22-A8FE-2A2D799D4FD9}" type="CELLRANGE">
+                    <a:fld id="{CAF333E1-D0DD-4E1B-9AE1-5BD73B6E6268}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1404,7 +1407,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8EB5C38D-2187-4F6D-BE7F-E2BA033ED757}" type="CELLRANGE">
+                    <a:fld id="{94AFF5CB-B7EF-4FCC-B19A-E19C35A86CE9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1438,7 +1441,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A8727C2E-D054-4E4A-8C4D-3F3D4FBA313C}" type="CELLRANGE">
+                    <a:fld id="{C1C42968-052D-4DDB-94B3-C13F726FF765}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1472,7 +1475,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD5BE07C-3152-41CD-8D7B-720D6911094D}" type="CELLRANGE">
+                    <a:fld id="{08E2AE1E-6C64-412C-A0A6-A09673EDCF42}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1506,7 +1509,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F9DB7E6-5445-4A20-ABDA-8A7AA6E508EB}" type="CELLRANGE">
+                    <a:fld id="{BA1F0082-C1B1-4E1A-9F53-C9E9821D55EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1540,7 +1543,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C51C551E-09C5-4F3D-9BEF-7111F06215A1}" type="CELLRANGE">
+                    <a:fld id="{A9A55A09-8446-46BF-B708-965463702694}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1574,7 +1577,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5906254F-3817-4ED5-A647-F5B001B5596C}" type="CELLRANGE">
+                    <a:fld id="{B6D1ABF9-1619-4984-AB78-BC54F6F0D162}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1608,7 +1611,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E128B0D2-1E27-493E-AD5D-A90A20E99182}" type="CELLRANGE">
+                    <a:fld id="{26F6861D-DCB6-4E8F-9050-5DE042CFA364}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1642,7 +1645,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{08F51735-227F-415D-A723-8A74A28F1266}" type="CELLRANGE">
+                    <a:fld id="{92CE3DE1-C2E0-4F83-BB86-D7F77AB9E38E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1676,7 +1679,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29835523-99F6-4F4C-A7C5-84E2BEAD6DCC}" type="CELLRANGE">
+                    <a:fld id="{4B7C0D96-06DB-486A-90C8-5949B95C63CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1710,7 +1713,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B1F51EAC-EB2E-4F46-A2D9-F3CFED8ACAE9}" type="CELLRANGE">
+                    <a:fld id="{8759C1C7-5249-458F-BDAA-E42F934B74EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1744,7 +1747,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A577F68F-B584-416D-94C6-BC2B3F3FC2E8}" type="CELLRANGE">
+                    <a:fld id="{DB90C7C5-9E1A-439E-A966-0E091A7CA391}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1778,7 +1781,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ACAAF75B-47DF-4629-BE01-2165D57980AE}" type="CELLRANGE">
+                    <a:fld id="{E879AC4B-A99F-44DF-B31C-6560EFEBA9A9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1812,7 +1815,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96B8A2A4-0E6E-4347-ADF8-8FA131F4FE2E}" type="CELLRANGE">
+                    <a:fld id="{3379FA92-35F2-4A30-A395-EC96ADFEF765}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1846,7 +1849,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7FA522A7-03FA-4DD2-BB22-4F7B4C75BF87}" type="CELLRANGE">
+                    <a:fld id="{1C2744F0-EC66-4B2D-BD94-813491C66A81}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1870,6 +1873,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-2FB8-4950-B2D1-FCD2790725B3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="46"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{02690BBC-6FF5-410F-A148-FFA883CF2B9C}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-6C2A-44F4-BD2F-56C82796355C}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1919,10 +1956,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$47</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
@@ -2059,6 +2096,9 @@
                   <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>11.25</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2066,10 +2106,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$47</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>2840</c:v>
                 </c:pt>
@@ -2206,6 +2246,9 @@
                   <c:v>3550</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2354,6 +2397,9 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="45">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="46">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3360,10 +3406,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D47" totalsRowShown="0">
-  <autoFilter ref="A1:D47" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D47">
-    <sortCondition ref="A1:A47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D48" totalsRowShown="0">
+  <autoFilter ref="A1:D48" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D48">
+    <sortCondition ref="A1:A48"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -3672,10 +3718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4337,15 +4383,30 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47">
+        <f>22.5/2</f>
+        <v>11.25</v>
+      </c>
+      <c r="C47">
+        <v>3800</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
         <v>29</v>
       </c>
-      <c r="B47">
+      <c r="B48">
         <v>6</v>
       </c>
-      <c r="C47">
+      <c r="C48">
         <v>2180</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Grand Park via Lake Eleanor
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58430F7B-76B5-41B7-8506-3D3D7258FA55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72F1ECA-E15F-429C-A1A8-337BD22E4247}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hike Difficulties" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Westside Road to North Puyallup</t>
+  </si>
+  <si>
+    <t>Grand Park via Lake Eleanor</t>
   </si>
 </sst>
 </file>
@@ -319,7 +322,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C75E656-154C-4561-A21F-E00DCD1EFF80}" type="CELLRANGE">
+                    <a:fld id="{38967F7C-7CD1-4345-81E1-C060ADE654DE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -353,7 +356,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7368B84E-5CA2-4D18-9DEE-40F2BB5A9E26}" type="CELLRANGE">
+                    <a:fld id="{3370CB3A-A0C8-4C07-8B42-E326AB5EE42A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -387,7 +390,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{577D542A-D522-4411-AC1F-A683F04B1034}" type="CELLRANGE">
+                    <a:fld id="{1F5331C9-D310-418E-B885-16EA6E6076C7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -421,7 +424,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC4A2F2C-848F-47F1-A7ED-AD8AA1446AF4}" type="CELLRANGE">
+                    <a:fld id="{59E9EE57-375E-4A41-B472-0506B5A6C143}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -455,7 +458,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1DE00B65-B614-4AC7-A7BE-536CADA668D9}" type="CELLRANGE">
+                    <a:fld id="{D384827B-1F10-47FA-8291-E6C2BF70865A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -489,7 +492,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F15982A1-EEFF-4348-90C8-16AA6CEBDFC3}" type="CELLRANGE">
+                    <a:fld id="{91E336E8-A250-425A-8190-EF839E936349}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -523,7 +526,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{273E9638-6C1F-4DA4-A2D4-B18BEBD9E610}" type="CELLRANGE">
+                    <a:fld id="{CFE7AB7E-6D14-48EE-B126-CF8AC3439D73}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -557,7 +560,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D2F7F8FE-F582-4F1F-BD63-786FA0F9F3F3}" type="CELLRANGE">
+                    <a:fld id="{92D89996-ED09-4E69-AFB6-D7B52AEE532F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -591,7 +594,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D00CBC90-5309-416D-9B6B-DDD15CB3B105}" type="CELLRANGE">
+                    <a:fld id="{3B2FA857-7987-4776-AD23-2E2A47D8AA02}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -625,7 +628,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32F63458-67F6-4DC2-8966-40DA51E07E82}" type="CELLRANGE">
+                    <a:fld id="{47F5C88F-7552-43A1-86BA-97E57799E7A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -659,7 +662,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9181B82-3275-42D9-AD5A-88451EDB0871}" type="CELLRANGE">
+                    <a:fld id="{9C550331-22BE-49B6-9FD4-9CB4936A98FB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -693,7 +696,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E81CE2ED-53E2-431F-8829-3662E1EE2EA6}" type="CELLRANGE">
+                    <a:fld id="{A4EA0DF2-AE6D-40FE-B121-8060314F4E5B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -727,7 +730,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{86693298-E020-488F-BFB1-9C71E60FD9C0}" type="CELLRANGE">
+                    <a:fld id="{9E765F21-E715-4892-922B-058F2F8C6A49}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -761,7 +764,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D8A69CE-5198-4F2E-96D0-A8CDEDE6DC51}" type="CELLRANGE">
+                    <a:fld id="{9BC69042-B95D-4B4F-968D-21067D5FC528}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -795,7 +798,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E333CFE-8E9C-4DF6-82C3-0257A6053543}" type="CELLRANGE">
+                    <a:fld id="{23B61035-39C9-4327-BFA6-FB8414AA1FBD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -829,7 +832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C454DAA8-DACE-48E5-A316-33E645E1EA87}" type="CELLRANGE">
+                    <a:fld id="{AFFA33DA-B67E-42D3-897B-23B78C741865}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -863,7 +866,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{39CA3282-CA02-458B-84A9-FD47C89CC125}" type="CELLRANGE">
+                    <a:fld id="{F60D8CE9-C9A2-464C-A967-84533339344D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -897,7 +900,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{006731DF-5CCB-482B-9801-DBEACD49234F}" type="CELLRANGE">
+                    <a:fld id="{D8688F76-C131-42A2-98EA-A2041E5F7AC3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -931,7 +934,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32A3DD83-9E86-4FD8-B78E-FC39878ACD73}" type="CELLRANGE">
+                    <a:fld id="{6FBC29A0-45B5-4283-AC98-B04C80916641}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -965,7 +968,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB176E0F-8FEC-4DFD-BE23-4FE89AFAF9F0}" type="CELLRANGE">
+                    <a:fld id="{8B4CDA36-A094-4ED0-8C09-471974E8C601}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -999,7 +1002,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79671C4B-FC74-4435-B719-CD2C90777837}" type="CELLRANGE">
+                    <a:fld id="{D27CE684-7C95-4FBC-AAF8-0610F6D999A2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1033,7 +1036,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{514BBCD7-DB80-42E5-97AD-2E5884ABCC72}" type="CELLRANGE">
+                    <a:fld id="{5EFCCA2F-7C9E-4E74-81BA-1D006E123B8F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1067,7 +1070,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2AF2C81E-6276-4682-8A20-32133C48907A}" type="CELLRANGE">
+                    <a:fld id="{FED3606D-B193-4E93-B078-057E18DB2E11}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1101,7 +1104,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E3245BE-106D-4517-A5BE-3C9BBAB57595}" type="CELLRANGE">
+                    <a:fld id="{7A1385B3-031B-4638-9162-6332653A4041}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1135,7 +1138,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6B992660-7A43-41C4-A3AF-D1D27441D972}" type="CELLRANGE">
+                    <a:fld id="{D7C46AC8-248A-487D-9561-AF8087856CBD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1169,7 +1172,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6DB5FBE0-7AAC-4A50-8939-91DB52BBD5C9}" type="CELLRANGE">
+                    <a:fld id="{27A0EEF6-EDEC-4BFA-93D3-49D3EF1E8051}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1203,7 +1206,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75977432-C09A-40D5-B92F-08ECDFE0FEEC}" type="CELLRANGE">
+                    <a:fld id="{35ACB3DC-25B4-4217-ABE2-A38B7EE5617A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1237,7 +1240,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B3589E52-70DA-4B89-96E8-D04A3864E4FE}" type="CELLRANGE">
+                    <a:fld id="{80FAE2B4-5380-457F-B81C-FBD201ACEDBE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1271,7 +1274,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{89EF1700-1EC6-4ED2-AADF-3CC910768305}" type="CELLRANGE">
+                    <a:fld id="{FDA35268-1037-4E2C-ACE7-1D473463592D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1305,7 +1308,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{451C6A2E-7DAA-45F7-8DB6-5F7CBF72DC5C}" type="CELLRANGE">
+                    <a:fld id="{1354AF55-37A7-4213-82C6-8912D046DC60}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1339,7 +1342,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F6120E8C-84F1-4731-B278-19F05352DF27}" type="CELLRANGE">
+                    <a:fld id="{E51719E7-10C2-4DC7-BC17-D88257F36750}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1373,7 +1376,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CAF333E1-D0DD-4E1B-9AE1-5BD73B6E6268}" type="CELLRANGE">
+                    <a:fld id="{82626C0C-2858-4966-872E-3C8F122A817B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1407,7 +1410,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{94AFF5CB-B7EF-4FCC-B19A-E19C35A86CE9}" type="CELLRANGE">
+                    <a:fld id="{54C38C4C-7C6E-47A7-9BAD-482EF7E8F8A9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1441,7 +1444,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C1C42968-052D-4DDB-94B3-C13F726FF765}" type="CELLRANGE">
+                    <a:fld id="{71C2D6AD-64F9-4E3F-86DE-2E58A0D3D135}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1475,7 +1478,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{08E2AE1E-6C64-412C-A0A6-A09673EDCF42}" type="CELLRANGE">
+                    <a:fld id="{B6129C67-AF17-45F1-8F63-518F3BF606CC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1509,7 +1512,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BA1F0082-C1B1-4E1A-9F53-C9E9821D55EB}" type="CELLRANGE">
+                    <a:fld id="{447D78BE-7115-4363-A07B-F36EE6A5D0DA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1543,7 +1546,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9A55A09-8446-46BF-B708-965463702694}" type="CELLRANGE">
+                    <a:fld id="{3B6123CC-C187-4547-93F5-3422D688F025}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1577,7 +1580,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6D1ABF9-1619-4984-AB78-BC54F6F0D162}" type="CELLRANGE">
+                    <a:fld id="{6FFB08DF-0EFA-4C26-9C74-E34E7164136A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1611,7 +1614,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{26F6861D-DCB6-4E8F-9050-5DE042CFA364}" type="CELLRANGE">
+                    <a:fld id="{DFB7E1B5-27BE-4454-842E-82CEF5BC3554}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1645,7 +1648,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{92CE3DE1-C2E0-4F83-BB86-D7F77AB9E38E}" type="CELLRANGE">
+                    <a:fld id="{D882DCCF-58C9-4940-BD00-76F0173650D1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1679,7 +1682,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4B7C0D96-06DB-486A-90C8-5949B95C63CB}" type="CELLRANGE">
+                    <a:fld id="{0CFD8D08-DB44-4568-9A43-8B02CCFC3264}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1713,7 +1716,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8759C1C7-5249-458F-BDAA-E42F934B74EE}" type="CELLRANGE">
+                    <a:fld id="{42BFDBA4-9796-4789-A8D8-93118AD8D4CC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1747,7 +1750,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DB90C7C5-9E1A-439E-A966-0E091A7CA391}" type="CELLRANGE">
+                    <a:fld id="{E682EF3B-80B8-4CFC-8C52-D0D872002462}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1781,7 +1784,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E879AC4B-A99F-44DF-B31C-6560EFEBA9A9}" type="CELLRANGE">
+                    <a:fld id="{6ADC13C1-7267-4255-8D6A-FDA5DB81D1BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1815,7 +1818,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3379FA92-35F2-4A30-A395-EC96ADFEF765}" type="CELLRANGE">
+                    <a:fld id="{D4326E70-CC95-4B2D-82E1-03B852F83214}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1849,7 +1852,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C2744F0-EC66-4B2D-BD94-813491C66A81}" type="CELLRANGE">
+                    <a:fld id="{4FD0E117-6552-447E-8F10-5001EC48E527}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1883,7 +1886,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02690BBC-6FF5-410F-A148-FFA883CF2B9C}" type="CELLRANGE">
+                    <a:fld id="{63604CFB-77BA-4A68-8541-6ABC47BB339F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1907,6 +1910,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-6C2A-44F4-BD2F-56C82796355C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="47"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{68253147-138C-417A-98C4-BAE416A832D1}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-13FE-4BE5-AAC1-73ACB9B149DB}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1956,10 +1993,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$48</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="47"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
@@ -2000,105 +2037,108 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>9.1</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>12.2</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>9.75</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>5.4</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>11.9</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="34">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2106,10 +2146,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$48</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="47"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>2840</c:v>
                 </c:pt>
@@ -2150,105 +2190,108 @@
                   <c:v>2780</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>1680</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>4800</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>4120</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>3420</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>1450</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>3160</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>880</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>1260</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2304,10 +2347,10 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="14">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="16">
                     <c:v>strenuous</c:v>
@@ -2319,25 +2362,25 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="19">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="21">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="22">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="23">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="23">
+                  <c:pt idx="24">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="24">
+                  <c:pt idx="25">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="26">
                     <c:v>easy</c:v>
@@ -2346,10 +2389,10 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="28">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="30">
                     <c:v>moderate</c:v>
@@ -2358,48 +2401,51 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="32">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="33">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="34">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="36">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="36">
+                  <c:pt idx="37">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="37">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="38">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="39">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="40">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="40">
+                  <c:pt idx="41">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="41">
+                  <c:pt idx="42">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="42">
+                  <c:pt idx="43">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="43">
+                  <c:pt idx="44">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="44">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="45">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="46">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3406,10 +3452,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D48" totalsRowShown="0">
-  <autoFilter ref="A1:D48" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D48">
-    <sortCondition ref="A1:A48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D49" totalsRowShown="0">
+  <autoFilter ref="A1:D49" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D49">
+    <sortCondition ref="A1:A49"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -3718,10 +3764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3931,13 +3977,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B15">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="C15">
-        <v>1580</v>
+        <v>1680</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
@@ -3945,41 +3991,41 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B16">
-        <v>5.2</v>
+        <v>9.1</v>
       </c>
       <c r="C16">
-        <v>1000</v>
+        <v>1580</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B17">
-        <v>14</v>
+        <v>5.2</v>
       </c>
       <c r="C17">
-        <v>4800</v>
+        <v>1000</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
         <v>14</v>
       </c>
-      <c r="B18">
-        <v>12.2</v>
-      </c>
       <c r="C18">
-        <v>4120</v>
+        <v>4800</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
@@ -3987,13 +4033,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19">
-        <v>12</v>
+        <v>12.2</v>
       </c>
       <c r="C19">
-        <v>3420</v>
+        <v>4120</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -4001,127 +4047,127 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>3420</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>37</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <f>19.5/2</f>
         <v>9.75</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <f>4400*7/8</f>
         <v>3850</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21">
-        <v>5.4</v>
-      </c>
-      <c r="C21">
-        <v>1450</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B22">
-        <v>11.9</v>
+        <v>5.4</v>
       </c>
       <c r="C22">
-        <v>3160</v>
+        <v>1450</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B23">
-        <v>11.4</v>
+        <v>11.9</v>
       </c>
       <c r="C23">
-        <v>2550</v>
+        <v>3160</v>
       </c>
       <c r="D23" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24">
-        <v>8.5</v>
+        <v>11.4</v>
       </c>
       <c r="C24">
-        <v>3350</v>
+        <v>2550</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B25">
-        <v>2.8</v>
+        <v>8.5</v>
       </c>
       <c r="C25">
-        <v>880</v>
+        <v>3350</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B26">
-        <v>10.4</v>
+        <v>2.8</v>
       </c>
       <c r="C26">
-        <v>1420</v>
+        <v>880</v>
       </c>
       <c r="D26" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B27">
-        <v>0.9</v>
+        <v>10.4</v>
       </c>
       <c r="C27">
-        <v>200</v>
+        <v>1420</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B28">
-        <v>4.8</v>
+        <v>0.9</v>
       </c>
       <c r="C28">
-        <v>1260</v>
+        <v>200</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -4129,13 +4175,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B29">
-        <v>1.4</v>
+        <v>4.8</v>
       </c>
       <c r="C29">
-        <v>375</v>
+        <v>1260</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -4143,41 +4189,41 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B30">
-        <v>13.6</v>
+        <v>1.4</v>
       </c>
       <c r="C30">
-        <v>3930</v>
+        <v>375</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B31">
-        <v>7</v>
+        <v>13.6</v>
       </c>
       <c r="C31">
-        <v>1670</v>
+        <v>3930</v>
       </c>
       <c r="D31" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B32">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="C32">
-        <v>2400</v>
+        <v>1670</v>
       </c>
       <c r="D32" t="s">
         <v>1</v>
@@ -4185,13 +4231,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B33">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C33">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D33" t="s">
         <v>1</v>
@@ -4199,27 +4245,27 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B34">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C34">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35">
         <v>4.8</v>
       </c>
       <c r="C35">
-        <v>1470</v>
+        <v>1300</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
@@ -4227,69 +4273,69 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C36">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D36" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B37">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C37">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D37" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B38">
-        <v>2.2000000000000002</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C38">
-        <v>750</v>
+        <v>3490</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B39">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C39">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D39" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C40">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D40" t="s">
         <v>1</v>
@@ -4297,116 +4343,130 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41">
+        <v>7.3</v>
+      </c>
+      <c r="C41">
+        <v>2250</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
         <v>25</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42">
-        <v>1.2</v>
-      </c>
-      <c r="C42">
-        <v>500</v>
-      </c>
-      <c r="D42" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B43">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C43">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B44">
-        <v>6.2</v>
+        <v>11</v>
       </c>
       <c r="C44">
-        <v>1890</v>
+        <v>3060</v>
       </c>
       <c r="D44" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B45">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C45">
-        <v>180</v>
+        <v>1890</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B46">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C46">
-        <v>3550</v>
+        <v>180</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47">
+        <v>7.3</v>
+      </c>
+      <c r="C47">
+        <v>3550</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
         <v>55</v>
       </c>
-      <c r="B47">
+      <c r="B48">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C47">
+      <c r="C48">
         <v>3800</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
         <v>29</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <v>6</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>2180</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix error in Grand Park from Sunrise distance
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72F1ECA-E15F-429C-A1A8-337BD22E4247}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CF383C-9688-491B-8BE0-75F6C50F327C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -322,7 +322,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{38967F7C-7CD1-4345-81E1-C060ADE654DE}" type="CELLRANGE">
+                    <a:fld id="{5F855BAE-59E0-45B0-A066-A7B9754089DF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -356,7 +356,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3370CB3A-A0C8-4C07-8B42-E326AB5EE42A}" type="CELLRANGE">
+                    <a:fld id="{F6465FD7-3805-416C-84EA-EC36FF24125A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -390,7 +390,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1F5331C9-D310-418E-B885-16EA6E6076C7}" type="CELLRANGE">
+                    <a:fld id="{4306E05D-896D-4038-A940-385259F9317A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -424,7 +424,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{59E9EE57-375E-4A41-B472-0506B5A6C143}" type="CELLRANGE">
+                    <a:fld id="{1FD46F92-324B-4D54-A8EC-99D392E264BD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -458,7 +458,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D384827B-1F10-47FA-8291-E6C2BF70865A}" type="CELLRANGE">
+                    <a:fld id="{012EC2CC-3E9A-4DD9-B21A-9C433AC7AF69}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -492,7 +492,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91E336E8-A250-425A-8190-EF839E936349}" type="CELLRANGE">
+                    <a:fld id="{F068AC08-45D6-4151-BEE0-EC0B1F074F0D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -526,7 +526,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CFE7AB7E-6D14-48EE-B126-CF8AC3439D73}" type="CELLRANGE">
+                    <a:fld id="{549C59F0-E940-4D78-A135-67DD6F6FA881}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -560,7 +560,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{92D89996-ED09-4E69-AFB6-D7B52AEE532F}" type="CELLRANGE">
+                    <a:fld id="{052CF848-F75F-476D-A372-1A8D5EFC945E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -594,7 +594,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B2FA857-7987-4776-AD23-2E2A47D8AA02}" type="CELLRANGE">
+                    <a:fld id="{A6D633D3-013C-45A1-92E1-0642900C5BEA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -628,7 +628,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47F5C88F-7552-43A1-86BA-97E57799E7A8}" type="CELLRANGE">
+                    <a:fld id="{1C2F779C-AB2B-4117-89DC-836A6AC3E8B6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -662,7 +662,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C550331-22BE-49B6-9FD4-9CB4936A98FB}" type="CELLRANGE">
+                    <a:fld id="{D935533D-C23A-4BF6-88DF-988D6D17E2C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -696,7 +696,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A4EA0DF2-AE6D-40FE-B121-8060314F4E5B}" type="CELLRANGE">
+                    <a:fld id="{58CA5EB1-85A8-48D4-8A44-A71557E86E2C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -730,7 +730,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E765F21-E715-4892-922B-058F2F8C6A49}" type="CELLRANGE">
+                    <a:fld id="{897C3121-5249-4ED9-88B2-768F310C36E6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -764,7 +764,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BC69042-B95D-4B4F-968D-21067D5FC528}" type="CELLRANGE">
+                    <a:fld id="{94B68370-7645-43B2-8D71-C452979B1399}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -798,7 +798,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23B61035-39C9-4327-BFA6-FB8414AA1FBD}" type="CELLRANGE">
+                    <a:fld id="{60F4B67D-6079-445B-9397-596A9DE66348}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -832,7 +832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AFFA33DA-B67E-42D3-897B-23B78C741865}" type="CELLRANGE">
+                    <a:fld id="{6F70EB01-F044-4FC9-8153-34AACE02B22B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -866,7 +866,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F60D8CE9-C9A2-464C-A967-84533339344D}" type="CELLRANGE">
+                    <a:fld id="{6CC6D88A-3162-4228-95C3-25A43E51DF3B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -900,7 +900,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8688F76-C131-42A2-98EA-A2041E5F7AC3}" type="CELLRANGE">
+                    <a:fld id="{230CE2DF-7746-48A0-AB82-B8494CB781B8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -934,7 +934,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6FBC29A0-45B5-4283-AC98-B04C80916641}" type="CELLRANGE">
+                    <a:fld id="{F488DBBA-1C8E-419C-B50F-AE05407358A3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -968,7 +968,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B4CDA36-A094-4ED0-8C09-471974E8C601}" type="CELLRANGE">
+                    <a:fld id="{8BA7479A-DF45-4A5C-A6F7-6C04D317290C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1002,7 +1002,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D27CE684-7C95-4FBC-AAF8-0610F6D999A2}" type="CELLRANGE">
+                    <a:fld id="{88E6CF40-1597-493E-B853-3B026E5453BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1036,7 +1036,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5EFCCA2F-7C9E-4E74-81BA-1D006E123B8F}" type="CELLRANGE">
+                    <a:fld id="{2E3F16A1-14CB-4DFD-919A-21F64C5A5ABC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1070,7 +1070,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FED3606D-B193-4E93-B078-057E18DB2E11}" type="CELLRANGE">
+                    <a:fld id="{D2A44FF0-DC0F-4B94-9308-59A04E1C7597}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1104,7 +1104,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7A1385B3-031B-4638-9162-6332653A4041}" type="CELLRANGE">
+                    <a:fld id="{3765BDAA-473A-4730-8CB8-8A0CCFDDC73B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1138,7 +1138,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D7C46AC8-248A-487D-9561-AF8087856CBD}" type="CELLRANGE">
+                    <a:fld id="{1D6CA709-6FD6-40DD-908C-DCC999E035D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1172,7 +1172,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{27A0EEF6-EDEC-4BFA-93D3-49D3EF1E8051}" type="CELLRANGE">
+                    <a:fld id="{73DEB595-0148-4110-A122-7B8303CC7A19}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1206,7 +1206,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35ACB3DC-25B4-4217-ABE2-A38B7EE5617A}" type="CELLRANGE">
+                    <a:fld id="{586E6397-8E5D-4C78-A084-EFCD44092D1A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1240,7 +1240,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{80FAE2B4-5380-457F-B81C-FBD201ACEDBE}" type="CELLRANGE">
+                    <a:fld id="{B6A29622-04F8-4BF5-AF5F-2C6ABD256D12}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1274,7 +1274,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FDA35268-1037-4E2C-ACE7-1D473463592D}" type="CELLRANGE">
+                    <a:fld id="{0FF43277-B591-4EEA-AF54-831FD6440EEA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1308,7 +1308,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1354AF55-37A7-4213-82C6-8912D046DC60}" type="CELLRANGE">
+                    <a:fld id="{CA543C71-60DC-461E-8A4A-4C80EA47767D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1342,7 +1342,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E51719E7-10C2-4DC7-BC17-D88257F36750}" type="CELLRANGE">
+                    <a:fld id="{1CC8606A-D595-441F-B111-587A365F3FC2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1376,7 +1376,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{82626C0C-2858-4966-872E-3C8F122A817B}" type="CELLRANGE">
+                    <a:fld id="{FA2A0693-4DBE-4451-9538-BD4326DA657C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1410,7 +1410,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{54C38C4C-7C6E-47A7-9BAD-482EF7E8F8A9}" type="CELLRANGE">
+                    <a:fld id="{7ABA858F-6DC8-4C0D-8FFB-93135D0F5FF3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1444,7 +1444,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{71C2D6AD-64F9-4E3F-86DE-2E58A0D3D135}" type="CELLRANGE">
+                    <a:fld id="{E57F9EA7-3C65-4DBE-9EAD-51E35F4622BD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1478,7 +1478,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6129C67-AF17-45F1-8F63-518F3BF606CC}" type="CELLRANGE">
+                    <a:fld id="{9FD3CC27-A34A-4A7A-A9AF-8439CDE0795C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1512,7 +1512,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{447D78BE-7115-4363-A07B-F36EE6A5D0DA}" type="CELLRANGE">
+                    <a:fld id="{A35596B3-0CB7-4C72-895A-0F905D96E0A9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1546,7 +1546,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B6123CC-C187-4547-93F5-3422D688F025}" type="CELLRANGE">
+                    <a:fld id="{6428A973-F3DB-40DB-91E4-C2A93E7B3DE2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1580,7 +1580,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6FFB08DF-0EFA-4C26-9C74-E34E7164136A}" type="CELLRANGE">
+                    <a:fld id="{83CA5217-2360-4148-88B8-1421E601058B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1614,7 +1614,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DFB7E1B5-27BE-4454-842E-82CEF5BC3554}" type="CELLRANGE">
+                    <a:fld id="{E3D6AB0E-BC0D-4523-A6A3-D8CC7F1BAF4B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1648,7 +1648,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D882DCCF-58C9-4940-BD00-76F0173650D1}" type="CELLRANGE">
+                    <a:fld id="{9C39EB9E-B352-4396-B33A-BCB5CB9BCBC3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1682,7 +1682,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0CFD8D08-DB44-4568-9A43-8B02CCFC3264}" type="CELLRANGE">
+                    <a:fld id="{16F13E43-C880-4BD5-AC23-0441541AF156}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1716,7 +1716,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42BFDBA4-9796-4789-A8D8-93118AD8D4CC}" type="CELLRANGE">
+                    <a:fld id="{76B756DD-1B2B-4B56-8AC8-9370AA9DF293}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1750,7 +1750,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E682EF3B-80B8-4CFC-8C52-D0D872002462}" type="CELLRANGE">
+                    <a:fld id="{0BC63603-7429-472D-A6B5-66E55D5F3DA7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1784,7 +1784,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6ADC13C1-7267-4255-8D6A-FDA5DB81D1BE}" type="CELLRANGE">
+                    <a:fld id="{11BF52B7-3459-4ABF-AEF3-F6F20ACC00E1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1818,7 +1818,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4326E70-CC95-4B2D-82E1-03B852F83214}" type="CELLRANGE">
+                    <a:fld id="{1B988058-6CD3-486A-A506-98B7CE6F0AF7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1852,7 +1852,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4FD0E117-6552-447E-8F10-5001EC48E527}" type="CELLRANGE">
+                    <a:fld id="{FE447269-1959-4D10-B087-B18FDF982A81}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1886,7 +1886,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63604CFB-77BA-4A68-8541-6ABC47BB339F}" type="CELLRANGE">
+                    <a:fld id="{EC971FD6-E7AE-4203-B6F7-42241F921365}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1920,7 +1920,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{68253147-138C-417A-98C4-BAE416A832D1}" type="CELLRANGE">
+                    <a:fld id="{D875DCC7-E055-4E06-8A66-D4A371A74301}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2034,7 +2034,7 @@
                   <c:v>11.6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>9</c:v>
@@ -3767,7 +3767,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3966,7 +3966,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>12.5</v>
       </c>
       <c r="C14">
         <v>2780</v>

</xml_diff>

<commit_message>
Add Paul Peak trail
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CF383C-9688-491B-8BE0-75F6C50F327C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971E59C6-1EE2-43B1-A327-97EB77354092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Grand Park via Lake Eleanor</t>
+  </si>
+  <si>
+    <t>Paul Peak Trail</t>
   </si>
 </sst>
 </file>
@@ -322,7 +325,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F855BAE-59E0-45B0-A066-A7B9754089DF}" type="CELLRANGE">
+                    <a:fld id="{D4DC9558-276A-4883-B30C-8AB294CC1522}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -356,7 +359,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F6465FD7-3805-416C-84EA-EC36FF24125A}" type="CELLRANGE">
+                    <a:fld id="{F3D821FD-E216-42A4-97BB-CD79F05F84F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -390,7 +393,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4306E05D-896D-4038-A940-385259F9317A}" type="CELLRANGE">
+                    <a:fld id="{4E6AACAB-24DD-4CDF-BDB3-953C70C7A36D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -424,7 +427,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1FD46F92-324B-4D54-A8EC-99D392E264BD}" type="CELLRANGE">
+                    <a:fld id="{C83AB602-A7B6-43D9-81A7-128276688A16}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -458,7 +461,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{012EC2CC-3E9A-4DD9-B21A-9C433AC7AF69}" type="CELLRANGE">
+                    <a:fld id="{3CBE3622-FCAD-4EC6-885E-390F0583841E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -492,7 +495,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F068AC08-45D6-4151-BEE0-EC0B1F074F0D}" type="CELLRANGE">
+                    <a:fld id="{FE8F25F3-C148-44EE-8B78-386AC4712B69}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -526,7 +529,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{549C59F0-E940-4D78-A135-67DD6F6FA881}" type="CELLRANGE">
+                    <a:fld id="{5C133477-591D-4766-85E9-8B04F501737F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -560,7 +563,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{052CF848-F75F-476D-A372-1A8D5EFC945E}" type="CELLRANGE">
+                    <a:fld id="{56814B48-91FF-4339-8298-8DA10F513991}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -594,7 +597,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A6D633D3-013C-45A1-92E1-0642900C5BEA}" type="CELLRANGE">
+                    <a:fld id="{B4EAA63E-313C-49B1-AB80-178A887EDB69}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -628,7 +631,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C2F779C-AB2B-4117-89DC-836A6AC3E8B6}" type="CELLRANGE">
+                    <a:fld id="{A29DE31C-D734-49C4-9725-7C4722A17B46}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -662,7 +665,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D935533D-C23A-4BF6-88DF-988D6D17E2C5}" type="CELLRANGE">
+                    <a:fld id="{4DFC0907-50D6-4BF5-A63E-D8B5CC1CC53D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -696,7 +699,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58CA5EB1-85A8-48D4-8A44-A71557E86E2C}" type="CELLRANGE">
+                    <a:fld id="{4B98B7F3-5120-4061-8CC8-8BB134FAAD88}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -730,7 +733,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{897C3121-5249-4ED9-88B2-768F310C36E6}" type="CELLRANGE">
+                    <a:fld id="{8F41EAA0-0C2C-483B-B47C-FBEE4A0E0B45}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -764,7 +767,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{94B68370-7645-43B2-8D71-C452979B1399}" type="CELLRANGE">
+                    <a:fld id="{F293DF27-8E4A-49B6-BE46-710DB9793034}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -798,7 +801,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60F4B67D-6079-445B-9397-596A9DE66348}" type="CELLRANGE">
+                    <a:fld id="{1ABE1264-AA62-41C6-9201-48FADE3E723B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -832,7 +835,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6F70EB01-F044-4FC9-8153-34AACE02B22B}" type="CELLRANGE">
+                    <a:fld id="{6D517D37-2E69-4A2C-B1C8-F950C5B23E3C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -866,7 +869,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CC6D88A-3162-4228-95C3-25A43E51DF3B}" type="CELLRANGE">
+                    <a:fld id="{BC8AB7AE-7F02-440E-BA61-49134809EAC5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -900,7 +903,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{230CE2DF-7746-48A0-AB82-B8494CB781B8}" type="CELLRANGE">
+                    <a:fld id="{3F086B12-D212-490C-B4A5-3613CBEC4024}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -934,7 +937,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F488DBBA-1C8E-419C-B50F-AE05407358A3}" type="CELLRANGE">
+                    <a:fld id="{51C263FD-AABC-4F43-9472-E19618974E33}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -968,7 +971,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8BA7479A-DF45-4A5C-A6F7-6C04D317290C}" type="CELLRANGE">
+                    <a:fld id="{57B7F884-C76C-49D9-8DEF-D746D5AAF148}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1002,7 +1005,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88E6CF40-1597-493E-B853-3B026E5453BA}" type="CELLRANGE">
+                    <a:fld id="{5558F014-96A0-429C-988C-83951BB8447A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1036,7 +1039,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E3F16A1-14CB-4DFD-919A-21F64C5A5ABC}" type="CELLRANGE">
+                    <a:fld id="{41126551-4398-4BFE-802B-2C1013BA24E0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1070,7 +1073,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D2A44FF0-DC0F-4B94-9308-59A04E1C7597}" type="CELLRANGE">
+                    <a:fld id="{FDE3DA6B-83C0-4E1A-86DA-A6C155F7D5A9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1104,7 +1107,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3765BDAA-473A-4730-8CB8-8A0CCFDDC73B}" type="CELLRANGE">
+                    <a:fld id="{C541D085-AB00-4AD7-BB53-AD25DF234FA8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1138,7 +1141,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1D6CA709-6FD6-40DD-908C-DCC999E035D7}" type="CELLRANGE">
+                    <a:fld id="{4C433C54-15DE-4D95-AB7F-D26316196935}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1172,7 +1175,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73DEB595-0148-4110-A122-7B8303CC7A19}" type="CELLRANGE">
+                    <a:fld id="{CA2B73A1-BEAA-4332-9B59-1A2ACBF52A1D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1206,7 +1209,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{586E6397-8E5D-4C78-A084-EFCD44092D1A}" type="CELLRANGE">
+                    <a:fld id="{5C1515DA-7059-4444-B826-C468A3D6662E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1240,7 +1243,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6A29622-04F8-4BF5-AF5F-2C6ABD256D12}" type="CELLRANGE">
+                    <a:fld id="{CAB025A4-086E-4D76-93F1-1C6EF908DBAB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1274,7 +1277,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0FF43277-B591-4EEA-AF54-831FD6440EEA}" type="CELLRANGE">
+                    <a:fld id="{0376A668-099B-4F74-86AA-5B8F201378FE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1308,7 +1311,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA543C71-60DC-461E-8A4A-4C80EA47767D}" type="CELLRANGE">
+                    <a:fld id="{AE80FA56-A0FD-406A-8E09-4C599729453F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1342,7 +1345,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1CC8606A-D595-441F-B111-587A365F3FC2}" type="CELLRANGE">
+                    <a:fld id="{E315571F-BF57-4EFF-8177-9D00693785B4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1376,7 +1379,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA2A0693-4DBE-4451-9538-BD4326DA657C}" type="CELLRANGE">
+                    <a:fld id="{9155BE2E-D25C-4BB4-B8EC-9EA32FDD8DDC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1410,7 +1413,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7ABA858F-6DC8-4C0D-8FFB-93135D0F5FF3}" type="CELLRANGE">
+                    <a:fld id="{4FE5B52A-46AE-4230-9B10-9AEBE8602817}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1444,7 +1447,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E57F9EA7-3C65-4DBE-9EAD-51E35F4622BD}" type="CELLRANGE">
+                    <a:fld id="{6A5F6F70-59AA-426D-AFC6-9FDF61F8F538}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1478,7 +1481,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9FD3CC27-A34A-4A7A-A9AF-8439CDE0795C}" type="CELLRANGE">
+                    <a:fld id="{A5C0C19A-8917-452C-A576-0EC22F36AF99}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1512,7 +1515,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A35596B3-0CB7-4C72-895A-0F905D96E0A9}" type="CELLRANGE">
+                    <a:fld id="{D64246EC-3E6A-4D9A-BCD5-D10A5C2EBB20}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1546,7 +1549,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6428A973-F3DB-40DB-91E4-C2A93E7B3DE2}" type="CELLRANGE">
+                    <a:fld id="{095400E1-ADA2-4BE9-A407-ACC08958DDBE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1580,7 +1583,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{83CA5217-2360-4148-88B8-1421E601058B}" type="CELLRANGE">
+                    <a:fld id="{59793891-434C-4C6C-92AA-6E1319EEFA2E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1614,7 +1617,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E3D6AB0E-BC0D-4523-A6A3-D8CC7F1BAF4B}" type="CELLRANGE">
+                    <a:fld id="{146B2D1C-A54D-4D02-BFAA-3B643064E5D1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1648,7 +1651,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C39EB9E-B352-4396-B33A-BCB5CB9BCBC3}" type="CELLRANGE">
+                    <a:fld id="{70CCE427-F472-49EE-BFF9-A5721C27FDC4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1682,7 +1685,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{16F13E43-C880-4BD5-AC23-0441541AF156}" type="CELLRANGE">
+                    <a:fld id="{636BD7DA-93E7-4CDD-B32A-8E9875DA578E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1716,7 +1719,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{76B756DD-1B2B-4B56-8AC8-9370AA9DF293}" type="CELLRANGE">
+                    <a:fld id="{446DD51B-9ED8-48EE-BE66-E41BE751EA73}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1750,7 +1753,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0BC63603-7429-472D-A6B5-66E55D5F3DA7}" type="CELLRANGE">
+                    <a:fld id="{B3BF0C54-C44F-4954-B173-598654FDF0B1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1784,7 +1787,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{11BF52B7-3459-4ABF-AEF3-F6F20ACC00E1}" type="CELLRANGE">
+                    <a:fld id="{460F30CB-F136-48BF-A4B5-023857AE06F1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1818,7 +1821,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B988058-6CD3-486A-A506-98B7CE6F0AF7}" type="CELLRANGE">
+                    <a:fld id="{F33FAAFE-F2A0-4DE7-AA53-C92F0EEE2C6F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1852,7 +1855,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FE447269-1959-4D10-B087-B18FDF982A81}" type="CELLRANGE">
+                    <a:fld id="{FBB2B8CD-EEC7-4C25-882B-F449756BD070}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1886,7 +1889,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC971FD6-E7AE-4203-B6F7-42241F921365}" type="CELLRANGE">
+                    <a:fld id="{EE7F9F2D-CA54-4598-A6D8-DFF52E973E27}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1920,7 +1923,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D875DCC7-E055-4E06-8A66-D4A371A74301}" type="CELLRANGE">
+                    <a:fld id="{44DC6DE5-C801-4F68-B704-3E7851207DF5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1944,6 +1947,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-13FE-4BE5-AAC1-73ACB9B149DB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="48"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{378CCE93-4427-4D86-B7D5-EBE25501F3A5}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-E885-43CA-B649-A1147A65F1AD}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1993,10 +2030,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$49</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
@@ -2100,45 +2137,48 @@
                   <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="34">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2146,10 +2186,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$49</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
                   <c:v>2840</c:v>
                 </c:pt>
@@ -2253,45 +2293,48 @@
                   <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="34">
+                  <c:v>1630</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2407,45 +2450,48 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="34">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="36">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="36">
+                  <c:pt idx="37">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="37">
+                  <c:pt idx="38">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="38">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="39">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="40">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="41">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="41">
+                  <c:pt idx="42">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="42">
+                  <c:pt idx="43">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="43">
+                  <c:pt idx="44">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="44">
+                  <c:pt idx="45">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="45">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="46">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="47">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="48">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3452,10 +3498,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D49" totalsRowShown="0">
-  <autoFilter ref="A1:D49" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D49">
-    <sortCondition ref="A1:A49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D50" totalsRowShown="0">
+  <autoFilter ref="A1:D50" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D50">
+    <sortCondition ref="A1:A50"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -3764,10 +3810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4273,83 +4319,83 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="B36">
-        <v>4.8</v>
+        <v>7.2</v>
       </c>
       <c r="C36">
-        <v>1470</v>
+        <v>1630</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C37">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D37" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B38">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C38">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D38" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B39">
-        <v>2.2000000000000002</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C39">
-        <v>750</v>
+        <v>3490</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B40">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C40">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D40" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B41">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C41">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
@@ -4357,116 +4403,130 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42">
+        <v>7.3</v>
+      </c>
+      <c r="C42">
+        <v>2250</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>25</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>49</v>
-      </c>
-      <c r="B43">
-        <v>1.2</v>
-      </c>
-      <c r="C43">
-        <v>500</v>
-      </c>
-      <c r="D43" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B44">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C44">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D44" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B45">
-        <v>6.2</v>
+        <v>11</v>
       </c>
       <c r="C45">
-        <v>1890</v>
+        <v>3060</v>
       </c>
       <c r="D45" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B46">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C46">
-        <v>180</v>
+        <v>1890</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B47">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C47">
-        <v>3550</v>
+        <v>180</v>
       </c>
       <c r="D47" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48">
+        <v>7.3</v>
+      </c>
+      <c r="C48">
+        <v>3550</v>
+      </c>
+      <c r="D48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
         <v>55</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>3800</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
         <v>29</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>6</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>2180</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4478,4 +4538,10 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Add Backbone Ridge trail
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A381E2-B539-4BE1-89C4-9939F6A76488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2A3358-922D-43F5-8DE5-3C322F54BDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Boundary Trail to Florence Peak</t>
+  </si>
+  <si>
+    <t>Backbone Ridge</t>
   </si>
 </sst>
 </file>
@@ -328,7 +331,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6F278B4-650D-4911-AB94-9324E17C830D}" type="CELLRANGE">
+                    <a:fld id="{6E5EFB28-5BDE-4391-9985-EB007C5A9081}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -362,7 +365,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C2E3D163-EAD0-42B9-9757-42B959DC5483}" type="CELLRANGE">
+                    <a:fld id="{80FC8114-2703-40C9-88E2-A8FD61800D1D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -396,7 +399,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{92F0C8ED-4372-4414-911D-F2EDE345E1D3}" type="CELLRANGE">
+                    <a:fld id="{DBB1E6AA-5BC1-480B-8574-C0CB60F5B33D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -430,7 +433,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C69EB9C-8106-496F-8F39-6E31C1051C8B}" type="CELLRANGE">
+                    <a:fld id="{7123F7FD-4C33-4BA8-B285-EF71F61859A2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -464,7 +467,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AF3E0D0B-5064-45E0-91D9-62E06517494F}" type="CELLRANGE">
+                    <a:fld id="{C22D2DE2-DDEA-412E-9E8C-9070F6417F5E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -498,7 +501,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C6A91E4-E26F-4366-8194-3936C3E6C304}" type="CELLRANGE">
+                    <a:fld id="{DDCF08FB-2411-4106-933D-C7EFCBF00C86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -532,7 +535,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B27754CA-E41D-4894-8C7D-1C6D54E9E43D}" type="CELLRANGE">
+                    <a:fld id="{A45AA860-0A37-4FB7-B628-497FD7F12D3D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -566,7 +569,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E6D41C8-22DE-44A5-97B5-82958BA3C82E}" type="CELLRANGE">
+                    <a:fld id="{9016758D-98DD-410C-9CFB-CACA2F8DAF04}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -600,7 +603,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C1C55EDC-DBD6-491F-9751-F6A83D3A1742}" type="CELLRANGE">
+                    <a:fld id="{F3878C62-0C81-4E8A-85B6-B9A0A8C7DFB1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -634,7 +637,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{76DED6FC-F910-4696-9CB3-F92E5B34DA4A}" type="CELLRANGE">
+                    <a:fld id="{7A124B87-515C-4C64-BC24-48BBD879E909}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -668,7 +671,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AEFD6A00-F966-4D50-A3BE-7F1861D59DA7}" type="CELLRANGE">
+                    <a:fld id="{F619F039-450A-4A13-85DC-4ED01ABE0E14}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -702,7 +705,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67F33545-D823-43C7-81E9-5003474C5F4C}" type="CELLRANGE">
+                    <a:fld id="{0F3B45C8-AEB6-4629-B0C7-0E8D0025A6B4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -736,7 +739,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{397582B0-7C25-4661-9C28-0BEE35C70206}" type="CELLRANGE">
+                    <a:fld id="{26E8E63A-E682-47FD-B0AC-1C763465F8CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -770,7 +773,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F93F4F7-2BB0-401A-AE84-B204CA0026D8}" type="CELLRANGE">
+                    <a:fld id="{4FEA0680-A21B-4A14-AB89-D71DC6D2043A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -804,7 +807,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F6260F99-8CBB-44AD-AB9A-727CF079DF1F}" type="CELLRANGE">
+                    <a:fld id="{5AAD2D13-D3FD-4EAD-9F98-FD851EF1835D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -838,7 +841,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DAE05A8A-88B4-4508-9DD1-74E476C34E18}" type="CELLRANGE">
+                    <a:fld id="{E6B84853-3EE3-4099-8C7C-24A107F29ED1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -872,7 +875,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4EB93B4D-E4E5-4161-93DA-C6CEE347C9D9}" type="CELLRANGE">
+                    <a:fld id="{FDBF4195-4917-44F1-945D-B48DDE1044AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -906,7 +909,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{918BE2BE-C779-4B9C-B4FC-04DBDBE0541F}" type="CELLRANGE">
+                    <a:fld id="{B6471DCF-E4AE-4AFD-BC8D-3B40E45D4B7F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -940,7 +943,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C42279E3-B5BB-48AC-A743-7C174F34C78C}" type="CELLRANGE">
+                    <a:fld id="{A72CC93E-50DF-4EDD-98CC-80D4F00A4EA8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -974,7 +977,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F90EB3B1-69BA-4DBE-A03E-9AEDBA406D02}" type="CELLRANGE">
+                    <a:fld id="{415BD3B9-7B14-469D-B7BC-D2D15CFD1259}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1008,7 +1011,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7627B5A5-B6DC-4B17-B987-848750902157}" type="CELLRANGE">
+                    <a:fld id="{02894FE2-36D5-4663-8598-57052CE2DA75}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1042,7 +1045,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC15F20A-4823-4358-AC7A-74D2E8FA9B7C}" type="CELLRANGE">
+                    <a:fld id="{799676E7-0EBD-4318-A863-4B5A87DD0035}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1076,7 +1079,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{986BF85F-B9AF-4C56-A230-D373BD142745}" type="CELLRANGE">
+                    <a:fld id="{B5351088-A981-4A0D-AE6E-1A8998904FE1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1110,7 +1113,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{645568E3-70AF-43D2-824C-D0C500F32692}" type="CELLRANGE">
+                    <a:fld id="{9BB1BDBD-F0C3-4A2E-919A-CAEF496217AF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1144,7 +1147,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{762BF04E-B4BD-405A-8E08-D6393697AF70}" type="CELLRANGE">
+                    <a:fld id="{51B30183-8CB5-470A-A100-51083D640D58}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1178,7 +1181,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AAB5A63C-79C8-455C-B36B-EDD502509F3A}" type="CELLRANGE">
+                    <a:fld id="{7D50CF8C-E201-472B-87F1-50D91B32595D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1212,7 +1215,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AC3E9885-60F6-4065-841C-F71201578F60}" type="CELLRANGE">
+                    <a:fld id="{002FC77A-DB58-476B-BAE0-9EA3C312465D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1246,7 +1249,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02C3C509-F8E5-4536-AC1F-14AA1C9DF2EE}" type="CELLRANGE">
+                    <a:fld id="{D0E36D8D-217B-40C1-AA33-C882E24FAB6C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1280,7 +1283,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4514A72A-E9B4-460F-AE57-2F5D9037A027}" type="CELLRANGE">
+                    <a:fld id="{CC47074E-86A3-44C1-949B-EF48663AE6BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1314,7 +1317,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F39F667-26A3-4B1C-9BBD-E8FE92F894E0}" type="CELLRANGE">
+                    <a:fld id="{FADF24F6-EA1E-418F-8EFD-FB0FCAE3BD5B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1348,7 +1351,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC3B844E-8D91-4F4E-8F9A-7D5CB4F0A10C}" type="CELLRANGE">
+                    <a:fld id="{7CD0755E-5B3B-4148-9D9B-9E8450EE9394}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1382,7 +1385,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0BC91EC0-8EDB-41CD-8DC2-C8F308A5EC2D}" type="CELLRANGE">
+                    <a:fld id="{335C42AD-A601-40AA-9F9F-0B61D3135854}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1416,7 +1419,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1802EB3F-558A-4C28-AD94-DAFB935B13E8}" type="CELLRANGE">
+                    <a:fld id="{3F9F46FD-4D72-4DB4-B9E0-3E2215444BEE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1450,7 +1453,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A34E98A9-C4DF-48D6-9F00-6086677A9C78}" type="CELLRANGE">
+                    <a:fld id="{868CF4AE-A1AC-404B-B3D7-8F8FC34D9627}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1484,7 +1487,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{59452C20-A749-4877-BF6B-59843495042C}" type="CELLRANGE">
+                    <a:fld id="{F2D8E44E-E90B-4EA6-863B-F8C7B8A0B168}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1518,7 +1521,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{43C3AE70-B9A8-4736-A3FB-CDED176ADDE1}" type="CELLRANGE">
+                    <a:fld id="{61661A6B-EA8B-449A-AE2D-7ABC912483F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1552,7 +1555,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7A94C6AC-686F-4301-A3FD-25218B536F0E}" type="CELLRANGE">
+                    <a:fld id="{D1A3D0EE-94D0-4309-8D09-46FCCCBA1925}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1586,7 +1589,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B2849735-6ADF-4871-97F1-F958EC07D9E5}" type="CELLRANGE">
+                    <a:fld id="{95CE04F0-7AAC-4C44-AF53-1C6C45BC06D9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1620,7 +1623,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D844AF8F-561A-4C0C-8A3E-0DFBCF495E0B}" type="CELLRANGE">
+                    <a:fld id="{3577D630-B002-4F3F-9077-0E889AF07E9D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1654,7 +1657,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B3352886-64A4-4A76-AE58-3D422C6FBEFE}" type="CELLRANGE">
+                    <a:fld id="{7BC38640-AD88-4EF1-84A9-32D59E6ADB3F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1688,7 +1691,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4037B56D-40F9-4BEC-BB61-0B72E3ABCE91}" type="CELLRANGE">
+                    <a:fld id="{2A8276FB-FDAA-403B-A99C-CCBAD578E07F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1722,7 +1725,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C294E72-4796-45FB-96A4-059FC24C836E}" type="CELLRANGE">
+                    <a:fld id="{6CB65385-1CDA-48F7-A8F6-C9F617FFBAA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1756,7 +1759,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9BC727C-527C-400D-97E9-75724ECF026A}" type="CELLRANGE">
+                    <a:fld id="{8BBA14A4-7F47-4A0B-B7E6-F9C41F689C1A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1790,7 +1793,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F1A725E1-BE95-47CB-AC28-0EC32E438E2F}" type="CELLRANGE">
+                    <a:fld id="{A51AAF32-0AC2-4D30-B890-0CC0C6CF5EAE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1824,7 +1827,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A02DC394-44A2-4EE4-8C47-54B63341AE26}" type="CELLRANGE">
+                    <a:fld id="{BDEB8FAB-E7CF-4532-BBD4-B997A834E052}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1858,7 +1861,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5AA55363-76C2-4DAB-B429-659BE905BD92}" type="CELLRANGE">
+                    <a:fld id="{7D6D7BD5-9AC7-4D46-B35B-2DCC702AB82E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1892,7 +1895,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4A19C08D-9668-4466-94BF-87FDE96229F1}" type="CELLRANGE">
+                    <a:fld id="{6BCC1FD8-E711-43C0-A022-3FDA33E9075A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1926,7 +1929,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{65E833BA-4F4D-4B8D-90D1-E3B50395427D}" type="CELLRANGE">
+                    <a:fld id="{4C8C1CEE-0AC1-4D71-9A19-314DC82F0233}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1960,7 +1963,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{43B36739-1A56-44A2-86BF-49CE37057BD6}" type="CELLRANGE">
+                    <a:fld id="{1B9AE679-11C1-4D52-B030-1934828E4920}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1994,7 +1997,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97BBB1AB-5AC8-4B95-8C1D-D4AFC97A885D}" type="CELLRANGE">
+                    <a:fld id="{450161B0-6B1F-4A2E-B69C-D87A2745D684}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2018,6 +2021,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-E12C-45AF-8FD6-270DCC9A88F5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="50"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A80AC26B-EA37-4A9B-888B-DD8DF20D0E99}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-A6AE-456F-B05B-25C923A280DB}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2067,158 +2104,161 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$51</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>7.6</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>11.866666666666667</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>10.3</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>7.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>2.9</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>7.1</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>9.8000000000000007</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>9.6</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>11.6</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>12.5</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>9.1</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>12.2</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>9.75</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>5.4</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>11.9</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>7.2</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2226,158 +2266,161 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$51</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
+                  <c:v>2990</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3950</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2840</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>4700</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2010</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>690</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2970</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>3030</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>1540</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>2880</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>3290</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>2660</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>2780</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>4800</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>4120</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>3420</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>1450</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>3160</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>880</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>1260</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>1630</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2394,28 +2437,28 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>omg yikes wtf</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>easy (but long)</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>moderate</c:v>
@@ -2424,25 +2467,25 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="11">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="13">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="14">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="15">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="16">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="18">
                     <c:v>strenuous</c:v>
@@ -2454,25 +2497,25 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="21">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="23">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="23">
+                  <c:pt idx="24">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="24">
+                  <c:pt idx="25">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="25">
+                  <c:pt idx="26">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="26">
+                  <c:pt idx="27">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="28">
                     <c:v>easy</c:v>
@@ -2481,10 +2524,10 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="30">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="31">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="32">
                     <c:v>moderate</c:v>
@@ -2493,51 +2536,54 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="34">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="36">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="36">
+                  <c:pt idx="37">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="37">
+                  <c:pt idx="38">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="38">
+                  <c:pt idx="39">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="39">
+                  <c:pt idx="40">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="40">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="41">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="42">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="43">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="43">
+                  <c:pt idx="44">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="44">
+                  <c:pt idx="45">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="45">
+                  <c:pt idx="46">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="46">
+                  <c:pt idx="47">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="47">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="48">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="49">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="50">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3544,10 +3590,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D51" totalsRowShown="0">
-  <autoFilter ref="A1:D51" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D51">
-    <sortCondition ref="A1:A51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D52" totalsRowShown="0">
+  <autoFilter ref="A1:D52" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D52">
+    <sortCondition ref="A1:A52"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -3856,10 +3902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3886,13 +3932,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B2">
-        <v>7.6</v>
+        <v>10.8</v>
       </c>
       <c r="C2">
-        <v>3950</v>
+        <v>2990</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -3900,98 +3946,98 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="B3">
-        <v>9.1999999999999993</v>
+        <v>7.6</v>
       </c>
       <c r="C3">
-        <v>2840</v>
+        <v>3950</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>8.5</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C4">
-        <v>4700</v>
+        <v>2840</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>8.5</v>
+      </c>
+      <c r="C5">
+        <v>4700</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <f>17.8*2/3</f>
         <v>11.866666666666667</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>2010</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>10.3</v>
-      </c>
-      <c r="C6">
-        <v>690</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>7.5</v>
+        <v>10.3</v>
       </c>
       <c r="C7">
-        <v>2970</v>
+        <v>690</v>
       </c>
       <c r="D7" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="C8">
-        <v>1000</v>
+        <v>2970</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9">
-        <v>2.9</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>1090</v>
+        <v>1000</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -3999,27 +4045,27 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B10">
-        <v>7.1</v>
+        <v>2.9</v>
       </c>
       <c r="C10">
-        <v>3030</v>
+        <v>1090</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B11">
-        <v>6.5</v>
+        <v>7.1</v>
       </c>
       <c r="C11">
-        <v>1540</v>
+        <v>3030</v>
       </c>
       <c r="D11" t="s">
         <v>1</v>
@@ -4027,13 +4073,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B12">
-        <v>9.8000000000000007</v>
+        <v>6.5</v>
       </c>
       <c r="C12">
-        <v>2880</v>
+        <v>1540</v>
       </c>
       <c r="D12" t="s">
         <v>1</v>
@@ -4041,69 +4087,69 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13">
-        <v>9.6</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C13">
-        <v>3290</v>
+        <v>2880</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="B14">
-        <v>11.6</v>
+        <v>9.6</v>
       </c>
       <c r="C14">
-        <v>2660</v>
+        <v>3290</v>
       </c>
       <c r="D14" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B15">
-        <v>12.5</v>
+        <v>11.6</v>
       </c>
       <c r="C15">
-        <v>2780</v>
+        <v>2660</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>12.5</v>
       </c>
       <c r="C16">
-        <v>1680</v>
+        <v>2780</v>
       </c>
       <c r="D16" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B17">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="C17">
-        <v>1580</v>
+        <v>1680</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
@@ -4111,41 +4157,41 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B18">
-        <v>5.2</v>
+        <v>9.1</v>
       </c>
       <c r="C18">
-        <v>1000</v>
+        <v>1580</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B19">
-        <v>14</v>
+        <v>5.2</v>
       </c>
       <c r="C19">
-        <v>4800</v>
+        <v>1000</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
         <v>14</v>
       </c>
-      <c r="B20">
-        <v>12.2</v>
-      </c>
       <c r="C20">
-        <v>4120</v>
+        <v>4800</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
@@ -4153,13 +4199,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21">
-        <v>12</v>
+        <v>12.2</v>
       </c>
       <c r="C21">
-        <v>3420</v>
+        <v>4120</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -4167,127 +4213,127 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>3420</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <f>19.5/2</f>
         <v>9.75</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <f>4400*7/8</f>
         <v>3850</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23">
-        <v>5.4</v>
-      </c>
-      <c r="C23">
-        <v>1450</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B24">
-        <v>11.9</v>
+        <v>5.4</v>
       </c>
       <c r="C24">
-        <v>3160</v>
+        <v>1450</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B25">
-        <v>11.4</v>
+        <v>11.9</v>
       </c>
       <c r="C25">
-        <v>2550</v>
+        <v>3160</v>
       </c>
       <c r="D25" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26">
-        <v>8.5</v>
+        <v>11.4</v>
       </c>
       <c r="C26">
-        <v>3350</v>
+        <v>2550</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B27">
-        <v>2.8</v>
+        <v>8.5</v>
       </c>
       <c r="C27">
-        <v>880</v>
+        <v>3350</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B28">
-        <v>10.4</v>
+        <v>2.8</v>
       </c>
       <c r="C28">
-        <v>1420</v>
+        <v>880</v>
       </c>
       <c r="D28" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B29">
-        <v>0.9</v>
+        <v>10.4</v>
       </c>
       <c r="C29">
-        <v>200</v>
+        <v>1420</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B30">
-        <v>4.8</v>
+        <v>0.9</v>
       </c>
       <c r="C30">
-        <v>1260</v>
+        <v>200</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -4295,13 +4341,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B31">
-        <v>1.4</v>
+        <v>4.8</v>
       </c>
       <c r="C31">
-        <v>375</v>
+        <v>1260</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -4309,41 +4355,41 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B32">
-        <v>13.6</v>
+        <v>1.4</v>
       </c>
       <c r="C32">
-        <v>3930</v>
+        <v>375</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>13.6</v>
       </c>
       <c r="C33">
-        <v>1670</v>
+        <v>3930</v>
       </c>
       <c r="D33" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B34">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="C34">
-        <v>2400</v>
+        <v>1670</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
@@ -4351,13 +4397,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B35">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C35">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D35" t="s">
         <v>1</v>
@@ -4365,111 +4411,111 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B36">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C36">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B37">
-        <v>7.2</v>
+        <v>4.8</v>
       </c>
       <c r="C37">
-        <v>1630</v>
+        <v>1300</v>
       </c>
       <c r="D37" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="B38">
-        <v>4.8</v>
+        <v>7.2</v>
       </c>
       <c r="C38">
-        <v>1470</v>
+        <v>1630</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B39">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C39">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D39" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B40">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C40">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B41">
-        <v>2.2000000000000002</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C41">
-        <v>750</v>
+        <v>3490</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B42">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C42">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D42" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B43">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C43">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
@@ -4477,116 +4523,130 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44">
+        <v>7.3</v>
+      </c>
+      <c r="C44">
+        <v>2250</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
         <v>25</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45">
-        <v>1.2</v>
-      </c>
-      <c r="C45">
-        <v>500</v>
-      </c>
-      <c r="D45" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B46">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C46">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B47">
-        <v>6.2</v>
+        <v>11</v>
       </c>
       <c r="C47">
-        <v>1890</v>
+        <v>3060</v>
       </c>
       <c r="D47" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B48">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C48">
-        <v>180</v>
+        <v>1890</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B49">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C49">
-        <v>3550</v>
+        <v>180</v>
       </c>
       <c r="D49" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50">
+        <v>7.3</v>
+      </c>
+      <c r="C50">
+        <v>3550</v>
+      </c>
+      <c r="D50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
         <v>55</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <v>3800</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
         <v>29</v>
       </c>
-      <c r="B51">
+      <c r="B52">
         <v>6</v>
       </c>
-      <c r="C51">
+      <c r="C52">
         <v>2180</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added not-hiked Tahoma Creek entry
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2A3358-922D-43F5-8DE5-3C322F54BDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C06003-5E03-4054-AE49-FEFA612A330C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Backbone Ridge</t>
+  </si>
+  <si>
+    <t>Tahoma Creek</t>
   </si>
 </sst>
 </file>
@@ -331,7 +334,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E5EFB28-5BDE-4391-9985-EB007C5A9081}" type="CELLRANGE">
+                    <a:fld id="{40F07B33-4437-43D3-BB94-A4955BD70528}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -365,7 +368,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{80FC8114-2703-40C9-88E2-A8FD61800D1D}" type="CELLRANGE">
+                    <a:fld id="{1EA1B3BF-4F08-4A0F-A2F9-F3A89882BCDF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -399,7 +402,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DBB1E6AA-5BC1-480B-8574-C0CB60F5B33D}" type="CELLRANGE">
+                    <a:fld id="{D3AFD5CB-E196-4910-9B96-AD85F7B18BBB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -433,7 +436,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7123F7FD-4C33-4BA8-B285-EF71F61859A2}" type="CELLRANGE">
+                    <a:fld id="{21AA1695-571E-44F7-BCB1-614B5606352E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -467,7 +470,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C22D2DE2-DDEA-412E-9E8C-9070F6417F5E}" type="CELLRANGE">
+                    <a:fld id="{050951AB-C4C2-4CAD-9BF3-DFEDEBB4AFDC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -501,7 +504,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DDCF08FB-2411-4106-933D-C7EFCBF00C86}" type="CELLRANGE">
+                    <a:fld id="{88425425-8AA3-4777-B308-873922CFF36F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -535,7 +538,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A45AA860-0A37-4FB7-B628-497FD7F12D3D}" type="CELLRANGE">
+                    <a:fld id="{CEA4E905-A776-4FA0-A2E4-6E20F5990E06}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -569,7 +572,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9016758D-98DD-410C-9CFB-CACA2F8DAF04}" type="CELLRANGE">
+                    <a:fld id="{04860A98-F623-4572-87D8-3C396B41E00A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -603,7 +606,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3878C62-0C81-4E8A-85B6-B9A0A8C7DFB1}" type="CELLRANGE">
+                    <a:fld id="{1CA85C20-3D73-45F7-A62F-B988645A93DB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -637,7 +640,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7A124B87-515C-4C64-BC24-48BBD879E909}" type="CELLRANGE">
+                    <a:fld id="{CE6294A2-BEDF-4872-8501-BCFF8C1F2501}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -671,7 +674,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F619F039-450A-4A13-85DC-4ED01ABE0E14}" type="CELLRANGE">
+                    <a:fld id="{4F66C29F-18D0-4513-A12C-AC381014A827}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -705,7 +708,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F3B45C8-AEB6-4629-B0C7-0E8D0025A6B4}" type="CELLRANGE">
+                    <a:fld id="{D1A991B3-271F-4DD0-B07B-F205781E307B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -739,7 +742,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{26E8E63A-E682-47FD-B0AC-1C763465F8CB}" type="CELLRANGE">
+                    <a:fld id="{644C2C22-15EB-4BBE-8CEE-BB37A014551B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -773,7 +776,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4FEA0680-A21B-4A14-AB89-D71DC6D2043A}" type="CELLRANGE">
+                    <a:fld id="{01B17B19-0433-4ED6-AED3-1E253E61F631}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -807,7 +810,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5AAD2D13-D3FD-4EAD-9F98-FD851EF1835D}" type="CELLRANGE">
+                    <a:fld id="{EBC63716-EF6A-41C8-B9E1-3FD9C5267769}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -841,7 +844,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E6B84853-3EE3-4099-8C7C-24A107F29ED1}" type="CELLRANGE">
+                    <a:fld id="{C5BD5B5F-10F4-478B-9FAA-1D1CD84399B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -875,7 +878,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FDBF4195-4917-44F1-945D-B48DDE1044AD}" type="CELLRANGE">
+                    <a:fld id="{5965E851-F6C5-493E-BE2D-39FC8F884D5B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -909,7 +912,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6471DCF-E4AE-4AFD-BC8D-3B40E45D4B7F}" type="CELLRANGE">
+                    <a:fld id="{4CFBC859-C6A4-4631-B975-27F6F6BDC66E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -943,7 +946,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A72CC93E-50DF-4EDD-98CC-80D4F00A4EA8}" type="CELLRANGE">
+                    <a:fld id="{36EF7186-0E64-42B1-986E-BEC6CDDD88F2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -977,7 +980,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{415BD3B9-7B14-469D-B7BC-D2D15CFD1259}" type="CELLRANGE">
+                    <a:fld id="{AA4963D7-FE2D-4AB6-9904-A0224C9C7C52}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1011,7 +1014,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02894FE2-36D5-4663-8598-57052CE2DA75}" type="CELLRANGE">
+                    <a:fld id="{8F2574A7-19F6-48A5-893C-0247D9170196}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1045,7 +1048,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{799676E7-0EBD-4318-A863-4B5A87DD0035}" type="CELLRANGE">
+                    <a:fld id="{C0FC69A6-9223-4E9F-87D4-63782C72760B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1079,7 +1082,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B5351088-A981-4A0D-AE6E-1A8998904FE1}" type="CELLRANGE">
+                    <a:fld id="{E0FA7EC0-2BD9-44FB-9E29-D850881DAF5A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1113,7 +1116,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BB1BDBD-F0C3-4A2E-919A-CAEF496217AF}" type="CELLRANGE">
+                    <a:fld id="{DC04343F-D3EF-47AC-88BB-2AD1D84D5D93}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1147,7 +1150,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{51B30183-8CB5-470A-A100-51083D640D58}" type="CELLRANGE">
+                    <a:fld id="{21D61FEE-9248-4823-B461-EE326F5405D1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1181,7 +1184,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D50CF8C-E201-472B-87F1-50D91B32595D}" type="CELLRANGE">
+                    <a:fld id="{9BD9AC4F-B384-4DAA-9F7B-EB47AE9FF5DC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1215,7 +1218,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{002FC77A-DB58-476B-BAE0-9EA3C312465D}" type="CELLRANGE">
+                    <a:fld id="{5C9A20AF-3643-4550-8FE2-4398AE2E0F66}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1249,7 +1252,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D0E36D8D-217B-40C1-AA33-C882E24FAB6C}" type="CELLRANGE">
+                    <a:fld id="{C3C88CD1-46DC-4DC0-866D-DC46275167FA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1283,7 +1286,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC47074E-86A3-44C1-949B-EF48663AE6BA}" type="CELLRANGE">
+                    <a:fld id="{62C369E5-9DDA-4531-827C-C911827AEFE2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1317,7 +1320,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FADF24F6-EA1E-418F-8EFD-FB0FCAE3BD5B}" type="CELLRANGE">
+                    <a:fld id="{A175BCCD-206B-4A1F-BC4F-6A63FDB85812}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1351,7 +1354,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7CD0755E-5B3B-4148-9D9B-9E8450EE9394}" type="CELLRANGE">
+                    <a:fld id="{606C5518-BDB0-4588-B600-4DE2313AEB8E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1385,7 +1388,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{335C42AD-A601-40AA-9F9F-0B61D3135854}" type="CELLRANGE">
+                    <a:fld id="{48C9B5FF-A90C-4C0C-9755-7E325453151A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1419,7 +1422,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F9F46FD-4D72-4DB4-B9E0-3E2215444BEE}" type="CELLRANGE">
+                    <a:fld id="{88056596-5F2A-4E02-8CC7-F5576C9B48B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1453,7 +1456,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{868CF4AE-A1AC-404B-B3D7-8F8FC34D9627}" type="CELLRANGE">
+                    <a:fld id="{6184ED51-F3FC-46A3-A33B-1B6C32D832DC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1487,7 +1490,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F2D8E44E-E90B-4EA6-863B-F8C7B8A0B168}" type="CELLRANGE">
+                    <a:fld id="{4BB9D54D-3CD4-4ED2-8285-7EC1CAE9C906}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1521,7 +1524,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{61661A6B-EA8B-449A-AE2D-7ABC912483F8}" type="CELLRANGE">
+                    <a:fld id="{FF19F88C-D7FB-41FC-8173-50919640E679}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1555,7 +1558,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1A3D0EE-94D0-4309-8D09-46FCCCBA1925}" type="CELLRANGE">
+                    <a:fld id="{D53C9AA0-4D0F-44B8-ABAA-D1FD4F452E3E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1589,7 +1592,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95CE04F0-7AAC-4C44-AF53-1C6C45BC06D9}" type="CELLRANGE">
+                    <a:fld id="{D52B3C80-2D70-452D-B638-63DE8581013E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1623,7 +1626,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3577D630-B002-4F3F-9077-0E889AF07E9D}" type="CELLRANGE">
+                    <a:fld id="{C3FD8CD9-EC17-41D7-9314-19349188CE4F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1657,7 +1660,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7BC38640-AD88-4EF1-84A9-32D59E6ADB3F}" type="CELLRANGE">
+                    <a:fld id="{ED98FC21-744D-465A-9F71-D75625A41BD3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1691,7 +1694,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A8276FB-FDAA-403B-A99C-CCBAD578E07F}" type="CELLRANGE">
+                    <a:fld id="{C1DE3567-1CA4-4E77-AC1B-EDBD0B360BBE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1725,7 +1728,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CB65385-1CDA-48F7-A8F6-C9F617FFBAA5}" type="CELLRANGE">
+                    <a:fld id="{12634BE7-3374-463E-8C94-C8791F6182B1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1759,7 +1762,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8BBA14A4-7F47-4A0B-B7E6-F9C41F689C1A}" type="CELLRANGE">
+                    <a:fld id="{69BAA711-8334-4323-930E-201EB114759E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1793,7 +1796,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A51AAF32-0AC2-4D30-B890-0CC0C6CF5EAE}" type="CELLRANGE">
+                    <a:fld id="{D9913B09-A392-4A4E-8E2C-0C2CF6641E05}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1827,7 +1830,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BDEB8FAB-E7CF-4532-BBD4-B997A834E052}" type="CELLRANGE">
+                    <a:fld id="{6057DA14-361A-4199-8453-7EB42CB6EE59}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1861,7 +1864,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D6D7BD5-9AC7-4D46-B35B-2DCC702AB82E}" type="CELLRANGE">
+                    <a:fld id="{D56ADFA8-3A9A-4741-BBF1-5B85D6E351D6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1895,7 +1898,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6BCC1FD8-E711-43C0-A022-3FDA33E9075A}" type="CELLRANGE">
+                    <a:fld id="{0DFA2CB9-4A42-4A8F-BE19-9E6F9E39E0F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1929,7 +1932,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4C8C1CEE-0AC1-4D71-9A19-314DC82F0233}" type="CELLRANGE">
+                    <a:fld id="{6A14DDB6-0387-4E12-8D5C-A90B8826A051}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1963,7 +1966,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B9AE679-11C1-4D52-B030-1934828E4920}" type="CELLRANGE">
+                    <a:fld id="{E62BF42A-6336-493A-8C05-D98576812164}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1997,7 +2000,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{450161B0-6B1F-4A2E-B69C-D87A2745D684}" type="CELLRANGE">
+                    <a:fld id="{507649EA-2F2D-4D0F-9ACC-A55DF08C9EDB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2031,7 +2034,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A80AC26B-EA37-4A9B-888B-DD8DF20D0E99}" type="CELLRANGE">
+                    <a:fld id="{ADF88FA7-1026-44E0-AD0B-9D5D516D95DD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2055,6 +2058,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-A6AE-456F-B05B-25C923A280DB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="51"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{6688146B-45CE-4C49-8A1B-22D422710989}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-BF83-4087-90C3-861EB29DC37E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2104,10 +2141,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$52</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="51"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -2247,18 +2284,21 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="46">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2266,10 +2306,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$52</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="51"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -2409,18 +2449,21 @@
                   <c:v>3060</c:v>
                 </c:pt>
                 <c:pt idx="46">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2575,15 +2618,18 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="47">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="48">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="48">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="49">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="50">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="51">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3590,10 +3636,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D52" totalsRowShown="0">
-  <autoFilter ref="A1:D52" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D52">
-    <sortCondition ref="A1:A52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D53" totalsRowShown="0">
+  <autoFilter ref="A1:D53" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D53">
+    <sortCondition ref="A1:A53"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -3902,10 +3948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4581,13 +4627,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B48">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
       <c r="C48">
-        <v>1890</v>
+        <v>1650</v>
       </c>
       <c r="D48" t="s">
         <v>1</v>
@@ -4595,58 +4641,72 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B49">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C49">
-        <v>180</v>
+        <v>1890</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B50">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C50">
-        <v>3550</v>
+        <v>180</v>
       </c>
       <c r="D50" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51">
+        <v>7.3</v>
+      </c>
+      <c r="C51">
+        <v>3550</v>
+      </c>
+      <c r="D51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
         <v>55</v>
       </c>
-      <c r="B51">
+      <c r="B52">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C51">
+      <c r="C52">
         <v>3800</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
         <v>29</v>
       </c>
-      <c r="B52">
+      <c r="B53">
         <v>6</v>
       </c>
-      <c r="C52">
+      <c r="C53">
         <v>2180</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Crystal Peak trail
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C06003-5E03-4054-AE49-FEFA612A330C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0487A98E-569C-4923-972A-9ED77286D415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>Tahoma Creek</t>
+  </si>
+  <si>
+    <t>Crystal Peak</t>
   </si>
 </sst>
 </file>
@@ -334,7 +337,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40F07B33-4437-43D3-BB94-A4955BD70528}" type="CELLRANGE">
+                    <a:fld id="{5FBE7195-A86A-4A3A-B8DE-11B5F9DD2C74}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -368,7 +371,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1EA1B3BF-4F08-4A0F-A2F9-F3A89882BCDF}" type="CELLRANGE">
+                    <a:fld id="{D081C1F0-D810-4BC1-906F-87334D295925}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -402,7 +405,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3AFD5CB-E196-4910-9B96-AD85F7B18BBB}" type="CELLRANGE">
+                    <a:fld id="{8B292D05-9179-4CA0-86E2-DE0B67A32695}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -436,7 +439,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{21AA1695-571E-44F7-BCB1-614B5606352E}" type="CELLRANGE">
+                    <a:fld id="{17EF5513-BEF3-475E-9B8D-23A84EC75E9A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -470,7 +473,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{050951AB-C4C2-4CAD-9BF3-DFEDEBB4AFDC}" type="CELLRANGE">
+                    <a:fld id="{F123809E-7BD8-4154-97B1-7217557EB1AA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -504,7 +507,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88425425-8AA3-4777-B308-873922CFF36F}" type="CELLRANGE">
+                    <a:fld id="{BA502FEA-A2A8-403A-862A-426E2DE50BFC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -538,7 +541,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CEA4E905-A776-4FA0-A2E4-6E20F5990E06}" type="CELLRANGE">
+                    <a:fld id="{1E51AFF0-9B33-41DC-955E-18F398675B9F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -572,7 +575,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{04860A98-F623-4572-87D8-3C396B41E00A}" type="CELLRANGE">
+                    <a:fld id="{FC485E3B-F8D1-4D85-ADA2-B5B3C362310D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -606,7 +609,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1CA85C20-3D73-45F7-A62F-B988645A93DB}" type="CELLRANGE">
+                    <a:fld id="{F68CD838-48DD-4CD2-AEAA-7FFF067A0394}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -640,7 +643,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE6294A2-BEDF-4872-8501-BCFF8C1F2501}" type="CELLRANGE">
+                    <a:fld id="{A4994B54-6CB2-4374-A96D-92A0A0AEFF5E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -674,7 +677,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F66C29F-18D0-4513-A12C-AC381014A827}" type="CELLRANGE">
+                    <a:fld id="{E7D9AA72-E990-4965-B427-1288C322704F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -708,7 +711,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1A991B3-271F-4DD0-B07B-F205781E307B}" type="CELLRANGE">
+                    <a:fld id="{04A10D27-5281-4636-98A8-3A8849E374F1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -742,7 +745,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{644C2C22-15EB-4BBE-8CEE-BB37A014551B}" type="CELLRANGE">
+                    <a:fld id="{045B1C2B-81E8-4E97-B0C6-4225865A66A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -776,7 +779,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{01B17B19-0433-4ED6-AED3-1E253E61F631}" type="CELLRANGE">
+                    <a:fld id="{06E7E72B-E578-4ACE-AB37-E5EDCB195DF2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -810,7 +813,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EBC63716-EF6A-41C8-B9E1-3FD9C5267769}" type="CELLRANGE">
+                    <a:fld id="{A5B15D60-2489-44DA-B3C6-AF9F451AFFEB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -844,7 +847,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5BD5B5F-10F4-478B-9FAA-1D1CD84399B0}" type="CELLRANGE">
+                    <a:fld id="{78CEFD81-5074-495B-97F6-EE43FC826E76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -878,7 +881,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5965E851-F6C5-493E-BE2D-39FC8F884D5B}" type="CELLRANGE">
+                    <a:fld id="{22931DA8-40BA-4AF5-B2D3-888E0991BA35}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -912,7 +915,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4CFBC859-C6A4-4631-B975-27F6F6BDC66E}" type="CELLRANGE">
+                    <a:fld id="{5EAE10EE-DCA5-45B4-BF93-0D6A42D8C0A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -946,7 +949,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36EF7186-0E64-42B1-986E-BEC6CDDD88F2}" type="CELLRANGE">
+                    <a:fld id="{58AFC650-7324-4692-875D-260C53D447B7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -980,7 +983,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AA4963D7-FE2D-4AB6-9904-A0224C9C7C52}" type="CELLRANGE">
+                    <a:fld id="{A6E5048E-D6F8-4E08-9EDE-6FE3CA15DD1C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1014,7 +1017,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8F2574A7-19F6-48A5-893C-0247D9170196}" type="CELLRANGE">
+                    <a:fld id="{6AAB9ADE-DE95-45C5-B8EB-91638EE96425}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1048,7 +1051,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0FC69A6-9223-4E9F-87D4-63782C72760B}" type="CELLRANGE">
+                    <a:fld id="{362FE50E-73E3-4B7B-8C74-C4123CEAB455}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1082,7 +1085,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E0FA7EC0-2BD9-44FB-9E29-D850881DAF5A}" type="CELLRANGE">
+                    <a:fld id="{EB331CCD-BB04-4D6B-A334-6B9D01D23D5B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1116,7 +1119,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC04343F-D3EF-47AC-88BB-2AD1D84D5D93}" type="CELLRANGE">
+                    <a:fld id="{31C3E4D4-1717-4627-B6ED-49394EA844C2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1150,7 +1153,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{21D61FEE-9248-4823-B461-EE326F5405D1}" type="CELLRANGE">
+                    <a:fld id="{45351E47-10CD-4083-ADC9-E3784D05272F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1184,7 +1187,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BD9AC4F-B384-4DAA-9F7B-EB47AE9FF5DC}" type="CELLRANGE">
+                    <a:fld id="{713111D7-337A-4958-9E9F-ED05F0C69733}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1218,7 +1221,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C9A20AF-3643-4550-8FE2-4398AE2E0F66}" type="CELLRANGE">
+                    <a:fld id="{E49DA96B-F0CB-455E-9075-AC21CA4F289B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1252,7 +1255,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3C88CD1-46DC-4DC0-866D-DC46275167FA}" type="CELLRANGE">
+                    <a:fld id="{AD0231C2-2971-4A9A-99F0-24FD161F2036}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1286,7 +1289,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{62C369E5-9DDA-4531-827C-C911827AEFE2}" type="CELLRANGE">
+                    <a:fld id="{17A38253-64CD-4FCE-969E-CA05A4ECDD3F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1320,7 +1323,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A175BCCD-206B-4A1F-BC4F-6A63FDB85812}" type="CELLRANGE">
+                    <a:fld id="{DE6C6A1A-AFD8-4476-8FA4-8755ECC93C1A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1354,7 +1357,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{606C5518-BDB0-4588-B600-4DE2313AEB8E}" type="CELLRANGE">
+                    <a:fld id="{C654DAE3-0603-4018-8AB7-D3CFBE017E5A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1388,7 +1391,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48C9B5FF-A90C-4C0C-9755-7E325453151A}" type="CELLRANGE">
+                    <a:fld id="{992D74CD-3E42-43C7-9C78-72BCE94CF7D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1422,7 +1425,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88056596-5F2A-4E02-8CC7-F5576C9B48B2}" type="CELLRANGE">
+                    <a:fld id="{8687BA3B-C273-4E9D-A32A-B0E16CA4DFB9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1456,7 +1459,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6184ED51-F3FC-46A3-A33B-1B6C32D832DC}" type="CELLRANGE">
+                    <a:fld id="{A71CD966-3BCD-4147-BFE5-D9A619EDD5BF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1490,7 +1493,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4BB9D54D-3CD4-4ED2-8285-7EC1CAE9C906}" type="CELLRANGE">
+                    <a:fld id="{157A5967-8820-4093-A5B2-511ABC38286F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1524,7 +1527,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF19F88C-D7FB-41FC-8173-50919640E679}" type="CELLRANGE">
+                    <a:fld id="{150C5DD7-61B8-4E96-9081-4CB6D57D340D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1558,7 +1561,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D53C9AA0-4D0F-44B8-ABAA-D1FD4F452E3E}" type="CELLRANGE">
+                    <a:fld id="{31F37708-BA16-4F4E-8204-74ED34C274D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1592,7 +1595,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D52B3C80-2D70-452D-B638-63DE8581013E}" type="CELLRANGE">
+                    <a:fld id="{B02186D4-30BF-41A8-BA85-454F4216D711}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1626,7 +1629,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3FD8CD9-EC17-41D7-9314-19349188CE4F}" type="CELLRANGE">
+                    <a:fld id="{79732C66-1701-43D1-8403-6622938C9702}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1660,7 +1663,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED98FC21-744D-465A-9F71-D75625A41BD3}" type="CELLRANGE">
+                    <a:fld id="{67FFCB87-FCB2-475E-B784-26E223C009C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1694,7 +1697,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C1DE3567-1CA4-4E77-AC1B-EDBD0B360BBE}" type="CELLRANGE">
+                    <a:fld id="{1EEF3867-FC6B-4AE3-943C-EFB0B6146824}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1728,7 +1731,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12634BE7-3374-463E-8C94-C8791F6182B1}" type="CELLRANGE">
+                    <a:fld id="{ACA5C9A8-8B7D-483B-B2FC-EF423B19952C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1762,7 +1765,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69BAA711-8334-4323-930E-201EB114759E}" type="CELLRANGE">
+                    <a:fld id="{8861CCCB-B961-47B2-8243-6CDF0BCF5913}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1796,7 +1799,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D9913B09-A392-4A4E-8E2C-0C2CF6641E05}" type="CELLRANGE">
+                    <a:fld id="{5756B74E-A697-4ED5-B95A-18795272777A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1830,7 +1833,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6057DA14-361A-4199-8453-7EB42CB6EE59}" type="CELLRANGE">
+                    <a:fld id="{8554F25B-136C-4B10-9FEF-E3B4B7A76B6F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1864,7 +1867,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D56ADFA8-3A9A-4741-BBF1-5B85D6E351D6}" type="CELLRANGE">
+                    <a:fld id="{F213770E-7E91-4701-A707-54100FDC287E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1898,7 +1901,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0DFA2CB9-4A42-4A8F-BE19-9E6F9E39E0F6}" type="CELLRANGE">
+                    <a:fld id="{0547C338-57F1-4EC6-97DA-DD5CB1DDFE76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1932,7 +1935,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6A14DDB6-0387-4E12-8D5C-A90B8826A051}" type="CELLRANGE">
+                    <a:fld id="{C453C4F9-3AFB-4B9A-93A4-F6E0F1CE5C06}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1966,7 +1969,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E62BF42A-6336-493A-8C05-D98576812164}" type="CELLRANGE">
+                    <a:fld id="{FE4F77DC-AA6A-4338-B203-EC583838D01E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2000,7 +2003,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{507649EA-2F2D-4D0F-9ACC-A55DF08C9EDB}" type="CELLRANGE">
+                    <a:fld id="{7B8CFAEE-8423-4A2D-ABBD-C9349B6EADCC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2034,7 +2037,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ADF88FA7-1026-44E0-AD0B-9D5D516D95DD}" type="CELLRANGE">
+                    <a:fld id="{706C3BB2-477D-488E-A4D4-6EBB949ABFE3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2068,7 +2071,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6688146B-45CE-4C49-8A1B-22D422710989}" type="CELLRANGE">
+                    <a:fld id="{30A90AF9-6DE8-43FC-B707-F592787AF97E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2092,6 +2095,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-BF83-4087-90C3-861EB29DC37E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="52"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{F8E181A9-A42F-4CE1-948F-61F7740F5529}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-45AB-473E-877A-98336F5637E5}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2141,10 +2178,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$53</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -2167,138 +2204,141 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>2.9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>7.1</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>9.8000000000000007</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>9.6</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>11.6</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>12.5</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>9.1</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>12.2</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>9.75</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>5.4</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>11.9</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>7.2</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2306,10 +2346,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$53</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -2332,138 +2372,141 @@
                   <c:v>2970</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>3110</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>3030</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>1540</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>2880</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>3290</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>2660</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>2780</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>4800</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>4120</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>3420</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>1450</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>3160</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>880</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>1260</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>1630</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2498,13 +2541,13 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="8">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>moderate</c:v>
@@ -2513,25 +2556,25 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="12">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="14">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="15">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="16">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="17">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="19">
                     <c:v>strenuous</c:v>
@@ -2543,25 +2586,25 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="22">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="23">
+                  <c:pt idx="24">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="24">
+                  <c:pt idx="25">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="25">
+                  <c:pt idx="26">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="26">
+                  <c:pt idx="27">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="27">
+                  <c:pt idx="28">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="29">
                     <c:v>easy</c:v>
@@ -2570,10 +2613,10 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="31">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="32">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="32">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="33">
                     <c:v>moderate</c:v>
@@ -2582,54 +2625,57 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="35">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="36">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="36">
+                  <c:pt idx="37">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="37">
+                  <c:pt idx="38">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="38">
+                  <c:pt idx="39">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="39">
+                  <c:pt idx="40">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="40">
+                  <c:pt idx="41">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="41">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="42">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="43">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="44">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="44">
+                  <c:pt idx="45">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="45">
+                  <c:pt idx="46">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="46">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="47">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="48">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="49">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="49">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="50">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="51">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="52">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3636,10 +3682,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D53" totalsRowShown="0">
-  <autoFilter ref="A1:D53" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D53">
-    <sortCondition ref="A1:A53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D54" totalsRowShown="0">
+  <autoFilter ref="A1:D54" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D54">
+    <sortCondition ref="A1:A54"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -3948,10 +3994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4077,27 +4123,27 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C9">
-        <v>1000</v>
+        <v>3110</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10">
-        <v>2.9</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>1090</v>
+        <v>1000</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -4105,27 +4151,27 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B11">
-        <v>7.1</v>
+        <v>2.9</v>
       </c>
       <c r="C11">
-        <v>3030</v>
+        <v>1090</v>
       </c>
       <c r="D11" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>6.5</v>
+        <v>7.1</v>
       </c>
       <c r="C12">
-        <v>1540</v>
+        <v>3030</v>
       </c>
       <c r="D12" t="s">
         <v>1</v>
@@ -4133,13 +4179,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B13">
-        <v>9.8000000000000007</v>
+        <v>6.5</v>
       </c>
       <c r="C13">
-        <v>2880</v>
+        <v>1540</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
@@ -4147,69 +4193,69 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14">
-        <v>9.6</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C14">
-        <v>3290</v>
+        <v>2880</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="B15">
-        <v>11.6</v>
+        <v>9.6</v>
       </c>
       <c r="C15">
-        <v>2660</v>
+        <v>3290</v>
       </c>
       <c r="D15" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B16">
-        <v>12.5</v>
+        <v>11.6</v>
       </c>
       <c r="C16">
-        <v>2780</v>
+        <v>2660</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="B17">
-        <v>9</v>
+        <v>12.5</v>
       </c>
       <c r="C17">
-        <v>1680</v>
+        <v>2780</v>
       </c>
       <c r="D17" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B18">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="C18">
-        <v>1580</v>
+        <v>1680</v>
       </c>
       <c r="D18" t="s">
         <v>1</v>
@@ -4217,41 +4263,41 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B19">
-        <v>5.2</v>
+        <v>9.1</v>
       </c>
       <c r="C19">
-        <v>1000</v>
+        <v>1580</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B20">
-        <v>14</v>
+        <v>5.2</v>
       </c>
       <c r="C20">
-        <v>4800</v>
+        <v>1000</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21">
         <v>14</v>
       </c>
-      <c r="B21">
-        <v>12.2</v>
-      </c>
       <c r="C21">
-        <v>4120</v>
+        <v>4800</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -4259,13 +4305,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22">
-        <v>12</v>
+        <v>12.2</v>
       </c>
       <c r="C22">
-        <v>3420</v>
+        <v>4120</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
@@ -4273,127 +4319,127 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>3420</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <f>19.5/2</f>
         <v>9.75</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <f>4400*7/8</f>
         <v>3850</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24">
-        <v>5.4</v>
-      </c>
-      <c r="C24">
-        <v>1450</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B25">
-        <v>11.9</v>
+        <v>5.4</v>
       </c>
       <c r="C25">
-        <v>3160</v>
+        <v>1450</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B26">
-        <v>11.4</v>
+        <v>11.9</v>
       </c>
       <c r="C26">
-        <v>2550</v>
+        <v>3160</v>
       </c>
       <c r="D26" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27">
-        <v>8.5</v>
+        <v>11.4</v>
       </c>
       <c r="C27">
-        <v>3350</v>
+        <v>2550</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B28">
-        <v>2.8</v>
+        <v>8.5</v>
       </c>
       <c r="C28">
-        <v>880</v>
+        <v>3350</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B29">
-        <v>10.4</v>
+        <v>2.8</v>
       </c>
       <c r="C29">
-        <v>1420</v>
+        <v>880</v>
       </c>
       <c r="D29" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B30">
-        <v>0.9</v>
+        <v>10.4</v>
       </c>
       <c r="C30">
-        <v>200</v>
+        <v>1420</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B31">
-        <v>4.8</v>
+        <v>0.9</v>
       </c>
       <c r="C31">
-        <v>1260</v>
+        <v>200</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -4401,13 +4447,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B32">
-        <v>1.4</v>
+        <v>4.8</v>
       </c>
       <c r="C32">
-        <v>375</v>
+        <v>1260</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
@@ -4415,41 +4461,41 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B33">
-        <v>13.6</v>
+        <v>1.4</v>
       </c>
       <c r="C33">
-        <v>3930</v>
+        <v>375</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B34">
-        <v>7</v>
+        <v>13.6</v>
       </c>
       <c r="C34">
-        <v>1670</v>
+        <v>3930</v>
       </c>
       <c r="D34" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B35">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="C35">
-        <v>2400</v>
+        <v>1670</v>
       </c>
       <c r="D35" t="s">
         <v>1</v>
@@ -4457,13 +4503,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B36">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C36">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D36" t="s">
         <v>1</v>
@@ -4471,111 +4517,111 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B37">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C37">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B38">
-        <v>7.2</v>
+        <v>4.8</v>
       </c>
       <c r="C38">
-        <v>1630</v>
+        <v>1300</v>
       </c>
       <c r="D38" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="B39">
-        <v>4.8</v>
+        <v>7.2</v>
       </c>
       <c r="C39">
-        <v>1470</v>
+        <v>1630</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B40">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C40">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D40" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B41">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C41">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B42">
-        <v>2.2000000000000002</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C42">
-        <v>750</v>
+        <v>3490</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B43">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C43">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D43" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B44">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C44">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D44" t="s">
         <v>1</v>
@@ -4583,71 +4629,71 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45">
+        <v>7.3</v>
+      </c>
+      <c r="C45">
+        <v>2250</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
         <v>25</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46">
-        <v>1.2</v>
-      </c>
-      <c r="C46">
-        <v>500</v>
-      </c>
-      <c r="D46" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B47">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C47">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D47" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B48">
-        <v>6.5</v>
+        <v>11</v>
       </c>
       <c r="C48">
-        <v>1650</v>
+        <v>3060</v>
       </c>
       <c r="D48" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B49">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
       <c r="C49">
-        <v>1890</v>
+        <v>1650</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
@@ -4655,58 +4701,72 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B50">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C50">
-        <v>180</v>
+        <v>1890</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B51">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C51">
-        <v>3550</v>
+        <v>180</v>
       </c>
       <c r="D51" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
+        <v>28</v>
+      </c>
+      <c r="B52">
+        <v>7.3</v>
+      </c>
+      <c r="C52">
+        <v>3550</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
         <v>55</v>
       </c>
-      <c r="B52">
+      <c r="B53">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C52">
+      <c r="C53">
         <v>3800</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
         <v>29</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <v>6</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>2180</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Upgrade Crystal Peak to strenuous
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0487A98E-569C-4923-972A-9ED77286D415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B407576C-2F71-41EB-B76E-A82C73420BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -337,7 +337,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5FBE7195-A86A-4A3A-B8DE-11B5F9DD2C74}" type="CELLRANGE">
+                    <a:fld id="{CD2F2669-3353-4373-918D-A1D686669D4D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -371,7 +371,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D081C1F0-D810-4BC1-906F-87334D295925}" type="CELLRANGE">
+                    <a:fld id="{FAC4626C-DE4D-481F-B6AC-B4A24D57DA67}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -405,7 +405,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B292D05-9179-4CA0-86E2-DE0B67A32695}" type="CELLRANGE">
+                    <a:fld id="{0DD818C6-CC85-448C-830B-F6FFA082B703}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -439,7 +439,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17EF5513-BEF3-475E-9B8D-23A84EC75E9A}" type="CELLRANGE">
+                    <a:fld id="{A7823DBD-6482-4B63-95A8-FB7DBBD82D2E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -473,7 +473,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F123809E-7BD8-4154-97B1-7217557EB1AA}" type="CELLRANGE">
+                    <a:fld id="{9F0B7C28-8A13-4171-A382-44A78AC65407}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -507,7 +507,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BA502FEA-A2A8-403A-862A-426E2DE50BFC}" type="CELLRANGE">
+                    <a:fld id="{AA02EDBB-A52E-4380-A82B-B8C026CB6652}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -541,7 +541,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1E51AFF0-9B33-41DC-955E-18F398675B9F}" type="CELLRANGE">
+                    <a:fld id="{D3E07BFE-E29D-4454-9096-BC179DA5F34E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -575,7 +575,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC485E3B-F8D1-4D85-ADA2-B5B3C362310D}" type="CELLRANGE">
+                    <a:fld id="{27016270-5E3B-4E6A-8D47-9B4A066EE2E1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -609,7 +609,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F68CD838-48DD-4CD2-AEAA-7FFF067A0394}" type="CELLRANGE">
+                    <a:fld id="{5F458672-9C4C-4606-89E6-5C16B266E7CF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -643,7 +643,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A4994B54-6CB2-4374-A96D-92A0A0AEFF5E}" type="CELLRANGE">
+                    <a:fld id="{73F05EDA-6C38-423D-953A-AD7935744200}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -677,7 +677,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7D9AA72-E990-4965-B427-1288C322704F}" type="CELLRANGE">
+                    <a:fld id="{572685EA-0FFD-4059-B8BC-7555871CF7A5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -711,7 +711,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{04A10D27-5281-4636-98A8-3A8849E374F1}" type="CELLRANGE">
+                    <a:fld id="{F0F30F77-89B1-4726-953B-855232F39F1A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -745,7 +745,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{045B1C2B-81E8-4E97-B0C6-4225865A66A8}" type="CELLRANGE">
+                    <a:fld id="{DE243EAF-72C8-4A8D-84E1-2C4FC5BB31DD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -779,7 +779,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06E7E72B-E578-4ACE-AB37-E5EDCB195DF2}" type="CELLRANGE">
+                    <a:fld id="{98852EEA-7CE5-4D7F-B299-9BF4708D098B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -813,7 +813,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5B15D60-2489-44DA-B3C6-AF9F451AFFEB}" type="CELLRANGE">
+                    <a:fld id="{C44E87C2-96BF-49ED-B91E-C664965564E6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -847,7 +847,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{78CEFD81-5074-495B-97F6-EE43FC826E76}" type="CELLRANGE">
+                    <a:fld id="{9623E32B-1035-41CA-BD52-0A29CC0075F0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -881,7 +881,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{22931DA8-40BA-4AF5-B2D3-888E0991BA35}" type="CELLRANGE">
+                    <a:fld id="{1FA5E1EA-9B8E-4964-A100-A7AEE20B13A2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -915,7 +915,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5EAE10EE-DCA5-45B4-BF93-0D6A42D8C0A8}" type="CELLRANGE">
+                    <a:fld id="{23CA3866-E524-4A20-B0C6-8E536D9223EF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -949,7 +949,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58AFC650-7324-4692-875D-260C53D447B7}" type="CELLRANGE">
+                    <a:fld id="{20F80C9B-B7EC-4792-BD5C-C05D1740A727}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -983,7 +983,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A6E5048E-D6F8-4E08-9EDE-6FE3CA15DD1C}" type="CELLRANGE">
+                    <a:fld id="{1C25B628-99C9-4E4A-BB88-7668FCDCF943}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1017,7 +1017,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6AAB9ADE-DE95-45C5-B8EB-91638EE96425}" type="CELLRANGE">
+                    <a:fld id="{1C5476E8-8B60-41AD-8058-CCA8363D8903}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1051,7 +1051,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{362FE50E-73E3-4B7B-8C74-C4123CEAB455}" type="CELLRANGE">
+                    <a:fld id="{A6E89E4E-C8FC-4D67-846E-700DFF298375}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1085,7 +1085,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB331CCD-BB04-4D6B-A334-6B9D01D23D5B}" type="CELLRANGE">
+                    <a:fld id="{543C0102-1B5F-48F2-8AC8-9A26FB6D1FD5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1119,7 +1119,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{31C3E4D4-1717-4627-B6ED-49394EA844C2}" type="CELLRANGE">
+                    <a:fld id="{3B2F6718-4AA7-4179-A06E-17A8C96F0F30}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1153,7 +1153,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{45351E47-10CD-4083-ADC9-E3784D05272F}" type="CELLRANGE">
+                    <a:fld id="{1CC0D210-EE80-4CE7-9062-ADFB04F15EF0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1187,7 +1187,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{713111D7-337A-4958-9E9F-ED05F0C69733}" type="CELLRANGE">
+                    <a:fld id="{B86C067C-ECC4-4448-84DE-D332F6156D05}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1221,7 +1221,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E49DA96B-F0CB-455E-9075-AC21CA4F289B}" type="CELLRANGE">
+                    <a:fld id="{660389C8-61A8-4207-9199-E175D2C51716}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1255,7 +1255,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD0231C2-2971-4A9A-99F0-24FD161F2036}" type="CELLRANGE">
+                    <a:fld id="{D525177C-E9FA-4DCF-8F9A-A852DE73B247}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1289,7 +1289,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17A38253-64CD-4FCE-969E-CA05A4ECDD3F}" type="CELLRANGE">
+                    <a:fld id="{5E189731-BE69-49B1-BB5E-633E1F3D5312}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1323,7 +1323,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE6C6A1A-AFD8-4476-8FA4-8755ECC93C1A}" type="CELLRANGE">
+                    <a:fld id="{808AA1CD-A3B5-4CA0-A17A-09EA3FAE9668}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1357,7 +1357,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C654DAE3-0603-4018-8AB7-D3CFBE017E5A}" type="CELLRANGE">
+                    <a:fld id="{39D2EE33-7142-481F-B9B0-D9A2C9E31005}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1391,7 +1391,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{992D74CD-3E42-43C7-9C78-72BCE94CF7D0}" type="CELLRANGE">
+                    <a:fld id="{8210932D-1C2A-43AD-B808-65CF0B6B6262}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1425,7 +1425,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8687BA3B-C273-4E9D-A32A-B0E16CA4DFB9}" type="CELLRANGE">
+                    <a:fld id="{06FE7701-8235-45F0-B02B-F14BCD19842B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1459,7 +1459,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A71CD966-3BCD-4147-BFE5-D9A619EDD5BF}" type="CELLRANGE">
+                    <a:fld id="{AC41F49E-A056-4BF3-B9D2-02E79BA71AEA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1493,7 +1493,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{157A5967-8820-4093-A5B2-511ABC38286F}" type="CELLRANGE">
+                    <a:fld id="{6C3C4A85-9B09-477A-BCEC-CF3A3D891F43}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1527,7 +1527,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{150C5DD7-61B8-4E96-9081-4CB6D57D340D}" type="CELLRANGE">
+                    <a:fld id="{D3123287-606F-46AE-8351-6E0895A797CC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1561,7 +1561,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{31F37708-BA16-4F4E-8204-74ED34C274D8}" type="CELLRANGE">
+                    <a:fld id="{27B733BF-7EE1-4279-BB8B-D895103DEEF5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1595,7 +1595,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B02186D4-30BF-41A8-BA85-454F4216D711}" type="CELLRANGE">
+                    <a:fld id="{CFD76D8A-1372-4172-AB62-1F258629AF08}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1629,7 +1629,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79732C66-1701-43D1-8403-6622938C9702}" type="CELLRANGE">
+                    <a:fld id="{848FCC92-29E3-43BF-B201-DC4331869903}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1663,7 +1663,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67FFCB87-FCB2-475E-B784-26E223C009C5}" type="CELLRANGE">
+                    <a:fld id="{F5444D1E-208F-41D9-842D-E26E229B52F4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1697,7 +1697,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1EEF3867-FC6B-4AE3-943C-EFB0B6146824}" type="CELLRANGE">
+                    <a:fld id="{5D2F67B6-831C-490A-AC59-964E7434DBD3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1731,7 +1731,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ACA5C9A8-8B7D-483B-B2FC-EF423B19952C}" type="CELLRANGE">
+                    <a:fld id="{BCB52C50-085E-4403-B750-8EB9F6E4E4BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1765,7 +1765,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8861CCCB-B961-47B2-8243-6CDF0BCF5913}" type="CELLRANGE">
+                    <a:fld id="{91FED40B-E6B8-4C10-A3E5-58513E8A24D5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1799,7 +1799,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5756B74E-A697-4ED5-B95A-18795272777A}" type="CELLRANGE">
+                    <a:fld id="{36D953F6-1EFF-4B8B-8C11-6A4D8F65E304}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1833,7 +1833,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8554F25B-136C-4B10-9FEF-E3B4B7A76B6F}" type="CELLRANGE">
+                    <a:fld id="{0B444287-B2B0-4D85-A2A9-F35E229DDBCF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1867,7 +1867,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F213770E-7E91-4701-A707-54100FDC287E}" type="CELLRANGE">
+                    <a:fld id="{2F05E8B3-8812-48B7-B88F-905C4447BA8D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1901,7 +1901,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0547C338-57F1-4EC6-97DA-DD5CB1DDFE76}" type="CELLRANGE">
+                    <a:fld id="{DA2FB6DC-74B7-401F-AC8F-F7B620C2E894}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1935,7 +1935,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C453C4F9-3AFB-4B9A-93A4-F6E0F1CE5C06}" type="CELLRANGE">
+                    <a:fld id="{3FA5881C-8588-4CE5-B71F-A454F0C0E92F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1969,7 +1969,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FE4F77DC-AA6A-4338-B203-EC583838D01E}" type="CELLRANGE">
+                    <a:fld id="{534FB94C-7709-4A38-BD47-B2532DCDBEA6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2003,7 +2003,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7B8CFAEE-8423-4A2D-ABBD-C9349B6EADCC}" type="CELLRANGE">
+                    <a:fld id="{A4D315C4-5491-413C-AF97-E49FF2D16EC5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2037,7 +2037,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{706C3BB2-477D-488E-A4D4-6EBB949ABFE3}" type="CELLRANGE">
+                    <a:fld id="{5824FF2D-3CA0-49CE-B4BF-1B4E224F6034}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2071,7 +2071,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{30A90AF9-6DE8-43FC-B707-F592787AF97E}" type="CELLRANGE">
+                    <a:fld id="{369BA944-43D9-4B76-ACD7-4400CCAFD59E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2105,7 +2105,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8E181A9-A42F-4CE1-948F-61F7740F5529}" type="CELLRANGE">
+                    <a:fld id="{147A401D-7CA8-40B0-95C1-CC6B1387F6E3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2541,7 +2541,7 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="8">
                     <c:v>easy</c:v>
@@ -3630,36 +3630,74 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>119063</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>52388</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>176213</xdr:rowOff>
+      <xdr:rowOff>61913</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="Straight Connector 11">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Freeform: Shape 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{108EB0C1-AEA3-465B-9817-63D9CEFA7709}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31FA77EC-1766-4C15-A73B-C6F56F0B2620}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7115175" y="2290763"/>
-          <a:ext cx="5695950" cy="1504950"/>
+          <a:off x="8053388" y="2971800"/>
+          <a:ext cx="4348162" cy="709613"/>
         </a:xfrm>
-        <a:prstGeom prst="line">
+        <a:custGeom>
           <a:avLst/>
-        </a:prstGeom>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 4348162 w 4348162"/>
+            <a:gd name="connsiteY0" fmla="*/ 709613 h 709613"/>
+            <a:gd name="connsiteX1" fmla="*/ 2562225 w 4348162"/>
+            <a:gd name="connsiteY1" fmla="*/ 276225 h 709613"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 4348162"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 709613"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="4348162" h="709613">
+              <a:moveTo>
+                <a:pt x="4348162" y="709613"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="3817540" y="552053"/>
+                <a:pt x="3286919" y="394494"/>
+                <a:pt x="2562225" y="276225"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1837531" y="157956"/>
+                <a:pt x="918765" y="78978"/>
+                <a:pt x="0" y="0"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -3675,7 +3713,15 @@
           <a:schemeClr val="tx1"/>
         </a:fontRef>
       </xdr:style>
-    </xdr:cxnSp>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3997,7 +4043,7 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4132,7 +4178,7 @@
         <v>3110</v>
       </c>
       <c r="D9" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Add Owyhigh Lakes from Deer Creek
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B407576C-2F71-41EB-B76E-A82C73420BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506F7B17-3092-47D2-88AC-7F3B3EDA0193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hike Difficulties" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="63">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Crystal Peak</t>
+  </si>
+  <si>
+    <t>Owyhigh Lakes from Deer Creek</t>
   </si>
 </sst>
 </file>
@@ -337,7 +340,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD2F2669-3353-4373-918D-A1D686669D4D}" type="CELLRANGE">
+                    <a:fld id="{1A3394B2-B4B0-4A1F-8E63-548655E016D2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -371,7 +374,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FAC4626C-DE4D-481F-B6AC-B4A24D57DA67}" type="CELLRANGE">
+                    <a:fld id="{871706F4-CC12-41AC-BC14-E3C1A7DADCFD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -405,7 +408,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0DD818C6-CC85-448C-830B-F6FFA082B703}" type="CELLRANGE">
+                    <a:fld id="{DE9DE608-0A34-48B1-BA1F-59AF5AECA0F7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -439,7 +442,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A7823DBD-6482-4B63-95A8-FB7DBBD82D2E}" type="CELLRANGE">
+                    <a:fld id="{D8122DF1-6EF7-4299-A660-804F160A6504}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -473,7 +476,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F0B7C28-8A13-4171-A382-44A78AC65407}" type="CELLRANGE">
+                    <a:fld id="{70968629-5CE0-4100-A33F-722CF74BEC97}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -507,7 +510,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AA02EDBB-A52E-4380-A82B-B8C026CB6652}" type="CELLRANGE">
+                    <a:fld id="{0F3D9EAF-85BB-4745-AF0E-4A49257B1295}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -541,7 +544,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3E07BFE-E29D-4454-9096-BC179DA5F34E}" type="CELLRANGE">
+                    <a:fld id="{A47295C7-DD67-413A-8D18-8B50CB12388B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -575,7 +578,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{27016270-5E3B-4E6A-8D47-9B4A066EE2E1}" type="CELLRANGE">
+                    <a:fld id="{093FF62D-6740-414B-8368-D9C0A8D13925}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -609,7 +612,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F458672-9C4C-4606-89E6-5C16B266E7CF}" type="CELLRANGE">
+                    <a:fld id="{E5768308-CCC5-4D13-B829-E5899421C83B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -643,7 +646,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73F05EDA-6C38-423D-953A-AD7935744200}" type="CELLRANGE">
+                    <a:fld id="{61451198-AF63-43C9-A999-59FC825D776A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -677,7 +680,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{572685EA-0FFD-4059-B8BC-7555871CF7A5}" type="CELLRANGE">
+                    <a:fld id="{0AE5FFB0-C95D-4FED-B90E-DA68E2183A6C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -711,7 +714,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0F30F77-89B1-4726-953B-855232F39F1A}" type="CELLRANGE">
+                    <a:fld id="{4E4E7457-565C-4E05-8717-35CC086E858E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -745,7 +748,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE243EAF-72C8-4A8D-84E1-2C4FC5BB31DD}" type="CELLRANGE">
+                    <a:fld id="{F2A02B86-3F6C-4E33-B7CA-7DFF762EC4BF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -779,7 +782,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{98852EEA-7CE5-4D7F-B299-9BF4708D098B}" type="CELLRANGE">
+                    <a:fld id="{815E6F84-D271-40CA-9315-5C0C2AA9EB18}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -813,7 +816,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C44E87C2-96BF-49ED-B91E-C664965564E6}" type="CELLRANGE">
+                    <a:fld id="{823FD3B1-1967-45DF-8BCF-5C491C16010D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -847,7 +850,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9623E32B-1035-41CA-BD52-0A29CC0075F0}" type="CELLRANGE">
+                    <a:fld id="{C8C71C66-2FA8-47DB-8D5E-48F69B308FA7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -881,7 +884,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1FA5E1EA-9B8E-4964-A100-A7AEE20B13A2}" type="CELLRANGE">
+                    <a:fld id="{A4D4CAC5-2791-4256-9095-7DFFDDE0800C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -915,7 +918,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23CA3866-E524-4A20-B0C6-8E536D9223EF}" type="CELLRANGE">
+                    <a:fld id="{32FD09FF-28FE-4532-A72A-5D06A5F81C52}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -949,7 +952,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{20F80C9B-B7EC-4792-BD5C-C05D1740A727}" type="CELLRANGE">
+                    <a:fld id="{80486582-3309-419E-BB5B-7A5760719F8A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -983,7 +986,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C25B628-99C9-4E4A-BB88-7668FCDCF943}" type="CELLRANGE">
+                    <a:fld id="{A60F1957-B59A-4580-94EC-68FF1CA58AFB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1017,7 +1020,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C5476E8-8B60-41AD-8058-CCA8363D8903}" type="CELLRANGE">
+                    <a:fld id="{26FB6D2D-5A80-4389-ADFC-7EA3583C9D0F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1051,7 +1054,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A6E89E4E-C8FC-4D67-846E-700DFF298375}" type="CELLRANGE">
+                    <a:fld id="{C78548DE-EC44-4854-817F-03A38EC397AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1085,7 +1088,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{543C0102-1B5F-48F2-8AC8-9A26FB6D1FD5}" type="CELLRANGE">
+                    <a:fld id="{C5014418-8659-4498-B180-768F84A74C6E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1119,7 +1122,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B2F6718-4AA7-4179-A06E-17A8C96F0F30}" type="CELLRANGE">
+                    <a:fld id="{E7963468-89FA-46B8-953D-737491FAA438}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1153,7 +1156,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1CC0D210-EE80-4CE7-9062-ADFB04F15EF0}" type="CELLRANGE">
+                    <a:fld id="{2A418A89-9723-408D-ADC0-57D99185ADE0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1187,7 +1190,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B86C067C-ECC4-4448-84DE-D332F6156D05}" type="CELLRANGE">
+                    <a:fld id="{64140D32-3709-4A75-9B65-FBF4EDBAF771}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1221,7 +1224,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{660389C8-61A8-4207-9199-E175D2C51716}" type="CELLRANGE">
+                    <a:fld id="{C54CB679-95D1-4AB7-A38B-587B3E309C9B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1255,7 +1258,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D525177C-E9FA-4DCF-8F9A-A852DE73B247}" type="CELLRANGE">
+                    <a:fld id="{5F0BA4F8-7E4A-4141-BF08-963D070EA2DF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1289,7 +1292,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5E189731-BE69-49B1-BB5E-633E1F3D5312}" type="CELLRANGE">
+                    <a:fld id="{14E0EBD1-1D39-40AB-B881-264214C8A2EA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1323,7 +1326,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{808AA1CD-A3B5-4CA0-A17A-09EA3FAE9668}" type="CELLRANGE">
+                    <a:fld id="{3FDB27BF-DA10-480B-BBB8-241B2E3082D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1357,7 +1360,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{39D2EE33-7142-481F-B9B0-D9A2C9E31005}" type="CELLRANGE">
+                    <a:fld id="{90ED0ADF-66DF-4CC9-83F5-A64EF5C944D6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1391,7 +1394,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8210932D-1C2A-43AD-B808-65CF0B6B6262}" type="CELLRANGE">
+                    <a:fld id="{008711DE-3B10-46C3-9A15-203C509C6784}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1425,7 +1428,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06FE7701-8235-45F0-B02B-F14BCD19842B}" type="CELLRANGE">
+                    <a:fld id="{575179EB-BC4F-47D5-B30C-1C374F169275}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1459,7 +1462,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AC41F49E-A056-4BF3-B9D2-02E79BA71AEA}" type="CELLRANGE">
+                    <a:fld id="{A001CC7E-A791-4132-864D-6164EC7C3C1B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1493,7 +1496,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C3C4A85-9B09-477A-BCEC-CF3A3D891F43}" type="CELLRANGE">
+                    <a:fld id="{5E5D952F-9E35-46D5-9092-4BF73EB52F66}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1527,7 +1530,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3123287-606F-46AE-8351-6E0895A797CC}" type="CELLRANGE">
+                    <a:fld id="{5B874C62-1EB5-4055-88C8-1DCD914C380D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1561,7 +1564,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{27B733BF-7EE1-4279-BB8B-D895103DEEF5}" type="CELLRANGE">
+                    <a:fld id="{5CB2C09B-D499-4801-B53D-3CE8F5C5FEA6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1595,7 +1598,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CFD76D8A-1372-4172-AB62-1F258629AF08}" type="CELLRANGE">
+                    <a:fld id="{5076FB9F-0EB9-43AE-AD69-5477C2D3B218}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1629,7 +1632,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{848FCC92-29E3-43BF-B201-DC4331869903}" type="CELLRANGE">
+                    <a:fld id="{E569D8E0-DBDE-4252-AA16-3105C017A319}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1663,7 +1666,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5444D1E-208F-41D9-842D-E26E229B52F4}" type="CELLRANGE">
+                    <a:fld id="{C017FF31-AC92-498C-9009-8B96A4F441EF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1697,7 +1700,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D2F67B6-831C-490A-AC59-964E7434DBD3}" type="CELLRANGE">
+                    <a:fld id="{A290E757-AB6E-482D-85D3-00A40DEEF286}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1731,7 +1734,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BCB52C50-085E-4403-B750-8EB9F6E4E4BA}" type="CELLRANGE">
+                    <a:fld id="{DD4E4851-9FE4-4422-8BC6-2E56D2498C7F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1765,7 +1768,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91FED40B-E6B8-4C10-A3E5-58513E8A24D5}" type="CELLRANGE">
+                    <a:fld id="{10394A75-3B06-4896-AD04-E5D8B32BC497}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1799,7 +1802,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36D953F6-1EFF-4B8B-8C11-6A4D8F65E304}" type="CELLRANGE">
+                    <a:fld id="{3102D146-F1C5-4156-A8FA-FDABE523421D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1833,7 +1836,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0B444287-B2B0-4D85-A2A9-F35E229DDBCF}" type="CELLRANGE">
+                    <a:fld id="{7AF294EB-7252-499D-B01A-37DDFFE1A901}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1867,7 +1870,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F05E8B3-8812-48B7-B88F-905C4447BA8D}" type="CELLRANGE">
+                    <a:fld id="{A5FA6E5F-5C86-4351-A4F1-395620BA3791}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1901,7 +1904,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DA2FB6DC-74B7-401F-AC8F-F7B620C2E894}" type="CELLRANGE">
+                    <a:fld id="{36425DA0-2F27-4005-A18F-C7DB4C170297}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1935,7 +1938,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3FA5881C-8588-4CE5-B71F-A454F0C0E92F}" type="CELLRANGE">
+                    <a:fld id="{2479AA1D-D9EF-4F7D-BD52-041BE679D175}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1969,7 +1972,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{534FB94C-7709-4A38-BD47-B2532DCDBEA6}" type="CELLRANGE">
+                    <a:fld id="{D339FE87-5E3B-45AE-BE9C-E7C801F6916A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2003,7 +2006,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A4D315C4-5491-413C-AF97-E49FF2D16EC5}" type="CELLRANGE">
+                    <a:fld id="{E788DB98-38E3-4238-A214-60E3494FC07E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2037,7 +2040,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5824FF2D-3CA0-49CE-B4BF-1B4E224F6034}" type="CELLRANGE">
+                    <a:fld id="{9D27CA1A-C96C-42AE-9FDE-AC151A330B99}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2071,7 +2074,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{369BA944-43D9-4B76-ACD7-4400CCAFD59E}" type="CELLRANGE">
+                    <a:fld id="{E3AA39D1-7FB9-4556-BA4D-CF17322CB63C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2105,7 +2108,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{147A401D-7CA8-40B0-95C1-CC6B1387F6E3}" type="CELLRANGE">
+                    <a:fld id="{AFC07119-73A3-4C7A-98A3-22EF0136A66F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2129,6 +2132,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-45AB-473E-877A-98336F5637E5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="53"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7041583C-8E9E-430D-920E-8F60CA280B62}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-1E06-4B7E-8BFA-5AA13E5BF977}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2178,10 +2215,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$54</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="54"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -2282,63 +2319,66 @@
                   <c:v>13.6</c:v>
                 </c:pt>
                 <c:pt idx="33">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>7.2</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2346,10 +2386,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$54</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="54"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -2450,63 +2490,66 @@
                   <c:v>3930</c:v>
                 </c:pt>
                 <c:pt idx="33">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>1630</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2619,7 +2662,7 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="33">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="34">
                     <c:v>moderate</c:v>
@@ -2628,54 +2671,57 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="36">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="37">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="37">
+                  <c:pt idx="38">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="38">
+                  <c:pt idx="39">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="39">
+                  <c:pt idx="40">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="40">
+                  <c:pt idx="41">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="41">
+                  <c:pt idx="42">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="42">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="43">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="44">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="45">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="45">
+                  <c:pt idx="46">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="46">
+                  <c:pt idx="47">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="47">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="48">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="49">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="50">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="50">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="51">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="52">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="53">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3728,10 +3774,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D54" totalsRowShown="0">
-  <autoFilter ref="A1:D54" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D54">
-    <sortCondition ref="A1:A54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D55" totalsRowShown="0">
+  <autoFilter ref="A1:D55" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D55">
+    <sortCondition ref="A1:A55"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -4040,10 +4086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4535,27 +4581,27 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B35">
-        <v>7</v>
+        <v>10.5</v>
       </c>
       <c r="C35">
-        <v>1670</v>
+        <v>3100</v>
       </c>
       <c r="D35" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="C36">
-        <v>2400</v>
+        <v>1670</v>
       </c>
       <c r="D36" t="s">
         <v>1</v>
@@ -4563,13 +4609,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B37">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C37">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D37" t="s">
         <v>1</v>
@@ -4577,111 +4623,111 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B38">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C38">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B39">
-        <v>7.2</v>
+        <v>4.8</v>
       </c>
       <c r="C39">
-        <v>1630</v>
+        <v>1300</v>
       </c>
       <c r="D39" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="B40">
-        <v>4.8</v>
+        <v>7.2</v>
       </c>
       <c r="C40">
-        <v>1470</v>
+        <v>1630</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B41">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C41">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D41" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B42">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C42">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B43">
-        <v>2.2000000000000002</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C43">
-        <v>750</v>
+        <v>3490</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B44">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C44">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D44" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B45">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C45">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D45" t="s">
         <v>1</v>
@@ -4689,71 +4735,71 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <v>7.3</v>
+      </c>
+      <c r="C46">
+        <v>2250</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
         <v>25</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47">
-        <v>1.2</v>
-      </c>
-      <c r="C47">
-        <v>500</v>
-      </c>
-      <c r="D47" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B48">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C48">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D48" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B49">
-        <v>6.5</v>
+        <v>11</v>
       </c>
       <c r="C49">
-        <v>1650</v>
+        <v>3060</v>
       </c>
       <c r="D49" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B50">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
       <c r="C50">
-        <v>1890</v>
+        <v>1650</v>
       </c>
       <c r="D50" t="s">
         <v>1</v>
@@ -4761,58 +4807,72 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B51">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C51">
-        <v>180</v>
+        <v>1890</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B52">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C52">
-        <v>3550</v>
+        <v>180</v>
       </c>
       <c r="D52" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53">
+        <v>7.3</v>
+      </c>
+      <c r="C53">
+        <v>3550</v>
+      </c>
+      <c r="D53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
         <v>55</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>3800</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
         <v>29</v>
       </c>
-      <c r="B54">
+      <c r="B55">
         <v>6</v>
       </c>
-      <c r="C54">
+      <c r="C55">
         <v>2180</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add West Fork White River
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506F7B17-3092-47D2-88AC-7F3B3EDA0193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A61DEB-9BC5-4B5D-BE22-712B603B36F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Owyhigh Lakes from Deer Creek</t>
+  </si>
+  <si>
+    <t>West Fork White River</t>
   </si>
 </sst>
 </file>
@@ -340,7 +343,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A3394B2-B4B0-4A1F-8E63-548655E016D2}" type="CELLRANGE">
+                    <a:fld id="{9503CD4A-13B0-4637-BEAC-7422AFDACD37}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -374,7 +377,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{871706F4-CC12-41AC-BC14-E3C1A7DADCFD}" type="CELLRANGE">
+                    <a:fld id="{29309738-E910-4628-919A-1400DEF6533C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -408,7 +411,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE9DE608-0A34-48B1-BA1F-59AF5AECA0F7}" type="CELLRANGE">
+                    <a:fld id="{D1A797C8-F792-4A45-AFAB-BE565B9F3352}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -442,7 +445,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8122DF1-6EF7-4299-A660-804F160A6504}" type="CELLRANGE">
+                    <a:fld id="{CC29263C-D047-4BEF-8C65-CB85FEEA2B81}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -476,7 +479,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70968629-5CE0-4100-A33F-722CF74BEC97}" type="CELLRANGE">
+                    <a:fld id="{9EDC3C2A-C38B-4EE1-9739-6418F89526CC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -510,7 +513,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F3D9EAF-85BB-4745-AF0E-4A49257B1295}" type="CELLRANGE">
+                    <a:fld id="{D1E22B7A-BBDC-4A4A-A483-24585C38489F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -544,7 +547,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A47295C7-DD67-413A-8D18-8B50CB12388B}" type="CELLRANGE">
+                    <a:fld id="{9406FF57-96DA-44F9-89B3-2D0D09479858}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -578,7 +581,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{093FF62D-6740-414B-8368-D9C0A8D13925}" type="CELLRANGE">
+                    <a:fld id="{BDF501B0-2C46-479E-80BC-29696BDDA3F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -612,7 +615,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E5768308-CCC5-4D13-B829-E5899421C83B}" type="CELLRANGE">
+                    <a:fld id="{4DDF1F9F-0DAC-4184-9A08-1D067C8B1163}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -646,7 +649,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{61451198-AF63-43C9-A999-59FC825D776A}" type="CELLRANGE">
+                    <a:fld id="{6D640914-4B67-42D7-8FAB-B1B27B4CE440}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -680,7 +683,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0AE5FFB0-C95D-4FED-B90E-DA68E2183A6C}" type="CELLRANGE">
+                    <a:fld id="{B378F913-EECD-41A3-B900-7029216013F0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -714,7 +717,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E4E7457-565C-4E05-8717-35CC086E858E}" type="CELLRANGE">
+                    <a:fld id="{D9ECEA4E-8A98-4885-84AE-DEEC7A371B1C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -748,7 +751,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F2A02B86-3F6C-4E33-B7CA-7DFF762EC4BF}" type="CELLRANGE">
+                    <a:fld id="{F03A7C7C-4820-4C8A-814B-2611EDDBAC08}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -782,7 +785,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{815E6F84-D271-40CA-9315-5C0C2AA9EB18}" type="CELLRANGE">
+                    <a:fld id="{8FE4FF0D-B6A4-4C7B-8917-E3F390618608}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -816,7 +819,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{823FD3B1-1967-45DF-8BCF-5C491C16010D}" type="CELLRANGE">
+                    <a:fld id="{F17C5161-493A-42EA-9EF1-88E5C2044E06}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -850,7 +853,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C8C71C66-2FA8-47DB-8D5E-48F69B308FA7}" type="CELLRANGE">
+                    <a:fld id="{16FE3356-6839-4289-A44F-F61A4CBB6DC7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -884,7 +887,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A4D4CAC5-2791-4256-9095-7DFFDDE0800C}" type="CELLRANGE">
+                    <a:fld id="{DE0C63D3-9ADB-406D-B7D9-A55E52812717}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -918,7 +921,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32FD09FF-28FE-4532-A72A-5D06A5F81C52}" type="CELLRANGE">
+                    <a:fld id="{503D8975-4824-45B8-9857-C64DC8C84679}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -952,7 +955,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{80486582-3309-419E-BB5B-7A5760719F8A}" type="CELLRANGE">
+                    <a:fld id="{D0926B54-64E5-44EF-A0E2-480CF6546027}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -986,7 +989,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A60F1957-B59A-4580-94EC-68FF1CA58AFB}" type="CELLRANGE">
+                    <a:fld id="{72AE9149-981F-4064-909B-49D5718358EF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1020,7 +1023,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{26FB6D2D-5A80-4389-ADFC-7EA3583C9D0F}" type="CELLRANGE">
+                    <a:fld id="{8BAABCD7-9620-42FE-B5ED-831612C3C11F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1054,7 +1057,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C78548DE-EC44-4854-817F-03A38EC397AC}" type="CELLRANGE">
+                    <a:fld id="{7DD34C7B-B279-4782-8867-FBC234C572D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1088,7 +1091,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5014418-8659-4498-B180-768F84A74C6E}" type="CELLRANGE">
+                    <a:fld id="{FC2D52BE-B8F1-4613-B325-06407C643FE4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1122,7 +1125,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7963468-89FA-46B8-953D-737491FAA438}" type="CELLRANGE">
+                    <a:fld id="{A9EBFF2B-CA49-444E-AE11-BB274FBAA64A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1156,7 +1159,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A418A89-9723-408D-ADC0-57D99185ADE0}" type="CELLRANGE">
+                    <a:fld id="{3AE41A9A-F378-4C30-91C5-C19F101803D2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1190,7 +1193,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{64140D32-3709-4A75-9B65-FBF4EDBAF771}" type="CELLRANGE">
+                    <a:fld id="{03DD53FD-776C-4363-942A-4C3054323733}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1224,7 +1227,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C54CB679-95D1-4AB7-A38B-587B3E309C9B}" type="CELLRANGE">
+                    <a:fld id="{B3299E44-2A2C-444B-B042-31F786703E41}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1258,7 +1261,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F0BA4F8-7E4A-4141-BF08-963D070EA2DF}" type="CELLRANGE">
+                    <a:fld id="{4D7275CB-CDB4-4AD2-986F-2B7154C28868}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1292,7 +1295,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14E0EBD1-1D39-40AB-B881-264214C8A2EA}" type="CELLRANGE">
+                    <a:fld id="{CAD215F9-5981-4DE2-B188-DB68DD6B135C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1326,7 +1329,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3FDB27BF-DA10-480B-BBB8-241B2E3082D7}" type="CELLRANGE">
+                    <a:fld id="{B15F46D1-7E05-477E-AB7D-C9AE6BB8B923}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1360,7 +1363,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{90ED0ADF-66DF-4CC9-83F5-A64EF5C944D6}" type="CELLRANGE">
+                    <a:fld id="{0FAD6C38-FBC9-4671-BB60-4752AB978A3A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1394,7 +1397,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{008711DE-3B10-46C3-9A15-203C509C6784}" type="CELLRANGE">
+                    <a:fld id="{63A17B5D-AE15-4001-9C08-99E79017BC87}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1428,7 +1431,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{575179EB-BC4F-47D5-B30C-1C374F169275}" type="CELLRANGE">
+                    <a:fld id="{9FECA5C1-3AD3-43B5-8815-493F1D002D81}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1462,7 +1465,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A001CC7E-A791-4132-864D-6164EC7C3C1B}" type="CELLRANGE">
+                    <a:fld id="{8ACB1442-19C7-41C1-9548-73AA0DC78599}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1496,7 +1499,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5E5D952F-9E35-46D5-9092-4BF73EB52F66}" type="CELLRANGE">
+                    <a:fld id="{70BC32DA-097B-4C9D-B5FB-BC64002CDE2E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1530,7 +1533,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B874C62-1EB5-4055-88C8-1DCD914C380D}" type="CELLRANGE">
+                    <a:fld id="{F7636994-ABCD-452A-8A0D-7D99EBC71F17}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1564,7 +1567,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5CB2C09B-D499-4801-B53D-3CE8F5C5FEA6}" type="CELLRANGE">
+                    <a:fld id="{B3FB8419-2091-42F8-AD6A-2808C24E5762}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1598,7 +1601,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5076FB9F-0EB9-43AE-AD69-5477C2D3B218}" type="CELLRANGE">
+                    <a:fld id="{7908134C-D313-4BF5-B93C-9B86649788DA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1632,7 +1635,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E569D8E0-DBDE-4252-AA16-3105C017A319}" type="CELLRANGE">
+                    <a:fld id="{75C53430-4A43-4160-B5CA-56EE32CB3DB3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1666,7 +1669,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C017FF31-AC92-498C-9009-8B96A4F441EF}" type="CELLRANGE">
+                    <a:fld id="{872B947D-A606-4CAB-A373-05472ECC8E74}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1700,7 +1703,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A290E757-AB6E-482D-85D3-00A40DEEF286}" type="CELLRANGE">
+                    <a:fld id="{A32D34C3-B1F4-42FA-B2ED-37061938EE66}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1734,7 +1737,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD4E4851-9FE4-4422-8BC6-2E56D2498C7F}" type="CELLRANGE">
+                    <a:fld id="{142F6F56-83AF-46E1-9B01-0A8B0E42DF45}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1768,7 +1771,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10394A75-3B06-4896-AD04-E5D8B32BC497}" type="CELLRANGE">
+                    <a:fld id="{7545B7F4-6533-443B-9A2F-635458B0EC1D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1802,7 +1805,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3102D146-F1C5-4156-A8FA-FDABE523421D}" type="CELLRANGE">
+                    <a:fld id="{B536DE74-8FBA-49D2-B62D-8A56222E1442}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1836,7 +1839,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7AF294EB-7252-499D-B01A-37DDFFE1A901}" type="CELLRANGE">
+                    <a:fld id="{0004FEDC-D26D-4503-860B-9F36A02F8A29}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1870,7 +1873,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5FA6E5F-5C86-4351-A4F1-395620BA3791}" type="CELLRANGE">
+                    <a:fld id="{62B44BC2-C87F-40F8-A209-F5AFF871B1EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1904,7 +1907,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36425DA0-2F27-4005-A18F-C7DB4C170297}" type="CELLRANGE">
+                    <a:fld id="{6D01164B-B9CD-4BC4-9984-0852F5805671}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1938,7 +1941,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2479AA1D-D9EF-4F7D-BD52-041BE679D175}" type="CELLRANGE">
+                    <a:fld id="{0B198010-1C69-4CB0-85D8-AED9827840CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1972,7 +1975,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D339FE87-5E3B-45AE-BE9C-E7C801F6916A}" type="CELLRANGE">
+                    <a:fld id="{4909AC4B-4679-41AE-8326-53F7D256FCFC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2006,7 +2009,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E788DB98-38E3-4238-A214-60E3494FC07E}" type="CELLRANGE">
+                    <a:fld id="{6AA83BDF-B9D4-4B48-88CB-78452A2BC133}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2040,7 +2043,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D27CA1A-C96C-42AE-9FDE-AC151A330B99}" type="CELLRANGE">
+                    <a:fld id="{397622B5-61DD-4F93-B31B-137FF204BB76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2074,7 +2077,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E3AA39D1-7FB9-4556-BA4D-CF17322CB63C}" type="CELLRANGE">
+                    <a:fld id="{E16170D0-3394-4B75-8AA9-5664E074897C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2108,7 +2111,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AFC07119-73A3-4C7A-98A3-22EF0136A66F}" type="CELLRANGE">
+                    <a:fld id="{270B0770-8F77-4783-89BC-72DD5640B98A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2142,7 +2145,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7041583C-8E9E-430D-920E-8F60CA280B62}" type="CELLRANGE">
+                    <a:fld id="{C681DAFF-E85D-4785-8FE2-B5A949F6AD48}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2166,6 +2169,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-1E06-4B7E-8BFA-5AA13E5BF977}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="54"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{D735D4A9-8514-4E0C-AF77-A5874500AB54}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-093C-4FD5-9234-0E1CB379EED9}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2215,10 +2252,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$55</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -2376,9 +2413,12 @@
                   <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="52">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="53">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2386,10 +2426,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$55</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -2547,9 +2587,12 @@
                   <c:v>3550</c:v>
                 </c:pt>
                 <c:pt idx="52">
+                  <c:v>2240</c:v>
+                </c:pt>
+                <c:pt idx="53">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2722,6 +2765,9 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="53">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3774,10 +3820,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D55" totalsRowShown="0">
-  <autoFilter ref="A1:D55" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D55">
-    <sortCondition ref="A1:A55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D56" totalsRowShown="0">
+  <autoFilter ref="A1:D56" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D56">
+    <sortCondition ref="A1:A56"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -4086,10 +4132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4849,30 +4895,44 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54">
+        <v>10.8</v>
+      </c>
+      <c r="C54">
+        <v>2240</v>
+      </c>
+      <c r="D54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
         <v>55</v>
       </c>
-      <c r="B54">
+      <c r="B55">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C54">
+      <c r="C55">
         <v>3800</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>29</v>
       </c>
-      <c r="B55">
+      <c r="B56">
         <v>6</v>
       </c>
-      <c r="C55">
+      <c r="C56">
         <v>2180</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix West Fork White River elevation gain
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A61DEB-9BC5-4B5D-BE22-712B603B36F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73511B55-79F9-41BA-8CF8-B04342799FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -343,7 +343,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9503CD4A-13B0-4637-BEAC-7422AFDACD37}" type="CELLRANGE">
+                    <a:fld id="{2AD3FA40-95B4-43E5-A482-5DA65135D122}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -377,7 +377,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29309738-E910-4628-919A-1400DEF6533C}" type="CELLRANGE">
+                    <a:fld id="{A9007D25-42C2-4AEB-A88A-32E29CA9052E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -411,7 +411,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1A797C8-F792-4A45-AFAB-BE565B9F3352}" type="CELLRANGE">
+                    <a:fld id="{C903DBB7-7763-4B58-B960-36843387F090}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -445,7 +445,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC29263C-D047-4BEF-8C65-CB85FEEA2B81}" type="CELLRANGE">
+                    <a:fld id="{729A4E7F-4FC8-4602-A642-0DB444927F54}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -479,7 +479,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9EDC3C2A-C38B-4EE1-9739-6418F89526CC}" type="CELLRANGE">
+                    <a:fld id="{C24B112A-B947-400C-B627-E2510100D11B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -513,7 +513,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1E22B7A-BBDC-4A4A-A483-24585C38489F}" type="CELLRANGE">
+                    <a:fld id="{C07D424C-A913-45DE-8A4D-6A6C23CFA28C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -547,7 +547,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9406FF57-96DA-44F9-89B3-2D0D09479858}" type="CELLRANGE">
+                    <a:fld id="{E2B0B49A-F87E-4552-8DC4-657F2E6BE3A3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -581,7 +581,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BDF501B0-2C46-479E-80BC-29696BDDA3F5}" type="CELLRANGE">
+                    <a:fld id="{E7A985FA-CD92-4A14-A34A-5EDDA6163B23}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -615,7 +615,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4DDF1F9F-0DAC-4184-9A08-1D067C8B1163}" type="CELLRANGE">
+                    <a:fld id="{878BA175-3DC5-48BC-8446-86E723F1E5BB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -649,7 +649,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D640914-4B67-42D7-8FAB-B1B27B4CE440}" type="CELLRANGE">
+                    <a:fld id="{95F0C71C-B48B-4E8F-88FA-FB94AA75BDE8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -683,7 +683,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B378F913-EECD-41A3-B900-7029216013F0}" type="CELLRANGE">
+                    <a:fld id="{A0F0DED1-784C-482D-9AF3-FB81A381A27A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -717,7 +717,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D9ECEA4E-8A98-4885-84AE-DEEC7A371B1C}" type="CELLRANGE">
+                    <a:fld id="{E2FD90AD-0C35-4AEE-8371-540C08648CFA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -751,7 +751,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F03A7C7C-4820-4C8A-814B-2611EDDBAC08}" type="CELLRANGE">
+                    <a:fld id="{B9BE9CF1-33B7-4E4C-A7DD-F21F7145116C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -785,7 +785,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8FE4FF0D-B6A4-4C7B-8917-E3F390618608}" type="CELLRANGE">
+                    <a:fld id="{B3A8E75E-4DA3-4EA7-B1CC-F375F665C1A5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -819,7 +819,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F17C5161-493A-42EA-9EF1-88E5C2044E06}" type="CELLRANGE">
+                    <a:fld id="{C77E07F4-05AF-4791-9C24-B5917BCC047D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -853,7 +853,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{16FE3356-6839-4289-A44F-F61A4CBB6DC7}" type="CELLRANGE">
+                    <a:fld id="{64D5FFE2-CC3D-432F-A8EC-E8871FAEB0C8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -887,7 +887,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE0C63D3-9ADB-406D-B7D9-A55E52812717}" type="CELLRANGE">
+                    <a:fld id="{9C4C5E70-69E8-4F6A-B0F7-C82892754464}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -921,7 +921,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{503D8975-4824-45B8-9857-C64DC8C84679}" type="CELLRANGE">
+                    <a:fld id="{0044E69A-B9A0-4F01-A118-1CEC31228097}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -955,7 +955,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D0926B54-64E5-44EF-A0E2-480CF6546027}" type="CELLRANGE">
+                    <a:fld id="{361E96C4-A693-45AD-924B-C364E208E1B7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -989,7 +989,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{72AE9149-981F-4064-909B-49D5718358EF}" type="CELLRANGE">
+                    <a:fld id="{FDB8A227-1E0F-4453-B814-841014398AB7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1023,7 +1023,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8BAABCD7-9620-42FE-B5ED-831612C3C11F}" type="CELLRANGE">
+                    <a:fld id="{A85F610F-37C8-489E-86CC-EF38D550EDC4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1057,7 +1057,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7DD34C7B-B279-4782-8867-FBC234C572D0}" type="CELLRANGE">
+                    <a:fld id="{D05E0EC5-DDF8-4653-B92D-3AD262115616}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1091,7 +1091,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC2D52BE-B8F1-4613-B325-06407C643FE4}" type="CELLRANGE">
+                    <a:fld id="{85BAFFAB-BC84-443F-A349-A87A57C23210}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1125,7 +1125,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9EBFF2B-CA49-444E-AE11-BB274FBAA64A}" type="CELLRANGE">
+                    <a:fld id="{79112CC3-EE27-4DC6-9FCE-0E6912B2EBCC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1159,7 +1159,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3AE41A9A-F378-4C30-91C5-C19F101803D2}" type="CELLRANGE">
+                    <a:fld id="{5C7AEA41-5BAE-4DBA-9B4F-A3F0B12B182E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1193,7 +1193,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{03DD53FD-776C-4363-942A-4C3054323733}" type="CELLRANGE">
+                    <a:fld id="{6B60C828-BDBB-4E7E-A14A-BE5726EC2C31}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1227,7 +1227,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B3299E44-2A2C-444B-B042-31F786703E41}" type="CELLRANGE">
+                    <a:fld id="{DBAC53D0-2C67-4127-A2D4-8758811249D4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1261,7 +1261,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D7275CB-CDB4-4AD2-986F-2B7154C28868}" type="CELLRANGE">
+                    <a:fld id="{0F357967-A073-4D4E-B590-B57F8CF9062F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1295,7 +1295,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CAD215F9-5981-4DE2-B188-DB68DD6B135C}" type="CELLRANGE">
+                    <a:fld id="{73CA5CF6-D229-4A55-BF49-3388F2FB854C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1329,7 +1329,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B15F46D1-7E05-477E-AB7D-C9AE6BB8B923}" type="CELLRANGE">
+                    <a:fld id="{ECDB4B4F-B077-4403-873D-7DA2FF79F584}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1363,7 +1363,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0FAD6C38-FBC9-4671-BB60-4752AB978A3A}" type="CELLRANGE">
+                    <a:fld id="{AFC604B4-C43C-45AB-ABA1-C97E310C6F5C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1397,7 +1397,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63A17B5D-AE15-4001-9C08-99E79017BC87}" type="CELLRANGE">
+                    <a:fld id="{21EC80DD-00A5-4062-BE6D-817076ECB5D4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1431,7 +1431,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9FECA5C1-3AD3-43B5-8815-493F1D002D81}" type="CELLRANGE">
+                    <a:fld id="{0742F8E2-20C0-48F2-8FC6-DF4ABA6AFADE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1465,7 +1465,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8ACB1442-19C7-41C1-9548-73AA0DC78599}" type="CELLRANGE">
+                    <a:fld id="{7FD7E7BC-741A-4A72-B4B7-B7A7FB466B3B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1499,7 +1499,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70BC32DA-097B-4C9D-B5FB-BC64002CDE2E}" type="CELLRANGE">
+                    <a:fld id="{2B613A2C-2C90-4DBD-8007-0C73F8CC4785}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1533,7 +1533,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F7636994-ABCD-452A-8A0D-7D99EBC71F17}" type="CELLRANGE">
+                    <a:fld id="{E0D62111-EFB3-44F1-A4B0-1749F309AC0D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1567,7 +1567,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B3FB8419-2091-42F8-AD6A-2808C24E5762}" type="CELLRANGE">
+                    <a:fld id="{8E4C5597-A23D-48BD-A168-0A4C37A2FE9F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1601,7 +1601,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7908134C-D313-4BF5-B93C-9B86649788DA}" type="CELLRANGE">
+                    <a:fld id="{F854DE22-C072-40DC-8DEB-7DA5437427BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1635,7 +1635,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75C53430-4A43-4160-B5CA-56EE32CB3DB3}" type="CELLRANGE">
+                    <a:fld id="{ED3E85A3-8215-4C99-8B47-3A3BB160D9A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1669,7 +1669,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{872B947D-A606-4CAB-A373-05472ECC8E74}" type="CELLRANGE">
+                    <a:fld id="{F5D92D2B-F2F7-48FD-91AB-C2770ACCDC26}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1703,7 +1703,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A32D34C3-B1F4-42FA-B2ED-37061938EE66}" type="CELLRANGE">
+                    <a:fld id="{29864A41-8610-4272-B998-DE1A8078BAFD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1737,7 +1737,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{142F6F56-83AF-46E1-9B01-0A8B0E42DF45}" type="CELLRANGE">
+                    <a:fld id="{75FF855E-C533-4E44-9155-10B34BE0B2C1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1771,7 +1771,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7545B7F4-6533-443B-9A2F-635458B0EC1D}" type="CELLRANGE">
+                    <a:fld id="{4C24E028-51C6-4B6A-A98E-423827B42ECE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1805,7 +1805,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B536DE74-8FBA-49D2-B62D-8A56222E1442}" type="CELLRANGE">
+                    <a:fld id="{AD6A2679-4E2C-4D2D-A00E-CD23B2330C21}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1839,7 +1839,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0004FEDC-D26D-4503-860B-9F36A02F8A29}" type="CELLRANGE">
+                    <a:fld id="{5E08ACC7-7F0D-41DF-942C-868BEB9B5B7A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1873,7 +1873,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{62B44BC2-C87F-40F8-A209-F5AFF871B1EE}" type="CELLRANGE">
+                    <a:fld id="{03F95561-B570-47E8-A235-55A3138C2F83}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1907,7 +1907,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D01164B-B9CD-4BC4-9984-0852F5805671}" type="CELLRANGE">
+                    <a:fld id="{CB4524DA-6B86-4AD8-BC09-09970B0AE8EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1941,7 +1941,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0B198010-1C69-4CB0-85D8-AED9827840CB}" type="CELLRANGE">
+                    <a:fld id="{5D96A28E-A822-44D0-A5E0-1CE60A556F94}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1975,7 +1975,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4909AC4B-4679-41AE-8326-53F7D256FCFC}" type="CELLRANGE">
+                    <a:fld id="{BEC42D93-A2E3-4063-848F-CF789CFBC141}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2009,7 +2009,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6AA83BDF-B9D4-4B48-88CB-78452A2BC133}" type="CELLRANGE">
+                    <a:fld id="{7EC6163A-C6D7-4F2D-8722-90B1BA92D63E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2043,7 +2043,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{397622B5-61DD-4F93-B31B-137FF204BB76}" type="CELLRANGE">
+                    <a:fld id="{B4691765-BFDB-48A7-ABCF-54B52E0DD214}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2077,7 +2077,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E16170D0-3394-4B75-8AA9-5664E074897C}" type="CELLRANGE">
+                    <a:fld id="{BBD817E1-2F26-43EC-8CA4-88CCAA6C0F5F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2111,7 +2111,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{270B0770-8F77-4783-89BC-72DD5640B98A}" type="CELLRANGE">
+                    <a:fld id="{32169870-D026-49C0-BE95-E8BF88488981}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2145,7 +2145,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C681DAFF-E85D-4785-8FE2-B5A949F6AD48}" type="CELLRANGE">
+                    <a:fld id="{D95871E2-1D2E-4496-B4AB-5B2B537758AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2179,7 +2179,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D735D4A9-8514-4E0C-AF77-A5874500AB54}" type="CELLRANGE">
+                    <a:fld id="{CD23A960-2D63-458C-A5CB-26CC217D0F48}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2587,7 +2587,7 @@
                   <c:v>3550</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2240</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>3800</c:v>
@@ -4134,8 +4134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4901,7 +4901,7 @@
         <v>10.8</v>
       </c>
       <c r="C54">
-        <v>2240</v>
+        <v>1800</v>
       </c>
       <c r="D54" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Add Silver Forest, Naches Peak, Deadwood Lakes
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73511B55-79F9-41BA-8CF8-B04342799FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05DF858-B46F-4692-A4D1-A1714EC80E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="68">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -225,6 +225,18 @@
   </si>
   <si>
     <t>West Fork White River</t>
+  </si>
+  <si>
+    <t>Deadwood Lakes</t>
+  </si>
+  <si>
+    <t>Silver Forest Trail</t>
+  </si>
+  <si>
+    <t>Naches Peak Loop</t>
+  </si>
+  <si>
+    <t>moderate (because rough)</t>
   </si>
 </sst>
 </file>
@@ -343,7 +355,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2AD3FA40-95B4-43E5-A482-5DA65135D122}" type="CELLRANGE">
+                    <a:fld id="{ED9F2AD5-02CC-4FED-82D3-1D761F57D823}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -377,7 +389,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9007D25-42C2-4AEB-A88A-32E29CA9052E}" type="CELLRANGE">
+                    <a:fld id="{F065E947-BA8D-4D6D-9D45-5FCD97187F79}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -411,7 +423,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C903DBB7-7763-4B58-B960-36843387F090}" type="CELLRANGE">
+                    <a:fld id="{332AFFC2-AACF-4754-AE3A-E0E2B6034AD2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -445,7 +457,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{729A4E7F-4FC8-4602-A642-0DB444927F54}" type="CELLRANGE">
+                    <a:fld id="{4601CEA0-19C9-4E89-99A1-082118F1FAFF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -479,7 +491,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C24B112A-B947-400C-B627-E2510100D11B}" type="CELLRANGE">
+                    <a:fld id="{1AFCD1AB-41E8-414C-9078-97768AAB53FF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -513,7 +525,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C07D424C-A913-45DE-8A4D-6A6C23CFA28C}" type="CELLRANGE">
+                    <a:fld id="{B8F5E892-BF48-4854-9CC0-DA80F66ECEE8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -547,7 +559,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E2B0B49A-F87E-4552-8DC4-657F2E6BE3A3}" type="CELLRANGE">
+                    <a:fld id="{8407393C-E243-46FD-B703-CBC9B2C39549}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -581,7 +593,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7A985FA-CD92-4A14-A34A-5EDDA6163B23}" type="CELLRANGE">
+                    <a:fld id="{AAFB1B89-4153-46A2-8E35-DAA1B6D67575}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -615,7 +627,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{878BA175-3DC5-48BC-8446-86E723F1E5BB}" type="CELLRANGE">
+                    <a:fld id="{8CC240B7-80A7-4E28-B9D0-2A8026435559}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -649,7 +661,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95F0C71C-B48B-4E8F-88FA-FB94AA75BDE8}" type="CELLRANGE">
+                    <a:fld id="{717E1828-A5A6-4F59-B8F5-5003ED14FCD6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -683,7 +695,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A0F0DED1-784C-482D-9AF3-FB81A381A27A}" type="CELLRANGE">
+                    <a:fld id="{BAD10E20-5F9A-40D6-B359-B7797B841258}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -717,7 +729,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E2FD90AD-0C35-4AEE-8371-540C08648CFA}" type="CELLRANGE">
+                    <a:fld id="{02DB093A-05CC-4BDF-9544-C21926CA0649}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -751,7 +763,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B9BE9CF1-33B7-4E4C-A7DD-F21F7145116C}" type="CELLRANGE">
+                    <a:fld id="{6C1BEE74-400B-472A-A6CB-5ECDF58B9C52}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -785,7 +797,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B3A8E75E-4DA3-4EA7-B1CC-F375F665C1A5}" type="CELLRANGE">
+                    <a:fld id="{C23128FB-0FD4-4FE6-A948-18FCFDD56AB4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -819,7 +831,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C77E07F4-05AF-4791-9C24-B5917BCC047D}" type="CELLRANGE">
+                    <a:fld id="{7338384E-1E51-4DAC-B610-D0EEAE95EBEB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -853,7 +865,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{64D5FFE2-CC3D-432F-A8EC-E8871FAEB0C8}" type="CELLRANGE">
+                    <a:fld id="{FA334FED-3D1D-4CA9-8F91-BE4D3C7A9B06}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -887,7 +899,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C4C5E70-69E8-4F6A-B0F7-C82892754464}" type="CELLRANGE">
+                    <a:fld id="{C1FAB9FA-A962-47B2-836E-A4977998EAF0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -921,7 +933,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0044E69A-B9A0-4F01-A118-1CEC31228097}" type="CELLRANGE">
+                    <a:fld id="{F612DA1F-1CB0-4E5D-81E3-145DFAFE1E05}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -955,7 +967,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{361E96C4-A693-45AD-924B-C364E208E1B7}" type="CELLRANGE">
+                    <a:fld id="{BD7B937C-3228-4FBA-82FE-78DF7445F45B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -989,7 +1001,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FDB8A227-1E0F-4453-B814-841014398AB7}" type="CELLRANGE">
+                    <a:fld id="{192AC8F2-2470-4673-99DA-E0AA90E6AFE2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1023,7 +1035,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A85F610F-37C8-489E-86CC-EF38D550EDC4}" type="CELLRANGE">
+                    <a:fld id="{C4B8847A-CD1B-4CDB-B483-E74C56C8CD07}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1057,7 +1069,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D05E0EC5-DDF8-4653-B92D-3AD262115616}" type="CELLRANGE">
+                    <a:fld id="{763287A5-D8E2-463D-8376-201F4281A5BC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1091,7 +1103,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{85BAFFAB-BC84-443F-A349-A87A57C23210}" type="CELLRANGE">
+                    <a:fld id="{4CD8A1A5-A396-4A12-86FF-A2F78AF1B878}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1125,7 +1137,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79112CC3-EE27-4DC6-9FCE-0E6912B2EBCC}" type="CELLRANGE">
+                    <a:fld id="{CB1BB88D-A062-4FA6-91BD-770148002A01}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1159,7 +1171,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C7AEA41-5BAE-4DBA-9B4F-A3F0B12B182E}" type="CELLRANGE">
+                    <a:fld id="{1A258165-4509-47A0-B8E2-9BD9B1C9F2E5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1193,7 +1205,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6B60C828-BDBB-4E7E-A14A-BE5726EC2C31}" type="CELLRANGE">
+                    <a:fld id="{3E13E460-6E2B-429C-AF15-7011A3A66156}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1227,7 +1239,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DBAC53D0-2C67-4127-A2D4-8758811249D4}" type="CELLRANGE">
+                    <a:fld id="{5B496C2C-5E24-4858-AF4C-F511721BCC8C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1261,7 +1273,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F357967-A073-4D4E-B590-B57F8CF9062F}" type="CELLRANGE">
+                    <a:fld id="{2A129E79-6069-405A-B119-7BD9FA8C5CA6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1295,7 +1307,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73CA5CF6-D229-4A55-BF49-3388F2FB854C}" type="CELLRANGE">
+                    <a:fld id="{D72939F4-D933-49AB-A9F7-F6C5D9E07470}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1329,7 +1341,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ECDB4B4F-B077-4403-873D-7DA2FF79F584}" type="CELLRANGE">
+                    <a:fld id="{FAD4AC5B-3111-4512-BA23-D02E7FA9EAFA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1363,7 +1375,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AFC604B4-C43C-45AB-ABA1-C97E310C6F5C}" type="CELLRANGE">
+                    <a:fld id="{582D3DD3-3D12-4622-B759-4D9ADF287D71}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1397,7 +1409,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{21EC80DD-00A5-4062-BE6D-817076ECB5D4}" type="CELLRANGE">
+                    <a:fld id="{F9931344-4CDE-49F9-934C-FBF54BF2F950}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1431,7 +1443,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0742F8E2-20C0-48F2-8FC6-DF4ABA6AFADE}" type="CELLRANGE">
+                    <a:fld id="{858D4D94-CF4A-4C1E-B100-4952FF8265DD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1465,7 +1477,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7FD7E7BC-741A-4A72-B4B7-B7A7FB466B3B}" type="CELLRANGE">
+                    <a:fld id="{CB2B724F-B978-44BB-A64F-EAE97E0B8CA0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1499,7 +1511,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2B613A2C-2C90-4DBD-8007-0C73F8CC4785}" type="CELLRANGE">
+                    <a:fld id="{32EC52DA-E9EC-4E61-9029-C421A31DBF53}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1533,7 +1545,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E0D62111-EFB3-44F1-A4B0-1749F309AC0D}" type="CELLRANGE">
+                    <a:fld id="{5C503A83-FE6C-405A-B76B-A9AEC8578FAA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1567,7 +1579,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8E4C5597-A23D-48BD-A168-0A4C37A2FE9F}" type="CELLRANGE">
+                    <a:fld id="{A5FC5F74-F8DE-47D6-8219-0DC6C36E2B80}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1601,7 +1613,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F854DE22-C072-40DC-8DEB-7DA5437427BA}" type="CELLRANGE">
+                    <a:fld id="{57107324-7FE3-40C2-8B4E-28001D449144}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1635,7 +1647,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED3E85A3-8215-4C99-8B47-3A3BB160D9A7}" type="CELLRANGE">
+                    <a:fld id="{62646499-51D0-4CD1-A68E-1BE4112C1BAD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1669,7 +1681,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5D92D2B-F2F7-48FD-91AB-C2770ACCDC26}" type="CELLRANGE">
+                    <a:fld id="{A035271B-086E-4E9A-AFD0-036C84828235}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1703,7 +1715,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29864A41-8610-4272-B998-DE1A8078BAFD}" type="CELLRANGE">
+                    <a:fld id="{56D40996-4474-4523-A4E0-3EBEBDCB1CCF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1737,7 +1749,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75FF855E-C533-4E44-9155-10B34BE0B2C1}" type="CELLRANGE">
+                    <a:fld id="{F8283D4B-1415-41CD-B71D-4021F7FECB43}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1771,7 +1783,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4C24E028-51C6-4B6A-A98E-423827B42ECE}" type="CELLRANGE">
+                    <a:fld id="{5462F2E5-B48E-4417-9A17-31BCF942F492}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1805,7 +1817,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD6A2679-4E2C-4D2D-A00E-CD23B2330C21}" type="CELLRANGE">
+                    <a:fld id="{A5C115F0-9227-4101-B5D8-122A62E26FCD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1839,7 +1851,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5E08ACC7-7F0D-41DF-942C-868BEB9B5B7A}" type="CELLRANGE">
+                    <a:fld id="{3E73376A-CEA1-4603-8119-5F18A90F8706}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1873,7 +1885,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{03F95561-B570-47E8-A235-55A3138C2F83}" type="CELLRANGE">
+                    <a:fld id="{8720C042-54C4-421A-BFCA-D63B7F600A7D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1907,7 +1919,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB4524DA-6B86-4AD8-BC09-09970B0AE8EE}" type="CELLRANGE">
+                    <a:fld id="{33663522-6F5C-4544-A881-9993BEDE4F93}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1941,7 +1953,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D96A28E-A822-44D0-A5E0-1CE60A556F94}" type="CELLRANGE">
+                    <a:fld id="{E55A17C3-3828-4B64-A7AB-A5136BC89779}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1975,7 +1987,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BEC42D93-A2E3-4063-848F-CF789CFBC141}" type="CELLRANGE">
+                    <a:fld id="{0142C367-D3CC-455E-8C25-2B4565049700}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2009,7 +2021,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7EC6163A-C6D7-4F2D-8722-90B1BA92D63E}" type="CELLRANGE">
+                    <a:fld id="{8063463C-2EE9-4D1B-B457-D8933D47B743}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2043,7 +2055,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B4691765-BFDB-48A7-ABCF-54B52E0DD214}" type="CELLRANGE">
+                    <a:fld id="{9BFA6D7B-1EEC-44ED-B70B-C407BDF469E3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2077,7 +2089,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BBD817E1-2F26-43EC-8CA4-88CCAA6C0F5F}" type="CELLRANGE">
+                    <a:fld id="{DF2ACE98-CEAD-48A5-BC78-3C3848E9FB61}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2111,7 +2123,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32169870-D026-49C0-BE95-E8BF88488981}" type="CELLRANGE">
+                    <a:fld id="{D09C936F-8590-4C24-AA3B-7C3F7DB5CD42}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2145,7 +2157,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D95871E2-1D2E-4496-B4AB-5B2B537758AD}" type="CELLRANGE">
+                    <a:fld id="{E88B20B7-1D5A-4975-9333-A874198AF5CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2179,7 +2191,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD23A960-2D63-458C-A5CB-26CC217D0F48}" type="CELLRANGE">
+                    <a:fld id="{69563121-CC3C-4F01-8FDA-F53564A9FF46}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2203,6 +2215,108 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-093C-4FD5-9234-0E1CB379EED9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="55"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{D10B270A-28F6-48E0-8E8F-2D17E0E48D8D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-2895-47D3-8EB5-D3385223803E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="56"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{DC4F1F1F-1B3B-4BCF-947A-A67650D7F2FC}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-2895-47D3-8EB5-D3385223803E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="57"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A914E940-CF3E-4F2C-883C-AC0189035910}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-2895-47D3-8EB5-D3385223803E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2252,10 +2366,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$56</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -2281,144 +2395,153 @@
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>2.9</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>7.1</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>9.8000000000000007</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>9.6</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>11.6</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>12.5</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>9.1</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>12.2</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>9.75</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>5.4</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>11.9</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>7.2</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="40">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="44">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="46">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="47">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="48">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="49">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="50">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="51">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="52">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="53">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="54">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="55">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="56">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="57">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2426,10 +2549,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$56</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -2455,144 +2578,153 @@
                   <c:v>3110</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>3030</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>1540</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>2880</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>3290</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>2660</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>2780</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>4800</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>4120</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>3420</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>1450</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>3160</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>880</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>1260</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>3100</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="39">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="40">
                   <c:v>1630</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="41">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="42">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="44">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="46">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="47">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="48">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="49">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="50">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="51">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="52">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="53">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="54">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="55">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="56">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="57">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2630,13 +2762,13 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>easy</c:v>
+                    <c:v>moderate (because rough)</c:v>
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>moderate</c:v>
@@ -2645,25 +2777,25 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="13">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="15">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="16">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="17">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="18">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="20">
                     <c:v>strenuous</c:v>
@@ -2675,25 +2807,25 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="23">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="24">
+                  <c:pt idx="25">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="25">
+                  <c:pt idx="26">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="26">
+                  <c:pt idx="27">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="27">
+                  <c:pt idx="28">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="28">
+                  <c:pt idx="29">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="30">
                     <c:v>easy</c:v>
@@ -2702,22 +2834,22 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="32">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="34">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="33">
+                  <c:pt idx="35">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="34">
-                    <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="35">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="36">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="37">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="38">
                     <c:v>moderate</c:v>
@@ -2729,45 +2861,54 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="41">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="42">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="43">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="42">
+                  <c:pt idx="44">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="43">
+                  <c:pt idx="45">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="46">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="44">
+                  <c:pt idx="47">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="45">
+                  <c:pt idx="48">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="46">
+                  <c:pt idx="49">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="47">
+                  <c:pt idx="50">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="48">
+                  <c:pt idx="51">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="49">
+                  <c:pt idx="52">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="50">
+                  <c:pt idx="53">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="51">
+                  <c:pt idx="54">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="52">
+                  <c:pt idx="55">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="53">
+                  <c:pt idx="56">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="54">
+                  <c:pt idx="57">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3820,10 +3961,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D56" totalsRowShown="0">
-  <autoFilter ref="A1:D56" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D56">
-    <sortCondition ref="A1:A56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D59" totalsRowShown="0">
+  <autoFilter ref="A1:D59" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D59">
+    <sortCondition ref="A1:A59"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -4132,10 +4273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4275,27 +4416,27 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="C10">
-        <v>1000</v>
+        <v>940</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11">
-        <v>2.9</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>1090</v>
+        <v>1000</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -4303,27 +4444,27 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B12">
-        <v>7.1</v>
+        <v>2.9</v>
       </c>
       <c r="C12">
-        <v>3030</v>
+        <v>1090</v>
       </c>
       <c r="D12" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B13">
-        <v>6.5</v>
+        <v>7.1</v>
       </c>
       <c r="C13">
-        <v>1540</v>
+        <v>3030</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
@@ -4331,13 +4472,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B14">
-        <v>9.8000000000000007</v>
+        <v>6.5</v>
       </c>
       <c r="C14">
-        <v>2880</v>
+        <v>1540</v>
       </c>
       <c r="D14" t="s">
         <v>1</v>
@@ -4345,69 +4486,69 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15">
-        <v>9.6</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C15">
-        <v>3290</v>
+        <v>2880</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="B16">
-        <v>11.6</v>
+        <v>9.6</v>
       </c>
       <c r="C16">
-        <v>2660</v>
+        <v>3290</v>
       </c>
       <c r="D16" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B17">
-        <v>12.5</v>
+        <v>11.6</v>
       </c>
       <c r="C17">
-        <v>2780</v>
+        <v>2660</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="B18">
-        <v>9</v>
+        <v>12.5</v>
       </c>
       <c r="C18">
-        <v>1680</v>
+        <v>2780</v>
       </c>
       <c r="D18" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B19">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="C19">
-        <v>1580</v>
+        <v>1680</v>
       </c>
       <c r="D19" t="s">
         <v>1</v>
@@ -4415,41 +4556,41 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B20">
-        <v>5.2</v>
+        <v>9.1</v>
       </c>
       <c r="C20">
-        <v>1000</v>
+        <v>1580</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B21">
-        <v>14</v>
+        <v>5.2</v>
       </c>
       <c r="C21">
-        <v>4800</v>
+        <v>1000</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
         <v>14</v>
       </c>
-      <c r="B22">
-        <v>12.2</v>
-      </c>
       <c r="C22">
-        <v>4120</v>
+        <v>4800</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
@@ -4457,13 +4598,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23">
-        <v>12</v>
+        <v>12.2</v>
       </c>
       <c r="C23">
-        <v>3420</v>
+        <v>4120</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -4471,127 +4612,127 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>3420</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>37</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <f>19.5/2</f>
         <v>9.75</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <f>4400*7/8</f>
         <v>3850</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25">
-        <v>5.4</v>
-      </c>
-      <c r="C25">
-        <v>1450</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B26">
-        <v>11.9</v>
+        <v>5.4</v>
       </c>
       <c r="C26">
-        <v>3160</v>
+        <v>1450</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B27">
-        <v>11.4</v>
+        <v>11.9</v>
       </c>
       <c r="C27">
-        <v>2550</v>
+        <v>3160</v>
       </c>
       <c r="D27" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28">
-        <v>8.5</v>
+        <v>11.4</v>
       </c>
       <c r="C28">
-        <v>3350</v>
+        <v>2550</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B29">
-        <v>2.8</v>
+        <v>8.5</v>
       </c>
       <c r="C29">
-        <v>880</v>
+        <v>3350</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B30">
-        <v>10.4</v>
+        <v>2.8</v>
       </c>
       <c r="C30">
-        <v>1420</v>
+        <v>880</v>
       </c>
       <c r="D30" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B31">
-        <v>0.9</v>
+        <v>10.4</v>
       </c>
       <c r="C31">
-        <v>200</v>
+        <v>1420</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B32">
-        <v>4.8</v>
+        <v>0.9</v>
       </c>
       <c r="C32">
-        <v>1260</v>
+        <v>200</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
@@ -4599,13 +4740,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B33">
-        <v>1.4</v>
+        <v>4.2</v>
       </c>
       <c r="C33">
-        <v>375</v>
+        <v>860</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -4613,69 +4754,69 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B34">
-        <v>13.6</v>
+        <v>4.8</v>
       </c>
       <c r="C34">
-        <v>3930</v>
+        <v>1260</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B35">
-        <v>10.5</v>
+        <v>1.4</v>
       </c>
       <c r="C35">
-        <v>3100</v>
+        <v>375</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B36">
-        <v>7</v>
+        <v>13.6</v>
       </c>
       <c r="C36">
-        <v>1670</v>
+        <v>3930</v>
       </c>
       <c r="D36" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B37">
-        <v>8.1</v>
+        <v>10.5</v>
       </c>
       <c r="C37">
-        <v>2400</v>
+        <v>3100</v>
       </c>
       <c r="D37" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B38">
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="C38">
-        <v>1850</v>
+        <v>1670</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
@@ -4683,27 +4824,27 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B39">
-        <v>4.8</v>
+        <v>8.1</v>
       </c>
       <c r="C39">
-        <v>1300</v>
+        <v>2400</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B40">
-        <v>7.2</v>
+        <v>5.5</v>
       </c>
       <c r="C40">
-        <v>1630</v>
+        <v>1850</v>
       </c>
       <c r="D40" t="s">
         <v>1</v>
@@ -4711,13 +4852,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B41">
         <v>4.8</v>
       </c>
       <c r="C41">
-        <v>1470</v>
+        <v>1300</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
@@ -4725,13 +4866,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B42">
-        <v>6.9</v>
+        <v>7.2</v>
       </c>
       <c r="C42">
-        <v>2000</v>
+        <v>1630</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
@@ -4739,200 +4880,242 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="B43">
-        <v>8.1999999999999993</v>
+        <v>4.8</v>
       </c>
       <c r="C43">
-        <v>3490</v>
+        <v>1470</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B44">
-        <v>2.2000000000000002</v>
+        <v>6.9</v>
       </c>
       <c r="C44">
-        <v>750</v>
+        <v>2000</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B45">
-        <v>11</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C45">
-        <v>2170</v>
+        <v>3490</v>
       </c>
       <c r="D45" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="B46">
-        <v>7.3</v>
+        <v>3.3</v>
       </c>
       <c r="C46">
-        <v>2250</v>
+        <v>600</v>
       </c>
       <c r="D46" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C47">
+        <v>750</v>
+      </c>
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48">
+        <v>11</v>
+      </c>
+      <c r="C48">
+        <v>2170</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49">
+        <v>7.3</v>
+      </c>
+      <c r="C49">
+        <v>2250</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
         <v>25</v>
       </c>
-      <c r="B47">
+      <c r="B50">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C47">
+      <c r="C50">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D50" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48">
-        <v>1.2</v>
-      </c>
-      <c r="C48">
-        <v>500</v>
-      </c>
-      <c r="D48" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B49">
-        <v>11</v>
-      </c>
-      <c r="C49">
-        <v>3060</v>
-      </c>
-      <c r="D49" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
-        <v>60</v>
-      </c>
-      <c r="B50">
-        <v>6.5</v>
-      </c>
-      <c r="C50">
-        <v>1650</v>
-      </c>
-      <c r="D50" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="B51">
-        <v>6.2</v>
+        <v>1.2</v>
       </c>
       <c r="C51">
-        <v>1890</v>
+        <v>500</v>
       </c>
       <c r="D51" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B52">
-        <v>0.4</v>
+        <v>11</v>
       </c>
       <c r="C52">
-        <v>180</v>
+        <v>3060</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B53">
-        <v>7.3</v>
+        <v>6.5</v>
       </c>
       <c r="C53">
-        <v>3550</v>
+        <v>1650</v>
       </c>
       <c r="D53" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="B54">
-        <v>10.8</v>
+        <v>6.2</v>
       </c>
       <c r="C54">
-        <v>1800</v>
+        <v>1890</v>
       </c>
       <c r="D54" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55">
+        <v>0.4</v>
+      </c>
+      <c r="C55">
+        <v>180</v>
+      </c>
+      <c r="D55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56">
+        <v>7.3</v>
+      </c>
+      <c r="C56">
+        <v>3550</v>
+      </c>
+      <c r="D56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57">
+        <v>10.8</v>
+      </c>
+      <c r="C57">
+        <v>1800</v>
+      </c>
+      <c r="D57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>55</v>
       </c>
-      <c r="B55">
+      <c r="B58">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C55">
+      <c r="C58">
         <v>3800</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D58" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
         <v>29</v>
       </c>
-      <c r="B56">
+      <c r="B59">
         <v>6</v>
       </c>
-      <c r="C56">
+      <c r="C59">
         <v>2180</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D59" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Pinnacle Saddle hike
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05DF858-B46F-4692-A4D1-A1714EC80E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3480EC-D5A7-44FD-A081-B019CA59B5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="69">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>moderate (because rough)</t>
+  </si>
+  <si>
+    <t>Pinnacle Saddle</t>
   </si>
 </sst>
 </file>
@@ -355,7 +358,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED9F2AD5-02CC-4FED-82D3-1D761F57D823}" type="CELLRANGE">
+                    <a:fld id="{A372089B-8F87-42B9-8E4D-7B3927EEA94C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -389,7 +392,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F065E947-BA8D-4D6D-9D45-5FCD97187F79}" type="CELLRANGE">
+                    <a:fld id="{512482B4-161C-40D7-8A87-B679818E6065}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -423,7 +426,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{332AFFC2-AACF-4754-AE3A-E0E2B6034AD2}" type="CELLRANGE">
+                    <a:fld id="{EB3B134F-5514-48D2-B36F-7DAA45723645}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -457,7 +460,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4601CEA0-19C9-4E89-99A1-082118F1FAFF}" type="CELLRANGE">
+                    <a:fld id="{8CAFAB71-930A-4438-9CEA-994188D9CE19}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -491,7 +494,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1AFCD1AB-41E8-414C-9078-97768AAB53FF}" type="CELLRANGE">
+                    <a:fld id="{1B1C4E86-0B2D-49C9-A2E7-62087198119D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -525,7 +528,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8F5E892-BF48-4854-9CC0-DA80F66ECEE8}" type="CELLRANGE">
+                    <a:fld id="{7D9AE965-8190-4F77-859F-BB1162FD97EA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -559,7 +562,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8407393C-E243-46FD-B703-CBC9B2C39549}" type="CELLRANGE">
+                    <a:fld id="{4B7E1991-43F1-45D6-BD30-D9EC95C0DC72}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -593,7 +596,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AAFB1B89-4153-46A2-8E35-DAA1B6D67575}" type="CELLRANGE">
+                    <a:fld id="{C24803BC-3C75-47F2-A44B-0786277A881B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -627,7 +630,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8CC240B7-80A7-4E28-B9D0-2A8026435559}" type="CELLRANGE">
+                    <a:fld id="{5CDCDF60-EDF6-4F0A-880F-36A689FF121C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -661,7 +664,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{717E1828-A5A6-4F59-B8F5-5003ED14FCD6}" type="CELLRANGE">
+                    <a:fld id="{5D6480A7-E33B-464A-8A49-6334B493CB58}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -695,7 +698,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BAD10E20-5F9A-40D6-B359-B7797B841258}" type="CELLRANGE">
+                    <a:fld id="{F5C2A9CB-2A3B-4377-AC03-6A5879FC7B30}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -729,7 +732,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02DB093A-05CC-4BDF-9544-C21926CA0649}" type="CELLRANGE">
+                    <a:fld id="{69892512-9628-41A9-87CA-EF718649421E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -763,7 +766,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C1BEE74-400B-472A-A6CB-5ECDF58B9C52}" type="CELLRANGE">
+                    <a:fld id="{C1198D48-2738-48B0-8C86-41B2F861EE7E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -797,7 +800,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C23128FB-0FD4-4FE6-A948-18FCFDD56AB4}" type="CELLRANGE">
+                    <a:fld id="{060C123C-731B-4425-B8D4-652EF7E22D65}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -831,7 +834,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7338384E-1E51-4DAC-B610-D0EEAE95EBEB}" type="CELLRANGE">
+                    <a:fld id="{5B2CFA04-9FFC-46AC-8F00-4AFF7EEFA7EA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -865,7 +868,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA334FED-3D1D-4CA9-8F91-BE4D3C7A9B06}" type="CELLRANGE">
+                    <a:fld id="{C5B696C7-E72D-4B5D-9DEA-EA54B048BA74}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -899,7 +902,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C1FAB9FA-A962-47B2-836E-A4977998EAF0}" type="CELLRANGE">
+                    <a:fld id="{E603DABB-091A-4FAA-9239-72C40B0A446B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -933,7 +936,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F612DA1F-1CB0-4E5D-81E3-145DFAFE1E05}" type="CELLRANGE">
+                    <a:fld id="{67D8A855-9371-428D-B9A6-70DF53EFFA1F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -967,7 +970,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BD7B937C-3228-4FBA-82FE-78DF7445F45B}" type="CELLRANGE">
+                    <a:fld id="{EECECF1C-1A84-4F0C-8300-45ADC26B8BDF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1001,7 +1004,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{192AC8F2-2470-4673-99DA-E0AA90E6AFE2}" type="CELLRANGE">
+                    <a:fld id="{1240D96B-EA5A-4767-B5A2-60B821A0E487}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1035,7 +1038,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C4B8847A-CD1B-4CDB-B483-E74C56C8CD07}" type="CELLRANGE">
+                    <a:fld id="{FE1A31B9-BA4C-4D39-A25B-1251211A1B20}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1069,7 +1072,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{763287A5-D8E2-463D-8376-201F4281A5BC}" type="CELLRANGE">
+                    <a:fld id="{6CFBE559-A4AD-49A0-9AF4-AB3C7A925625}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1103,7 +1106,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4CD8A1A5-A396-4A12-86FF-A2F78AF1B878}" type="CELLRANGE">
+                    <a:fld id="{04EE7028-CD7D-4BF5-817E-741916B15CE9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1137,7 +1140,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB1BB88D-A062-4FA6-91BD-770148002A01}" type="CELLRANGE">
+                    <a:fld id="{D69877B0-1880-4C9E-A245-932EBDD25969}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1171,7 +1174,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A258165-4509-47A0-B8E2-9BD9B1C9F2E5}" type="CELLRANGE">
+                    <a:fld id="{42E7655F-EE47-475B-815F-3711CCB71094}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1205,7 +1208,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E13E460-6E2B-429C-AF15-7011A3A66156}" type="CELLRANGE">
+                    <a:fld id="{BCF1DF81-B309-48F5-8CCE-E4E3743734EC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1239,7 +1242,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B496C2C-5E24-4858-AF4C-F511721BCC8C}" type="CELLRANGE">
+                    <a:fld id="{FA7C7A97-C192-485F-ADDA-7798D270A14B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1273,7 +1276,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A129E79-6069-405A-B119-7BD9FA8C5CA6}" type="CELLRANGE">
+                    <a:fld id="{43CDBE4A-6B9C-4AF8-AE7A-6612D013DCC1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1307,7 +1310,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D72939F4-D933-49AB-A9F7-F6C5D9E07470}" type="CELLRANGE">
+                    <a:fld id="{711D58E2-1E87-4501-A5A6-6EB3407626EF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1341,7 +1344,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FAD4AC5B-3111-4512-BA23-D02E7FA9EAFA}" type="CELLRANGE">
+                    <a:fld id="{5DB9A196-1DB4-468F-88FD-E9A3BEE7C259}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1375,7 +1378,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{582D3DD3-3D12-4622-B759-4D9ADF287D71}" type="CELLRANGE">
+                    <a:fld id="{DD01C71A-55F0-41BF-A9EE-B5CF90F5A97C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1409,7 +1412,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F9931344-4CDE-49F9-934C-FBF54BF2F950}" type="CELLRANGE">
+                    <a:fld id="{C3D6E2A3-5BF2-482B-B6D4-1EFB74814023}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1443,7 +1446,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{858D4D94-CF4A-4C1E-B100-4952FF8265DD}" type="CELLRANGE">
+                    <a:fld id="{4366147D-65D6-4AD6-BB90-D9160BC85DBC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1477,7 +1480,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB2B724F-B978-44BB-A64F-EAE97E0B8CA0}" type="CELLRANGE">
+                    <a:fld id="{A9FE4AF7-A777-496A-9BE3-766566B5BD65}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1511,7 +1514,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32EC52DA-E9EC-4E61-9029-C421A31DBF53}" type="CELLRANGE">
+                    <a:fld id="{DEB1D87D-538A-4C64-9A0F-AC277E681D2A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1545,7 +1548,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C503A83-FE6C-405A-B76B-A9AEC8578FAA}" type="CELLRANGE">
+                    <a:fld id="{74A39C1D-73B6-4035-8E97-298A52D49A20}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1579,7 +1582,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5FC5F74-F8DE-47D6-8219-0DC6C36E2B80}" type="CELLRANGE">
+                    <a:fld id="{8B5692F6-BD79-4388-91B6-FD8F75A7A7B6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1613,7 +1616,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{57107324-7FE3-40C2-8B4E-28001D449144}" type="CELLRANGE">
+                    <a:fld id="{5AD3DF49-0565-4972-85DA-62C50209019C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1647,7 +1650,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{62646499-51D0-4CD1-A68E-1BE4112C1BAD}" type="CELLRANGE">
+                    <a:fld id="{E50FAF55-5345-4C78-9A32-8588805E598D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1681,7 +1684,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A035271B-086E-4E9A-AFD0-036C84828235}" type="CELLRANGE">
+                    <a:fld id="{B8B7FD1E-3348-4E26-8BF9-C4648EAFC3B6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1715,7 +1718,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56D40996-4474-4523-A4E0-3EBEBDCB1CCF}" type="CELLRANGE">
+                    <a:fld id="{A9C68958-DB61-4761-9391-F73771BFDF6B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1749,7 +1752,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8283D4B-1415-41CD-B71D-4021F7FECB43}" type="CELLRANGE">
+                    <a:fld id="{7912A50F-95F8-4CE0-A076-C55E94FA8CA8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1783,7 +1786,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5462F2E5-B48E-4417-9A17-31BCF942F492}" type="CELLRANGE">
+                    <a:fld id="{947F57F6-9B02-4511-A764-179295E76676}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1817,7 +1820,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5C115F0-9227-4101-B5D8-122A62E26FCD}" type="CELLRANGE">
+                    <a:fld id="{52A45758-75F1-4D27-B723-65D181246E56}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1851,7 +1854,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E73376A-CEA1-4603-8119-5F18A90F8706}" type="CELLRANGE">
+                    <a:fld id="{5EFD6AFC-E600-44FB-A021-2EC8503C3F76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1885,7 +1888,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8720C042-54C4-421A-BFCA-D63B7F600A7D}" type="CELLRANGE">
+                    <a:fld id="{90E4C024-47DC-4013-A28D-CDF0BF0BEF6A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1919,7 +1922,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33663522-6F5C-4544-A881-9993BEDE4F93}" type="CELLRANGE">
+                    <a:fld id="{8134CDB0-AEF9-4E55-90B4-733C82CAAE45}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1953,7 +1956,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E55A17C3-3828-4B64-A7AB-A5136BC89779}" type="CELLRANGE">
+                    <a:fld id="{AD25A549-29DE-4D67-AC68-CBAEA6D325C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1987,7 +1990,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0142C367-D3CC-455E-8C25-2B4565049700}" type="CELLRANGE">
+                    <a:fld id="{D6E004A1-F52B-47FB-B8F6-C8DC42F546DF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2021,7 +2024,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8063463C-2EE9-4D1B-B457-D8933D47B743}" type="CELLRANGE">
+                    <a:fld id="{21DF14CE-7B64-46B6-9586-3606025941B6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2055,7 +2058,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BFA6D7B-1EEC-44ED-B70B-C407BDF469E3}" type="CELLRANGE">
+                    <a:fld id="{078F7353-C8FE-4424-9AA1-96E6D46A8074}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2089,7 +2092,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF2ACE98-CEAD-48A5-BC78-3C3848E9FB61}" type="CELLRANGE">
+                    <a:fld id="{28608DA7-E8D5-4097-9F31-DE02211F9EDD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2123,7 +2126,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D09C936F-8590-4C24-AA3B-7C3F7DB5CD42}" type="CELLRANGE">
+                    <a:fld id="{0E59666E-3FB0-473D-A71B-1B092ABCA5D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2157,7 +2160,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E88B20B7-1D5A-4975-9333-A874198AF5CB}" type="CELLRANGE">
+                    <a:fld id="{8BFAD955-16E1-48A7-95F0-AAA0E14DE1B5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2191,7 +2194,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69563121-CC3C-4F01-8FDA-F53564A9FF46}" type="CELLRANGE">
+                    <a:fld id="{97795565-B263-4DD1-88BC-74A7F07AE7D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2225,7 +2228,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D10B270A-28F6-48E0-8E8F-2D17E0E48D8D}" type="CELLRANGE">
+                    <a:fld id="{33010B7B-2FBF-4B27-8C9E-AFFBA2D89F45}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2259,7 +2262,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC4F1F1F-1B3B-4BCF-947A-A67650D7F2FC}" type="CELLRANGE">
+                    <a:fld id="{6B895A9F-2FD3-4FB3-AD95-18AAB4FF66A6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2293,7 +2296,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A914E940-CF3E-4F2C-883C-AC0189035910}" type="CELLRANGE">
+                    <a:fld id="{516C4A18-0048-4927-ABDA-2069DEB0D3CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2317,6 +2320,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-2895-47D3-8EB5-D3385223803E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="58"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{35F99D25-7790-4625-8C66-1B6D2DAF9D2A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-B3A9-4001-928F-B974AB9C15F2}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2366,10 +2403,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$59</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="59"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -2494,54 +2531,57 @@
                   <c:v>7.2</c:v>
                 </c:pt>
                 <c:pt idx="41">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>3.3</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2549,10 +2589,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$59</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="59"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -2677,54 +2717,57 @@
                   <c:v>1630</c:v>
                 </c:pt>
                 <c:pt idx="41">
+                  <c:v>1090</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2864,43 +2907,43 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="42">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="43">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="43">
+                  <c:pt idx="44">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="44">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="45">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="46">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="47">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="48">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="49">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="49">
+                  <c:pt idx="50">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="50">
+                  <c:pt idx="51">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="51">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="52">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="53">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="54">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="55">
                     <c:v>strenuous</c:v>
@@ -2909,6 +2952,9 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="57">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="58">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -3961,10 +4007,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D59" totalsRowShown="0">
-  <autoFilter ref="A1:D59" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D59">
-    <sortCondition ref="A1:A59"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D60" totalsRowShown="0">
+  <autoFilter ref="A1:D60" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D60">
+    <sortCondition ref="A1:A60"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -4273,10 +4319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4880,13 +4926,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="B43">
-        <v>4.8</v>
+        <v>2.7</v>
       </c>
       <c r="C43">
-        <v>1470</v>
+        <v>1090</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
@@ -4894,55 +4940,55 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B44">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C44">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D44" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B45">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C45">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D45" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B46">
-        <v>3.3</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C46">
-        <v>600</v>
+        <v>3490</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B47">
-        <v>2.2000000000000002</v>
+        <v>3.3</v>
       </c>
       <c r="C47">
-        <v>750</v>
+        <v>600</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
@@ -4950,27 +4996,27 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B48">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C48">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D48" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B49">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C49">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
@@ -4978,71 +5024,71 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50">
+        <v>7.3</v>
+      </c>
+      <c r="C50">
+        <v>2250</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
         <v>25</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51">
-        <v>1.2</v>
-      </c>
-      <c r="C51">
-        <v>500</v>
-      </c>
-      <c r="D51" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B52">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C52">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D52" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B53">
-        <v>6.5</v>
+        <v>11</v>
       </c>
       <c r="C53">
-        <v>1650</v>
+        <v>3060</v>
       </c>
       <c r="D53" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B54">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
       <c r="C54">
-        <v>1890</v>
+        <v>1650</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
@@ -5050,41 +5096,41 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B55">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C55">
-        <v>180</v>
+        <v>1890</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B56">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C56">
-        <v>3550</v>
+        <v>180</v>
       </c>
       <c r="D56" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B57">
-        <v>10.8</v>
+        <v>7.3</v>
       </c>
       <c r="C57">
-        <v>1800</v>
+        <v>3550</v>
       </c>
       <c r="D57" t="s">
         <v>10</v>
@@ -5092,30 +5138,44 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58">
+        <v>10.8</v>
+      </c>
+      <c r="C58">
+        <v>1800</v>
+      </c>
+      <c r="D58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
         <v>55</v>
       </c>
-      <c r="B58">
+      <c r="B59">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C58">
+      <c r="C59">
         <v>3800</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
         <v>29</v>
       </c>
-      <c r="B59">
+      <c r="B60">
         <v>6</v>
       </c>
-      <c r="C59">
+      <c r="C60">
         <v>2180</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Eastside Trail and Eastside PCT Loop
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3480EC-D5A7-44FD-A081-B019CA59B5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6145C62C-7DD1-4B65-9731-12EE0CCC5B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="72">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -240,6 +240,15 @@
   </si>
   <si>
     <t>Pinnacle Saddle</t>
+  </si>
+  <si>
+    <t>Eastside PCT Loop</t>
+  </si>
+  <si>
+    <t>Eastside Trail (full)</t>
+  </si>
+  <si>
+    <t>Eastside Trail (part)</t>
   </si>
 </sst>
 </file>
@@ -358,7 +367,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A372089B-8F87-42B9-8E4D-7B3927EEA94C}" type="CELLRANGE">
+                    <a:fld id="{BD46433F-065B-4673-9988-2EE9582C6F6A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -392,7 +401,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{512482B4-161C-40D7-8A87-B679818E6065}" type="CELLRANGE">
+                    <a:fld id="{F13BB831-373E-4B68-8CCB-1A04C7A26B9B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -426,7 +435,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB3B134F-5514-48D2-B36F-7DAA45723645}" type="CELLRANGE">
+                    <a:fld id="{1BC752E5-9BA9-4DB9-8FE4-634612D253C3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -460,7 +469,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8CAFAB71-930A-4438-9CEA-994188D9CE19}" type="CELLRANGE">
+                    <a:fld id="{E48B4625-F882-4281-988F-A66E1AFE40D1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -494,7 +503,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B1C4E86-0B2D-49C9-A2E7-62087198119D}" type="CELLRANGE">
+                    <a:fld id="{411F037C-BBBA-45B5-84BD-5E2AE89A5FB3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -528,7 +537,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D9AE965-8190-4F77-859F-BB1162FD97EA}" type="CELLRANGE">
+                    <a:fld id="{B6FC95CB-3E37-420F-8BA8-5DBED903F645}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -562,7 +571,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4B7E1991-43F1-45D6-BD30-D9EC95C0DC72}" type="CELLRANGE">
+                    <a:fld id="{9FE8D6C4-20C3-45E4-BD06-F25F25D0425A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -596,7 +605,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C24803BC-3C75-47F2-A44B-0786277A881B}" type="CELLRANGE">
+                    <a:fld id="{06E3AB67-6086-40E4-BE8D-3A40C00BB270}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -630,7 +639,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5CDCDF60-EDF6-4F0A-880F-36A689FF121C}" type="CELLRANGE">
+                    <a:fld id="{4C365140-E43B-42D6-AC00-7FEDB3808E73}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -664,7 +673,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D6480A7-E33B-464A-8A49-6334B493CB58}" type="CELLRANGE">
+                    <a:fld id="{66C90860-1160-4EEA-AA81-CDBCD70A98B1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -698,7 +707,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5C2A9CB-2A3B-4377-AC03-6A5879FC7B30}" type="CELLRANGE">
+                    <a:fld id="{46046A83-1BA1-45D0-916F-A5751BC40FB0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -732,7 +741,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69892512-9628-41A9-87CA-EF718649421E}" type="CELLRANGE">
+                    <a:fld id="{A456033C-782A-4AC6-B1D5-3CD1FC4D09F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -766,7 +775,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C1198D48-2738-48B0-8C86-41B2F861EE7E}" type="CELLRANGE">
+                    <a:fld id="{86101427-BB2C-4BCD-BC27-9B0AF87D983B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -800,7 +809,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{060C123C-731B-4425-B8D4-652EF7E22D65}" type="CELLRANGE">
+                    <a:fld id="{2D93DFB2-C375-4CAE-A487-3D7323D08AF4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -834,7 +843,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B2CFA04-9FFC-46AC-8F00-4AFF7EEFA7EA}" type="CELLRANGE">
+                    <a:fld id="{441410B8-576A-4239-8EED-B3F57BF1A6AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -868,7 +877,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5B696C7-E72D-4B5D-9DEA-EA54B048BA74}" type="CELLRANGE">
+                    <a:fld id="{13538562-691E-4DEC-B9DB-8E5870A10E9A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -902,7 +911,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E603DABB-091A-4FAA-9239-72C40B0A446B}" type="CELLRANGE">
+                    <a:fld id="{7EBB6AD1-D3EE-445C-A19C-E2D0C8D49DB5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -936,7 +945,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67D8A855-9371-428D-B9A6-70DF53EFFA1F}" type="CELLRANGE">
+                    <a:fld id="{0550C648-D44F-4EC6-A362-0657761A4E09}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -970,7 +979,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EECECF1C-1A84-4F0C-8300-45ADC26B8BDF}" type="CELLRANGE">
+                    <a:fld id="{4CC4E2A9-38EE-401E-B16E-03A6EC0CE36E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1004,7 +1013,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1240D96B-EA5A-4767-B5A2-60B821A0E487}" type="CELLRANGE">
+                    <a:fld id="{471D5592-D28D-4F3A-B82C-F327B31CFD9F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1038,7 +1047,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FE1A31B9-BA4C-4D39-A25B-1251211A1B20}" type="CELLRANGE">
+                    <a:fld id="{8B57E40A-05F5-46F1-86B5-5EB859485E22}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1072,7 +1081,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CFBE559-A4AD-49A0-9AF4-AB3C7A925625}" type="CELLRANGE">
+                    <a:fld id="{2D139036-C280-4AA4-AA01-92B7FF0792CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1106,7 +1115,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{04EE7028-CD7D-4BF5-817E-741916B15CE9}" type="CELLRANGE">
+                    <a:fld id="{4860425F-60D5-454E-B08B-B21822642F7D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1140,7 +1149,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D69877B0-1880-4C9E-A245-932EBDD25969}" type="CELLRANGE">
+                    <a:fld id="{F1780D0A-819E-4812-A539-C656DE5A0035}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1174,7 +1183,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42E7655F-EE47-475B-815F-3711CCB71094}" type="CELLRANGE">
+                    <a:fld id="{AC536F06-3762-4CDC-9151-4780BB9360F7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1208,7 +1217,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BCF1DF81-B309-48F5-8CCE-E4E3743734EC}" type="CELLRANGE">
+                    <a:fld id="{30EB3AB1-5900-4A72-A4EC-3D8183C4C737}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1242,7 +1251,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA7C7A97-C192-485F-ADDA-7798D270A14B}" type="CELLRANGE">
+                    <a:fld id="{381223BA-1AAD-4B8D-BC24-C09754916E53}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1276,7 +1285,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{43CDBE4A-6B9C-4AF8-AE7A-6612D013DCC1}" type="CELLRANGE">
+                    <a:fld id="{D51AD406-C8C2-4207-8076-92AD13B217DB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1310,7 +1319,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{711D58E2-1E87-4501-A5A6-6EB3407626EF}" type="CELLRANGE">
+                    <a:fld id="{7968B6F8-7EC2-4A1F-B08D-792B0C1242B8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1344,7 +1353,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5DB9A196-1DB4-468F-88FD-E9A3BEE7C259}" type="CELLRANGE">
+                    <a:fld id="{B6BEFAD2-3636-40EC-A573-ADC98C6EE342}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1378,7 +1387,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD01C71A-55F0-41BF-A9EE-B5CF90F5A97C}" type="CELLRANGE">
+                    <a:fld id="{B104C5CC-369E-40B5-976C-FD3990276690}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1412,7 +1421,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3D6E2A3-5BF2-482B-B6D4-1EFB74814023}" type="CELLRANGE">
+                    <a:fld id="{9DF04331-C08B-4890-88F7-3FE3BD5CC31E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1446,7 +1455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4366147D-65D6-4AD6-BB90-D9160BC85DBC}" type="CELLRANGE">
+                    <a:fld id="{7E62DB5E-0C25-4AA9-9E79-836DBE527937}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1480,7 +1489,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9FE4AF7-A777-496A-9BE3-766566B5BD65}" type="CELLRANGE">
+                    <a:fld id="{D052F3C2-CEAA-466A-BD8B-F0513F795AF1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1514,7 +1523,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DEB1D87D-538A-4C64-9A0F-AC277E681D2A}" type="CELLRANGE">
+                    <a:fld id="{0BFB51EA-9D4E-4E43-8A29-0C52D73942D6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1548,7 +1557,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{74A39C1D-73B6-4035-8E97-298A52D49A20}" type="CELLRANGE">
+                    <a:fld id="{7502AA44-200A-4429-980A-10CAD3F551A0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1582,7 +1591,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B5692F6-BD79-4388-91B6-FD8F75A7A7B6}" type="CELLRANGE">
+                    <a:fld id="{749CDD92-714E-425C-9007-19C3DCA0056C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1616,7 +1625,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5AD3DF49-0565-4972-85DA-62C50209019C}" type="CELLRANGE">
+                    <a:fld id="{5C86A46F-00D4-46BF-9485-D43A20C7A476}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1650,7 +1659,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E50FAF55-5345-4C78-9A32-8588805E598D}" type="CELLRANGE">
+                    <a:fld id="{8E95A253-F72B-43CC-9139-C08581C31E8B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1684,7 +1693,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8B7FD1E-3348-4E26-8BF9-C4648EAFC3B6}" type="CELLRANGE">
+                    <a:fld id="{7692E00C-E3A8-4483-9469-93A79565144C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1718,7 +1727,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9C68958-DB61-4761-9391-F73771BFDF6B}" type="CELLRANGE">
+                    <a:fld id="{22622574-A7D1-428D-B8A6-130791DF2BDA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1752,7 +1761,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7912A50F-95F8-4CE0-A076-C55E94FA8CA8}" type="CELLRANGE">
+                    <a:fld id="{8230167D-E23A-4098-9676-F0BF1605BBA9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1786,7 +1795,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{947F57F6-9B02-4511-A764-179295E76676}" type="CELLRANGE">
+                    <a:fld id="{FF1EC917-DDBE-48E1-95AF-61CD053DD31B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1820,7 +1829,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{52A45758-75F1-4D27-B723-65D181246E56}" type="CELLRANGE">
+                    <a:fld id="{9FF0135F-90B7-4B0D-A561-500BC38B6BD5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1854,7 +1863,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5EFD6AFC-E600-44FB-A021-2EC8503C3F76}" type="CELLRANGE">
+                    <a:fld id="{F9A0BD12-3B12-4571-9F21-FFE05F5E7916}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1888,7 +1897,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{90E4C024-47DC-4013-A28D-CDF0BF0BEF6A}" type="CELLRANGE">
+                    <a:fld id="{157C201F-3BDB-4D63-B013-4CEE31357837}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1922,7 +1931,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8134CDB0-AEF9-4E55-90B4-733C82CAAE45}" type="CELLRANGE">
+                    <a:fld id="{43759E04-7B95-4920-A035-3F60877A9434}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1956,7 +1965,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD25A549-29DE-4D67-AC68-CBAEA6D325C5}" type="CELLRANGE">
+                    <a:fld id="{DA84EA4F-2F0D-4FE1-B1AB-2AD30138C3DE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1990,7 +1999,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D6E004A1-F52B-47FB-B8F6-C8DC42F546DF}" type="CELLRANGE">
+                    <a:fld id="{93FD2043-56E0-4B95-8178-93EE0300FD0B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2024,7 +2033,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{21DF14CE-7B64-46B6-9586-3606025941B6}" type="CELLRANGE">
+                    <a:fld id="{7043E125-0CFC-49FB-9BB4-45AFB814C58A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2058,7 +2067,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{078F7353-C8FE-4424-9AA1-96E6D46A8074}" type="CELLRANGE">
+                    <a:fld id="{A148BB59-E433-4823-8526-7FBD6EC1A5B8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2092,7 +2101,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{28608DA7-E8D5-4097-9F31-DE02211F9EDD}" type="CELLRANGE">
+                    <a:fld id="{E28406A9-22F9-4D5C-BE6B-11850820AEB3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2126,7 +2135,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E59666E-3FB0-473D-A71B-1B092ABCA5D0}" type="CELLRANGE">
+                    <a:fld id="{F0A33F66-100A-4F2A-BF18-C0C4636D2947}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2160,7 +2169,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8BFAD955-16E1-48A7-95F0-AAA0E14DE1B5}" type="CELLRANGE">
+                    <a:fld id="{C5CEE638-A756-4CD6-98C0-7F0B804F4D82}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2194,7 +2203,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97795565-B263-4DD1-88BC-74A7F07AE7D8}" type="CELLRANGE">
+                    <a:fld id="{549D934B-15C7-4715-9BB9-36E682BCDD0C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2228,7 +2237,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33010B7B-2FBF-4B27-8C9E-AFFBA2D89F45}" type="CELLRANGE">
+                    <a:fld id="{AE7591C7-6C86-4EA0-82E8-4E55C0F2C2C6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2262,7 +2271,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6B895A9F-2FD3-4FB3-AD95-18AAB4FF66A6}" type="CELLRANGE">
+                    <a:fld id="{B98A31C9-86A4-4CF0-AB11-B77B037BDF8E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2296,7 +2305,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{516C4A18-0048-4927-ABDA-2069DEB0D3CB}" type="CELLRANGE">
+                    <a:fld id="{45D853C8-204F-4ED8-B23C-6CA64EE5673A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2330,7 +2339,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35F99D25-7790-4625-8C66-1B6D2DAF9D2A}" type="CELLRANGE">
+                    <a:fld id="{5C666437-B51E-4943-ADEE-B6D70F7CD60B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2354,6 +2363,108 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-B3A9-4001-928F-B974AB9C15F2}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="59"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{447B562B-3537-4ED7-BED6-8CC4C045C400}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-E3F8-4332-A80A-1122A9B34D5D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="60"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7139C286-8701-4AFC-BC46-5B510CDCEB08}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-E3F8-4332-A80A-1122A9B34D5D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="61"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2EB7A0BE-50D9-4E1F-9712-617992E791AE}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-E3F8-4332-A80A-1122A9B34D5D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2403,10 +2514,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$60</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="62"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -2444,144 +2555,153 @@
                   <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>9.8000000000000007</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>9.6</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>11.6</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>12.5</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>9.1</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>12.2</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>9.75</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>5.4</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>11.9</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="29">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="30">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="31">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="32">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="33">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="34">
                   <c:v>4.2</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="35">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="36">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="37">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="38">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="39">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="40">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="41">
                   <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="43">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="47">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="48">
                   <c:v>3.3</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="49">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="50">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="51">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="52">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="53">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="54">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="55">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="56">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="57">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="58">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="59">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="60">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="61">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2589,10 +2709,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$60</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="62"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -2630,144 +2750,153 @@
                   <c:v>3030</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3850</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>1540</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>2880</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>3290</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>2660</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>2780</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>4800</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>4120</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>3420</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>1450</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>3160</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="29">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="30">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="31">
                   <c:v>880</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="32">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="33">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="34">
                   <c:v>860</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="35">
                   <c:v>1260</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="36">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="37">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="38">
                   <c:v>3100</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="39">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="40">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="41">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="42">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="43">
                   <c:v>1630</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="44">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="45">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="46">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="47">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="48">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="49">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="50">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="51">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="52">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="53">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="54">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="55">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="56">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="57">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="58">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="59">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="60">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="61">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2817,94 +2946,94 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>strenuous</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="15">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="16">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="18">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="19">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="23">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>easy</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="25">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="26">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="27">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="29">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="30">
-                    <c:v>easy</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="31">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="32">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="33">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="34">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="36">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="37">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="38">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="36">
+                  <c:pt idx="39">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="37">
-                    <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="38">
-                    <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="39">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="40">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="41">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="42">
                     <c:v>easy</c:v>
@@ -2913,48 +3042,57 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="44">
-                    <c:v>strenuous</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="45">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="46">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="48">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="47">
+                  <c:pt idx="49">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="50">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="48">
+                  <c:pt idx="51">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="49">
+                  <c:pt idx="52">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="50">
+                  <c:pt idx="53">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="51">
+                  <c:pt idx="54">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="52">
+                  <c:pt idx="55">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="53">
+                  <c:pt idx="56">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="54">
+                  <c:pt idx="57">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="55">
+                  <c:pt idx="58">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="56">
+                  <c:pt idx="59">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="57">
+                  <c:pt idx="60">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="58">
+                  <c:pt idx="61">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -4007,10 +4145,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D60" totalsRowShown="0">
-  <autoFilter ref="A1:D60" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D60">
-    <sortCondition ref="A1:A60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D63" totalsRowShown="0">
+  <autoFilter ref="A1:D63" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D63">
+    <sortCondition ref="A1:A63"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -4319,10 +4457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4518,55 +4656,55 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B14">
-        <v>6.5</v>
+        <v>7.9</v>
       </c>
       <c r="C14">
-        <v>1540</v>
+        <v>3200</v>
       </c>
       <c r="D14" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="B15">
-        <v>9.8000000000000007</v>
+        <v>11.3</v>
       </c>
       <c r="C15">
-        <v>2880</v>
+        <v>3850</v>
       </c>
       <c r="D15" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="B16">
-        <v>9.6</v>
+        <v>6.8</v>
       </c>
       <c r="C16">
-        <v>3290</v>
+        <v>1200</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B17">
-        <v>11.6</v>
+        <v>6.5</v>
       </c>
       <c r="C17">
-        <v>2660</v>
+        <v>1540</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
@@ -4574,41 +4712,41 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B18">
-        <v>12.5</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C18">
-        <v>2780</v>
+        <v>2880</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B19">
-        <v>9</v>
+        <v>9.6</v>
       </c>
       <c r="C19">
-        <v>1680</v>
+        <v>3290</v>
       </c>
       <c r="D19" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="B20">
-        <v>9.1</v>
+        <v>11.6</v>
       </c>
       <c r="C20">
-        <v>1580</v>
+        <v>2660</v>
       </c>
       <c r="D20" t="s">
         <v>1</v>
@@ -4616,155 +4754,155 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B21">
-        <v>5.2</v>
+        <v>12.5</v>
       </c>
       <c r="C21">
-        <v>1000</v>
+        <v>2780</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="B22">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C22">
-        <v>4800</v>
+        <v>1680</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B23">
-        <v>12.2</v>
+        <v>9.1</v>
       </c>
       <c r="C23">
-        <v>4120</v>
+        <v>1580</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B24">
-        <v>12</v>
+        <v>5.2</v>
       </c>
       <c r="C24">
-        <v>3420</v>
+        <v>1000</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>4800</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <v>12.2</v>
+      </c>
+      <c r="C26">
+        <v>4120</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>3420</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>37</v>
       </c>
-      <c r="B25">
+      <c r="B28">
         <f>19.5/2</f>
         <v>9.75</v>
       </c>
-      <c r="C25">
+      <c r="C28">
         <f>4400*7/8</f>
         <v>3850</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D28" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26">
-        <v>5.4</v>
-      </c>
-      <c r="C26">
-        <v>1450</v>
-      </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27">
-        <v>11.9</v>
-      </c>
-      <c r="C27">
-        <v>3160</v>
-      </c>
-      <c r="D27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28">
-        <v>11.4</v>
-      </c>
-      <c r="C28">
-        <v>2550</v>
-      </c>
-      <c r="D28" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B29">
-        <v>8.5</v>
+        <v>5.4</v>
       </c>
       <c r="C29">
-        <v>3350</v>
+        <v>1450</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B30">
-        <v>2.8</v>
+        <v>11.9</v>
       </c>
       <c r="C30">
-        <v>880</v>
+        <v>3160</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B31">
-        <v>10.4</v>
+        <v>11.4</v>
       </c>
       <c r="C31">
-        <v>1420</v>
+        <v>2550</v>
       </c>
       <c r="D31" t="s">
         <v>1</v>
@@ -4772,27 +4910,27 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B32">
-        <v>0.9</v>
+        <v>8.5</v>
       </c>
       <c r="C32">
-        <v>200</v>
+        <v>3350</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B33">
-        <v>4.2</v>
+        <v>2.8</v>
       </c>
       <c r="C33">
-        <v>860</v>
+        <v>880</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -4800,27 +4938,27 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="B34">
-        <v>4.8</v>
+        <v>10.4</v>
       </c>
       <c r="C34">
-        <v>1260</v>
+        <v>1420</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35">
-        <v>1.4</v>
+        <v>0.9</v>
       </c>
       <c r="C35">
-        <v>375</v>
+        <v>200</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
@@ -4828,97 +4966,97 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="B36">
-        <v>13.6</v>
+        <v>4.2</v>
       </c>
       <c r="C36">
-        <v>3930</v>
+        <v>860</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B37">
-        <v>10.5</v>
+        <v>4.8</v>
       </c>
       <c r="C37">
-        <v>3100</v>
+        <v>1260</v>
       </c>
       <c r="D37" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B38">
+        <v>1.4</v>
+      </c>
+      <c r="C38">
+        <v>375</v>
+      </c>
+      <c r="D38" t="s">
         <v>7</v>
-      </c>
-      <c r="C38">
-        <v>1670</v>
-      </c>
-      <c r="D38" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B39">
-        <v>8.1</v>
+        <v>13.6</v>
       </c>
       <c r="C39">
-        <v>2400</v>
+        <v>3930</v>
       </c>
       <c r="D39" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="B40">
-        <v>5.5</v>
+        <v>10.5</v>
       </c>
       <c r="C40">
-        <v>1850</v>
+        <v>3100</v>
       </c>
       <c r="D40" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B41">
-        <v>4.8</v>
+        <v>7</v>
       </c>
       <c r="C41">
-        <v>1300</v>
+        <v>1670</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B42">
-        <v>7.2</v>
+        <v>8.1</v>
       </c>
       <c r="C42">
-        <v>1630</v>
+        <v>2400</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
@@ -4926,27 +5064,27 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="B43">
-        <v>2.7</v>
+        <v>5.5</v>
       </c>
       <c r="C43">
-        <v>1090</v>
+        <v>1850</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B44">
         <v>4.8</v>
       </c>
       <c r="C44">
-        <v>1470</v>
+        <v>1300</v>
       </c>
       <c r="D44" t="s">
         <v>7</v>
@@ -4954,13 +5092,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B45">
-        <v>6.9</v>
+        <v>7.2</v>
       </c>
       <c r="C45">
-        <v>2000</v>
+        <v>1630</v>
       </c>
       <c r="D45" t="s">
         <v>1</v>
@@ -4968,27 +5106,27 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="B46">
-        <v>8.1999999999999993</v>
+        <v>2.7</v>
       </c>
       <c r="C46">
-        <v>3490</v>
+        <v>1090</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="B47">
-        <v>3.3</v>
+        <v>4.8</v>
       </c>
       <c r="C47">
-        <v>600</v>
+        <v>1470</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
@@ -4996,186 +5134,228 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B48">
-        <v>2.2000000000000002</v>
+        <v>6.9</v>
       </c>
       <c r="C48">
-        <v>750</v>
+        <v>2000</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B49">
-        <v>11</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C49">
-        <v>2170</v>
+        <v>3490</v>
       </c>
       <c r="D49" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="B50">
-        <v>7.3</v>
+        <v>3.3</v>
       </c>
       <c r="C50">
-        <v>2250</v>
+        <v>600</v>
       </c>
       <c r="D50" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C51">
+        <v>750</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52">
+        <v>11</v>
+      </c>
+      <c r="C52">
+        <v>2170</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53">
+        <v>7.3</v>
+      </c>
+      <c r="C53">
+        <v>2250</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
         <v>25</v>
       </c>
-      <c r="B51">
+      <c r="B54">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C51">
+      <c r="C54">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D54" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52">
-        <v>1.2</v>
-      </c>
-      <c r="C52">
-        <v>500</v>
-      </c>
-      <c r="D52" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B53">
-        <v>11</v>
-      </c>
-      <c r="C53">
-        <v>3060</v>
-      </c>
-      <c r="D53" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54">
-        <v>6.5</v>
-      </c>
-      <c r="C54">
-        <v>1650</v>
-      </c>
-      <c r="D54" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="B55">
-        <v>6.2</v>
+        <v>1.2</v>
       </c>
       <c r="C55">
-        <v>1890</v>
+        <v>500</v>
       </c>
       <c r="D55" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B56">
-        <v>0.4</v>
+        <v>11</v>
       </c>
       <c r="C56">
-        <v>180</v>
+        <v>3060</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B57">
-        <v>7.3</v>
+        <v>6.5</v>
       </c>
       <c r="C57">
-        <v>3550</v>
+        <v>1650</v>
       </c>
       <c r="D57" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="B58">
-        <v>10.8</v>
+        <v>6.2</v>
       </c>
       <c r="C58">
-        <v>1800</v>
+        <v>1890</v>
       </c>
       <c r="D58" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59">
+        <v>0.4</v>
+      </c>
+      <c r="C59">
+        <v>180</v>
+      </c>
+      <c r="D59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>28</v>
+      </c>
+      <c r="B60">
+        <v>7.3</v>
+      </c>
+      <c r="C60">
+        <v>3550</v>
+      </c>
+      <c r="D60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61">
+        <v>10.8</v>
+      </c>
+      <c r="C61">
+        <v>1800</v>
+      </c>
+      <c r="D61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
         <v>55</v>
       </c>
-      <c r="B59">
+      <c r="B62">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C59">
+      <c r="C62">
         <v>3800</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D62" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
         <v>29</v>
       </c>
-      <c r="B60">
+      <c r="B63">
         <v>6</v>
       </c>
-      <c r="C60">
+      <c r="C63">
         <v>2180</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D63" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Chenuis Falls Trail
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083B3AAF-4983-4A37-B0B8-2F4B550D7BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19856091-8F75-454D-A74E-764A6ADE5073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>Tamanos Mountain</t>
+  </si>
+  <si>
+    <t>Chenuis Falls Trail</t>
   </si>
 </sst>
 </file>
@@ -370,7 +373,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1DF093F9-227D-4646-B1A1-8EE3C9C5FBA3}" type="CELLRANGE">
+                    <a:fld id="{7420417C-1CD7-4D01-9E64-48ED4CC48D91}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -404,7 +407,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E242334D-E57B-4877-9E15-7CB2B02FE97C}" type="CELLRANGE">
+                    <a:fld id="{24A31AAD-8170-470E-9225-8A0244307A0C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -438,7 +441,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2048C943-60BE-419D-AF3C-DA20AE2C6B5C}" type="CELLRANGE">
+                    <a:fld id="{2739F49E-8B22-4436-9572-628D59922C58}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -472,7 +475,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC69E976-2914-4177-A50A-501D454BCC48}" type="CELLRANGE">
+                    <a:fld id="{9D2EAABD-9A7E-4C78-850C-0110550ACDCF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -506,7 +509,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{72255C94-4713-4863-8157-C53187FED0EA}" type="CELLRANGE">
+                    <a:fld id="{BB532C5E-CFE0-4D77-9C20-6EAA5DE6518C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -540,7 +543,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9CBB434C-8BB9-419B-A25E-49DD61FC49D5}" type="CELLRANGE">
+                    <a:fld id="{7CE7439F-ADCA-41B1-BF3F-C6C9CCBF2DE6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -574,7 +577,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4C6D20D6-DAE6-4986-A698-A30372A0C646}" type="CELLRANGE">
+                    <a:fld id="{71E732FF-3772-43E6-AEF9-206005394B47}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -608,7 +611,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{18B7FE67-1C19-4D4C-B03B-9E41CDDBABD4}" type="CELLRANGE">
+                    <a:fld id="{E74C0D14-264F-4B88-9964-BCD4096F40A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -642,7 +645,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F1BC4D0-34C7-4741-8FF3-72E86101E1EB}" type="CELLRANGE">
+                    <a:fld id="{4BB512E6-F5A7-4DC9-B4F7-F9388726386E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -676,7 +679,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CF3F8112-7108-4C6C-87CA-4EBA12D60177}" type="CELLRANGE">
+                    <a:fld id="{66195BB1-3491-4EBD-89CA-32EA5E331163}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -710,7 +713,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{05BA55BC-C990-41B4-BF0F-D73E29C195D3}" type="CELLRANGE">
+                    <a:fld id="{B8E23886-E100-4FB5-AEE7-1233FFF9148E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -744,7 +747,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C40AB7A-0C3C-4A24-A9FA-0DBD762A500C}" type="CELLRANGE">
+                    <a:fld id="{3DE586D6-08EC-4A0B-9955-7C15004ED19D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -778,7 +781,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9AF17704-508F-45D9-8FAB-6C93F513329B}" type="CELLRANGE">
+                    <a:fld id="{B1DE8702-AFED-40FE-8B47-33FC7ABD24CA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -812,7 +815,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{05BDB9F8-C329-435C-9DA2-60453FF2B48C}" type="CELLRANGE">
+                    <a:fld id="{1EC709B3-08F6-446D-B52D-63B3C2596028}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -846,7 +849,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{57248735-7458-4A35-837B-FE2E9DAC2AFB}" type="CELLRANGE">
+                    <a:fld id="{2A9AA5DD-611A-4C06-AE96-AA91860DA652}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -880,7 +883,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7EC5F9B7-4CF2-4930-8087-BCC5FB083483}" type="CELLRANGE">
+                    <a:fld id="{BCCC5026-2B2D-4A43-901C-EDBAAD499196}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -914,7 +917,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA9F6824-BA8D-4FC2-B227-2AF625A698A2}" type="CELLRANGE">
+                    <a:fld id="{1C797EA1-D8BE-460B-832B-4734416202C0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -948,7 +951,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{00184375-C026-49B2-ACAB-694734C7A41A}" type="CELLRANGE">
+                    <a:fld id="{63C4E74F-47E2-4BA5-81CB-C10E6D95E67D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -982,7 +985,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91315F16-B09E-4CAF-90DB-8E0D0209EFD2}" type="CELLRANGE">
+                    <a:fld id="{F59CA824-1B8F-43F0-AFB3-C5B00866A987}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1016,7 +1019,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2410EB6D-70D2-4F3F-A074-A263C357285E}" type="CELLRANGE">
+                    <a:fld id="{D3C9B8A0-24DD-419F-A637-A5C214474610}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1050,7 +1053,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E84DCF8-C917-45F7-BCA2-A8884394A4CB}" type="CELLRANGE">
+                    <a:fld id="{A4EE921A-D8BF-43B3-9271-D9815F3D3FAB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1084,7 +1087,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5945CC35-FFB7-4792-9B6C-0E91306763A4}" type="CELLRANGE">
+                    <a:fld id="{60B8B38B-8D52-41ED-BADA-72DD0078E86C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1118,7 +1121,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{609A5485-7D49-42C7-A053-54AAE101340A}" type="CELLRANGE">
+                    <a:fld id="{E9BC3FE2-F6FA-401D-8AF3-EF358000522A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1152,7 +1155,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{92B76A21-B0E0-41D6-98B4-B61261406FCC}" type="CELLRANGE">
+                    <a:fld id="{694BB8C2-EE14-4BF0-A2E5-E102B6781F6C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1186,7 +1189,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C386BF2-3780-49E4-B256-B75B8B89F6AF}" type="CELLRANGE">
+                    <a:fld id="{384FC6EE-219E-4C2F-BA35-B45B4FD6B1B9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1220,7 +1223,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33A1804D-B268-4731-A180-0391A71FF8E0}" type="CELLRANGE">
+                    <a:fld id="{7DEF3857-B133-48D6-89E6-73B41BF94762}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1254,7 +1257,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B0F157E-C95C-4FCB-8855-B13A5791AC12}" type="CELLRANGE">
+                    <a:fld id="{661C1889-D337-408E-8099-68A5241EC058}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1288,7 +1291,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5E294C0F-0CC6-40EF-B230-63CF9108F762}" type="CELLRANGE">
+                    <a:fld id="{068961D1-5012-4C00-B473-810E9AD1D06E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1322,7 +1325,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D43BDBF-B6D4-4A32-B0AF-CB5B13931C98}" type="CELLRANGE">
+                    <a:fld id="{41F87B82-4948-4803-9890-BCC5C6F9A5C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1356,7 +1359,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E99EFAA5-26DC-47E9-838C-457A05F41BB8}" type="CELLRANGE">
+                    <a:fld id="{8338D7C7-355B-4266-8B31-199F951180B6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1390,7 +1393,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7EC545DB-C2DB-455B-BF4C-9EB8BB8993B7}" type="CELLRANGE">
+                    <a:fld id="{C0320690-8886-4362-9A4B-A83D8467408E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1424,7 +1427,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{25862AA5-9126-4F39-BABF-E15C178A276C}" type="CELLRANGE">
+                    <a:fld id="{ABC8583C-8D9E-4857-A7D6-B7B10464D7DB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1458,7 +1461,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{85485E90-CCD0-46B6-BB1C-A64576460FDD}" type="CELLRANGE">
+                    <a:fld id="{EC8E3BEE-2BFC-436C-B65A-71203FBBF071}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1492,7 +1495,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8621C76-46F1-4CE7-8CA1-884A3AB3EE53}" type="CELLRANGE">
+                    <a:fld id="{E9888994-CAA7-4D74-AB95-8D71376D3B3D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1526,7 +1529,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CBA71CBE-A4A1-426E-B574-6451EBE28F06}" type="CELLRANGE">
+                    <a:fld id="{E3A28890-E063-49BD-BD83-0B19B0C4941D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1560,7 +1563,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB89ED04-623B-45E6-B60C-10A7FCE31C98}" type="CELLRANGE">
+                    <a:fld id="{57D6D53D-ECFF-4119-9BA9-33138FD27D83}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1594,7 +1597,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{20388D4D-FEE2-4244-B96D-C57EC8F4BC11}" type="CELLRANGE">
+                    <a:fld id="{E9869D5A-E18E-42A4-920F-04D0E93AD1BD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1628,7 +1631,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D11DE322-09CA-496E-8861-004934A948CE}" type="CELLRANGE">
+                    <a:fld id="{8BAE4E8C-4A93-4AAA-9BBC-2E2CDC3E288B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1662,7 +1665,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8E2C3716-F161-44AA-AB2F-10AE492EA63B}" type="CELLRANGE">
+                    <a:fld id="{7F11F2A4-6CCB-41EB-BF3B-D644061EADA3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1696,7 +1699,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{440FFCF2-3934-4418-94E3-FC2295F49777}" type="CELLRANGE">
+                    <a:fld id="{F88382E0-B952-4ED0-9CA1-3905BE3DC4D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1730,7 +1733,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7D0AF92-A425-467E-B005-15B55AC1B8F9}" type="CELLRANGE">
+                    <a:fld id="{2CD7E73C-627B-4663-81CF-C9FF66285E16}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1764,7 +1767,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8971871E-6331-4036-BF6D-7786A1C9E6F9}" type="CELLRANGE">
+                    <a:fld id="{B72DADC6-0DE6-49E1-8E49-50F6D2957F8E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1798,7 +1801,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{54BC7FD9-718B-4451-8E1A-C586054F29D4}" type="CELLRANGE">
+                    <a:fld id="{35CC0317-E590-41DA-9ED5-92F22814BFA6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1832,7 +1835,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0ABC81C5-3767-4004-957C-D69EBBD867CB}" type="CELLRANGE">
+                    <a:fld id="{D18AE2F1-672C-4257-88E8-AC96153E4A08}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1866,7 +1869,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4705414D-7D0C-43DF-B4E3-08E5B61A1567}" type="CELLRANGE">
+                    <a:fld id="{F245DEAF-36C1-42F2-AA17-EA6B791D0531}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1900,7 +1903,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A90C08D-A04B-4084-BEDA-CAC1E1792655}" type="CELLRANGE">
+                    <a:fld id="{68195A60-CAC0-483D-AFC2-56B2CF1DB211}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1934,7 +1937,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{534ECDF3-91E2-439F-BD3A-696D076B339E}" type="CELLRANGE">
+                    <a:fld id="{A7782E41-76C4-41C3-B7D3-143848E3B969}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1968,7 +1971,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{41266692-2050-493A-9F0A-1BD2CE77F795}" type="CELLRANGE">
+                    <a:fld id="{1505E7CF-3F11-4E2B-A9B8-25D95BB614F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2002,7 +2005,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{71C218A8-8140-49EE-B1E7-29218084CACD}" type="CELLRANGE">
+                    <a:fld id="{C6CC7CEB-F6BE-468A-B8F7-52D104003C99}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2036,7 +2039,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C68AC7DB-F64C-4692-BD20-CEAC21E633C2}" type="CELLRANGE">
+                    <a:fld id="{7F7B189B-474F-40F1-B614-30E4589DDC2A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2070,7 +2073,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CAB58A2F-0717-4723-B3A8-ED43A420B590}" type="CELLRANGE">
+                    <a:fld id="{F1B7BB12-466A-47C4-87AF-574DF1138F4C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2104,7 +2107,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F3D7F89-33EC-444F-A192-228BED5FDE46}" type="CELLRANGE">
+                    <a:fld id="{89DC1754-1677-46BF-B8DE-825A05AA9BC5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2138,7 +2141,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FB706793-3B4E-4529-B7DE-BAE03C4E93D8}" type="CELLRANGE">
+                    <a:fld id="{B181C08E-5980-492D-9AA6-886C46FC8819}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2172,7 +2175,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E4A045DC-B29A-4464-A5C0-FCA2F77FF46F}" type="CELLRANGE">
+                    <a:fld id="{FEB109CD-30DF-4FB9-A556-84A53694BB3B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2206,7 +2209,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2EE06CD1-5D66-4D9B-8A04-A3FC6471C390}" type="CELLRANGE">
+                    <a:fld id="{79E11B34-8FDD-4073-B3C0-BA8E999D1A8E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2240,7 +2243,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF27F118-2FFF-418C-B58F-DF698E85C6DC}" type="CELLRANGE">
+                    <a:fld id="{06C9F075-B161-49F6-A233-A52A0B6774DB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2274,7 +2277,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA627F43-4C9F-465A-B811-042B0B4975BA}" type="CELLRANGE">
+                    <a:fld id="{1DBDF5B3-4B55-4268-AD61-FBFAB5DAC42D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2308,7 +2311,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{55894F78-1201-4875-AF35-D705333B56E9}" type="CELLRANGE">
+                    <a:fld id="{B0635626-4191-43C1-AE3A-6143CF42677C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2342,7 +2345,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{061AAD44-0BAA-4B5C-96BA-177706AB7993}" type="CELLRANGE">
+                    <a:fld id="{7E4E2CD9-30E8-48F1-80DC-D2047D097CFA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2376,7 +2379,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1244E54C-BBDA-4329-B5B1-0DCCF0F5A43B}" type="CELLRANGE">
+                    <a:fld id="{36C5FD39-EEE5-4C0F-82FC-EB62F7475B97}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2410,7 +2413,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF944532-6746-4284-9EA8-93529677B8FC}" type="CELLRANGE">
+                    <a:fld id="{646BA5E4-90AC-4667-BC54-D565F741EFBB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2444,7 +2447,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9585BC5A-5B0C-4690-B4C7-861230126B1F}" type="CELLRANGE">
+                    <a:fld id="{D11FD703-CC77-41D5-9C55-7FBB841AF364}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2478,7 +2481,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4B015F13-8612-473A-A7EA-7161E5E1BF72}" type="CELLRANGE">
+                    <a:fld id="{3F6B4A6A-7E27-49F2-8E87-069070197858}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2502,6 +2505,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-6227-4D30-994E-D7B0AF6E6DEF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="63"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{6E80B751-27D4-4C23-AF74-D1015DE01F19}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-CF74-4E88-9A3C-E443B85DDBA8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2551,10 +2588,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$64</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="63"/>
+                <c:ptCount val="64"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -2574,174 +2611,177 @@
                   <c:v>10.3</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>7.5</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>3.4</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>2.9</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>7.1</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>7.9</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>11.3</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>6.8</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>9.8000000000000007</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>9.6</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>11.6</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>12.5</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>9.1</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>12.2</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>9.75</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>5.4</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>11.9</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>4.2</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>7.2</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>2.7</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>3.3</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>9.9</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2749,10 +2789,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$64</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="63"/>
+                <c:ptCount val="64"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -2772,174 +2812,177 @@
                   <c:v>690</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>1270</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2970</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>3110</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>940</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>3030</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>3200</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>1200</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>1540</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>2880</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>3290</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>2660</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>2780</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>4800</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>4120</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>3420</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>1450</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>3160</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>880</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>860</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>1260</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>3100</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>1630</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>3180</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -2974,55 +3017,55 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="7">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
                     <c:v>moderate (because rough)</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="11">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="13">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="14">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="16">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="17">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="19">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="20">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="21">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="22">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="24">
                     <c:v>strenuous</c:v>
@@ -3034,25 +3077,25 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="27">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="28">
+                  <c:pt idx="29">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="29">
+                  <c:pt idx="30">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="30">
+                  <c:pt idx="31">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="31">
+                  <c:pt idx="32">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="32">
+                  <c:pt idx="33">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="33">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="34">
                     <c:v>easy</c:v>
@@ -3064,13 +3107,13 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="37">
-                    <c:v>strenuous</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="38">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="39">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="40">
                     <c:v>moderate</c:v>
@@ -3079,58 +3122,58 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="42">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="43">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="43">
+                  <c:pt idx="44">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="44">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="45">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="46">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="47">
+                  <c:pt idx="48">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="48">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="49">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="50">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="51">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="52">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="53">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="53">
+                  <c:pt idx="54">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="54">
+                  <c:pt idx="55">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="55">
+                  <c:pt idx="56">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="56">
+                  <c:pt idx="57">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="57">
+                  <c:pt idx="58">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="58">
+                  <c:pt idx="59">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="59">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="60">
                     <c:v>strenuous</c:v>
@@ -3139,6 +3182,9 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="62">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="63">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -4191,10 +4237,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D64" totalsRowShown="0">
-  <autoFilter ref="A1:D64" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D64">
-    <sortCondition ref="A1:A64"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D65" totalsRowShown="0">
+  <autoFilter ref="A1:D65" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D65">
+    <sortCondition ref="A1:A65"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -4503,10 +4549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4618,13 +4664,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="B8">
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>2970</v>
+        <v>1270</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
@@ -4632,55 +4678,55 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B9">
-        <v>8.1999999999999993</v>
+        <v>7.5</v>
       </c>
       <c r="C9">
-        <v>3110</v>
+        <v>2970</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B10">
-        <v>3.4</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C10">
-        <v>940</v>
+        <v>3110</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="C11">
-        <v>1000</v>
+        <v>940</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12">
-        <v>2.9</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>1090</v>
+        <v>1000</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -4688,41 +4734,41 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B13">
-        <v>7.1</v>
+        <v>2.9</v>
       </c>
       <c r="C13">
-        <v>3030</v>
+        <v>1090</v>
       </c>
       <c r="D13" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="B14">
-        <v>7.9</v>
+        <v>7.1</v>
       </c>
       <c r="C14">
-        <v>3200</v>
+        <v>3030</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15">
-        <v>11.3</v>
+        <v>7.9</v>
       </c>
       <c r="C15">
-        <v>3850</v>
+        <v>3200</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
@@ -4730,41 +4776,41 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16">
-        <v>6.8</v>
+        <v>11.3</v>
       </c>
       <c r="C16">
-        <v>1200</v>
+        <v>3850</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B17">
-        <v>6.5</v>
+        <v>6.8</v>
       </c>
       <c r="C17">
-        <v>1540</v>
+        <v>1200</v>
       </c>
       <c r="D17" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B18">
-        <v>9.8000000000000007</v>
+        <v>6.5</v>
       </c>
       <c r="C18">
-        <v>2880</v>
+        <v>1540</v>
       </c>
       <c r="D18" t="s">
         <v>1</v>
@@ -4772,69 +4818,69 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19">
-        <v>9.6</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C19">
-        <v>3290</v>
+        <v>2880</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>11.6</v>
+        <v>9.6</v>
       </c>
       <c r="C20">
-        <v>2660</v>
+        <v>3290</v>
       </c>
       <c r="D20" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B21">
-        <v>12.5</v>
+        <v>11.6</v>
       </c>
       <c r="C21">
-        <v>2780</v>
+        <v>2660</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>12.5</v>
       </c>
       <c r="C22">
-        <v>1680</v>
+        <v>2780</v>
       </c>
       <c r="D22" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B23">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>1580</v>
+        <v>1680</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
@@ -4842,41 +4888,41 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B24">
-        <v>5.2</v>
+        <v>9.1</v>
       </c>
       <c r="C24">
-        <v>1000</v>
+        <v>1580</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B25">
-        <v>14</v>
+        <v>5.2</v>
       </c>
       <c r="C25">
-        <v>4800</v>
+        <v>1000</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
         <v>14</v>
       </c>
-      <c r="B26">
-        <v>12.2</v>
-      </c>
       <c r="C26">
-        <v>4120</v>
+        <v>4800</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
@@ -4884,13 +4930,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27">
-        <v>12</v>
+        <v>12.2</v>
       </c>
       <c r="C27">
-        <v>3420</v>
+        <v>4120</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
@@ -4898,127 +4944,127 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>3420</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>37</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <f>19.5/2</f>
         <v>9.75</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <f>4400*7/8</f>
         <v>3850</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29">
-        <v>5.4</v>
-      </c>
-      <c r="C29">
-        <v>1450</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B30">
-        <v>11.9</v>
+        <v>5.4</v>
       </c>
       <c r="C30">
-        <v>3160</v>
+        <v>1450</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B31">
-        <v>11.4</v>
+        <v>11.9</v>
       </c>
       <c r="C31">
-        <v>2550</v>
+        <v>3160</v>
       </c>
       <c r="D31" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B32">
-        <v>8.5</v>
+        <v>11.4</v>
       </c>
       <c r="C32">
-        <v>3350</v>
+        <v>2550</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B33">
-        <v>2.8</v>
+        <v>8.5</v>
       </c>
       <c r="C33">
-        <v>880</v>
+        <v>3350</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B34">
-        <v>10.4</v>
+        <v>2.8</v>
       </c>
       <c r="C34">
-        <v>1420</v>
+        <v>880</v>
       </c>
       <c r="D34" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B35">
-        <v>0.9</v>
+        <v>10.4</v>
       </c>
       <c r="C35">
-        <v>200</v>
+        <v>1420</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B36">
-        <v>4.2</v>
+        <v>0.9</v>
       </c>
       <c r="C36">
-        <v>860</v>
+        <v>200</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
@@ -5026,13 +5072,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B37">
-        <v>4.8</v>
+        <v>4.2</v>
       </c>
       <c r="C37">
-        <v>1260</v>
+        <v>860</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>
@@ -5040,13 +5086,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B38">
-        <v>1.4</v>
+        <v>4.8</v>
       </c>
       <c r="C38">
-        <v>375</v>
+        <v>1260</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
@@ -5054,27 +5100,27 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B39">
-        <v>13.6</v>
+        <v>1.4</v>
       </c>
       <c r="C39">
-        <v>3930</v>
+        <v>375</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B40">
-        <v>10.5</v>
+        <v>13.6</v>
       </c>
       <c r="C40">
-        <v>3100</v>
+        <v>3930</v>
       </c>
       <c r="D40" t="s">
         <v>10</v>
@@ -5082,27 +5128,27 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B41">
-        <v>7</v>
+        <v>10.5</v>
       </c>
       <c r="C41">
-        <v>1670</v>
+        <v>3100</v>
       </c>
       <c r="D41" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B42">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="C42">
-        <v>2400</v>
+        <v>1670</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
@@ -5110,13 +5156,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B43">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C43">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
@@ -5124,55 +5170,55 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B44">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C44">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B45">
-        <v>7.2</v>
+        <v>4.8</v>
       </c>
       <c r="C45">
-        <v>1630</v>
+        <v>1300</v>
       </c>
       <c r="D45" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B46">
-        <v>2.7</v>
+        <v>7.2</v>
       </c>
       <c r="C46">
-        <v>1090</v>
+        <v>1630</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="B47">
-        <v>4.8</v>
+        <v>2.7</v>
       </c>
       <c r="C47">
-        <v>1470</v>
+        <v>1090</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
@@ -5180,55 +5226,55 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B48">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C48">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D48" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B49">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C49">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D49" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B50">
-        <v>3.3</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C50">
-        <v>600</v>
+        <v>3490</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B51">
-        <v>2.2000000000000002</v>
+        <v>3.3</v>
       </c>
       <c r="C51">
-        <v>750</v>
+        <v>600</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -5236,27 +5282,27 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B52">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C52">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D52" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B53">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C53">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D53" t="s">
         <v>1</v>
@@ -5264,127 +5310,127 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54">
+        <v>7.3</v>
+      </c>
+      <c r="C54">
+        <v>2250</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
         <v>25</v>
       </c>
-      <c r="B54">
+      <c r="B55">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C54">
+      <c r="C55">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
-        <v>49</v>
-      </c>
-      <c r="B55">
-        <v>1.2</v>
-      </c>
-      <c r="C55">
-        <v>500</v>
-      </c>
-      <c r="D55" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B56">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C56">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D56" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B57">
-        <v>6.5</v>
+        <v>11</v>
       </c>
       <c r="C57">
-        <v>1650</v>
+        <v>3060</v>
       </c>
       <c r="D57" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B58">
-        <v>9.9</v>
+        <v>6.5</v>
       </c>
       <c r="C58">
-        <v>3180</v>
+        <v>1650</v>
       </c>
       <c r="D58" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="B59">
-        <v>6.2</v>
+        <v>9.9</v>
       </c>
       <c r="C59">
-        <v>1890</v>
+        <v>3180</v>
       </c>
       <c r="D59" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B60">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C60">
-        <v>180</v>
+        <v>1890</v>
       </c>
       <c r="D60" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B61">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C61">
-        <v>3550</v>
+        <v>180</v>
       </c>
       <c r="D61" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B62">
-        <v>10.8</v>
+        <v>7.3</v>
       </c>
       <c r="C62">
-        <v>1800</v>
+        <v>3550</v>
       </c>
       <c r="D62" t="s">
         <v>10</v>
@@ -5392,30 +5438,44 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63">
+        <v>10.8</v>
+      </c>
+      <c r="C63">
+        <v>1800</v>
+      </c>
+      <c r="D63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
         <v>55</v>
       </c>
-      <c r="B63">
+      <c r="B64">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C63">
+      <c r="C64">
         <v>3800</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D64" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
         <v>29</v>
       </c>
-      <c r="B64">
+      <c r="B65">
         <v>6</v>
       </c>
-      <c r="C64">
+      <c r="C65">
         <v>2180</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Nisqually Boundary Trail
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19856091-8F75-454D-A74E-764A6ADE5073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFB4364-D483-45DC-911E-A8F949D138D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hike Difficulties" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>Chenuis Falls Trail</t>
+  </si>
+  <si>
+    <t>Nisqually Boundary Trail</t>
   </si>
 </sst>
 </file>
@@ -373,7 +376,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7420417C-1CD7-4D01-9E64-48ED4CC48D91}" type="CELLRANGE">
+                    <a:fld id="{14022948-127C-4AD1-9EB7-842FCCCB6187}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -407,7 +410,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{24A31AAD-8170-470E-9225-8A0244307A0C}" type="CELLRANGE">
+                    <a:fld id="{F737B911-4D3B-4EA4-B32E-D2F9762093E7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -441,7 +444,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2739F49E-8B22-4436-9572-628D59922C58}" type="CELLRANGE">
+                    <a:fld id="{CBD4A2D9-C19A-49D2-A18D-724E85544089}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -475,7 +478,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D2EAABD-9A7E-4C78-850C-0110550ACDCF}" type="CELLRANGE">
+                    <a:fld id="{F5494828-9454-4A03-B22B-4B758062A1FB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -509,7 +512,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB532C5E-CFE0-4D77-9C20-6EAA5DE6518C}" type="CELLRANGE">
+                    <a:fld id="{986A1EAE-8B19-43F4-8E28-0338FE4E499E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -543,7 +546,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7CE7439F-ADCA-41B1-BF3F-C6C9CCBF2DE6}" type="CELLRANGE">
+                    <a:fld id="{CE71D489-3DCE-44CC-81E9-3B5EB7D543BC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -577,7 +580,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{71E732FF-3772-43E6-AEF9-206005394B47}" type="CELLRANGE">
+                    <a:fld id="{C28512EB-A2AB-47DE-927C-934A265B2611}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -611,7 +614,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E74C0D14-264F-4B88-9964-BCD4096F40A1}" type="CELLRANGE">
+                    <a:fld id="{3ADDAFE9-FDDA-4871-AC1F-387903AFBE01}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -645,7 +648,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4BB512E6-F5A7-4DC9-B4F7-F9388726386E}" type="CELLRANGE">
+                    <a:fld id="{FD364940-8C5B-40E4-A1A6-324DFB5AC85C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -679,7 +682,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{66195BB1-3491-4EBD-89CA-32EA5E331163}" type="CELLRANGE">
+                    <a:fld id="{54F48A47-16D2-4512-8832-A326387FC971}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -713,7 +716,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8E23886-E100-4FB5-AEE7-1233FFF9148E}" type="CELLRANGE">
+                    <a:fld id="{E84A788B-DE70-447E-973F-34ABE1653D86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -747,7 +750,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3DE586D6-08EC-4A0B-9955-7C15004ED19D}" type="CELLRANGE">
+                    <a:fld id="{05CDAA7D-8321-446F-AEAC-A81207DC68A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -781,7 +784,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B1DE8702-AFED-40FE-8B47-33FC7ABD24CA}" type="CELLRANGE">
+                    <a:fld id="{14C2DA0B-2033-4B35-931D-1FCAA33E351C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -815,7 +818,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1EC709B3-08F6-446D-B52D-63B3C2596028}" type="CELLRANGE">
+                    <a:fld id="{8AB217D1-B31F-49D2-895A-98ADEFC0E464}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -849,7 +852,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A9AA5DD-611A-4C06-AE96-AA91860DA652}" type="CELLRANGE">
+                    <a:fld id="{A041D249-E4AA-475F-BA9C-A1C8FFFC6CCD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -883,7 +886,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BCCC5026-2B2D-4A43-901C-EDBAAD499196}" type="CELLRANGE">
+                    <a:fld id="{D9BFE083-F734-4B19-A9D5-174B2B79BFB2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -917,7 +920,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C797EA1-D8BE-460B-832B-4734416202C0}" type="CELLRANGE">
+                    <a:fld id="{7006F81A-547D-4452-907F-443290B7499C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -951,7 +954,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63C4E74F-47E2-4BA5-81CB-C10E6D95E67D}" type="CELLRANGE">
+                    <a:fld id="{E733F791-890A-4884-B74C-E55B0D11AC4D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -985,7 +988,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F59CA824-1B8F-43F0-AFB3-C5B00866A987}" type="CELLRANGE">
+                    <a:fld id="{A9BD83A6-C9C3-4461-B0F5-2C71BA0505F1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1019,7 +1022,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3C9B8A0-24DD-419F-A637-A5C214474610}" type="CELLRANGE">
+                    <a:fld id="{1D765793-68F6-40FE-88E5-172A1720E0B7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1053,7 +1056,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A4EE921A-D8BF-43B3-9271-D9815F3D3FAB}" type="CELLRANGE">
+                    <a:fld id="{53CEDD71-6458-4EBE-B56A-3A821EB22762}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1087,7 +1090,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60B8B38B-8D52-41ED-BADA-72DD0078E86C}" type="CELLRANGE">
+                    <a:fld id="{B11CCCFE-D5CA-45C2-8855-0E4604FDD7AF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1121,7 +1124,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9BC3FE2-F6FA-401D-8AF3-EF358000522A}" type="CELLRANGE">
+                    <a:fld id="{F68E30E2-423F-46D4-B2BF-967B1AE559BF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1155,7 +1158,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{694BB8C2-EE14-4BF0-A2E5-E102B6781F6C}" type="CELLRANGE">
+                    <a:fld id="{7D5914A5-E7E5-4F45-816C-BE774D04AA54}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1189,7 +1192,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{384FC6EE-219E-4C2F-BA35-B45B4FD6B1B9}" type="CELLRANGE">
+                    <a:fld id="{FC07574F-17B5-42F7-8294-4BD3B770B8FB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1223,7 +1226,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7DEF3857-B133-48D6-89E6-73B41BF94762}" type="CELLRANGE">
+                    <a:fld id="{6EA4EA50-986E-4BF2-9B50-97B59E1619C4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1257,7 +1260,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{661C1889-D337-408E-8099-68A5241EC058}" type="CELLRANGE">
+                    <a:fld id="{1EA819D9-8DA1-4EE0-BB47-905A850F302C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1291,7 +1294,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{068961D1-5012-4C00-B473-810E9AD1D06E}" type="CELLRANGE">
+                    <a:fld id="{A2635884-4DB2-4279-AD80-9EBE0A75F706}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1325,7 +1328,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{41F87B82-4948-4803-9890-BCC5C6F9A5C5}" type="CELLRANGE">
+                    <a:fld id="{B29D5AC5-8DDA-4342-A371-A2A578991D29}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1359,7 +1362,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8338D7C7-355B-4266-8B31-199F951180B6}" type="CELLRANGE">
+                    <a:fld id="{F8A44E09-4458-4B0C-9825-6B1658FADE0E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1393,7 +1396,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0320690-8886-4362-9A4B-A83D8467408E}" type="CELLRANGE">
+                    <a:fld id="{3DD965CB-4EA7-4414-A2FA-21F47121B989}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1427,7 +1430,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ABC8583C-8D9E-4857-A7D6-B7B10464D7DB}" type="CELLRANGE">
+                    <a:fld id="{FAB5CA12-FE07-499C-85AD-E9E71478EF82}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1461,7 +1464,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC8E3BEE-2BFC-436C-B65A-71203FBBF071}" type="CELLRANGE">
+                    <a:fld id="{CE1FFC94-5E51-4C5D-AE84-30FF935EDFFC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1495,7 +1498,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9888994-CAA7-4D74-AB95-8D71376D3B3D}" type="CELLRANGE">
+                    <a:fld id="{1616778F-B86A-4DE7-9512-11220693AAE3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1529,7 +1532,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E3A28890-E063-49BD-BD83-0B19B0C4941D}" type="CELLRANGE">
+                    <a:fld id="{1D241687-6FCD-4349-8291-CCB1E08D06D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1563,7 +1566,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{57D6D53D-ECFF-4119-9BA9-33138FD27D83}" type="CELLRANGE">
+                    <a:fld id="{924B0A6F-77B6-4EF7-B10B-9CC510D32923}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1597,7 +1600,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9869D5A-E18E-42A4-920F-04D0E93AD1BD}" type="CELLRANGE">
+                    <a:fld id="{9CC6B440-9A4E-4EFC-9F00-6C7556BA0B6F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1631,7 +1634,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8BAE4E8C-4A93-4AAA-9BBC-2E2CDC3E288B}" type="CELLRANGE">
+                    <a:fld id="{A91FF528-3C9D-40EC-B6E3-28B2799D4277}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1665,7 +1668,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F11F2A4-6CCB-41EB-BF3B-D644061EADA3}" type="CELLRANGE">
+                    <a:fld id="{882F2C9D-6DF4-4B0D-9079-2CECAA8E202F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1699,7 +1702,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F88382E0-B952-4ED0-9CA1-3905BE3DC4D8}" type="CELLRANGE">
+                    <a:fld id="{63B84441-F13A-4639-AD6A-494FD849485D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1733,7 +1736,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2CD7E73C-627B-4663-81CF-C9FF66285E16}" type="CELLRANGE">
+                    <a:fld id="{F89CC352-36DF-43F4-980B-BC504BFA6403}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1767,7 +1770,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B72DADC6-0DE6-49E1-8E49-50F6D2957F8E}" type="CELLRANGE">
+                    <a:fld id="{354DFDD3-7113-42EC-A092-D35BD7D94D67}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1801,7 +1804,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35CC0317-E590-41DA-9ED5-92F22814BFA6}" type="CELLRANGE">
+                    <a:fld id="{26E408B0-6442-4068-B003-4D8084A77203}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1835,7 +1838,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D18AE2F1-672C-4257-88E8-AC96153E4A08}" type="CELLRANGE">
+                    <a:fld id="{DCC99824-E7A7-4649-9028-4C067EF5BAE4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1869,7 +1872,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F245DEAF-36C1-42F2-AA17-EA6B791D0531}" type="CELLRANGE">
+                    <a:fld id="{44AC92A5-29D8-4CA7-BE4E-0B30FDE768B3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1903,7 +1906,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{68195A60-CAC0-483D-AFC2-56B2CF1DB211}" type="CELLRANGE">
+                    <a:fld id="{A1217FC7-6A34-403D-B896-4436AC1E12B3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1937,7 +1940,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A7782E41-76C4-41C3-B7D3-143848E3B969}" type="CELLRANGE">
+                    <a:fld id="{E7AACE3C-F35C-4037-A6EF-85C0828FC088}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1971,7 +1974,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1505E7CF-3F11-4E2B-A9B8-25D95BB614F8}" type="CELLRANGE">
+                    <a:fld id="{8DB111A9-EE57-4D63-8C95-09B991BF6045}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2005,7 +2008,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C6CC7CEB-F6BE-468A-B8F7-52D104003C99}" type="CELLRANGE">
+                    <a:fld id="{949907F4-BF74-4184-BDCF-7EBC434A2E7F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2039,7 +2042,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F7B189B-474F-40F1-B614-30E4589DDC2A}" type="CELLRANGE">
+                    <a:fld id="{467A1854-D677-4D9D-9F82-B31F408CF37C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2073,7 +2076,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F1B7BB12-466A-47C4-87AF-574DF1138F4C}" type="CELLRANGE">
+                    <a:fld id="{A7B29E1E-CB2E-44D9-9C35-5463A7CDE5BF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2107,7 +2110,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{89DC1754-1677-46BF-B8DE-825A05AA9BC5}" type="CELLRANGE">
+                    <a:fld id="{CF635A13-0FC4-49BB-B90D-988D5A6C9C00}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2141,7 +2144,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B181C08E-5980-492D-9AA6-886C46FC8819}" type="CELLRANGE">
+                    <a:fld id="{9959408C-B640-4E94-A9BA-ADDBC5FF6F3B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2175,7 +2178,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FEB109CD-30DF-4FB9-A556-84A53694BB3B}" type="CELLRANGE">
+                    <a:fld id="{A3D97CD1-73B2-4928-B3DF-FD05B195704A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2209,7 +2212,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79E11B34-8FDD-4073-B3C0-BA8E999D1A8E}" type="CELLRANGE">
+                    <a:fld id="{2F77E9B6-0039-4469-B745-4AEE09BDD3CF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2243,7 +2246,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06C9F075-B161-49F6-A233-A52A0B6774DB}" type="CELLRANGE">
+                    <a:fld id="{BB2ECDA0-D890-482D-A414-36BE48FE4EFC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2277,7 +2280,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1DBDF5B3-4B55-4268-AD61-FBFAB5DAC42D}" type="CELLRANGE">
+                    <a:fld id="{2E98D3A3-80C9-42B4-B863-6D24449B0A94}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2311,7 +2314,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B0635626-4191-43C1-AE3A-6143CF42677C}" type="CELLRANGE">
+                    <a:fld id="{FF07C6A3-A70C-40DF-BAE5-1DE06E5618E7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2345,7 +2348,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E4E2CD9-30E8-48F1-80DC-D2047D097CFA}" type="CELLRANGE">
+                    <a:fld id="{A329446F-6E05-4EC6-8956-CB140946B76E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2379,7 +2382,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36C5FD39-EEE5-4C0F-82FC-EB62F7475B97}" type="CELLRANGE">
+                    <a:fld id="{2DD85133-7C5C-422D-ACCF-D4E1ABB43DFB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2413,7 +2416,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{646BA5E4-90AC-4667-BC54-D565F741EFBB}" type="CELLRANGE">
+                    <a:fld id="{15F09CC7-EDF4-473C-AA16-AD89B3883A81}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2447,7 +2450,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D11FD703-CC77-41D5-9C55-7FBB841AF364}" type="CELLRANGE">
+                    <a:fld id="{AE76EEAB-BE72-4100-99B9-822046A7A316}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2481,7 +2484,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F6B4A6A-7E27-49F2-8E87-069070197858}" type="CELLRANGE">
+                    <a:fld id="{2729926A-4E33-48A8-8D98-E55E5C019D06}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2515,7 +2518,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E80B751-27D4-4C23-AF74-D1015DE01F19}" type="CELLRANGE">
+                    <a:fld id="{2E4C1E47-B5FF-416A-8C6C-272C8DC72676}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2539,6 +2542,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-CF74-4E88-9A3C-E443B85DDBA8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="64"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{23C63C9C-E00D-47F9-B3D2-45F9D53EF75C}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-9EE3-4056-960A-4CAD4E543A52}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2588,10 +2625,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$65</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="64"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -2704,84 +2741,87 @@
                   <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="37">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>7.2</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>2.7</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>3.3</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>9.9</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2789,10 +2829,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$65</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="64"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -2905,84 +2945,87 @@
                   <c:v>1260</c:v>
                 </c:pt>
                 <c:pt idx="37">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>3100</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>1630</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>3180</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -3107,16 +3150,16 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="37">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="38">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="38">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="39">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="40">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="41">
                     <c:v>moderate</c:v>
@@ -3125,58 +3168,58 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="43">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="44">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="44">
+                  <c:pt idx="45">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="45">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="46">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="47">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="48">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="48">
+                  <c:pt idx="49">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="49">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="50">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="51">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="52">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="53">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="54">
+                  <c:pt idx="55">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="55">
+                  <c:pt idx="56">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="56">
+                  <c:pt idx="57">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="57">
+                  <c:pt idx="58">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="58">
+                  <c:pt idx="59">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="59">
+                  <c:pt idx="60">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="60">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="61">
                     <c:v>strenuous</c:v>
@@ -3185,6 +3228,9 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="63">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="64">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -4237,10 +4283,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D65" totalsRowShown="0">
-  <autoFilter ref="A1:D65" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D65">
-    <sortCondition ref="A1:A65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D66" totalsRowShown="0">
+  <autoFilter ref="A1:D66" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D66">
+    <sortCondition ref="A1:A66"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -4549,21 +4595,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.06640625" customWidth="1"/>
-    <col min="2" max="2" width="9.53125" customWidth="1"/>
-    <col min="3" max="3" width="10.1328125" customWidth="1"/>
-    <col min="4" max="4" width="9.86328125" customWidth="1"/>
+    <col min="1" max="1" width="28.08984375" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -4577,7 +4623,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -4591,7 +4637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -4605,7 +4651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -4619,7 +4665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4633,7 +4679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -4648,7 +4694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4662,7 +4708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -4676,7 +4722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -4690,7 +4736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -4704,7 +4750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -4718,7 +4764,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -4732,7 +4778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -4746,7 +4792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -4760,7 +4806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -4774,7 +4820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -4788,7 +4834,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -4802,7 +4848,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -4816,7 +4862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -4830,7 +4876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -4844,7 +4890,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -4858,7 +4904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -4872,7 +4918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -4886,7 +4932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -4900,7 +4946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -4914,7 +4960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -4928,7 +4974,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -4942,7 +4988,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -4956,7 +5002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -4972,7 +5018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -4986,7 +5032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -5000,7 +5046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -5014,7 +5060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -5028,7 +5074,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -5042,7 +5088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -5056,7 +5102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -5070,7 +5116,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -5084,7 +5130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -5098,384 +5144,398 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>2600</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>52</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <v>1.4</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>375</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>47</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>13.6</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <v>3930</v>
-      </c>
-      <c r="D40" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41">
-        <v>10.5</v>
-      </c>
-      <c r="C41">
-        <v>3100</v>
       </c>
       <c r="D41" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42">
+        <v>10.5</v>
+      </c>
+      <c r="C42">
+        <v>3100</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>34</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <v>7</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <v>1670</v>
-      </c>
-      <c r="D42" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43">
-        <v>8.1</v>
-      </c>
-      <c r="C43">
-        <v>2400</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B44">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C44">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D44" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45">
+        <v>5.5</v>
+      </c>
+      <c r="C45">
+        <v>1850</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>21</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <v>4.8</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <v>1300</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>57</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <v>7.2</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <v>1630</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>68</v>
       </c>
-      <c r="B47">
+      <c r="B48">
         <v>2.7</v>
       </c>
-      <c r="C47">
+      <c r="C48">
         <v>1090</v>
-      </c>
-      <c r="D47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>22</v>
-      </c>
-      <c r="B48">
-        <v>4.8</v>
-      </c>
-      <c r="C48">
-        <v>1470</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49">
+        <v>4.8</v>
+      </c>
+      <c r="C49">
+        <v>1470</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>23</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>6.9</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>2000</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>45</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <v>8.1999999999999993</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <v>3490</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>65</v>
       </c>
-      <c r="B51">
+      <c r="B52">
         <v>3.3</v>
       </c>
-      <c r="C51">
+      <c r="C52">
         <v>600</v>
-      </c>
-      <c r="D51" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
-        <v>40</v>
-      </c>
-      <c r="B52">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C52">
-        <v>750</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C53">
+        <v>750</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>38</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <v>11</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>2170</v>
-      </c>
-      <c r="D53" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
-        <v>24</v>
-      </c>
-      <c r="B54">
-        <v>7.3</v>
-      </c>
-      <c r="C54">
-        <v>2250</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55">
+        <v>7.3</v>
+      </c>
+      <c r="C55">
+        <v>2250</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>25</v>
       </c>
-      <c r="B55">
+      <c r="B56">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C55">
+      <c r="C56">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>49</v>
       </c>
-      <c r="B56">
+      <c r="B57">
         <v>1.2</v>
       </c>
-      <c r="C56">
+      <c r="C57">
         <v>500</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>26</v>
       </c>
-      <c r="B57">
+      <c r="B58">
         <v>11</v>
       </c>
-      <c r="C57">
+      <c r="C58">
         <v>3060</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>60</v>
       </c>
-      <c r="B58">
+      <c r="B59">
         <v>6.5</v>
       </c>
-      <c r="C58">
+      <c r="C59">
         <v>1650</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>72</v>
       </c>
-      <c r="B59">
+      <c r="B60">
         <v>9.9</v>
       </c>
-      <c r="C59">
+      <c r="C60">
         <v>3180</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>27</v>
       </c>
-      <c r="B60">
+      <c r="B61">
         <v>6.2</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <v>1890</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D61" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>48</v>
       </c>
-      <c r="B61">
+      <c r="B62">
         <v>0.4</v>
       </c>
-      <c r="C61">
+      <c r="C62">
         <v>180</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>28</v>
       </c>
-      <c r="B62">
+      <c r="B63">
         <v>7.3</v>
       </c>
-      <c r="C62">
+      <c r="C63">
         <v>3550</v>
-      </c>
-      <c r="D62" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63">
-        <v>10.8</v>
-      </c>
-      <c r="C63">
-        <v>1800</v>
       </c>
       <c r="D63" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>10.8</v>
+      </c>
+      <c r="C64">
+        <v>1800</v>
+      </c>
+      <c r="D64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>55</v>
       </c>
-      <c r="B64">
+      <c r="B65">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C64">
+      <c r="C65">
         <v>3800</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>29</v>
       </c>
-      <c r="B65">
+      <c r="B66">
         <v>6</v>
       </c>
-      <c r="C65">
+      <c r="C66">
         <v>2180</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D66" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add option to sort hikes by length, elevation, or steepness
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFB4364-D483-45DC-911E-A8F949D138D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9562ABB4-84F7-41BE-A33A-FE24D068C919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -376,7 +376,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14022948-127C-4AD1-9EB7-842FCCCB6187}" type="CELLRANGE">
+                    <a:fld id="{DEF8EEDE-F7B4-4D64-9688-B4973A43CCFF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -410,7 +410,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F737B911-4D3B-4EA4-B32E-D2F9762093E7}" type="CELLRANGE">
+                    <a:fld id="{2DC9F2F5-993D-46D5-8D51-66308D644CA6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -444,7 +444,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CBD4A2D9-C19A-49D2-A18D-724E85544089}" type="CELLRANGE">
+                    <a:fld id="{FF21E0A9-4601-456C-BC88-E8F71DB224D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -478,7 +478,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5494828-9454-4A03-B22B-4B758062A1FB}" type="CELLRANGE">
+                    <a:fld id="{416F107E-33E2-4162-A453-CD120DFB4462}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -512,7 +512,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{986A1EAE-8B19-43F4-8E28-0338FE4E499E}" type="CELLRANGE">
+                    <a:fld id="{420CF2D8-6BA5-4785-AC4D-2A9E1BC66D92}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -546,7 +546,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE71D489-3DCE-44CC-81E9-3B5EB7D543BC}" type="CELLRANGE">
+                    <a:fld id="{9BAE3CAD-0921-4CF8-9B9D-DF3CEC09D541}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -580,7 +580,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C28512EB-A2AB-47DE-927C-934A265B2611}" type="CELLRANGE">
+                    <a:fld id="{2225751F-56AE-4D56-8926-68131EC69855}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -614,7 +614,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3ADDAFE9-FDDA-4871-AC1F-387903AFBE01}" type="CELLRANGE">
+                    <a:fld id="{691624DF-9346-4A55-821F-242A8ED7CC6F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -648,7 +648,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD364940-8C5B-40E4-A1A6-324DFB5AC85C}" type="CELLRANGE">
+                    <a:fld id="{DE6C0C1E-9490-4505-94A8-E2A4C20625C0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -682,7 +682,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{54F48A47-16D2-4512-8832-A326387FC971}" type="CELLRANGE">
+                    <a:fld id="{0AE0808D-DCD1-49E2-A4B6-66F474A52477}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -716,7 +716,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E84A788B-DE70-447E-973F-34ABE1653D86}" type="CELLRANGE">
+                    <a:fld id="{C3925B3C-7E53-4966-B770-C5BD05A54548}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -750,7 +750,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{05CDAA7D-8321-446F-AEAC-A81207DC68A8}" type="CELLRANGE">
+                    <a:fld id="{88091F96-5128-413A-A7E3-345C471922CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -784,7 +784,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14C2DA0B-2033-4B35-931D-1FCAA33E351C}" type="CELLRANGE">
+                    <a:fld id="{5EFF3594-C768-40F5-A0DD-4FF874E471FC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -818,7 +818,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8AB217D1-B31F-49D2-895A-98ADEFC0E464}" type="CELLRANGE">
+                    <a:fld id="{10FDDA66-9AA6-463D-A0E7-1A086542756A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -852,7 +852,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A041D249-E4AA-475F-BA9C-A1C8FFFC6CCD}" type="CELLRANGE">
+                    <a:fld id="{077510B6-0F06-4979-B1F7-14E8C4C31822}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -886,7 +886,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D9BFE083-F734-4B19-A9D5-174B2B79BFB2}" type="CELLRANGE">
+                    <a:fld id="{BA5A212A-5464-4471-8E79-421E99B1CD65}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -920,7 +920,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7006F81A-547D-4452-907F-443290B7499C}" type="CELLRANGE">
+                    <a:fld id="{B43EBA02-A3C2-4B0B-9573-D80FC1307AD1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -954,7 +954,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E733F791-890A-4884-B74C-E55B0D11AC4D}" type="CELLRANGE">
+                    <a:fld id="{6AA24949-AA98-404B-A6D0-BD4CAF96E293}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -988,7 +988,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9BD83A6-C9C3-4461-B0F5-2C71BA0505F1}" type="CELLRANGE">
+                    <a:fld id="{7F298EEE-8AEE-4A28-9C03-0BF4AFC4872A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1022,7 +1022,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1D765793-68F6-40FE-88E5-172A1720E0B7}" type="CELLRANGE">
+                    <a:fld id="{EAA32A50-A102-417D-9C77-AC4F554D6602}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1056,7 +1056,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{53CEDD71-6458-4EBE-B56A-3A821EB22762}" type="CELLRANGE">
+                    <a:fld id="{6CD4B1FF-2D68-4964-955E-CCF6EBEDAB1B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1090,7 +1090,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B11CCCFE-D5CA-45C2-8855-0E4604FDD7AF}" type="CELLRANGE">
+                    <a:fld id="{4D095FA9-9E28-4BF0-A582-6613B105D643}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1124,7 +1124,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F68E30E2-423F-46D4-B2BF-967B1AE559BF}" type="CELLRANGE">
+                    <a:fld id="{2B24DE9A-7545-497D-8BA2-EBD5D60E2D87}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1158,7 +1158,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D5914A5-E7E5-4F45-816C-BE774D04AA54}" type="CELLRANGE">
+                    <a:fld id="{2E6AFCB4-2A38-49FE-A1E0-7F30762D5787}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1192,7 +1192,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC07574F-17B5-42F7-8294-4BD3B770B8FB}" type="CELLRANGE">
+                    <a:fld id="{01B67AC5-DA80-49A2-AB82-4AD5768E4787}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1226,7 +1226,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6EA4EA50-986E-4BF2-9B50-97B59E1619C4}" type="CELLRANGE">
+                    <a:fld id="{42C29704-C9B0-48B5-AFBD-EB694908EA61}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1260,7 +1260,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1EA819D9-8DA1-4EE0-BB47-905A850F302C}" type="CELLRANGE">
+                    <a:fld id="{FF2DF13F-828B-4E4B-9BE7-02894DA20DC0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1294,7 +1294,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A2635884-4DB2-4279-AD80-9EBE0A75F706}" type="CELLRANGE">
+                    <a:fld id="{91B8308B-F0BD-49B0-9636-55D05DE1618B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1328,7 +1328,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B29D5AC5-8DDA-4342-A371-A2A578991D29}" type="CELLRANGE">
+                    <a:fld id="{39DF87C2-EBDA-476D-83FC-999DCBE63A1D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1362,7 +1362,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8A44E09-4458-4B0C-9825-6B1658FADE0E}" type="CELLRANGE">
+                    <a:fld id="{DFF4A1E2-5282-4D13-B26F-47E417739097}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1396,7 +1396,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3DD965CB-4EA7-4414-A2FA-21F47121B989}" type="CELLRANGE">
+                    <a:fld id="{119186D1-CD6B-42B7-9250-CDB9594DDB6B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1430,7 +1430,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FAB5CA12-FE07-499C-85AD-E9E71478EF82}" type="CELLRANGE">
+                    <a:fld id="{3BD5195F-94F1-4F63-9587-8F62B41A39AF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1464,7 +1464,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE1FFC94-5E51-4C5D-AE84-30FF935EDFFC}" type="CELLRANGE">
+                    <a:fld id="{929C62FB-731F-4A89-9548-B69A64EBEF02}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1498,7 +1498,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1616778F-B86A-4DE7-9512-11220693AAE3}" type="CELLRANGE">
+                    <a:fld id="{C7C6C793-A323-441A-99E6-92F8D6A35F80}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1532,7 +1532,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1D241687-6FCD-4349-8291-CCB1E08D06D0}" type="CELLRANGE">
+                    <a:fld id="{C6CAAE57-278D-41C5-973D-DF7A51325AB1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1566,7 +1566,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{924B0A6F-77B6-4EF7-B10B-9CC510D32923}" type="CELLRANGE">
+                    <a:fld id="{0986A94C-B4D4-48EE-A1F7-972FF0FAF541}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1600,7 +1600,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9CC6B440-9A4E-4EFC-9F00-6C7556BA0B6F}" type="CELLRANGE">
+                    <a:fld id="{494EE4A2-6CE5-4831-BA64-F4A59BFA8AA3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1634,7 +1634,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A91FF528-3C9D-40EC-B6E3-28B2799D4277}" type="CELLRANGE">
+                    <a:fld id="{E7EDCA34-68C3-4D90-BEF3-1A0C00399639}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1668,7 +1668,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{882F2C9D-6DF4-4B0D-9079-2CECAA8E202F}" type="CELLRANGE">
+                    <a:fld id="{33C0C9E0-34A8-45EC-9D5D-8B06CD772AF8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1702,7 +1702,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63B84441-F13A-4639-AD6A-494FD849485D}" type="CELLRANGE">
+                    <a:fld id="{D1DA23E0-91F9-40BC-A9C8-5EF0DCA2BFDB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1736,7 +1736,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F89CC352-36DF-43F4-980B-BC504BFA6403}" type="CELLRANGE">
+                    <a:fld id="{5A3FC1B1-7A31-47F6-A76A-3AAE75CB700B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1770,7 +1770,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{354DFDD3-7113-42EC-A092-D35BD7D94D67}" type="CELLRANGE">
+                    <a:fld id="{3218C0DC-02D2-45BD-BBFB-25D2121CA599}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1804,7 +1804,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{26E408B0-6442-4068-B003-4D8084A77203}" type="CELLRANGE">
+                    <a:fld id="{D6D02669-8F9F-45D1-9A2A-C56027A8B4FD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1838,7 +1838,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DCC99824-E7A7-4649-9028-4C067EF5BAE4}" type="CELLRANGE">
+                    <a:fld id="{7B17C9E1-5B2F-406A-982F-F71A1310EFAC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1872,7 +1872,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{44AC92A5-29D8-4CA7-BE4E-0B30FDE768B3}" type="CELLRANGE">
+                    <a:fld id="{C65E7EC9-AC0B-43D5-B400-9A16E15A4B51}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1906,7 +1906,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A1217FC7-6A34-403D-B896-4436AC1E12B3}" type="CELLRANGE">
+                    <a:fld id="{352C18F0-132E-4BDA-B7EB-D0C03A07CF40}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1940,7 +1940,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7AACE3C-F35C-4037-A6EF-85C0828FC088}" type="CELLRANGE">
+                    <a:fld id="{493E18E6-8896-496D-9D88-A52E43FDCFD3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1974,7 +1974,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8DB111A9-EE57-4D63-8C95-09B991BF6045}" type="CELLRANGE">
+                    <a:fld id="{006FC954-F206-4F5F-BA11-EE1985A80221}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2008,7 +2008,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{949907F4-BF74-4184-BDCF-7EBC434A2E7F}" type="CELLRANGE">
+                    <a:fld id="{7CFC330F-3D61-401F-932C-97A580B6FA54}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2042,7 +2042,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{467A1854-D677-4D9D-9F82-B31F408CF37C}" type="CELLRANGE">
+                    <a:fld id="{8223B97D-C9FB-4E5F-B31C-07BC733D0CCC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2076,7 +2076,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A7B29E1E-CB2E-44D9-9C35-5463A7CDE5BF}" type="CELLRANGE">
+                    <a:fld id="{0D7ADD61-6136-4467-AA07-075B881B3E5D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2110,7 +2110,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CF635A13-0FC4-49BB-B90D-988D5A6C9C00}" type="CELLRANGE">
+                    <a:fld id="{20FFC496-9E75-4545-8B7A-A397D4203C40}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2144,7 +2144,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9959408C-B640-4E94-A9BA-ADDBC5FF6F3B}" type="CELLRANGE">
+                    <a:fld id="{0F4E3503-B108-4939-8FBE-DED8FAE90A5A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2178,7 +2178,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A3D97CD1-73B2-4928-B3DF-FD05B195704A}" type="CELLRANGE">
+                    <a:fld id="{4599811F-AE04-4757-9606-E62621BF28D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2212,7 +2212,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F77E9B6-0039-4469-B745-4AEE09BDD3CF}" type="CELLRANGE">
+                    <a:fld id="{A2DF2BF0-B46D-4345-AE87-67759F2765E5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2246,7 +2246,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB2ECDA0-D890-482D-A414-36BE48FE4EFC}" type="CELLRANGE">
+                    <a:fld id="{9BD8D374-4B46-4345-80A1-B46C66D5C185}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2280,7 +2280,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E98D3A3-80C9-42B4-B863-6D24449B0A94}" type="CELLRANGE">
+                    <a:fld id="{CBCD0B3F-8059-4D2F-B36B-CFD2ABECA72B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2314,7 +2314,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF07C6A3-A70C-40DF-BAE5-1DE06E5618E7}" type="CELLRANGE">
+                    <a:fld id="{4AFD5034-5308-4BAE-A727-679E060B20AF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2348,7 +2348,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A329446F-6E05-4EC6-8956-CB140946B76E}" type="CELLRANGE">
+                    <a:fld id="{0B5BA583-6A48-45FF-A707-C95570E2D953}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2382,7 +2382,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2DD85133-7C5C-422D-ACCF-D4E1ABB43DFB}" type="CELLRANGE">
+                    <a:fld id="{0A73F553-FB28-4193-9032-9AA85E4D1FF8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2416,7 +2416,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{15F09CC7-EDF4-473C-AA16-AD89B3883A81}" type="CELLRANGE">
+                    <a:fld id="{A769AA22-9956-46C9-9AB8-3DF5D79A4110}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2450,7 +2450,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE76EEAB-BE72-4100-99B9-822046A7A316}" type="CELLRANGE">
+                    <a:fld id="{E47FCFD7-F91F-4336-8E93-D00C29DF0EEB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2484,7 +2484,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2729926A-4E33-48A8-8D98-E55E5C019D06}" type="CELLRANGE">
+                    <a:fld id="{B461B431-E3E3-490F-8AA8-4DFDE95700FB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2518,7 +2518,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E4C1E47-B5FF-416A-8C6C-272C8DC72676}" type="CELLRANGE">
+                    <a:fld id="{58AFB4AD-AC3B-4024-9D23-20CCB20F834A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2552,7 +2552,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23C63C9C-E00D-47F9-B3D2-45F9D53EF75C}" type="CELLRANGE">
+                    <a:fld id="{96CAF0D7-1797-441C-B6D7-B5A623CDBD66}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3014,7 +3014,7 @@
                   <c:v>1890</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>180</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>3550</c:v>
@@ -4597,8 +4597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5476,7 +5476,7 @@
         <v>0.4</v>
       </c>
       <c r="C62">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Add West Boundary Trail
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9562ABB4-84F7-41BE-A33A-FE24D068C919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AB726D-AAF0-42C9-A112-B7308EBD5EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="76">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>Nisqually Boundary Trail</t>
+  </si>
+  <si>
+    <t>West Boundary Trail</t>
   </si>
 </sst>
 </file>
@@ -376,7 +379,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DEF8EEDE-F7B4-4D64-9688-B4973A43CCFF}" type="CELLRANGE">
+                    <a:fld id="{71D40D56-A4D5-44CF-8565-1A28AF11110F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -410,7 +413,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2DC9F2F5-993D-46D5-8D51-66308D644CA6}" type="CELLRANGE">
+                    <a:fld id="{0AE89BC6-A858-4CF1-9E9E-C3AD61610BE1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -444,7 +447,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF21E0A9-4601-456C-BC88-E8F71DB224D3}" type="CELLRANGE">
+                    <a:fld id="{6EE440CB-9293-45C5-BF86-CE70DD1EEEA4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -478,7 +481,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{416F107E-33E2-4162-A453-CD120DFB4462}" type="CELLRANGE">
+                    <a:fld id="{87CCCCEC-9FDB-472B-90AD-DA8633AF29BF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -512,7 +515,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{420CF2D8-6BA5-4785-AC4D-2A9E1BC66D92}" type="CELLRANGE">
+                    <a:fld id="{35FA939C-71F2-464B-B48B-DFDEAA997392}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -546,7 +549,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BAE3CAD-0921-4CF8-9B9D-DF3CEC09D541}" type="CELLRANGE">
+                    <a:fld id="{4F1A9D09-297C-4450-A891-6E5CEB92CCB9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -580,7 +583,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2225751F-56AE-4D56-8926-68131EC69855}" type="CELLRANGE">
+                    <a:fld id="{37A2C06E-B4B5-4D9E-B16C-BFB5D02AE306}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -614,7 +617,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{691624DF-9346-4A55-821F-242A8ED7CC6F}" type="CELLRANGE">
+                    <a:fld id="{8EB668CC-E40B-4679-A5A9-BA6389564644}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -648,7 +651,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE6C0C1E-9490-4505-94A8-E2A4C20625C0}" type="CELLRANGE">
+                    <a:fld id="{29EB0F96-959D-4EBD-8E87-9FB856BFEDA9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -682,7 +685,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0AE0808D-DCD1-49E2-A4B6-66F474A52477}" type="CELLRANGE">
+                    <a:fld id="{34541857-E757-45D7-A81E-052BA76DD056}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -716,7 +719,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3925B3C-7E53-4966-B770-C5BD05A54548}" type="CELLRANGE">
+                    <a:fld id="{977F821B-1694-45F0-BD42-1D8AC254DB8D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -750,7 +753,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88091F96-5128-413A-A7E3-345C471922CB}" type="CELLRANGE">
+                    <a:fld id="{BC006C67-C35B-45AD-8E89-FBB068AF5DE7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -784,7 +787,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5EFF3594-C768-40F5-A0DD-4FF874E471FC}" type="CELLRANGE">
+                    <a:fld id="{EC672B41-BB49-4D3C-A742-4BE42F7CC4C3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -818,7 +821,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10FDDA66-9AA6-463D-A0E7-1A086542756A}" type="CELLRANGE">
+                    <a:fld id="{42EB9272-D67C-49C3-A291-63A5F63CD82E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -852,7 +855,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{077510B6-0F06-4979-B1F7-14E8C4C31822}" type="CELLRANGE">
+                    <a:fld id="{A96C66E8-2795-4A4A-ABC1-8A560C140EBE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -886,7 +889,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BA5A212A-5464-4471-8E79-421E99B1CD65}" type="CELLRANGE">
+                    <a:fld id="{CE9DFFF3-BABB-404E-939C-18F003069194}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -920,7 +923,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B43EBA02-A3C2-4B0B-9573-D80FC1307AD1}" type="CELLRANGE">
+                    <a:fld id="{D5D344B5-27FD-4CFC-B360-857B9001FD43}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -954,7 +957,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6AA24949-AA98-404B-A6D0-BD4CAF96E293}" type="CELLRANGE">
+                    <a:fld id="{AA48724F-1CEA-4646-88C8-80F0BACF2755}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -988,7 +991,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F298EEE-8AEE-4A28-9C03-0BF4AFC4872A}" type="CELLRANGE">
+                    <a:fld id="{7E35E769-5C81-4ADC-812C-992BB7D1C511}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1022,7 +1025,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EAA32A50-A102-417D-9C77-AC4F554D6602}" type="CELLRANGE">
+                    <a:fld id="{2E69F557-0526-4C6D-BCF3-79E733487A7D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1056,7 +1059,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CD4B1FF-2D68-4964-955E-CCF6EBEDAB1B}" type="CELLRANGE">
+                    <a:fld id="{DDDEF68C-7001-4BDE-801C-CDD0142351AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1090,7 +1093,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D095FA9-9E28-4BF0-A582-6613B105D643}" type="CELLRANGE">
+                    <a:fld id="{5CB0629C-46D7-4F0D-91DB-14A7F1C63503}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1124,7 +1127,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2B24DE9A-7545-497D-8BA2-EBD5D60E2D87}" type="CELLRANGE">
+                    <a:fld id="{35CEEFF1-841B-4841-A05A-1CF07DF57CEE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1158,7 +1161,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E6AFCB4-2A38-49FE-A1E0-7F30762D5787}" type="CELLRANGE">
+                    <a:fld id="{C07F297B-439A-44EC-99CF-0D03E179A9EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1192,7 +1195,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{01B67AC5-DA80-49A2-AB82-4AD5768E4787}" type="CELLRANGE">
+                    <a:fld id="{C38EA5E3-8E37-40A9-97F2-A2723BB73202}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1226,7 +1229,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42C29704-C9B0-48B5-AFBD-EB694908EA61}" type="CELLRANGE">
+                    <a:fld id="{489E69E0-8422-4612-9E71-CFB94352E7F0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1260,7 +1263,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF2DF13F-828B-4E4B-9BE7-02894DA20DC0}" type="CELLRANGE">
+                    <a:fld id="{0394790C-50D5-460C-80D6-AAAD4DF6B282}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1294,7 +1297,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91B8308B-F0BD-49B0-9636-55D05DE1618B}" type="CELLRANGE">
+                    <a:fld id="{AF364E28-4A33-4823-8478-20FA6545A7F1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1328,7 +1331,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{39DF87C2-EBDA-476D-83FC-999DCBE63A1D}" type="CELLRANGE">
+                    <a:fld id="{F99A316D-F556-4A88-9EAE-F12C5333B8B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1362,7 +1365,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DFF4A1E2-5282-4D13-B26F-47E417739097}" type="CELLRANGE">
+                    <a:fld id="{9B0E1A70-60C6-44DB-BB7D-9AF75DD3FC9E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1396,7 +1399,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{119186D1-CD6B-42B7-9250-CDB9594DDB6B}" type="CELLRANGE">
+                    <a:fld id="{DC53C201-F247-4B75-9516-EA0BB3C70AB7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1430,7 +1433,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3BD5195F-94F1-4F63-9587-8F62B41A39AF}" type="CELLRANGE">
+                    <a:fld id="{CB749DCB-4C7D-42BE-BFD3-919D94DF9F9F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1464,7 +1467,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{929C62FB-731F-4A89-9548-B69A64EBEF02}" type="CELLRANGE">
+                    <a:fld id="{FB319B6A-A6A5-423D-B19A-89E4ADB44987}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1498,7 +1501,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7C6C793-A323-441A-99E6-92F8D6A35F80}" type="CELLRANGE">
+                    <a:fld id="{6F965725-D988-41AA-9E2C-FAEC92FFCA0F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1532,7 +1535,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C6CAAE57-278D-41C5-973D-DF7A51325AB1}" type="CELLRANGE">
+                    <a:fld id="{6A5C6AA3-CAFE-4E17-938C-53725F0F488F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1566,7 +1569,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0986A94C-B4D4-48EE-A1F7-972FF0FAF541}" type="CELLRANGE">
+                    <a:fld id="{DE81AD6F-A636-4692-B1C4-5ED88606ADAC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1600,7 +1603,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{494EE4A2-6CE5-4831-BA64-F4A59BFA8AA3}" type="CELLRANGE">
+                    <a:fld id="{C0853AC4-E1F1-40BA-92D9-C85943DB9330}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1634,7 +1637,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7EDCA34-68C3-4D90-BEF3-1A0C00399639}" type="CELLRANGE">
+                    <a:fld id="{EBD774D0-F77B-4EFA-BFC9-94DAA5571F66}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1668,7 +1671,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33C0C9E0-34A8-45EC-9D5D-8B06CD772AF8}" type="CELLRANGE">
+                    <a:fld id="{B09A7E17-A021-4D2B-839A-64D50482E789}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1702,7 +1705,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1DA23E0-91F9-40BC-A9C8-5EF0DCA2BFDB}" type="CELLRANGE">
+                    <a:fld id="{CBABF1AD-BCA3-44FC-8B41-E815A352EACC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1736,7 +1739,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A3FC1B1-7A31-47F6-A76A-3AAE75CB700B}" type="CELLRANGE">
+                    <a:fld id="{CD3ACEF9-0536-42CE-8523-924F1638FE37}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1770,7 +1773,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3218C0DC-02D2-45BD-BBFB-25D2121CA599}" type="CELLRANGE">
+                    <a:fld id="{1929F187-3804-4013-9746-95082DD0752F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1804,7 +1807,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D6D02669-8F9F-45D1-9A2A-C56027A8B4FD}" type="CELLRANGE">
+                    <a:fld id="{36D47067-088A-4DF8-B373-0BED43AD74D2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1838,7 +1841,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7B17C9E1-5B2F-406A-982F-F71A1310EFAC}" type="CELLRANGE">
+                    <a:fld id="{4FE4CE2B-E50D-4713-934A-457EB84243CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1872,7 +1875,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C65E7EC9-AC0B-43D5-B400-9A16E15A4B51}" type="CELLRANGE">
+                    <a:fld id="{2A5DA2FC-96C2-43BA-A337-42E3105A9C77}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1906,7 +1909,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{352C18F0-132E-4BDA-B7EB-D0C03A07CF40}" type="CELLRANGE">
+                    <a:fld id="{CBD0B970-D199-46D3-A469-CC7F8CDB0CEC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1940,7 +1943,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{493E18E6-8896-496D-9D88-A52E43FDCFD3}" type="CELLRANGE">
+                    <a:fld id="{91785809-0B32-4F4A-A408-5B4F6D1BE6F3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1974,7 +1977,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{006FC954-F206-4F5F-BA11-EE1985A80221}" type="CELLRANGE">
+                    <a:fld id="{1CBE4E43-BD9E-46A0-BAFA-0337ECACE37F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2008,7 +2011,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7CFC330F-3D61-401F-932C-97A580B6FA54}" type="CELLRANGE">
+                    <a:fld id="{902EB4EE-7070-4BB1-B57D-55B47E413BE4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2042,7 +2045,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8223B97D-C9FB-4E5F-B31C-07BC733D0CCC}" type="CELLRANGE">
+                    <a:fld id="{6FEE2079-1EB8-48D5-B746-2445CF928980}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2076,7 +2079,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D7ADD61-6136-4467-AA07-075B881B3E5D}" type="CELLRANGE">
+                    <a:fld id="{98ED0577-5B22-47EB-ABCA-0DAC8C5D473D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2110,7 +2113,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{20FFC496-9E75-4545-8B7A-A397D4203C40}" type="CELLRANGE">
+                    <a:fld id="{A6E20208-9009-4132-AA22-5BD8EE8029E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2144,7 +2147,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F4E3503-B108-4939-8FBE-DED8FAE90A5A}" type="CELLRANGE">
+                    <a:fld id="{2222AAFA-E250-45A5-B55D-0DF52F1D65B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2178,7 +2181,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4599811F-AE04-4757-9606-E62621BF28D0}" type="CELLRANGE">
+                    <a:fld id="{F5140372-D91A-4A38-8DC4-26457A2AC8C6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2212,7 +2215,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A2DF2BF0-B46D-4345-AE87-67759F2765E5}" type="CELLRANGE">
+                    <a:fld id="{E04ED7F9-2835-430F-AA02-77B05B41CB72}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2246,7 +2249,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BD8D374-4B46-4345-80A1-B46C66D5C185}" type="CELLRANGE">
+                    <a:fld id="{E8DAEA73-50EF-4A9B-A2B0-AAD4793A0AE0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2280,7 +2283,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CBCD0B3F-8059-4D2F-B36B-CFD2ABECA72B}" type="CELLRANGE">
+                    <a:fld id="{7EE623A9-B68A-4C47-92A7-25CA6A7B7FAC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2314,7 +2317,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4AFD5034-5308-4BAE-A727-679E060B20AF}" type="CELLRANGE">
+                    <a:fld id="{0B227442-B927-4A72-84F0-BE0DB1038865}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2348,7 +2351,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0B5BA583-6A48-45FF-A707-C95570E2D953}" type="CELLRANGE">
+                    <a:fld id="{9C7184BD-32C0-443C-8AA0-A7FAA40AEFDA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2382,7 +2385,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A73F553-FB28-4193-9032-9AA85E4D1FF8}" type="CELLRANGE">
+                    <a:fld id="{DDF32010-439F-40FD-AE98-C55965CD73AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2416,7 +2419,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A769AA22-9956-46C9-9AB8-3DF5D79A4110}" type="CELLRANGE">
+                    <a:fld id="{45A6C730-1DEF-4EB1-B1E7-833607F5664B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2450,7 +2453,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E47FCFD7-F91F-4336-8E93-D00C29DF0EEB}" type="CELLRANGE">
+                    <a:fld id="{3C54C59A-16B6-40A0-B195-858C925B3BA2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2484,7 +2487,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B461B431-E3E3-490F-8AA8-4DFDE95700FB}" type="CELLRANGE">
+                    <a:fld id="{FC60C2CF-6F59-424B-97B6-C6E82F905F2E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2518,7 +2521,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58AFB4AD-AC3B-4024-9D23-20CCB20F834A}" type="CELLRANGE">
+                    <a:fld id="{7D0074B5-D883-4E77-B4A4-C7F5ED8145AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2552,7 +2555,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96CAF0D7-1797-441C-B6D7-B5A623CDBD66}" type="CELLRANGE">
+                    <a:fld id="{062299B0-42B3-47AD-B6DE-2CA6BB74BC11}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2576,6 +2579,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-9EE3-4056-960A-4CAD4E543A52}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="65"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{36B2A222-E9F3-48F6-95B8-C0DB5EC240B1}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-15E5-41FB-A622-C3C92D097AC9}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2625,10 +2662,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$66</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="65"/>
+                <c:ptCount val="66"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -2816,12 +2853,15 @@
                   <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="62">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="63">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2829,10 +2869,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$66</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="65"/>
+                <c:ptCount val="66"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -3020,12 +3060,15 @@
                   <c:v>3550</c:v>
                 </c:pt>
                 <c:pt idx="62">
+                  <c:v>1680</c:v>
+                </c:pt>
+                <c:pt idx="63">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -3225,12 +3268,15 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="62">
-                    <c:v>strenuous</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="63">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="64">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="65">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -4283,10 +4329,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D66" totalsRowShown="0">
-  <autoFilter ref="A1:D66" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D66">
-    <sortCondition ref="A1:A66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D67" totalsRowShown="0">
+  <autoFilter ref="A1:D67" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D67">
+    <sortCondition ref="A1:A67"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -4595,10 +4641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5498,44 +5544,58 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B64">
-        <v>10.8</v>
+        <v>5.6</v>
       </c>
       <c r="C64">
-        <v>1800</v>
+        <v>1680</v>
       </c>
       <c r="D64" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>10.8</v>
+      </c>
+      <c r="C65">
+        <v>1800</v>
+      </c>
+      <c r="D65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>55</v>
       </c>
-      <c r="B65">
+      <c r="B66">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C65">
+      <c r="C66">
         <v>3800</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D66" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>29</v>
       </c>
-      <c r="B66">
+      <c r="B67">
         <v>6</v>
       </c>
-      <c r="C66">
+      <c r="C67">
         <v>2180</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Skyscraper Mountain. Add thumbnail images for pages that show lists of other hikes. Fix various minor bugs.
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AB726D-AAF0-42C9-A112-B7308EBD5EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0477773A-0C4C-498A-93A8-C07FABAF947A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="77">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>West Boundary Trail</t>
+  </si>
+  <si>
+    <t>Skyscraper Mountain</t>
   </si>
 </sst>
 </file>
@@ -379,7 +382,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{71D40D56-A4D5-44CF-8565-1A28AF11110F}" type="CELLRANGE">
+                    <a:fld id="{0C35CA22-2FEA-4E38-A9BA-A9B65D755DF5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -413,7 +416,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0AE89BC6-A858-4CF1-9E9E-C3AD61610BE1}" type="CELLRANGE">
+                    <a:fld id="{74CF0B84-B636-44C7-93F7-661FD5D65DA0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -447,7 +450,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6EE440CB-9293-45C5-BF86-CE70DD1EEEA4}" type="CELLRANGE">
+                    <a:fld id="{8CE822AE-FB06-4149-82BA-720E89D472F1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -481,7 +484,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{87CCCCEC-9FDB-472B-90AD-DA8633AF29BF}" type="CELLRANGE">
+                    <a:fld id="{88DB037D-1A8D-4B6A-BA31-82FD2E13CA8F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -515,7 +518,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35FA939C-71F2-464B-B48B-DFDEAA997392}" type="CELLRANGE">
+                    <a:fld id="{61BCF6C9-FB59-457C-BEB4-DD7A9D898534}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -549,7 +552,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F1A9D09-297C-4450-A891-6E5CEB92CCB9}" type="CELLRANGE">
+                    <a:fld id="{E4C22B06-D993-4CE0-BCE4-6FE66F4CDD76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -583,7 +586,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{37A2C06E-B4B5-4D9E-B16C-BFB5D02AE306}" type="CELLRANGE">
+                    <a:fld id="{E7894004-4084-4085-A007-CEF9572EADA8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -617,7 +620,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8EB668CC-E40B-4679-A5A9-BA6389564644}" type="CELLRANGE">
+                    <a:fld id="{417F7B45-01A8-484B-AE23-800F106175F3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -651,7 +654,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29EB0F96-959D-4EBD-8E87-9FB856BFEDA9}" type="CELLRANGE">
+                    <a:fld id="{E52A0D44-E44D-4C66-A78C-28B9AA2123D2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -685,7 +688,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34541857-E757-45D7-A81E-052BA76DD056}" type="CELLRANGE">
+                    <a:fld id="{C764DDE9-E668-479B-A5FA-D7BE3FC6763B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -719,7 +722,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{977F821B-1694-45F0-BD42-1D8AC254DB8D}" type="CELLRANGE">
+                    <a:fld id="{B8EE060C-D737-4152-B669-2EBE167B40A9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -753,7 +756,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BC006C67-C35B-45AD-8E89-FBB068AF5DE7}" type="CELLRANGE">
+                    <a:fld id="{0825D66A-113F-4111-9C8F-E73CEBE6E5B8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -787,7 +790,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC672B41-BB49-4D3C-A742-4BE42F7CC4C3}" type="CELLRANGE">
+                    <a:fld id="{7F0FC1B8-75AA-4710-AF41-52EB385DD7D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -821,7 +824,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42EB9272-D67C-49C3-A291-63A5F63CD82E}" type="CELLRANGE">
+                    <a:fld id="{E3CB1C46-BD7E-4A5B-8E40-987295B0ED42}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -855,7 +858,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A96C66E8-2795-4A4A-ABC1-8A560C140EBE}" type="CELLRANGE">
+                    <a:fld id="{12FDAC0F-15A4-46FA-A072-598780094CE2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -889,7 +892,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE9DFFF3-BABB-404E-939C-18F003069194}" type="CELLRANGE">
+                    <a:fld id="{ADA34A8D-3794-48BA-8109-3472E25669F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -923,7 +926,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D5D344B5-27FD-4CFC-B360-857B9001FD43}" type="CELLRANGE">
+                    <a:fld id="{0AA68414-7075-4C6E-83E4-423383F28788}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -957,7 +960,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AA48724F-1CEA-4646-88C8-80F0BACF2755}" type="CELLRANGE">
+                    <a:fld id="{20B45460-9EE9-4B28-BC26-1FF9F6F456B6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -991,7 +994,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E35E769-5C81-4ADC-812C-992BB7D1C511}" type="CELLRANGE">
+                    <a:fld id="{DE237E0F-7B00-49C8-84C3-9389BE4A3913}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1025,7 +1028,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E69F557-0526-4C6D-BCF3-79E733487A7D}" type="CELLRANGE">
+                    <a:fld id="{6E95F3AB-F08D-407D-9470-EF5C3162BC3F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1059,7 +1062,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DDDEF68C-7001-4BDE-801C-CDD0142351AD}" type="CELLRANGE">
+                    <a:fld id="{336BD114-A722-4DCE-8DC1-4BE91A5C0AFB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1093,7 +1096,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5CB0629C-46D7-4F0D-91DB-14A7F1C63503}" type="CELLRANGE">
+                    <a:fld id="{3F767CF2-4478-49DC-BB8D-A6DA6DDEA347}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1127,7 +1130,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35CEEFF1-841B-4841-A05A-1CF07DF57CEE}" type="CELLRANGE">
+                    <a:fld id="{F1A54A99-697D-4535-97A2-425CE3FE7609}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1161,7 +1164,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C07F297B-439A-44EC-99CF-0D03E179A9EE}" type="CELLRANGE">
+                    <a:fld id="{9AA15DEB-602A-4EEC-B9A4-AF70435E44A6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1195,7 +1198,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C38EA5E3-8E37-40A9-97F2-A2723BB73202}" type="CELLRANGE">
+                    <a:fld id="{D6BEC079-5779-4863-BEFC-A5E15AAAAA07}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1229,7 +1232,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{489E69E0-8422-4612-9E71-CFB94352E7F0}" type="CELLRANGE">
+                    <a:fld id="{BCB65087-B55A-45B5-9C1C-8C58F3B40ED1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1263,7 +1266,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0394790C-50D5-460C-80D6-AAAD4DF6B282}" type="CELLRANGE">
+                    <a:fld id="{7AE92343-776E-4402-8594-21123675D3C1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1297,7 +1300,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AF364E28-4A33-4823-8478-20FA6545A7F1}" type="CELLRANGE">
+                    <a:fld id="{E9B1875C-106B-43F1-9A7A-56378147589B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1331,7 +1334,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F99A316D-F556-4A88-9EAE-F12C5333B8B2}" type="CELLRANGE">
+                    <a:fld id="{2A78F1E8-E325-4F94-8C4E-4118DA4A89CC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1365,7 +1368,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B0E1A70-60C6-44DB-BB7D-9AF75DD3FC9E}" type="CELLRANGE">
+                    <a:fld id="{AA63A7A4-DEA6-4A04-B572-E35D16A80E3C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1399,7 +1402,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC53C201-F247-4B75-9516-EA0BB3C70AB7}" type="CELLRANGE">
+                    <a:fld id="{6A287D00-E9FC-4A4D-9270-4FFD393FB1B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1433,7 +1436,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB749DCB-4C7D-42BE-BFD3-919D94DF9F9F}" type="CELLRANGE">
+                    <a:fld id="{0BB82393-3BCA-42AB-8F92-E9CB4ACD221F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1467,7 +1470,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FB319B6A-A6A5-423D-B19A-89E4ADB44987}" type="CELLRANGE">
+                    <a:fld id="{95C8A20B-5BB3-4F4E-AA45-1FC93A2001A5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1501,7 +1504,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6F965725-D988-41AA-9E2C-FAEC92FFCA0F}" type="CELLRANGE">
+                    <a:fld id="{261FC2DF-4668-4D45-A0E7-D57E0E08BFD3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1535,7 +1538,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6A5C6AA3-CAFE-4E17-938C-53725F0F488F}" type="CELLRANGE">
+                    <a:fld id="{8CD47500-27FF-44F6-B2B5-E66CE650E41A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1569,7 +1572,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE81AD6F-A636-4692-B1C4-5ED88606ADAC}" type="CELLRANGE">
+                    <a:fld id="{425135EB-7AC6-4772-839A-AA54577E2DC8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1603,7 +1606,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0853AC4-E1F1-40BA-92D9-C85943DB9330}" type="CELLRANGE">
+                    <a:fld id="{BEF30B60-CBE3-4FBD-9C9D-A1EED7E1E939}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1637,7 +1640,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EBD774D0-F77B-4EFA-BFC9-94DAA5571F66}" type="CELLRANGE">
+                    <a:fld id="{EFB1ABCE-495B-42ED-94A6-E312FDE8BC93}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1671,7 +1674,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B09A7E17-A021-4D2B-839A-64D50482E789}" type="CELLRANGE">
+                    <a:fld id="{E138FF5C-81A2-4307-B212-0D62CCE012E3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1705,7 +1708,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CBABF1AD-BCA3-44FC-8B41-E815A352EACC}" type="CELLRANGE">
+                    <a:fld id="{9D9C9F0E-5E77-4637-AB9B-0EEE414D9217}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1739,7 +1742,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD3ACEF9-0536-42CE-8523-924F1638FE37}" type="CELLRANGE">
+                    <a:fld id="{503DE915-4A0C-4229-A727-13340D89EE9B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1773,7 +1776,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1929F187-3804-4013-9746-95082DD0752F}" type="CELLRANGE">
+                    <a:fld id="{7C37CA5E-05B3-4A66-8AD4-811B86C97009}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1807,7 +1810,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36D47067-088A-4DF8-B373-0BED43AD74D2}" type="CELLRANGE">
+                    <a:fld id="{D35F81DF-E3A5-4C4F-BEF1-8E3B21AF6BC2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1841,7 +1844,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4FE4CE2B-E50D-4713-934A-457EB84243CB}" type="CELLRANGE">
+                    <a:fld id="{1728036F-9FBF-49CF-A2C9-5BAA33C6383C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1875,7 +1878,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A5DA2FC-96C2-43BA-A337-42E3105A9C77}" type="CELLRANGE">
+                    <a:fld id="{86CFABCE-A1E6-4C2E-B478-8C7BBA8D0695}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1909,7 +1912,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CBD0B970-D199-46D3-A469-CC7F8CDB0CEC}" type="CELLRANGE">
+                    <a:fld id="{0951A49E-3170-4B66-AB97-A6CCDD09E533}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1943,7 +1946,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91785809-0B32-4F4A-A408-5B4F6D1BE6F3}" type="CELLRANGE">
+                    <a:fld id="{3E8E4921-AF3C-4A4C-A396-94EA68DE541C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1977,7 +1980,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1CBE4E43-BD9E-46A0-BAFA-0337ECACE37F}" type="CELLRANGE">
+                    <a:fld id="{829D7B99-7A2F-4FF2-AB0E-5F2659024E71}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2011,7 +2014,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{902EB4EE-7070-4BB1-B57D-55B47E413BE4}" type="CELLRANGE">
+                    <a:fld id="{0D76F86D-C79F-4DEA-907B-4B1F4868BFEE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2045,7 +2048,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6FEE2079-1EB8-48D5-B746-2445CF928980}" type="CELLRANGE">
+                    <a:fld id="{072556CD-4D37-4DD1-A6C6-0AF1F3BBAE71}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2079,7 +2082,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{98ED0577-5B22-47EB-ABCA-0DAC8C5D473D}" type="CELLRANGE">
+                    <a:fld id="{9450B97D-651C-4324-AECA-9116E10622E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2113,7 +2116,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A6E20208-9009-4132-AA22-5BD8EE8029E4}" type="CELLRANGE">
+                    <a:fld id="{4E6FB41F-D6DA-45CE-B923-8686B6C03555}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2147,7 +2150,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2222AAFA-E250-45A5-B55D-0DF52F1D65B2}" type="CELLRANGE">
+                    <a:fld id="{5FF7956B-769D-4708-86D1-02371F7A7EE2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2181,7 +2184,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5140372-D91A-4A38-8DC4-26457A2AC8C6}" type="CELLRANGE">
+                    <a:fld id="{8BBB1AA5-7737-4B56-A03A-B2D954579F57}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2215,7 +2218,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E04ED7F9-2835-430F-AA02-77B05B41CB72}" type="CELLRANGE">
+                    <a:fld id="{4844D908-934C-4863-BC8C-FFC3C6B92892}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2249,7 +2252,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E8DAEA73-50EF-4A9B-A2B0-AAD4793A0AE0}" type="CELLRANGE">
+                    <a:fld id="{E5009AFC-959E-4EBE-96E2-EF5C518EACFF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2283,7 +2286,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7EE623A9-B68A-4C47-92A7-25CA6A7B7FAC}" type="CELLRANGE">
+                    <a:fld id="{78C7F40A-E266-4881-9D7A-15A5B5C81E31}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2317,7 +2320,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0B227442-B927-4A72-84F0-BE0DB1038865}" type="CELLRANGE">
+                    <a:fld id="{508EC25D-08A8-4B47-B703-9BEAE341DBD6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2351,7 +2354,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C7184BD-32C0-443C-8AA0-A7FAA40AEFDA}" type="CELLRANGE">
+                    <a:fld id="{77A95878-8BA4-4ABF-8FDE-036EC571275A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2385,7 +2388,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DDF32010-439F-40FD-AE98-C55965CD73AC}" type="CELLRANGE">
+                    <a:fld id="{DD2FF92E-7792-4230-AC20-4B0D73D53B53}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2419,7 +2422,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{45A6C730-1DEF-4EB1-B1E7-833607F5664B}" type="CELLRANGE">
+                    <a:fld id="{32762B96-355B-4066-B819-2AF584E1A0A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2453,7 +2456,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C54C59A-16B6-40A0-B195-858C925B3BA2}" type="CELLRANGE">
+                    <a:fld id="{89F24AF5-DF62-4A99-8F19-3A52BD1D8D8E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2487,7 +2490,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC60C2CF-6F59-424B-97B6-C6E82F905F2E}" type="CELLRANGE">
+                    <a:fld id="{C2B413D7-47B8-4440-A2CE-1392E5D368E1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2521,7 +2524,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D0074B5-D883-4E77-B4A4-C7F5ED8145AC}" type="CELLRANGE">
+                    <a:fld id="{35EF4410-6CFB-4203-841C-7FAC77C6AEB9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2555,7 +2558,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{062299B0-42B3-47AD-B6DE-2CA6BB74BC11}" type="CELLRANGE">
+                    <a:fld id="{A1E043D7-7AD3-4403-9FB8-9A4930C23D73}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2589,7 +2592,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36B2A222-E9F3-48F6-95B8-C0DB5EC240B1}" type="CELLRANGE">
+                    <a:fld id="{B16B8893-40AD-4ADF-9BB4-CAB68A4C2205}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2613,6 +2616,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-15E5-41FB-A622-C3C92D097AC9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="66"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{155A8E65-7FC6-410B-9D32-632CDE51E3F3}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-71AE-4949-92BE-2A5186CA13D0}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2662,10 +2699,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$67</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -2820,48 +2857,51 @@
                   <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="51">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>9.9</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>5.6</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2869,10 +2909,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$67</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -3027,48 +3067,51 @@
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="51">
+                  <c:v>1930</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>3180</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -3235,48 +3278,51 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="51">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="52">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="52">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="53">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="54">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="55">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="55">
+                  <c:pt idx="56">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="56">
+                  <c:pt idx="57">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="57">
+                  <c:pt idx="58">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="58">
+                  <c:pt idx="59">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="59">
+                  <c:pt idx="60">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="60">
+                  <c:pt idx="61">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="61">
+                  <c:pt idx="62">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="62">
+                  <c:pt idx="63">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="63">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="64">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="65">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="66">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -4329,10 +4375,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D67" totalsRowShown="0">
-  <autoFilter ref="A1:D67" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D67">
-    <sortCondition ref="A1:A67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D68" totalsRowShown="0">
+  <autoFilter ref="A1:D68" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D68">
+    <sortCondition ref="A1:A68"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -4641,10 +4687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5388,41 +5434,41 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B53">
-        <v>2.2000000000000002</v>
+        <v>8.5</v>
       </c>
       <c r="C53">
-        <v>750</v>
+        <v>1930</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B54">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C54">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D54" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B55">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C55">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D55" t="s">
         <v>1</v>
@@ -5430,172 +5476,186 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56">
+        <v>7.3</v>
+      </c>
+      <c r="C56">
+        <v>2250</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>25</v>
       </c>
-      <c r="B56">
+      <c r="B57">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C56">
+      <c r="C57">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>49</v>
-      </c>
-      <c r="B57">
-        <v>1.2</v>
-      </c>
-      <c r="C57">
-        <v>500</v>
-      </c>
-      <c r="D57" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B58">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C58">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D58" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B59">
-        <v>6.5</v>
+        <v>11</v>
       </c>
       <c r="C59">
-        <v>1650</v>
+        <v>3060</v>
       </c>
       <c r="D59" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B60">
-        <v>9.9</v>
+        <v>6.5</v>
       </c>
       <c r="C60">
-        <v>3180</v>
+        <v>1650</v>
       </c>
       <c r="D60" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="B61">
-        <v>6.2</v>
+        <v>9.9</v>
       </c>
       <c r="C61">
-        <v>1890</v>
+        <v>3180</v>
       </c>
       <c r="D61" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B62">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C62">
-        <v>100</v>
+        <v>1890</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B63">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C63">
-        <v>3550</v>
+        <v>100</v>
       </c>
       <c r="D63" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="B64">
-        <v>5.6</v>
+        <v>7.3</v>
       </c>
       <c r="C64">
-        <v>1680</v>
+        <v>3550</v>
       </c>
       <c r="D64" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B65">
-        <v>10.8</v>
+        <v>5.6</v>
       </c>
       <c r="C65">
-        <v>1800</v>
+        <v>1680</v>
       </c>
       <c r="D65" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66">
+        <v>10.8</v>
+      </c>
+      <c r="C66">
+        <v>1800</v>
+      </c>
+      <c r="D66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>55</v>
       </c>
-      <c r="B66">
+      <c r="B67">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C66">
+      <c r="C67">
         <v>3800</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>29</v>
       </c>
-      <c r="B67">
+      <c r="B68">
         <v>6</v>
       </c>
-      <c r="C67">
+      <c r="C68">
         <v>2180</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Glacier View Wilderness, and GOAL ACCOMPLISHED!
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3287A404-F4F6-4C4C-957B-47D2DCCA8F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAEDC59-BE2B-45FF-B908-441D704C1487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="83">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>Eastside Loop</t>
+  </si>
+  <si>
+    <t>Glacier View Wilderness</t>
   </si>
 </sst>
 </file>
@@ -397,7 +400,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7452F1C8-B458-44F0-BF49-C576493E06E3}" type="CELLRANGE">
+                    <a:fld id="{F1D5EA67-9493-4DCA-818D-6C83C15101B8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -431,7 +434,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F85AA2D1-2CA4-42DC-9526-0FD6F45DA115}" type="CELLRANGE">
+                    <a:fld id="{A25B33E4-C3D4-43B2-8506-B40A7EE9BA0F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -465,7 +468,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7B1A525B-DA2C-4C96-B10E-B51FF786C4DE}" type="CELLRANGE">
+                    <a:fld id="{E576A120-B096-4DEF-AAA9-EBAF57E8F24F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -499,7 +502,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6F2E696E-8C18-4997-889C-3C02D51E8768}" type="CELLRANGE">
+                    <a:fld id="{98F5BEBE-392E-498A-BE85-FA0A9F9E582D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -533,7 +536,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{964EF4FB-0389-4C65-A1FD-FF4D84BE6399}" type="CELLRANGE">
+                    <a:fld id="{22BF2244-6DB5-4B8B-87BE-9811FDC46687}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -567,7 +570,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE47F1B2-0394-48A9-941E-99E726496D77}" type="CELLRANGE">
+                    <a:fld id="{5074E491-D616-47ED-AB4D-8294D0A3F959}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -601,7 +604,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{114D968B-0220-47C7-9B32-00026CF5D480}" type="CELLRANGE">
+                    <a:fld id="{0EA9A0FA-D8A1-44E6-A0B8-216820CFBD6E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -635,7 +638,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{78BB2740-C3B4-402B-95CF-BECB05716B31}" type="CELLRANGE">
+                    <a:fld id="{B37B76DE-835D-4FB1-8302-E94478EC36B9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -669,7 +672,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E555931-3727-44D7-95CF-47F4C010D37C}" type="CELLRANGE">
+                    <a:fld id="{5345FACE-6ADF-4D8D-B682-A55710B4BB14}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -703,7 +706,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B06EBD4-C6A1-430D-B4DE-5E056D0F6762}" type="CELLRANGE">
+                    <a:fld id="{B4B6E06E-6CB8-40E8-B4F7-D8D0DB5E3087}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -737,7 +740,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{737704E0-BB70-4D5E-AA90-61322FCFA7F7}" type="CELLRANGE">
+                    <a:fld id="{CA695A09-E9E3-41C9-A87F-3D99DE106574}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -771,7 +774,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ABCD5BC4-8276-47AF-A92A-ADC7FB1288D6}" type="CELLRANGE">
+                    <a:fld id="{FBC6E596-AB2C-436D-B276-FD8B3C7C7CAB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -805,7 +808,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6817726A-E3A5-4BCA-9713-F4612EA10F51}" type="CELLRANGE">
+                    <a:fld id="{0DD41674-11C7-4A97-B111-525D4A0C49E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -839,7 +842,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EFB1DF8C-95B0-4BC5-9978-488A8AD8E0AE}" type="CELLRANGE">
+                    <a:fld id="{AAFC3F66-FD6F-4084-8577-B35D5B9EA223}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -873,7 +876,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{080DFC76-0964-48B0-ABB9-1A9C6327B96C}" type="CELLRANGE">
+                    <a:fld id="{90FB0E55-DEFD-41FC-A868-EE8594B2FC61}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -907,7 +910,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F14ADD73-5B5D-4B39-9A2B-C3BEAA7779F7}" type="CELLRANGE">
+                    <a:fld id="{A31C9C65-2429-4C6A-B5B2-A424F26595A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -941,7 +944,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2267E4C2-0E6C-4250-8E68-27DC25D2014D}" type="CELLRANGE">
+                    <a:fld id="{85B4593B-D155-442C-AAB3-A8CC20388BF2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -975,7 +978,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D39EEB5-C27D-4185-B9EC-18B9A1F43F9B}" type="CELLRANGE">
+                    <a:fld id="{BEF2ACFC-4AC9-4F44-968E-4437FD71045A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1009,7 +1012,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BE2C3BE0-982E-4F1E-96E5-98CEEE398BBA}" type="CELLRANGE">
+                    <a:fld id="{96D76723-EBEA-4DAE-A097-4C4F091BF09E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1043,7 +1046,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{50FCF42D-27F8-47B9-A75D-12C6C19C28D0}" type="CELLRANGE">
+                    <a:fld id="{B9500702-5BE5-457D-8CDA-8CD7CBADB627}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1077,7 +1080,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D647B5E-8F66-4922-A179-D3E7A327DB4E}" type="CELLRANGE">
+                    <a:fld id="{A165DAD6-0581-4F87-AD9A-21AD04B29AB8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1111,7 +1114,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BC1DEC40-DEA5-4545-A7EA-66A7F2E45F6D}" type="CELLRANGE">
+                    <a:fld id="{5259C38A-2111-4F7F-8611-A6546BB86E5E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1145,7 +1148,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E09ECD1D-CD4F-405C-9F98-E9D905495790}" type="CELLRANGE">
+                    <a:fld id="{8C14A859-8931-4E63-BF83-F874BB9357D6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1179,7 +1182,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4F9CFEB-366A-4E7F-9BBE-F008FFD2FEEF}" type="CELLRANGE">
+                    <a:fld id="{1D3F5603-69F2-420E-B5B6-A5AF6EB499B8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1213,7 +1216,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2912CB77-875A-4D3D-A6F2-61C072167FC0}" type="CELLRANGE">
+                    <a:fld id="{5FF444A1-C957-4D5B-9A9C-1EE236EE0359}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1247,7 +1250,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A233BF5-2A23-4DCB-B074-ECDDFFB1A7A3}" type="CELLRANGE">
+                    <a:fld id="{B4F41D06-6FD2-4BB6-8CBE-DCCE87E6A68D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1281,7 +1284,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{588BF5D1-3DB1-4D50-B56B-1EDE6D3BC74F}" type="CELLRANGE">
+                    <a:fld id="{29EC1CBB-11BD-4A86-B4EC-19957837E39E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1315,7 +1318,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EE0E3B3A-69E2-42C2-9075-EEE5C4E7F2CB}" type="CELLRANGE">
+                    <a:fld id="{18C05E16-AB1D-4C20-9552-692E643A6529}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1349,7 +1352,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F61E127A-10ED-4796-8B7D-5F11E4BEEC21}" type="CELLRANGE">
+                    <a:fld id="{F2956D31-0B1B-4145-89D4-D949D1F7A871}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1383,7 +1386,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5426369A-4573-4B49-B3F0-78BA0BD8B4AD}" type="CELLRANGE">
+                    <a:fld id="{4CF2B311-D04F-425E-B4CC-B500EBB36AE4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1417,7 +1420,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2FF870BA-A0CD-419C-BC7A-1EB8045B9D1F}" type="CELLRANGE">
+                    <a:fld id="{29AE7E4F-06A2-41BE-89A7-052A6DAB9061}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1451,7 +1454,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4019F676-F3A0-427E-BB72-DBC5811B6403}" type="CELLRANGE">
+                    <a:fld id="{CA7F7AFE-1AF3-4248-AD54-B950A17EA850}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1485,7 +1488,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1215264D-975A-4AB2-B044-BFA6D0AE1ECE}" type="CELLRANGE">
+                    <a:fld id="{A9F99482-2F4D-4968-BA0F-FC5708D01915}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1519,7 +1522,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14A99D51-6180-4DE7-BDB9-E545D69E1B2A}" type="CELLRANGE">
+                    <a:fld id="{17DA4F78-D051-42C7-BEB7-8703B502CCD8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1553,7 +1556,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{025022D2-8886-4438-87CC-EDEA4C05BDD8}" type="CELLRANGE">
+                    <a:fld id="{A5E96F2A-76BC-4816-BA1D-B81377DF536F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1587,7 +1590,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B102E7CC-8425-4B88-BA24-F276FA653AD9}" type="CELLRANGE">
+                    <a:fld id="{CF09B3AE-9841-4640-A3B0-3B3368CEC548}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1621,7 +1624,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC8BF75C-BC87-4249-86D4-10FCA4691E1F}" type="CELLRANGE">
+                    <a:fld id="{760C8D0B-30EC-4E76-9FCC-DA4A6FE68BF7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1655,7 +1658,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C8E0538A-3DAE-475D-A72D-D2B2C386280E}" type="CELLRANGE">
+                    <a:fld id="{DB4C7765-E3FB-43D3-856C-87756CA0ACD0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1689,7 +1692,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E6B8B28-5E2F-4437-8F2B-48F525158DE5}" type="CELLRANGE">
+                    <a:fld id="{E4A5D550-2CF1-4A64-B7D7-BC46232671AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1723,7 +1726,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67A4F3C7-1397-4B54-8156-1DF4075A33AF}" type="CELLRANGE">
+                    <a:fld id="{7E0F23C6-CE17-40DA-B867-934936006663}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1757,7 +1760,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69DFE0EF-8D08-4116-B2C9-9E0485740EF3}" type="CELLRANGE">
+                    <a:fld id="{37086C60-C86D-460D-8A0A-B3BA3EE2470D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1791,7 +1794,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B9B02EFD-64DB-4EDB-8679-80A2D8B2F303}" type="CELLRANGE">
+                    <a:fld id="{3092B727-19BB-4273-BD1F-909D5A229A73}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1825,7 +1828,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8D2163E-A0A5-4D6F-9117-B1F1A55EA0E4}" type="CELLRANGE">
+                    <a:fld id="{289CCB5E-0E74-4BEA-B911-4C2744ADE0DC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1859,7 +1862,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7262B541-5180-499B-BC73-607297FBC315}" type="CELLRANGE">
+                    <a:fld id="{3434CB3C-28C4-4474-9276-7CA4D3718B9F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1893,7 +1896,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{812994D1-9E98-407C-9DB8-E86EFF95E449}" type="CELLRANGE">
+                    <a:fld id="{735A275C-72A4-4A29-82B9-AA171C5A0838}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1927,7 +1930,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14E25F58-50DF-4896-AB03-9FFBA0DAC83B}" type="CELLRANGE">
+                    <a:fld id="{DAD5EF8A-5AB4-4DD3-8628-49026AB4B90B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1961,7 +1964,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{533CA18D-DBFE-4B44-9D4B-6896C552872D}" type="CELLRANGE">
+                    <a:fld id="{4A607215-5E72-4F13-9322-642DD22D7856}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1995,7 +1998,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{330C62F4-5554-4D55-B8BE-C5F1241830E0}" type="CELLRANGE">
+                    <a:fld id="{3611410B-89C9-41EC-B61C-C2FDC7D29816}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2029,7 +2032,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD22440E-A3D7-4196-8601-E0699BEAD747}" type="CELLRANGE">
+                    <a:fld id="{E739F4F6-F03E-453D-BDD1-985E50B5E5DE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2063,7 +2066,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A8E24592-B7B1-4347-9E92-0CE790510D25}" type="CELLRANGE">
+                    <a:fld id="{AAF6CC88-0394-4EFC-9E6F-8FF2E5E7520A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2097,7 +2100,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33416717-F19E-4154-94AA-3B21CD2D0D16}" type="CELLRANGE">
+                    <a:fld id="{24F206BB-BF1B-4EDD-B187-DCC28897D710}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2131,7 +2134,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF9CB9AA-7627-4C3E-9C8A-4B311B6EDB38}" type="CELLRANGE">
+                    <a:fld id="{D91AE6F5-816B-404D-8D2D-119218042A35}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2165,7 +2168,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FFD89F79-9448-4555-B719-107A84FFA2F4}" type="CELLRANGE">
+                    <a:fld id="{C643B941-E538-4540-971E-28EECD1A8606}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2199,7 +2202,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F4E9D32E-7C3C-460E-926F-8C32EC9B2BBE}" type="CELLRANGE">
+                    <a:fld id="{24C288F4-AED8-4875-B90F-B440A4640FE7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2233,7 +2236,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D49A75F4-CA81-4360-8628-6460501DC083}" type="CELLRANGE">
+                    <a:fld id="{D7EC5CC8-259D-4816-9BA6-F4556A43397F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2267,7 +2270,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9AF2172-D91B-4B98-B577-201BDF7888BE}" type="CELLRANGE">
+                    <a:fld id="{93BE2470-3B7E-44C3-AFAD-5D4735D1F784}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2301,7 +2304,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1444857B-997C-46C2-82B4-66B3C4FBA315}" type="CELLRANGE">
+                    <a:fld id="{D5514921-520C-4F13-92AF-03DFBF10D994}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2335,7 +2338,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E76BEA6-C4AB-49D2-8084-470D80114E9C}" type="CELLRANGE">
+                    <a:fld id="{BB4F3B8D-4F3C-4FDB-A31C-5C3AC4B62028}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2369,7 +2372,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{64CD82EF-95BA-48AF-87A1-C24105F64221}" type="CELLRANGE">
+                    <a:fld id="{AA3C0708-5D75-4DDF-A0DA-F1C00361F4A4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2403,7 +2406,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B196EEC0-E15C-4C4E-ACC8-9CADB9CC0B86}" type="CELLRANGE">
+                    <a:fld id="{B72EB4F6-DAA2-443E-8DE8-47D71935FAA2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2437,7 +2440,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B41D5A90-D524-4E90-BAA0-367C94C76980}" type="CELLRANGE">
+                    <a:fld id="{1CA35C1D-7DB6-459D-A742-4CCCB988C7EA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2471,7 +2474,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F9EC03E8-27F7-49E2-ABCB-9278B56061FB}" type="CELLRANGE">
+                    <a:fld id="{793A6547-835F-442C-8E07-1E84BBC00E5C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2505,7 +2508,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{09D88DFA-D860-4919-89C6-67F54230E7E8}" type="CELLRANGE">
+                    <a:fld id="{361CCE17-4D48-4C23-A7DE-43A1160AA912}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2539,7 +2542,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{61F009BF-68C7-4C46-9845-211E17AE6348}" type="CELLRANGE">
+                    <a:fld id="{C8F6C3E8-C303-4AC5-869E-4D12CE9B79A4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2573,7 +2576,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E4B1724D-0C93-472A-9AC9-E921444F20D3}" type="CELLRANGE">
+                    <a:fld id="{13606D1A-3C1D-4C7F-AA10-A3D9A13757D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2607,7 +2610,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C849305-486E-4CDB-94A6-2746FE356E40}" type="CELLRANGE">
+                    <a:fld id="{80D057AA-8DBE-428E-B86C-AA7F690E8FE0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2641,7 +2644,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0343555-35A5-47AF-A137-30E88A037D40}" type="CELLRANGE">
+                    <a:fld id="{BB89B855-9034-44D6-8013-315FCC8FE52D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2675,7 +2678,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC8327F1-FB75-4D40-842D-BE23531FF7C4}" type="CELLRANGE">
+                    <a:fld id="{8420B9D1-E603-49DF-B5E6-03378633A6DE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2709,7 +2712,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7AC3A460-B187-4076-8FFF-01D223E34A90}" type="CELLRANGE">
+                    <a:fld id="{9C71DEFE-81A0-4022-A249-57F0F5FB26A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2743,7 +2746,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{120E88DE-EE01-456E-9269-FF6FD65BE81F}" type="CELLRANGE">
+                    <a:fld id="{4E8F4FD3-EEF1-4958-B607-B129E1FC7AEC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2777,7 +2780,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA4466E3-4C13-4F96-8542-DDE38C2B3643}" type="CELLRANGE">
+                    <a:fld id="{90FC813B-A3B4-48A2-8A49-F249864F00AA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2811,7 +2814,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17817A20-0028-493A-94E3-941D34E726E2}" type="CELLRANGE">
+                    <a:fld id="{0916F819-041D-4967-8C0D-C091EC4B2AD2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2835,6 +2838,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-E100-4598-89EB-D4D54BCB330E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="72"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{4E0C757A-C03F-40C8-BACF-07CDBC49BBBD}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-7F91-4CC8-93F8-66436583A52F}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2884,10 +2921,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$73</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -2952,156 +2989,159 @@
                   <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>11.6</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>12.5</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>9.1</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>9.5500000000000007</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>12.2</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>9.75</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>5.4</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>11.9</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>4.2</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>7.2</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>2.7</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>3.3</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>9.9</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="69">
                   <c:v>5.6</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -3109,10 +3149,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$73</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -3177,156 +3217,159 @@
                   <c:v>3290</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>2660</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>2780</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>2425</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>4100</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>4800</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>4120</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>3420</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>2050</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>1450</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>3160</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>880</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>860</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>1260</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>2600</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>3100</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>1630</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>1930</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>3180</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="69">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -3406,22 +3449,22 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="22">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="24">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="25">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="26">
+                  <c:pt idx="27">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="28">
                     <c:v>strenuous</c:v>
@@ -3436,28 +3479,28 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="32">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="33">
+                  <c:pt idx="34">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="34">
+                  <c:pt idx="35">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="36">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="36">
+                  <c:pt idx="37">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="37">
+                  <c:pt idx="38">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="38">
+                  <c:pt idx="39">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="39">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="40">
                     <c:v>easy</c:v>
@@ -3466,19 +3509,19 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="42">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="43">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="43">
+                  <c:pt idx="44">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="44">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="45">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="46">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="47">
                     <c:v>moderate</c:v>
@@ -3487,72 +3530,75 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="49">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="50">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="50">
+                  <c:pt idx="51">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="51">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="52">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="53">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="54">
+                  <c:pt idx="55">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="55">
+                  <c:pt idx="56">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="56">
+                  <c:pt idx="57">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="57">
+                  <c:pt idx="58">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="58">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="59">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="60">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="61">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="61">
+                  <c:pt idx="62">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="62">
+                  <c:pt idx="63">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="63">
+                  <c:pt idx="64">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="64">
+                  <c:pt idx="65">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="65">
+                  <c:pt idx="66">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="66">
+                  <c:pt idx="67">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="67">
+                  <c:pt idx="68">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="68">
+                  <c:pt idx="69">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="69">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="70">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="71">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="72">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -4605,10 +4651,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D73" totalsRowShown="0">
-  <autoFilter ref="A1:D73" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D73">
-    <sortCondition ref="A1:A73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D74" totalsRowShown="0">
+  <autoFilter ref="A1:D74" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D74">
+    <sortCondition ref="A1:A74"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -4917,10 +4963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5244,13 +5290,15 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="B23">
-        <v>11.6</v>
+        <f>14.6/2</f>
+        <v>7.3</v>
       </c>
       <c r="C23">
-        <v>2660</v>
+        <f>3160/2</f>
+        <v>1580</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
@@ -5258,41 +5306,41 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B24">
-        <v>12.5</v>
+        <v>11.6</v>
       </c>
       <c r="C24">
-        <v>2780</v>
+        <v>2660</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="B25">
-        <v>9</v>
+        <v>12.5</v>
       </c>
       <c r="C25">
-        <v>1680</v>
+        <v>2780</v>
       </c>
       <c r="D25" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B26">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="C26">
-        <v>1580</v>
+        <v>1680</v>
       </c>
       <c r="D26" t="s">
         <v>1</v>
@@ -5300,57 +5348,57 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B27">
-        <v>5.2</v>
+        <v>9.1</v>
       </c>
       <c r="C27">
-        <v>1000</v>
+        <v>1580</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>5.2</v>
+      </c>
+      <c r="C28">
+        <v>1000</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>79</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <f>19.1/2</f>
         <v>9.5500000000000007</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <f>4850/2</f>
         <v>2425</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29">
-        <v>9.5</v>
-      </c>
-      <c r="C29">
-        <v>4100</v>
-      </c>
-      <c r="D29" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="B30">
-        <v>14</v>
+        <v>9.5</v>
       </c>
       <c r="C30">
-        <v>4800</v>
+        <v>4100</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
@@ -5358,13 +5406,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31">
         <v>14</v>
       </c>
-      <c r="B31">
-        <v>12.2</v>
-      </c>
       <c r="C31">
-        <v>4120</v>
+        <v>4800</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
@@ -5372,13 +5420,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B32">
-        <v>12</v>
+        <v>12.2</v>
       </c>
       <c r="C32">
-        <v>3420</v>
+        <v>4120</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
@@ -5386,141 +5434,141 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <v>12</v>
+      </c>
+      <c r="C33">
+        <v>3420</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>37</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <f>19.5/2</f>
         <v>9.75</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <f>4400*7/8</f>
         <v>3850</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34">
-        <v>6.9</v>
-      </c>
-      <c r="C34">
-        <v>2050</v>
-      </c>
-      <c r="D34" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="B35">
-        <v>5.4</v>
+        <v>6.9</v>
       </c>
       <c r="C35">
-        <v>1450</v>
+        <v>2050</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B36">
-        <v>11.9</v>
+        <v>5.4</v>
       </c>
       <c r="C36">
-        <v>3160</v>
+        <v>1450</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B37">
-        <v>11.4</v>
+        <v>11.9</v>
       </c>
       <c r="C37">
-        <v>2550</v>
+        <v>3160</v>
       </c>
       <c r="D37" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38">
-        <v>8.5</v>
+        <v>11.4</v>
       </c>
       <c r="C38">
-        <v>3350</v>
+        <v>2550</v>
       </c>
       <c r="D38" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B39">
-        <v>2.8</v>
+        <v>8.5</v>
       </c>
       <c r="C39">
-        <v>880</v>
+        <v>3350</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B40">
-        <v>10.4</v>
+        <v>2.8</v>
       </c>
       <c r="C40">
-        <v>1420</v>
+        <v>880</v>
       </c>
       <c r="D40" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B41">
-        <v>0.9</v>
+        <v>10.4</v>
       </c>
       <c r="C41">
-        <v>200</v>
+        <v>1420</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B42">
-        <v>4.2</v>
+        <v>0.9</v>
       </c>
       <c r="C42">
-        <v>860</v>
+        <v>200</v>
       </c>
       <c r="D42" t="s">
         <v>7</v>
@@ -5528,13 +5576,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B43">
-        <v>4.8</v>
+        <v>4.2</v>
       </c>
       <c r="C43">
-        <v>1260</v>
+        <v>860</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
@@ -5542,55 +5590,55 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B44">
-        <v>4</v>
+        <v>4.8</v>
       </c>
       <c r="C44">
-        <v>2600</v>
+        <v>1260</v>
       </c>
       <c r="D44" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B45">
-        <v>1.4</v>
+        <v>4</v>
       </c>
       <c r="C45">
-        <v>375</v>
+        <v>2600</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B46">
-        <v>13.6</v>
+        <v>1.4</v>
       </c>
       <c r="C46">
-        <v>3930</v>
+        <v>375</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B47">
-        <v>10.5</v>
+        <v>13.6</v>
       </c>
       <c r="C47">
-        <v>3100</v>
+        <v>3930</v>
       </c>
       <c r="D47" t="s">
         <v>10</v>
@@ -5598,27 +5646,27 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B48">
-        <v>7</v>
+        <v>10.5</v>
       </c>
       <c r="C48">
-        <v>1670</v>
+        <v>3100</v>
       </c>
       <c r="D48" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B49">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="C49">
-        <v>2400</v>
+        <v>1670</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
@@ -5626,13 +5674,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B50">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C50">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D50" t="s">
         <v>1</v>
@@ -5640,55 +5688,55 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B51">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C51">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B52">
-        <v>7.2</v>
+        <v>4.8</v>
       </c>
       <c r="C52">
-        <v>1630</v>
+        <v>1300</v>
       </c>
       <c r="D52" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B53">
-        <v>2.7</v>
+        <v>7.2</v>
       </c>
       <c r="C53">
-        <v>1090</v>
+        <v>1630</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="B54">
-        <v>4.8</v>
+        <v>2.7</v>
       </c>
       <c r="C54">
-        <v>1470</v>
+        <v>1090</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
@@ -5696,97 +5744,97 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B55">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C55">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D55" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B56">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C56">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D56" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B57">
-        <v>3.3</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C57">
-        <v>600</v>
+        <v>3490</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B58">
-        <v>8.5</v>
+        <v>3.3</v>
       </c>
       <c r="C58">
-        <v>1930</v>
+        <v>600</v>
       </c>
       <c r="D58" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B59">
-        <v>2.2000000000000002</v>
+        <v>8.5</v>
       </c>
       <c r="C59">
-        <v>750</v>
+        <v>1930</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B60">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C60">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D60" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B61">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C61">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D61" t="s">
         <v>1</v>
@@ -5794,172 +5842,186 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62">
+        <v>7.3</v>
+      </c>
+      <c r="C62">
+        <v>2250</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>25</v>
       </c>
-      <c r="B62">
+      <c r="B63">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C62">
+      <c r="C63">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D63" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>49</v>
-      </c>
-      <c r="B63">
-        <v>1.2</v>
-      </c>
-      <c r="C63">
-        <v>500</v>
-      </c>
-      <c r="D63" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B64">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C64">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D64" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B65">
-        <v>6.5</v>
+        <v>11</v>
       </c>
       <c r="C65">
-        <v>1650</v>
+        <v>3060</v>
       </c>
       <c r="D65" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B66">
-        <v>9.9</v>
+        <v>6.5</v>
       </c>
       <c r="C66">
-        <v>3180</v>
+        <v>1650</v>
       </c>
       <c r="D66" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="B67">
-        <v>6.2</v>
+        <v>9.9</v>
       </c>
       <c r="C67">
-        <v>1890</v>
+        <v>3180</v>
       </c>
       <c r="D67" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B68">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C68">
-        <v>100</v>
+        <v>1890</v>
       </c>
       <c r="D68" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B69">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C69">
-        <v>3550</v>
+        <v>100</v>
       </c>
       <c r="D69" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="B70">
-        <v>5.6</v>
+        <v>7.3</v>
       </c>
       <c r="C70">
-        <v>1680</v>
+        <v>3550</v>
       </c>
       <c r="D70" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B71">
-        <v>10.8</v>
+        <v>5.6</v>
       </c>
       <c r="C71">
-        <v>1800</v>
+        <v>1680</v>
       </c>
       <c r="D71" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>63</v>
+      </c>
+      <c r="B72">
+        <v>10.8</v>
+      </c>
+      <c r="C72">
+        <v>1800</v>
+      </c>
+      <c r="D72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>55</v>
       </c>
-      <c r="B72">
+      <c r="B73">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C72">
+      <c r="C73">
         <v>3800</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D73" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>29</v>
       </c>
-      <c r="B73">
+      <c r="B74">
         <v>6</v>
       </c>
-      <c r="C73">
+      <c r="C74">
         <v>2180</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D74" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Cowlitz Divide Trail
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F755AD-DDF2-4326-B4E0-BA5EED8BA810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3287A404-F4F6-4C4C-957B-47D2DCCA8F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="82">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -273,6 +273,12 @@
   </si>
   <si>
     <t>Huckleberry / Grand Park Loop</t>
+  </si>
+  <si>
+    <t>Cowlitz Divide Trail</t>
+  </si>
+  <si>
+    <t>Eastside Loop</t>
   </si>
 </sst>
 </file>
@@ -391,7 +397,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B7408E5F-1C2A-4A05-A1F5-0F860195DD08}" type="CELLRANGE">
+                    <a:fld id="{7452F1C8-B458-44F0-BF49-C576493E06E3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -425,7 +431,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{119DA670-D196-4704-9F23-693E4554DE22}" type="CELLRANGE">
+                    <a:fld id="{F85AA2D1-2CA4-42DC-9526-0FD6F45DA115}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -459,7 +465,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9CB0529D-4C71-4C8F-85F7-321F47283AEC}" type="CELLRANGE">
+                    <a:fld id="{7B1A525B-DA2C-4C96-B10E-B51FF786C4DE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -493,7 +499,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4AB42ED6-0BAF-4402-990B-B890846F5C70}" type="CELLRANGE">
+                    <a:fld id="{6F2E696E-8C18-4997-889C-3C02D51E8768}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -527,7 +533,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{108E5349-6F8D-4132-9DE2-97B9EB757CFA}" type="CELLRANGE">
+                    <a:fld id="{964EF4FB-0389-4C65-A1FD-FF4D84BE6399}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -561,7 +567,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{613DA924-54AF-4B1C-BF8C-B05290B09D52}" type="CELLRANGE">
+                    <a:fld id="{DE47F1B2-0394-48A9-941E-99E726496D77}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -595,7 +601,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D83136AB-7EF6-494B-AA49-54DFE9ED5D3C}" type="CELLRANGE">
+                    <a:fld id="{114D968B-0220-47C7-9B32-00026CF5D480}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -629,7 +635,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BA24AD4A-E3F2-4D84-86E1-0EAE8251EAC3}" type="CELLRANGE">
+                    <a:fld id="{78BB2740-C3B4-402B-95CF-BECB05716B31}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -663,7 +669,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE8B4954-18CC-4656-8630-02E2AA5B6BD0}" type="CELLRANGE">
+                    <a:fld id="{7E555931-3727-44D7-95CF-47F4C010D37C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -697,7 +703,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8D07DABE-92E9-4AF7-B1CA-1E7B9185FAE7}" type="CELLRANGE">
+                    <a:fld id="{5B06EBD4-C6A1-430D-B4DE-5E056D0F6762}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -731,7 +737,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7C94BEB-56CF-4F48-B483-FAFC1691CC60}" type="CELLRANGE">
+                    <a:fld id="{737704E0-BB70-4D5E-AA90-61322FCFA7F7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -765,7 +771,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E86C4201-D720-4B1D-9220-31C7E1B1C9D9}" type="CELLRANGE">
+                    <a:fld id="{ABCD5BC4-8276-47AF-A92A-ADC7FB1288D6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -799,7 +805,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7749AAAA-FF98-49E9-BCDB-1F16EE403F56}" type="CELLRANGE">
+                    <a:fld id="{6817726A-E3A5-4BCA-9713-F4612EA10F51}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -833,7 +839,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{449AA21D-10BF-409C-A006-00AA44BFCDE3}" type="CELLRANGE">
+                    <a:fld id="{EFB1DF8C-95B0-4BC5-9978-488A8AD8E0AE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -867,7 +873,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BD3700C8-8860-420C-8474-9B468CAA2C10}" type="CELLRANGE">
+                    <a:fld id="{080DFC76-0964-48B0-ABB9-1A9C6327B96C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -901,7 +907,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{13C6EB57-C2D6-4E56-982B-9256885E4761}" type="CELLRANGE">
+                    <a:fld id="{F14ADD73-5B5D-4B39-9A2B-C3BEAA7779F7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -935,7 +941,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6B5C9566-1EBD-40C9-821F-F687BFB245EF}" type="CELLRANGE">
+                    <a:fld id="{2267E4C2-0E6C-4250-8E68-27DC25D2014D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -969,7 +975,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{46970AD5-8426-496E-9E91-2068E90A8F0B}" type="CELLRANGE">
+                    <a:fld id="{4D39EEB5-C27D-4185-B9EC-18B9A1F43F9B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1003,7 +1009,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{04997E42-AB4C-4798-B592-190EB62EB8FC}" type="CELLRANGE">
+                    <a:fld id="{BE2C3BE0-982E-4F1E-96E5-98CEEE398BBA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1037,7 +1043,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E5B686EC-465D-46D4-81CD-4D1B1553D08D}" type="CELLRANGE">
+                    <a:fld id="{50FCF42D-27F8-47B9-A75D-12C6C19C28D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1071,7 +1077,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97B8FAEB-4241-46E5-9808-A8EA6E145AA6}" type="CELLRANGE">
+                    <a:fld id="{9D647B5E-8F66-4922-A179-D3E7A327DB4E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1105,7 +1111,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8155FEA8-F066-49D6-8A47-373E22855665}" type="CELLRANGE">
+                    <a:fld id="{BC1DEC40-DEA5-4545-A7EA-66A7F2E45F6D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1139,7 +1145,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{07664132-707B-4782-A7F5-B1B50DCB03C7}" type="CELLRANGE">
+                    <a:fld id="{E09ECD1D-CD4F-405C-9F98-E9D905495790}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1173,7 +1179,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{875364A1-C65A-4F4D-BB32-65445D6C8A40}" type="CELLRANGE">
+                    <a:fld id="{D4F9CFEB-366A-4E7F-9BBE-F008FFD2FEEF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1207,7 +1213,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FADDCE67-7977-48F9-B9A3-CA7C437D5D53}" type="CELLRANGE">
+                    <a:fld id="{2912CB77-875A-4D3D-A6F2-61C072167FC0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1241,7 +1247,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63EFC3EB-AA59-4CCB-B3C6-D88550D25C7E}" type="CELLRANGE">
+                    <a:fld id="{1A233BF5-2A23-4DCB-B074-ECDDFFB1A7A3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1275,7 +1281,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8D445E5-CE84-492F-A88A-36F81B0ADAEC}" type="CELLRANGE">
+                    <a:fld id="{588BF5D1-3DB1-4D50-B56B-1EDE6D3BC74F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1309,7 +1315,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EFBEA209-BDDF-4DCE-82BB-26B735E7C2F9}" type="CELLRANGE">
+                    <a:fld id="{EE0E3B3A-69E2-42C2-9075-EEE5C4E7F2CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1343,7 +1349,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D1E4050-F065-4456-821E-D4D64A33FF72}" type="CELLRANGE">
+                    <a:fld id="{F61E127A-10ED-4796-8B7D-5F11E4BEEC21}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1377,7 +1383,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CDDFCB20-E1FC-4EDF-B80C-DAF4E374DED0}" type="CELLRANGE">
+                    <a:fld id="{5426369A-4573-4B49-B3F0-78BA0BD8B4AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1411,7 +1417,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D61B852B-C66C-49EE-91A0-99517DCC22EC}" type="CELLRANGE">
+                    <a:fld id="{2FF870BA-A0CD-419C-BC7A-1EB8045B9D1F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1445,7 +1451,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F19E2DC8-C041-4046-979F-9A7D905FAE36}" type="CELLRANGE">
+                    <a:fld id="{4019F676-F3A0-427E-BB72-DBC5811B6403}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1479,7 +1485,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5CB0833F-8981-491D-8E37-F1FF6C20AFF5}" type="CELLRANGE">
+                    <a:fld id="{1215264D-975A-4AB2-B044-BFA6D0AE1ECE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1513,7 +1519,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F9F23226-A229-4D44-A529-F2E64E90A1C6}" type="CELLRANGE">
+                    <a:fld id="{14A99D51-6180-4DE7-BDB9-E545D69E1B2A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1547,7 +1553,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F87EB4A6-E7C2-4234-A9FD-D4DCBF843782}" type="CELLRANGE">
+                    <a:fld id="{025022D2-8886-4438-87CC-EDEA4C05BDD8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1581,7 +1587,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8D9CD449-20EB-493D-8A81-93593AFF9ABC}" type="CELLRANGE">
+                    <a:fld id="{B102E7CC-8425-4B88-BA24-F276FA653AD9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1615,7 +1621,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5EB260EF-5CC7-4F4D-B819-C2FE328F0FF7}" type="CELLRANGE">
+                    <a:fld id="{DC8BF75C-BC87-4249-86D4-10FCA4691E1F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1649,7 +1655,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2B52D915-A129-4803-B224-FDE29E35386F}" type="CELLRANGE">
+                    <a:fld id="{C8E0538A-3DAE-475D-A72D-D2B2C386280E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1683,7 +1689,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{09828E1D-9F24-43AE-A94F-67F903565422}" type="CELLRANGE">
+                    <a:fld id="{6E6B8B28-5E2F-4437-8F2B-48F525158DE5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1717,7 +1723,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B4E9E9A3-48BE-48D6-AD12-D0992F8BB947}" type="CELLRANGE">
+                    <a:fld id="{67A4F3C7-1397-4B54-8156-1DF4075A33AF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1751,7 +1757,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56183F87-D17D-4194-BDB5-D23F053C7A28}" type="CELLRANGE">
+                    <a:fld id="{69DFE0EF-8D08-4116-B2C9-9E0485740EF3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1785,7 +1791,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0EDA8BCC-50CF-478F-BC8F-A109ECE59721}" type="CELLRANGE">
+                    <a:fld id="{B9B02EFD-64DB-4EDB-8679-80A2D8B2F303}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1819,7 +1825,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9313A6E7-CCCD-4FE7-8545-A20EA141097D}" type="CELLRANGE">
+                    <a:fld id="{B8D2163E-A0A5-4D6F-9117-B1F1A55EA0E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1853,7 +1859,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{575FC21B-117C-4BD5-9145-E40140320C2B}" type="CELLRANGE">
+                    <a:fld id="{7262B541-5180-499B-BC73-607297FBC315}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1887,7 +1893,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{395D4FDE-EFF3-4AF1-BE5F-BA3AA65BF865}" type="CELLRANGE">
+                    <a:fld id="{812994D1-9E98-407C-9DB8-E86EFF95E449}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1921,7 +1927,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F77A88A9-E59A-450D-8199-7C2017A9B431}" type="CELLRANGE">
+                    <a:fld id="{14E25F58-50DF-4896-AB03-9FFBA0DAC83B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1955,7 +1961,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AF354E67-5F01-4957-8A25-7748B90D1008}" type="CELLRANGE">
+                    <a:fld id="{533CA18D-DBFE-4B44-9D4B-6896C552872D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1989,7 +1995,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{287EF8F6-1ED9-4E54-9310-8996B7C40EC1}" type="CELLRANGE">
+                    <a:fld id="{330C62F4-5554-4D55-B8BE-C5F1241830E0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2023,7 +2029,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{951A60DD-6F80-4F08-88B0-501AD6A2D224}" type="CELLRANGE">
+                    <a:fld id="{AD22440E-A3D7-4196-8601-E0699BEAD747}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2057,7 +2063,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{07D18596-53F2-4794-B39D-657A1749996F}" type="CELLRANGE">
+                    <a:fld id="{A8E24592-B7B1-4347-9E92-0CE790510D25}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2091,7 +2097,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B405453A-B65E-49FE-B80B-F77F8E5ADC0F}" type="CELLRANGE">
+                    <a:fld id="{33416717-F19E-4154-94AA-3B21CD2D0D16}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2125,7 +2131,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6F9FA69-1E5B-4BE4-A5A2-F2009DA846A5}" type="CELLRANGE">
+                    <a:fld id="{FF9CB9AA-7627-4C3E-9C8A-4B311B6EDB38}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2159,7 +2165,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B3FA2988-8E22-4C92-A199-5A512F296564}" type="CELLRANGE">
+                    <a:fld id="{FFD89F79-9448-4555-B719-107A84FFA2F4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2193,7 +2199,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B6E5E2F-EB8E-409C-8B43-316A539C3D73}" type="CELLRANGE">
+                    <a:fld id="{F4E9D32E-7C3C-460E-926F-8C32EC9B2BBE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2227,7 +2233,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E3BC0543-4988-42E2-97C3-9A95DA10D56F}" type="CELLRANGE">
+                    <a:fld id="{D49A75F4-CA81-4360-8628-6460501DC083}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2261,7 +2267,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B95A490-2DBB-40EF-A596-09DAED799F59}" type="CELLRANGE">
+                    <a:fld id="{A9AF2172-D91B-4B98-B577-201BDF7888BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2295,7 +2301,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97EDF557-12A2-48F9-8057-A8263E4D75D5}" type="CELLRANGE">
+                    <a:fld id="{1444857B-997C-46C2-82B4-66B3C4FBA315}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2329,7 +2335,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{15492699-7804-43E3-A8C9-44D1831B9A31}" type="CELLRANGE">
+                    <a:fld id="{0E76BEA6-C4AB-49D2-8084-470D80114E9C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2363,7 +2369,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DFFF05E6-2DE2-4A6B-96BE-2B6E66B28F06}" type="CELLRANGE">
+                    <a:fld id="{64CD82EF-95BA-48AF-87A1-C24105F64221}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2397,7 +2403,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42F737DA-FBBF-4330-BEC1-BEBB5C912446}" type="CELLRANGE">
+                    <a:fld id="{B196EEC0-E15C-4C4E-ACC8-9CADB9CC0B86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2431,7 +2437,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{216AA73B-19AD-44FF-A1D9-F81222628225}" type="CELLRANGE">
+                    <a:fld id="{B41D5A90-D524-4E90-BAA0-367C94C76980}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2465,7 +2471,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BED060E6-2EB4-4980-9A8B-62B596C5D7C6}" type="CELLRANGE">
+                    <a:fld id="{F9EC03E8-27F7-49E2-ABCB-9278B56061FB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2499,7 +2505,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E66FF51-328B-4203-9872-3FB604A22811}" type="CELLRANGE">
+                    <a:fld id="{09D88DFA-D860-4919-89C6-67F54230E7E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2533,7 +2539,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B29C82C1-BAD2-44EE-A48A-D5460C9867A0}" type="CELLRANGE">
+                    <a:fld id="{61F009BF-68C7-4C46-9845-211E17AE6348}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2567,7 +2573,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0089FC36-C400-44C7-A912-5F94C4C15DB9}" type="CELLRANGE">
+                    <a:fld id="{E4B1724D-0C93-472A-9AC9-E921444F20D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2601,7 +2607,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EDF2FB30-1203-485F-A418-A8A8B3265FC2}" type="CELLRANGE">
+                    <a:fld id="{5C849305-486E-4CDB-94A6-2746FE356E40}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2635,7 +2641,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8213344A-9688-4606-955B-D5EF941C5D5F}" type="CELLRANGE">
+                    <a:fld id="{F0343555-35A5-47AF-A137-30E88A037D40}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2669,7 +2675,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0281BDE9-D9D9-43EB-BC45-D098680A3EB7}" type="CELLRANGE">
+                    <a:fld id="{DC8327F1-FB75-4D40-842D-BE23531FF7C4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2703,7 +2709,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9DF74AEC-3625-417C-86B0-DA681946E9E4}" type="CELLRANGE">
+                    <a:fld id="{7AC3A460-B187-4076-8FFF-01D223E34A90}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2737,7 +2743,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F4EC5C9-8139-40B1-BFCC-42E26D9DF59E}" type="CELLRANGE">
+                    <a:fld id="{120E88DE-EE01-456E-9269-FF6FD65BE81F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2761,6 +2767,74 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-5502-470D-857D-2D78F0BD0C14}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="70"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{CA4466E3-4C13-4F96-8542-DDE38C2B3643}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-E100-4598-89EB-D4D54BCB330E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="71"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{17817A20-0028-493A-94E3-941D34E726E2}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-E100-4598-89EB-D4D54BCB330E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2810,10 +2884,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$71</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -2836,192 +2910,198 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>7.5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>3.4</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>2.9</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>7.1</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
+                  <c:v>8.75</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>7.9</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>11.3</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>6.8</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>9.8000000000000007</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>9.6</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>11.6</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>12.5</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>9.1</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>9.5500000000000007</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>12.2</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>9.75</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>5.4</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>11.9</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="39">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="40">
                   <c:v>4.2</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="41">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="42">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="44">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="45">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="47">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="48">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="49">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="50">
                   <c:v>7.2</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="51">
                   <c:v>2.7</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="52">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="53">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="54">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="55">
                   <c:v>3.3</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="56">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="57">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="58">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="59">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="60">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="61">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="62">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="63">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="64">
                   <c:v>9.9</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="65">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="66">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="67">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="68">
                   <c:v>5.6</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="69">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="70">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="71">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -3029,10 +3109,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$71</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -3055,192 +3135,198 @@
                   <c:v>1270</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>2970</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>3110</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>940</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>3030</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>3200</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>1200</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>1540</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>2880</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>3290</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>2660</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>2780</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>2425</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>4100</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>4800</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>4120</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>3420</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>2050</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>1450</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>3160</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>880</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="39">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="40">
                   <c:v>860</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="41">
                   <c:v>1260</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="42">
                   <c:v>2600</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="44">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="45">
                   <c:v>3100</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="47">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="48">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="49">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="50">
                   <c:v>1630</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="51">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="52">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="53">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="54">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="55">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="56">
                   <c:v>1930</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="57">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="58">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="59">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="60">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="61">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="62">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="63">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="64">
                   <c:v>3180</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="65">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="66">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="67">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="68">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="69">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="70">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="71">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -3278,37 +3364,37 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="8">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="10">
                     <c:v>moderate (because rough)</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="12">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="14">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="16">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="17">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="18">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="19">
                     <c:v>moderate</c:v>
@@ -3320,19 +3406,19 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="22">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="24">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>strenuous</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="26">
-                    <c:v>strenuous</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="27">
                     <c:v>strenuous</c:v>
@@ -3344,58 +3430,58 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="30">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="32">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="31">
+                  <c:pt idx="33">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="32">
-                    <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="33">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="34">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="35">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="36">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="37">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="38">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="39">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="40">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="41">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="42">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="43">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="44">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="43">
+                  <c:pt idx="45">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="44">
-                    <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="45">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="46">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="47">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="48">
                     <c:v>moderate</c:v>
@@ -3404,19 +3490,19 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="50">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="51">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="51">
+                  <c:pt idx="52">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="53">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="52">
+                  <c:pt idx="54">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="53">
-                    <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="54">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="55">
                     <c:v>easy</c:v>
@@ -3425,19 +3511,19 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="57">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="58">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="58">
-                    <c:v>strenuous</c:v>
-                  </c:pt>
                   <c:pt idx="59">
-                    <c:v>easy</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="60">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="61">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="62">
                     <c:v>strenuous</c:v>
@@ -3446,21 +3532,27 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="64">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="65">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="66">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="65">
-                    <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="66">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="67">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="68">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="69">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="69">
+                  <c:pt idx="70">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="71">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -4513,10 +4605,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D71" totalsRowShown="0">
-  <autoFilter ref="A1:D71" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D71">
-    <sortCondition ref="A1:A71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D73" totalsRowShown="0">
+  <autoFilter ref="A1:D73" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D73">
+    <sortCondition ref="A1:A73"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -4825,10 +4917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4954,13 +5046,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="B9">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>2970</v>
+        <v>2400</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
@@ -4968,55 +5060,55 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B10">
-        <v>8.1999999999999993</v>
+        <v>7.5</v>
       </c>
       <c r="C10">
-        <v>3110</v>
+        <v>2970</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B11">
-        <v>3.4</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C11">
-        <v>940</v>
+        <v>3110</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="C12">
-        <v>1000</v>
+        <v>940</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13">
-        <v>2.9</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>1090</v>
+        <v>1000</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -5024,111 +5116,113 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B14">
-        <v>7.1</v>
+        <v>2.9</v>
       </c>
       <c r="C14">
-        <v>3030</v>
+        <v>1090</v>
       </c>
       <c r="D14" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="B15">
-        <v>7.9</v>
+        <v>7.1</v>
       </c>
       <c r="C15">
-        <v>3200</v>
+        <v>3030</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B16">
-        <v>11.3</v>
+        <f>35/4</f>
+        <v>8.75</v>
       </c>
       <c r="C16">
-        <v>3850</v>
+        <f>9000/4</f>
+        <v>2250</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B17">
-        <v>6.8</v>
+        <v>7.9</v>
       </c>
       <c r="C17">
-        <v>1200</v>
+        <v>3200</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B18">
-        <v>6.5</v>
+        <v>11.3</v>
       </c>
       <c r="C18">
-        <v>1540</v>
+        <v>3850</v>
       </c>
       <c r="D18" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="B19">
-        <v>9.8000000000000007</v>
+        <v>6.8</v>
       </c>
       <c r="C19">
-        <v>2880</v>
+        <v>1200</v>
       </c>
       <c r="D19" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B20">
-        <v>9.6</v>
+        <v>6.5</v>
       </c>
       <c r="C20">
-        <v>3290</v>
+        <v>1540</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B21">
-        <v>11.6</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C21">
-        <v>2660</v>
+        <v>2880</v>
       </c>
       <c r="D21" t="s">
         <v>1</v>
@@ -5136,13 +5230,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B22">
-        <v>12.5</v>
+        <v>9.6</v>
       </c>
       <c r="C22">
-        <v>2780</v>
+        <v>3290</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
@@ -5150,13 +5244,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B23">
-        <v>9</v>
+        <v>11.6</v>
       </c>
       <c r="C23">
-        <v>1680</v>
+        <v>2660</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
@@ -5164,85 +5258,85 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24">
-        <v>9.1</v>
+        <v>12.5</v>
       </c>
       <c r="C24">
-        <v>1580</v>
+        <v>2780</v>
       </c>
       <c r="D24" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B25">
-        <v>5.2</v>
+        <v>9</v>
       </c>
       <c r="C25">
-        <v>1000</v>
+        <v>1680</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <v>9.1</v>
+      </c>
+      <c r="C26">
+        <v>1580</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>5.2</v>
+      </c>
+      <c r="C27">
+        <v>1000</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>79</v>
       </c>
-      <c r="B26">
+      <c r="B28">
         <f>19.1/2</f>
         <v>9.5500000000000007</v>
       </c>
-      <c r="C26">
+      <c r="C28">
         <f>4850/2</f>
         <v>2425</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D28" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27">
-        <v>9.5</v>
-      </c>
-      <c r="C27">
-        <v>4100</v>
-      </c>
-      <c r="D27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28">
-        <v>14</v>
-      </c>
-      <c r="C28">
-        <v>4800</v>
-      </c>
-      <c r="D28" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="B29">
-        <v>12.2</v>
+        <v>9.5</v>
       </c>
       <c r="C29">
-        <v>4120</v>
+        <v>4100</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
@@ -5250,13 +5344,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B30">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C30">
-        <v>3420</v>
+        <v>4800</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
@@ -5264,85 +5358,85 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>12.2</v>
+      </c>
+      <c r="C31">
+        <v>4120</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <v>3420</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>37</v>
       </c>
-      <c r="B31">
+      <c r="B33">
         <f>19.5/2</f>
         <v>9.75</v>
       </c>
-      <c r="C31">
+      <c r="C33">
         <f>4400*7/8</f>
         <v>3850</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D33" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32">
-        <v>6.9</v>
-      </c>
-      <c r="C32">
-        <v>2050</v>
-      </c>
-      <c r="D32" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33">
-        <v>5.4</v>
-      </c>
-      <c r="C33">
-        <v>1450</v>
-      </c>
-      <c r="D33" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="B34">
-        <v>11.9</v>
+        <v>6.9</v>
       </c>
       <c r="C34">
-        <v>3160</v>
+        <v>2050</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35">
-        <v>11.4</v>
+        <v>5.4</v>
       </c>
       <c r="C35">
-        <v>2550</v>
+        <v>1450</v>
       </c>
       <c r="D35" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B36">
-        <v>8.5</v>
+        <v>11.9</v>
       </c>
       <c r="C36">
-        <v>3350</v>
+        <v>3160</v>
       </c>
       <c r="D36" t="s">
         <v>10</v>
@@ -5350,41 +5444,41 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="B37">
-        <v>2.8</v>
+        <v>11.4</v>
       </c>
       <c r="C37">
-        <v>880</v>
+        <v>2550</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38">
-        <v>10.4</v>
+        <v>8.5</v>
       </c>
       <c r="C38">
-        <v>1420</v>
+        <v>3350</v>
       </c>
       <c r="D38" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B39">
-        <v>0.9</v>
+        <v>2.8</v>
       </c>
       <c r="C39">
-        <v>200</v>
+        <v>880</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
@@ -5392,27 +5486,27 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="B40">
-        <v>4.2</v>
+        <v>10.4</v>
       </c>
       <c r="C40">
-        <v>860</v>
+        <v>1420</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B41">
-        <v>4.8</v>
+        <v>0.9</v>
       </c>
       <c r="C41">
-        <v>1260</v>
+        <v>200</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
@@ -5420,27 +5514,27 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="C42">
-        <v>2600</v>
+        <v>860</v>
       </c>
       <c r="D42" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B43">
-        <v>1.4</v>
+        <v>4.8</v>
       </c>
       <c r="C43">
-        <v>375</v>
+        <v>1260</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
@@ -5448,69 +5542,69 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B44">
-        <v>13.6</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>3930</v>
+        <v>2600</v>
       </c>
       <c r="D44" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B45">
-        <v>10.5</v>
+        <v>1.4</v>
       </c>
       <c r="C45">
-        <v>3100</v>
+        <v>375</v>
       </c>
       <c r="D45" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B46">
-        <v>7</v>
+        <v>13.6</v>
       </c>
       <c r="C46">
-        <v>1670</v>
+        <v>3930</v>
       </c>
       <c r="D46" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B47">
-        <v>8.1</v>
+        <v>10.5</v>
       </c>
       <c r="C47">
-        <v>2400</v>
+        <v>3100</v>
       </c>
       <c r="D47" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B48">
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="C48">
-        <v>1850</v>
+        <v>1670</v>
       </c>
       <c r="D48" t="s">
         <v>1</v>
@@ -5518,27 +5612,27 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B49">
-        <v>4.8</v>
+        <v>8.1</v>
       </c>
       <c r="C49">
-        <v>1300</v>
+        <v>2400</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B50">
-        <v>7.2</v>
+        <v>5.5</v>
       </c>
       <c r="C50">
-        <v>1630</v>
+        <v>1850</v>
       </c>
       <c r="D50" t="s">
         <v>1</v>
@@ -5546,13 +5640,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="B51">
-        <v>2.7</v>
+        <v>4.8</v>
       </c>
       <c r="C51">
-        <v>1090</v>
+        <v>1300</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -5560,83 +5654,83 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="B52">
-        <v>4.8</v>
+        <v>7.2</v>
       </c>
       <c r="C52">
-        <v>1470</v>
+        <v>1630</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="B53">
-        <v>6.9</v>
+        <v>2.7</v>
       </c>
       <c r="C53">
-        <v>2000</v>
+        <v>1090</v>
       </c>
       <c r="D53" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="B54">
-        <v>8.1999999999999993</v>
+        <v>4.8</v>
       </c>
       <c r="C54">
-        <v>3490</v>
+        <v>1470</v>
       </c>
       <c r="D54" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B55">
-        <v>3.3</v>
+        <v>6.9</v>
       </c>
       <c r="C55">
-        <v>600</v>
+        <v>2000</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="B56">
-        <v>8.5</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C56">
-        <v>1930</v>
+        <v>3490</v>
       </c>
       <c r="D56" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B57">
-        <v>2.2000000000000002</v>
+        <v>3.3</v>
       </c>
       <c r="C57">
-        <v>750</v>
+        <v>600</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -5644,13 +5738,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B58">
-        <v>11</v>
+        <v>8.5</v>
       </c>
       <c r="C58">
-        <v>2170</v>
+        <v>1930</v>
       </c>
       <c r="D58" t="s">
         <v>1</v>
@@ -5658,85 +5752,85 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B59">
-        <v>7.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C59">
-        <v>2250</v>
+        <v>750</v>
       </c>
       <c r="D59" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60">
+        <v>11</v>
+      </c>
+      <c r="C60">
+        <v>2170</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61">
+        <v>7.3</v>
+      </c>
+      <c r="C61">
+        <v>2250</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>25</v>
       </c>
-      <c r="B60">
+      <c r="B62">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C60">
+      <c r="C62">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>49</v>
-      </c>
-      <c r="B61">
-        <v>1.2</v>
-      </c>
-      <c r="C61">
-        <v>500</v>
-      </c>
-      <c r="D61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62">
-        <v>11</v>
-      </c>
-      <c r="C62">
-        <v>3060</v>
-      </c>
       <c r="D62" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B63">
-        <v>6.5</v>
+        <v>1.2</v>
       </c>
       <c r="C63">
-        <v>1650</v>
+        <v>500</v>
       </c>
       <c r="D63" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="B64">
-        <v>9.9</v>
+        <v>11</v>
       </c>
       <c r="C64">
-        <v>3180</v>
+        <v>3060</v>
       </c>
       <c r="D64" t="s">
         <v>10</v>
@@ -5744,13 +5838,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B65">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
       <c r="C65">
-        <v>1890</v>
+        <v>1650</v>
       </c>
       <c r="D65" t="s">
         <v>1</v>
@@ -5758,55 +5852,55 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="B66">
-        <v>0.4</v>
+        <v>9.9</v>
       </c>
       <c r="C66">
-        <v>100</v>
+        <v>3180</v>
       </c>
       <c r="D66" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B67">
-        <v>7.3</v>
+        <v>6.2</v>
       </c>
       <c r="C67">
-        <v>3550</v>
+        <v>1890</v>
       </c>
       <c r="D67" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="B68">
-        <v>5.6</v>
+        <v>0.4</v>
       </c>
       <c r="C68">
-        <v>1680</v>
+        <v>100</v>
       </c>
       <c r="D68" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B69">
-        <v>10.8</v>
+        <v>7.3</v>
       </c>
       <c r="C69">
-        <v>1800</v>
+        <v>3550</v>
       </c>
       <c r="D69" t="s">
         <v>10</v>
@@ -5814,30 +5908,58 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70">
+        <v>5.6</v>
+      </c>
+      <c r="C70">
+        <v>1680</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71">
+        <v>10.8</v>
+      </c>
+      <c r="C71">
+        <v>1800</v>
+      </c>
+      <c r="D71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>55</v>
       </c>
-      <c r="B70">
+      <c r="B72">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C70">
+      <c r="C72">
         <v>3800</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D72" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>29</v>
       </c>
-      <c r="B71">
+      <c r="B73">
         <v>6</v>
       </c>
-      <c r="C71">
+      <c r="C73">
         <v>2180</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D73" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Split Glacier Basin and Emmons Moraine
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014A8713-AB46-4417-996E-73ECAFA559AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32043E41-B83A-463A-8A31-CB0385A82805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="85">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>Cowlitz Gap</t>
+  </si>
+  <si>
+    <t>Emmons Moraine</t>
   </si>
 </sst>
 </file>
@@ -403,7 +406,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E1EC9277-92D5-41A9-A9A3-AABA8BAD412C}" type="CELLRANGE">
+                    <a:fld id="{8B6BA183-77C9-4D71-A416-E0ACAC75CA6B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -437,7 +440,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{875FE6C4-49F2-4C94-AF1A-089145FFDC04}" type="CELLRANGE">
+                    <a:fld id="{12C64069-373E-49D4-AFC0-46BAB795CF12}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -471,7 +474,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A658ADD1-5A44-4B86-8ABC-14B6C270ED97}" type="CELLRANGE">
+                    <a:fld id="{7C1A8C53-A111-4361-88D5-6698BE6D7E4F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -505,7 +508,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{86B8173A-FA56-4342-BDEE-E5477F588688}" type="CELLRANGE">
+                    <a:fld id="{0E1387B0-D174-4BB9-B09B-6D32381AAE29}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -539,7 +542,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{07DE93E8-30B7-4B8A-9C6A-ED0C276CB51C}" type="CELLRANGE">
+                    <a:fld id="{48E9B296-9696-49A2-9A4D-7FAC924EC049}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -573,7 +576,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{855100B6-5AA5-49B2-96E9-60ACC321F2B6}" type="CELLRANGE">
+                    <a:fld id="{2A356DDD-5BDE-48CA-888B-7BD82559A54B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -607,7 +610,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F7EBB40-F73C-41E8-81BD-04C740E1AC66}" type="CELLRANGE">
+                    <a:fld id="{37514A75-B166-4B87-94B6-BD047FB75049}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -641,7 +644,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D5CC8CB4-C881-4697-9F27-834D356F5CDA}" type="CELLRANGE">
+                    <a:fld id="{2C3D1715-F50C-4E00-9FA6-A5366BE80F56}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -675,7 +678,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5AD7D950-654B-4E83-B212-B74D137A4B52}" type="CELLRANGE">
+                    <a:fld id="{335169C4-1350-45D5-8A19-867800F6127F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -709,7 +712,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8A0C71B-FEFB-4F0A-8765-3A6B37968AD3}" type="CELLRANGE">
+                    <a:fld id="{A5BC26E7-1FC7-4A2B-9432-A1F9EF186553}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -743,7 +746,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88047F64-B6C6-44E6-BCFC-5584C0B64ED8}" type="CELLRANGE">
+                    <a:fld id="{3E7F1A3A-1F26-4730-A38D-AA61DB6A7E72}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -777,7 +780,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BCC41688-CF55-4863-A299-077314AAC2E9}" type="CELLRANGE">
+                    <a:fld id="{4A62CFB7-DD78-4D64-81A5-021884D95375}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -811,7 +814,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5F6F879-BA40-445C-B430-96AF1EA15832}" type="CELLRANGE">
+                    <a:fld id="{29877F09-CEEE-4318-A0C2-9A4DAFB6480D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -845,7 +848,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AC508E8D-D6A8-4448-982F-2989CE453C34}" type="CELLRANGE">
+                    <a:fld id="{0EAE13CD-2982-4854-A7E4-4C62F90FC416}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -879,7 +882,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A3F1AF75-AB03-4D43-968E-D72775C2D8CB}" type="CELLRANGE">
+                    <a:fld id="{153A496F-B467-472B-B336-9A0962FE7540}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -913,7 +916,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5EA4E39-24D7-4259-90B8-C1F5551502BD}" type="CELLRANGE">
+                    <a:fld id="{509D57B9-A9C8-46E2-80D7-2AC1FF9EA510}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -947,7 +950,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3FD5D084-A6DA-47FD-BEAD-1EF34A0D4D34}" type="CELLRANGE">
+                    <a:fld id="{D75FA810-7F82-4BCB-803F-95656D553303}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -981,7 +984,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42E6D5F7-C159-4385-9FDC-C8DBCF517520}" type="CELLRANGE">
+                    <a:fld id="{961832CC-AFC4-48C9-9E03-1CE71FA8FAD2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1015,7 +1018,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{98C4F052-DC8A-4D15-B032-1AFA3EA40855}" type="CELLRANGE">
+                    <a:fld id="{16FEA4B3-F16A-4047-A302-92570C9514E1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1049,7 +1052,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96BCD944-EE32-477B-889C-D44FEFC1C5FE}" type="CELLRANGE">
+                    <a:fld id="{3C00C10B-9886-4F0E-8978-E321D4735691}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1083,7 +1086,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D55416CB-D555-4775-8E36-AA87BBD5A306}" type="CELLRANGE">
+                    <a:fld id="{F8D3A7CE-C8D3-430D-876F-424845080074}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1117,7 +1120,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A39288C1-5223-4A9C-A163-62C067E93676}" type="CELLRANGE">
+                    <a:fld id="{C38D1CD7-2350-405D-BC08-53E7DE3B9A10}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1151,7 +1154,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34E0CA17-31DC-4A3E-9F1F-A0996CBFE7F3}" type="CELLRANGE">
+                    <a:fld id="{E4BE3EDE-2C11-44F3-87E2-73381F57B41A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1185,7 +1188,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0405E122-696C-4384-9D8E-1EA695F537F2}" type="CELLRANGE">
+                    <a:fld id="{49BB43B3-4224-4B95-9DBD-F389776462EF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1219,7 +1222,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{048878EF-B928-418B-9D13-BCDF6935A787}" type="CELLRANGE">
+                    <a:fld id="{F224A18E-9D67-4A76-870E-FD21EA21BCEE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1253,7 +1256,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D25E8D97-412F-4ABB-AE7B-C67251FC8167}" type="CELLRANGE">
+                    <a:fld id="{696736F3-D793-41BB-82D6-ABFEE1EEDD64}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1287,7 +1290,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8304D764-62DF-45AF-9A46-C57888557777}" type="CELLRANGE">
+                    <a:fld id="{B915873C-67F3-4AEC-AA2B-869B42F3BC2D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1321,7 +1324,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70AB88B5-37BC-472F-A054-E141982AC09D}" type="CELLRANGE">
+                    <a:fld id="{4059E81F-32F9-4338-B1A5-F06AB5987EC0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1355,7 +1358,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B557507E-A1CC-45F4-8F66-AA337957B117}" type="CELLRANGE">
+                    <a:fld id="{30BDAFD7-E207-477C-A0F7-6C73388A43E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1389,7 +1392,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3AEE735B-BDCE-400A-829D-987D0EA77933}" type="CELLRANGE">
+                    <a:fld id="{1D19187C-B65C-4D77-8C53-B3EF0AA18AF0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1423,7 +1426,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19A0DC7C-CC76-4D50-8823-399BC8E099BF}" type="CELLRANGE">
+                    <a:fld id="{5B6AC520-4DC3-40D6-88E7-8B6EDBACD514}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1457,7 +1460,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4C8EB64-85A5-42EB-94C2-174906B789B3}" type="CELLRANGE">
+                    <a:fld id="{7DDAF1FB-C024-49C3-B631-5A665BB31781}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1491,7 +1494,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD99C933-B6A3-4189-85D2-CAF0749489E9}" type="CELLRANGE">
+                    <a:fld id="{E9552C25-9D53-4228-9682-8B41511719E0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1525,7 +1528,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70E6F8FB-5B89-4376-863F-381F956797A2}" type="CELLRANGE">
+                    <a:fld id="{2CC6E6A7-03E2-4421-BCA7-5677F87E9FBD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1559,7 +1562,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E8F413A6-C7B2-400C-B84F-095E9ABEE44F}" type="CELLRANGE">
+                    <a:fld id="{057A3604-1FF4-4E93-A26D-38DCD3993046}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1593,7 +1596,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7A5E1CF6-AC83-44D7-9721-0887A17C8B5D}" type="CELLRANGE">
+                    <a:fld id="{026934DD-6400-49A7-8691-A36C0FC7A3F4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1627,7 +1630,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C1DB088-13D8-42D3-A948-0CFCA2092411}" type="CELLRANGE">
+                    <a:fld id="{2B8A40F8-C352-4740-B9FD-6C45140CB37A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1661,7 +1664,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{83DA45E4-FF5B-4725-8F66-06966E4ED7B3}" type="CELLRANGE">
+                    <a:fld id="{C6610DC3-5513-4AEB-BFC1-79210B5F0BCC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1695,7 +1698,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D63D00B-725F-4B99-9DEB-D8015F6DAC0E}" type="CELLRANGE">
+                    <a:fld id="{EB32F6C4-7436-4E75-8DA4-DEBBA44C1EF5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1729,7 +1732,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D6046C3-5667-4D3E-BD55-ADE2903F3FA8}" type="CELLRANGE">
+                    <a:fld id="{F17E49C4-6C79-41B5-9173-72F667F1C4CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1763,7 +1766,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4CA04646-F474-4B53-AE89-9FD0C1E46D63}" type="CELLRANGE">
+                    <a:fld id="{80F9E5E2-A798-4AD2-A19E-0EF0CF15406F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1797,7 +1800,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{13895B44-8D20-43EB-9EB3-A94885CAFAE9}" type="CELLRANGE">
+                    <a:fld id="{D90EE91C-B115-4861-9F10-71BEF6945629}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1831,7 +1834,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A4F522AE-08EC-44AE-81B1-39D5E72C62A4}" type="CELLRANGE">
+                    <a:fld id="{F090BFD5-1FA1-4615-8477-953F9CC0E835}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1865,7 +1868,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9833F4CD-C02F-4892-96C4-1DC3E108F6DC}" type="CELLRANGE">
+                    <a:fld id="{94C05EAE-C7F7-4DFC-B3EC-BCD62E46876B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1899,7 +1902,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{948C62DB-F141-4CD1-A3AB-C42547207699}" type="CELLRANGE">
+                    <a:fld id="{2D1C42B1-332A-4C07-ABA1-EB5E8BD9A114}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1933,7 +1936,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{744A7676-4D85-4EC0-91F9-92C93FE47843}" type="CELLRANGE">
+                    <a:fld id="{8D0A0BD1-47EF-4E03-9AD1-CB8EA321964E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1967,7 +1970,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6BBD0958-DAED-4219-AE45-07E2286108C1}" type="CELLRANGE">
+                    <a:fld id="{BFA9B394-53EF-4C93-9F40-7DAA145CD46F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2001,7 +2004,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E5866D87-B035-42A0-95E4-BAE41CF068AC}" type="CELLRANGE">
+                    <a:fld id="{7B51B1F8-2F8B-4B09-AB58-EC2B4579DAA0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2035,7 +2038,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B347A6AB-B67A-41EE-81E9-FDFE73FD726F}" type="CELLRANGE">
+                    <a:fld id="{CB3FBA2A-E245-4FBF-9988-029A35E36707}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2069,7 +2072,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{07ED5639-3FAF-4544-B9A5-4F3859A56028}" type="CELLRANGE">
+                    <a:fld id="{B2D45E12-F919-4B19-B393-41F48764B218}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2103,7 +2106,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67ED076F-F9CE-4844-82C6-B3735EDA90FF}" type="CELLRANGE">
+                    <a:fld id="{ED43A707-4820-4536-B2E8-867E28C4F71A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2137,7 +2140,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3004D0F-CBFB-453B-B0F6-CF593BE60C88}" type="CELLRANGE">
+                    <a:fld id="{EBE00B18-1DAF-4040-8E28-959C708C7B9E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2171,7 +2174,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E20E31DF-F578-40A0-A735-506FB8B095BD}" type="CELLRANGE">
+                    <a:fld id="{0BD78186-1B91-456E-8DEF-75D0C075A2ED}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2205,7 +2208,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FEFC406F-3065-4935-A08D-271C3DC50EFC}" type="CELLRANGE">
+                    <a:fld id="{B0C264D3-046B-4347-8508-5E8E1D3DFE28}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2239,7 +2242,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14720225-A68A-4392-BDF9-620B32B38554}" type="CELLRANGE">
+                    <a:fld id="{AC01B721-D24E-4009-BAE2-1236991BB226}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2273,7 +2276,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F9CB893-4E95-40A1-BD15-124925786488}" type="CELLRANGE">
+                    <a:fld id="{10BB482C-996A-4861-88A3-92BED1E302F7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2307,7 +2310,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47E4983E-36B6-4B2B-B0D3-C26E318FCD79}" type="CELLRANGE">
+                    <a:fld id="{C6E9CB7F-C791-4516-A5AD-252A64761EF2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2341,7 +2344,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{139D1B4E-FCA5-4153-A268-AB789E5954D5}" type="CELLRANGE">
+                    <a:fld id="{DF75B0D9-2B13-4923-A502-91202F59A874}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2375,7 +2378,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5CF0BEB-3860-4C0E-8381-BCE6B214B16A}" type="CELLRANGE">
+                    <a:fld id="{EB9B0B5F-A1C6-4864-898F-BB99E8E20C74}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2409,7 +2412,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6C29664-BBCE-4458-B20F-7CE5773C3526}" type="CELLRANGE">
+                    <a:fld id="{B3A77ED0-00BD-4E11-B652-B7CC93D12C44}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2443,7 +2446,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{44A41E6A-D366-473F-A0EB-757DC42E9E8F}" type="CELLRANGE">
+                    <a:fld id="{905184F4-B8C7-45D5-BCB4-BDCC477E1863}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2477,7 +2480,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0401ADB6-5083-4628-862B-A15E4358F619}" type="CELLRANGE">
+                    <a:fld id="{7121A9A4-77B1-4085-87C6-CF36B87FCEA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2511,7 +2514,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A458234B-840B-4190-95F0-87D371D763B5}" type="CELLRANGE">
+                    <a:fld id="{A8023539-2402-4024-923D-7AB06EBE3170}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2545,7 +2548,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B2746948-49A6-4E39-B3FA-97EAF6AF0A37}" type="CELLRANGE">
+                    <a:fld id="{26FB0F57-47C6-4FBD-AD51-B37FA7CFCAED}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2579,7 +2582,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10F1CB9F-3ADE-4160-ADF6-2C15ED2142B1}" type="CELLRANGE">
+                    <a:fld id="{DF85DCEC-8891-4F64-8891-CF349FE5CB7F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2613,7 +2616,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{31706341-C3AE-4997-9AC8-D2D25F798935}" type="CELLRANGE">
+                    <a:fld id="{B207B172-615D-4567-8EC6-BD10F3650FC9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2647,7 +2650,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CBDC6F68-E15D-43BE-AC52-18A170FBAAD4}" type="CELLRANGE">
+                    <a:fld id="{33BF6708-2498-49B0-A1B1-C9A57A35C271}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2681,7 +2684,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{997EAF93-C3FB-4615-A5AC-7968AF7E8008}" type="CELLRANGE">
+                    <a:fld id="{7BB488D8-2EA1-43D4-8F66-621B7B0CAFFA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2715,7 +2718,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C31FE7B-0E06-48D3-B3A7-C5456802DC3C}" type="CELLRANGE">
+                    <a:fld id="{9FC81DE6-A315-40A2-8028-363A8282CD49}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2749,7 +2752,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91D0C355-5965-402D-9C98-9D550FE58B33}" type="CELLRANGE">
+                    <a:fld id="{8B8E7D7A-D0D7-4836-BE5F-99EEE59BE552}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2783,7 +2786,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7526A205-6641-4747-A863-B2E50B48D831}" type="CELLRANGE">
+                    <a:fld id="{30FEBC55-55DB-40F1-A0D1-C420B940F7A2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2817,7 +2820,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{87E74A4B-C3A5-4C93-B5EF-E47B04227AF1}" type="CELLRANGE">
+                    <a:fld id="{9DCB2948-569A-43B8-A521-91D52AA251CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2851,7 +2854,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D5FA19FD-4A19-440A-AEA4-8B9A511642AD}" type="CELLRANGE">
+                    <a:fld id="{3B2CB7A5-E3FD-4468-8083-5AB8E1386EEF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2885,7 +2888,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58DBC59E-4C99-491D-A331-60A49CD4ABE2}" type="CELLRANGE">
+                    <a:fld id="{A564ACBD-B51B-4724-80E9-F31C70656D11}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2909,6 +2912,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-1000-4668-87B3-27164E012883}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="74"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2C2A589C-6295-4059-B9B9-C668621A8C6E}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-199E-419A-8EE0-80CDE2F856E3}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2958,10 +2995,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$75</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="74"/>
+                <c:ptCount val="75"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -3020,168 +3057,171 @@
                   <c:v>6.8</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>9.8000000000000007</c:v>
-                </c:pt>
                 <c:pt idx="21">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>9.6</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>11.6</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>12.5</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>9.1</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>9.5500000000000007</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>12.2</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>9.75</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>5.4</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>11.9</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>4.2</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>7.2</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>2.7</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>3.3</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>9.9</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="69">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>5.6</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="73">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="74">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -3189,10 +3229,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$75</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="74"/>
+                <c:ptCount val="75"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -3251,168 +3291,171 @@
                   <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>1540</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>2880</c:v>
-                </c:pt>
                 <c:pt idx="21">
+                  <c:v>2380</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>3290</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>2660</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>2780</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>2425</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>4100</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>4800</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>4120</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>3420</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>2050</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>1450</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>3160</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>880</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>860</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>1260</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>2600</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>3100</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>1630</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>1930</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>3180</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="69">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="73">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="74">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -3483,37 +3526,37 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="20">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="21">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="23">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="24">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="26">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="27">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="28">
+                  <c:pt idx="29">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="30">
                     <c:v>strenuous</c:v>
@@ -3528,28 +3571,28 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="34">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="36">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="36">
+                  <c:pt idx="37">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="37">
+                  <c:pt idx="38">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="38">
+                  <c:pt idx="39">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="39">
+                  <c:pt idx="40">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="40">
+                  <c:pt idx="41">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="41">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="42">
                     <c:v>easy</c:v>
@@ -3558,19 +3601,19 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="44">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="45">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="45">
+                  <c:pt idx="46">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="46">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="47">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="48">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="49">
                     <c:v>moderate</c:v>
@@ -3579,72 +3622,75 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="51">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="52">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="52">
+                  <c:pt idx="53">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="53">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="54">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="55">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="56">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="56">
+                  <c:pt idx="57">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="57">
+                  <c:pt idx="58">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="58">
+                  <c:pt idx="59">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="59">
+                  <c:pt idx="60">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="60">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="61">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="62">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="63">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="63">
+                  <c:pt idx="64">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="64">
+                  <c:pt idx="65">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="65">
+                  <c:pt idx="66">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="66">
+                  <c:pt idx="67">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="67">
+                  <c:pt idx="68">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="68">
+                  <c:pt idx="69">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="69">
+                  <c:pt idx="70">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="70">
+                  <c:pt idx="71">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="71">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="72">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="73">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="74">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -4697,10 +4743,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D75" totalsRowShown="0">
-  <autoFilter ref="A1:D75" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D75">
-    <sortCondition ref="A1:A75"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D76" totalsRowShown="0">
+  <autoFilter ref="A1:D76" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D76">
+    <sortCondition ref="A1:A76"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -5009,10 +5055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5308,27 +5354,27 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="B21">
-        <v>6.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C21">
-        <v>1540</v>
+        <v>960</v>
       </c>
       <c r="D21" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B22">
-        <v>9.8000000000000007</v>
+        <v>6.5</v>
       </c>
       <c r="C22">
-        <v>2880</v>
+        <v>1540</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
@@ -5336,85 +5382,85 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23">
-        <v>9.6</v>
+        <v>8.5</v>
       </c>
       <c r="C23">
-        <v>3290</v>
+        <v>2380</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>9.6</v>
+      </c>
+      <c r="C24">
+        <v>3290</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>82</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <f>14.6/2</f>
         <v>7.3</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <f>3160/2</f>
         <v>1580</v>
       </c>
-      <c r="D24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25">
-        <v>11.6</v>
-      </c>
-      <c r="C25">
-        <v>2660</v>
-      </c>
       <c r="D25" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B26">
-        <v>12.5</v>
+        <v>11.6</v>
       </c>
       <c r="C26">
-        <v>2780</v>
+        <v>2660</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="B27">
-        <v>9</v>
+        <v>12.5</v>
       </c>
       <c r="C27">
-        <v>1680</v>
+        <v>2780</v>
       </c>
       <c r="D27" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B28">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="C28">
-        <v>1580</v>
+        <v>1680</v>
       </c>
       <c r="D28" t="s">
         <v>1</v>
@@ -5422,57 +5468,57 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B29">
-        <v>5.2</v>
+        <v>9.1</v>
       </c>
       <c r="C29">
-        <v>1000</v>
+        <v>1580</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30">
+        <v>5.2</v>
+      </c>
+      <c r="C30">
+        <v>1000</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>79</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <f>19.1/2</f>
         <v>9.5500000000000007</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <f>4850/2</f>
         <v>2425</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31">
-        <v>9.5</v>
-      </c>
-      <c r="C31">
-        <v>4100</v>
-      </c>
-      <c r="D31" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="B32">
-        <v>14</v>
+        <v>9.5</v>
       </c>
       <c r="C32">
-        <v>4800</v>
+        <v>4100</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
@@ -5480,13 +5526,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33">
         <v>14</v>
       </c>
-      <c r="B33">
-        <v>12.2</v>
-      </c>
       <c r="C33">
-        <v>4120</v>
+        <v>4800</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
@@ -5494,13 +5540,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B34">
-        <v>12</v>
+        <v>12.2</v>
       </c>
       <c r="C34">
-        <v>3420</v>
+        <v>4120</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
@@ -5508,141 +5554,141 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>3420</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <f>19.5/2</f>
         <v>9.75</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <f>4400*7/8</f>
         <v>3850</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36">
-        <v>6.9</v>
-      </c>
-      <c r="C36">
-        <v>2050</v>
-      </c>
-      <c r="D36" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="B37">
-        <v>5.4</v>
+        <v>6.9</v>
       </c>
       <c r="C37">
-        <v>1450</v>
+        <v>2050</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B38">
-        <v>11.9</v>
+        <v>5.4</v>
       </c>
       <c r="C38">
-        <v>3160</v>
+        <v>1450</v>
       </c>
       <c r="D38" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B39">
-        <v>11.4</v>
+        <v>11.9</v>
       </c>
       <c r="C39">
-        <v>2550</v>
+        <v>3160</v>
       </c>
       <c r="D39" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B40">
-        <v>8.5</v>
+        <v>11.4</v>
       </c>
       <c r="C40">
-        <v>3350</v>
+        <v>2550</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B41">
-        <v>2.8</v>
+        <v>8.5</v>
       </c>
       <c r="C41">
-        <v>880</v>
+        <v>3350</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B42">
-        <v>10.4</v>
+        <v>2.8</v>
       </c>
       <c r="C42">
-        <v>1420</v>
+        <v>880</v>
       </c>
       <c r="D42" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B43">
-        <v>0.9</v>
+        <v>10.4</v>
       </c>
       <c r="C43">
-        <v>200</v>
+        <v>1420</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B44">
-        <v>4.2</v>
+        <v>0.9</v>
       </c>
       <c r="C44">
-        <v>860</v>
+        <v>200</v>
       </c>
       <c r="D44" t="s">
         <v>7</v>
@@ -5650,13 +5696,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B45">
-        <v>4.8</v>
+        <v>4.2</v>
       </c>
       <c r="C45">
-        <v>1260</v>
+        <v>860</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
@@ -5664,55 +5710,55 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>4.8</v>
       </c>
       <c r="C46">
-        <v>2600</v>
+        <v>1260</v>
       </c>
       <c r="D46" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B47">
-        <v>1.4</v>
+        <v>4</v>
       </c>
       <c r="C47">
-        <v>375</v>
+        <v>2600</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B48">
-        <v>13.6</v>
+        <v>1.4</v>
       </c>
       <c r="C48">
-        <v>3930</v>
+        <v>375</v>
       </c>
       <c r="D48" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B49">
-        <v>10.5</v>
+        <v>13.6</v>
       </c>
       <c r="C49">
-        <v>3100</v>
+        <v>3930</v>
       </c>
       <c r="D49" t="s">
         <v>10</v>
@@ -5720,27 +5766,27 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B50">
-        <v>7</v>
+        <v>10.5</v>
       </c>
       <c r="C50">
-        <v>1670</v>
+        <v>3100</v>
       </c>
       <c r="D50" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B51">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="C51">
-        <v>2400</v>
+        <v>1670</v>
       </c>
       <c r="D51" t="s">
         <v>1</v>
@@ -5748,13 +5794,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B52">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C52">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D52" t="s">
         <v>1</v>
@@ -5762,55 +5808,55 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B53">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C53">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B54">
-        <v>7.2</v>
+        <v>4.8</v>
       </c>
       <c r="C54">
-        <v>1630</v>
+        <v>1300</v>
       </c>
       <c r="D54" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B55">
-        <v>2.7</v>
+        <v>7.2</v>
       </c>
       <c r="C55">
-        <v>1090</v>
+        <v>1630</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="B56">
-        <v>4.8</v>
+        <v>2.7</v>
       </c>
       <c r="C56">
-        <v>1470</v>
+        <v>1090</v>
       </c>
       <c r="D56" t="s">
         <v>7</v>
@@ -5818,97 +5864,97 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B57">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C57">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D57" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B58">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C58">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D58" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B59">
-        <v>3.3</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C59">
-        <v>600</v>
+        <v>3490</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B60">
-        <v>8.5</v>
+        <v>3.3</v>
       </c>
       <c r="C60">
-        <v>1930</v>
+        <v>600</v>
       </c>
       <c r="D60" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B61">
-        <v>2.2000000000000002</v>
+        <v>8.5</v>
       </c>
       <c r="C61">
-        <v>750</v>
+        <v>1930</v>
       </c>
       <c r="D61" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B62">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C62">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D62" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B63">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C63">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D63" t="s">
         <v>1</v>
@@ -5916,172 +5962,186 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64">
+        <v>7.3</v>
+      </c>
+      <c r="C64">
+        <v>2250</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>25</v>
       </c>
-      <c r="B64">
+      <c r="B65">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C64">
+      <c r="C65">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>49</v>
-      </c>
-      <c r="B65">
-        <v>1.2</v>
-      </c>
-      <c r="C65">
-        <v>500</v>
-      </c>
-      <c r="D65" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B66">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C66">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D66" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B67">
-        <v>6.5</v>
+        <v>11</v>
       </c>
       <c r="C67">
-        <v>1650</v>
+        <v>3060</v>
       </c>
       <c r="D67" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B68">
-        <v>9.9</v>
+        <v>6.5</v>
       </c>
       <c r="C68">
-        <v>3180</v>
+        <v>1650</v>
       </c>
       <c r="D68" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="B69">
-        <v>6.2</v>
+        <v>9.9</v>
       </c>
       <c r="C69">
-        <v>1890</v>
+        <v>3180</v>
       </c>
       <c r="D69" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B70">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C70">
-        <v>100</v>
+        <v>1890</v>
       </c>
       <c r="D70" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B71">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C71">
-        <v>3550</v>
+        <v>100</v>
       </c>
       <c r="D71" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="B72">
-        <v>5.6</v>
+        <v>7.3</v>
       </c>
       <c r="C72">
-        <v>1680</v>
+        <v>3550</v>
       </c>
       <c r="D72" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B73">
-        <v>10.8</v>
+        <v>5.6</v>
       </c>
       <c r="C73">
-        <v>1800</v>
+        <v>1680</v>
       </c>
       <c r="D73" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
+        <v>63</v>
+      </c>
+      <c r="B74">
+        <v>10.8</v>
+      </c>
+      <c r="C74">
+        <v>1800</v>
+      </c>
+      <c r="D74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>55</v>
       </c>
-      <c r="B74">
+      <c r="B75">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C74">
+      <c r="C75">
         <v>3800</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D75" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>29</v>
       </c>
-      <c r="B75">
+      <c r="B76">
         <v>6</v>
       </c>
-      <c r="C75">
+      <c r="C76">
         <v>2180</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Longmire Stewardship Campground
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32043E41-B83A-463A-8A31-CB0385A82805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065DD3DF-D716-46C6-83E7-24FDAFF8C69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="86">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>Emmons Moraine</t>
+  </si>
+  <si>
+    <t>Longmire Stewardship Campground</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B6BA183-77C9-4D71-A416-E0ACAC75CA6B}" type="CELLRANGE">
+                    <a:fld id="{F0B39BE0-ECDE-4BE9-B07F-71CB2CCB66A0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -440,7 +443,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12C64069-373E-49D4-AFC0-46BAB795CF12}" type="CELLRANGE">
+                    <a:fld id="{10AF186E-38F1-4B0B-A3D2-88ACA2327DE5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -474,7 +477,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7C1A8C53-A111-4361-88D5-6698BE6D7E4F}" type="CELLRANGE">
+                    <a:fld id="{A66206BF-3CD3-485B-BA3D-03DB9C2DFE05}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -508,7 +511,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E1387B0-D174-4BB9-B09B-6D32381AAE29}" type="CELLRANGE">
+                    <a:fld id="{C8D8B6DD-A46C-4B42-A595-04870F3753FE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -542,7 +545,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48E9B296-9696-49A2-9A4D-7FAC924EC049}" type="CELLRANGE">
+                    <a:fld id="{630A8632-EA72-448F-AB47-FF39C5FB3052}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -576,7 +579,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A356DDD-5BDE-48CA-888B-7BD82559A54B}" type="CELLRANGE">
+                    <a:fld id="{0577AF11-C3F8-4BE7-A19F-E9BF09879DC4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -610,7 +613,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{37514A75-B166-4B87-94B6-BD047FB75049}" type="CELLRANGE">
+                    <a:fld id="{862D23BB-483C-479E-A063-AB5A7EF12594}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -644,7 +647,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C3D1715-F50C-4E00-9FA6-A5366BE80F56}" type="CELLRANGE">
+                    <a:fld id="{EEEE213B-15CC-4FD1-87A8-AD23637EA1A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -678,7 +681,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{335169C4-1350-45D5-8A19-867800F6127F}" type="CELLRANGE">
+                    <a:fld id="{69870C59-A777-4076-9211-6CB5A7B4B4BC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -712,7 +715,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5BC26E7-1FC7-4A2B-9432-A1F9EF186553}" type="CELLRANGE">
+                    <a:fld id="{45FE33B7-F1CE-4BEB-BCB5-61951B772A11}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -746,7 +749,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E7F1A3A-1F26-4730-A38D-AA61DB6A7E72}" type="CELLRANGE">
+                    <a:fld id="{2E5417CB-4E6F-49ED-9D5B-CD004635E4C3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -780,7 +783,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4A62CFB7-DD78-4D64-81A5-021884D95375}" type="CELLRANGE">
+                    <a:fld id="{3F01BD3B-4DC6-4C92-B7AF-68C9889932FA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -814,7 +817,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29877F09-CEEE-4318-A0C2-9A4DAFB6480D}" type="CELLRANGE">
+                    <a:fld id="{D801A403-477A-4B14-9DA3-A128476F0329}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -848,7 +851,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0EAE13CD-2982-4854-A7E4-4C62F90FC416}" type="CELLRANGE">
+                    <a:fld id="{3E30EB25-EA22-472D-B185-9767ABC3E82E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -882,7 +885,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{153A496F-B467-472B-B336-9A0962FE7540}" type="CELLRANGE">
+                    <a:fld id="{509B6979-B58C-464C-8BC7-1BF455E7D6E9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -916,7 +919,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{509D57B9-A9C8-46E2-80D7-2AC1FF9EA510}" type="CELLRANGE">
+                    <a:fld id="{34703DB1-7E36-4508-BD0F-126D799B60E3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -950,7 +953,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D75FA810-7F82-4BCB-803F-95656D553303}" type="CELLRANGE">
+                    <a:fld id="{351DCD96-1828-4F59-8A54-2426DF94F025}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -984,7 +987,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{961832CC-AFC4-48C9-9E03-1CE71FA8FAD2}" type="CELLRANGE">
+                    <a:fld id="{FC8BA4BE-8401-4FCB-8BA6-893F542A1A02}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1018,7 +1021,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{16FEA4B3-F16A-4047-A302-92570C9514E1}" type="CELLRANGE">
+                    <a:fld id="{B70369B8-B0DA-4565-9171-869FE29B1679}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1052,7 +1055,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C00C10B-9886-4F0E-8978-E321D4735691}" type="CELLRANGE">
+                    <a:fld id="{B7DEE7C9-158F-4AD4-9125-BCA83F2301D4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1086,7 +1089,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8D3A7CE-C8D3-430D-876F-424845080074}" type="CELLRANGE">
+                    <a:fld id="{B197A628-7407-4A1E-B20A-67AD13672913}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1120,7 +1123,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C38D1CD7-2350-405D-BC08-53E7DE3B9A10}" type="CELLRANGE">
+                    <a:fld id="{A597A935-A679-465D-BA36-CE3C7BBCD2E5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1154,7 +1157,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E4BE3EDE-2C11-44F3-87E2-73381F57B41A}" type="CELLRANGE">
+                    <a:fld id="{6BE2731F-DA97-4AFF-967A-18B59E071E94}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1188,7 +1191,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{49BB43B3-4224-4B95-9DBD-F389776462EF}" type="CELLRANGE">
+                    <a:fld id="{876ACD0C-C3DC-43E9-A11F-DC1F831C88F1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1222,7 +1225,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F224A18E-9D67-4A76-870E-FD21EA21BCEE}" type="CELLRANGE">
+                    <a:fld id="{C6651F9F-ADA2-4D70-BAEB-5A9FB40958DB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1256,7 +1259,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{696736F3-D793-41BB-82D6-ABFEE1EEDD64}" type="CELLRANGE">
+                    <a:fld id="{63403692-3C4A-481C-84D2-E7A42566F5F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1290,7 +1293,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B915873C-67F3-4AEC-AA2B-869B42F3BC2D}" type="CELLRANGE">
+                    <a:fld id="{BB075985-BA28-4B8E-9FDB-29F924FC975B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1324,7 +1327,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4059E81F-32F9-4338-B1A5-F06AB5987EC0}" type="CELLRANGE">
+                    <a:fld id="{6F15B6EE-8CB4-40A5-AB4A-723DAB098B8F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1358,7 +1361,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{30BDAFD7-E207-477C-A0F7-6C73388A43E4}" type="CELLRANGE">
+                    <a:fld id="{22BD07BF-C3E9-4806-B6FB-B5810C725B2E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1392,7 +1395,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1D19187C-B65C-4D77-8C53-B3EF0AA18AF0}" type="CELLRANGE">
+                    <a:fld id="{B43BF7C7-0CA6-4BFE-A84B-59AB3EAEC0DE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1426,7 +1429,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B6AC520-4DC3-40D6-88E7-8B6EDBACD514}" type="CELLRANGE">
+                    <a:fld id="{B8365A81-D22B-4151-A6EE-F20F6800810C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1460,7 +1463,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7DDAF1FB-C024-49C3-B631-5A665BB31781}" type="CELLRANGE">
+                    <a:fld id="{2775CB39-45D3-476B-975C-B3DEE57449B6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1494,7 +1497,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9552C25-9D53-4228-9682-8B41511719E0}" type="CELLRANGE">
+                    <a:fld id="{C9EB857B-1ABB-4B60-B7F8-4A5E45DECD2A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1528,7 +1531,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2CC6E6A7-03E2-4421-BCA7-5677F87E9FBD}" type="CELLRANGE">
+                    <a:fld id="{68FE1545-E440-45CF-9158-CD86C8A04A8D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1562,7 +1565,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{057A3604-1FF4-4E93-A26D-38DCD3993046}" type="CELLRANGE">
+                    <a:fld id="{B859A590-F4F6-4802-8C0D-5D581F9015B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1596,7 +1599,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{026934DD-6400-49A7-8691-A36C0FC7A3F4}" type="CELLRANGE">
+                    <a:fld id="{3BC389D1-9591-453C-BD5A-5476A8E06F42}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1630,7 +1633,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2B8A40F8-C352-4740-B9FD-6C45140CB37A}" type="CELLRANGE">
+                    <a:fld id="{900A479A-ED84-4A28-AC46-FBAF7ED71B37}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1664,7 +1667,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C6610DC3-5513-4AEB-BFC1-79210B5F0BCC}" type="CELLRANGE">
+                    <a:fld id="{90D20C92-F0A6-47F5-B45F-0D8B5A29C5F9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1698,7 +1701,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB32F6C4-7436-4E75-8DA4-DEBBA44C1EF5}" type="CELLRANGE">
+                    <a:fld id="{7F089E5F-7A7B-494D-A451-E222727284A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1732,7 +1735,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F17E49C4-6C79-41B5-9173-72F667F1C4CB}" type="CELLRANGE">
+                    <a:fld id="{10109EB2-7288-4E7E-9CFD-FFB621C20F8C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1766,7 +1769,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{80F9E5E2-A798-4AD2-A19E-0EF0CF15406F}" type="CELLRANGE">
+                    <a:fld id="{D23AE8AB-0984-4268-9743-89927E663E7B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1800,7 +1803,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D90EE91C-B115-4861-9F10-71BEF6945629}" type="CELLRANGE">
+                    <a:fld id="{4E2D2BBC-14CB-4A04-BC79-EF9E72D48EF8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1834,7 +1837,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F090BFD5-1FA1-4615-8477-953F9CC0E835}" type="CELLRANGE">
+                    <a:fld id="{AB03046A-A85B-4750-9271-5FDA086491CE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1868,7 +1871,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{94C05EAE-C7F7-4DFC-B3EC-BCD62E46876B}" type="CELLRANGE">
+                    <a:fld id="{DDEE1C3A-1E1C-482E-8C98-D0F11E81C6E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1902,7 +1905,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D1C42B1-332A-4C07-ABA1-EB5E8BD9A114}" type="CELLRANGE">
+                    <a:fld id="{04336D28-21F5-433E-9461-916D83E02636}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1936,7 +1939,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8D0A0BD1-47EF-4E03-9AD1-CB8EA321964E}" type="CELLRANGE">
+                    <a:fld id="{874E2EA2-87F7-4905-90E2-34B4AA9DC20B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1970,7 +1973,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BFA9B394-53EF-4C93-9F40-7DAA145CD46F}" type="CELLRANGE">
+                    <a:fld id="{8AC5811D-471E-4686-97DA-407DF6136C27}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2004,7 +2007,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7B51B1F8-2F8B-4B09-AB58-EC2B4579DAA0}" type="CELLRANGE">
+                    <a:fld id="{3C23937F-62E7-4934-87DC-F0A70A95CAA6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2038,7 +2041,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB3FBA2A-E245-4FBF-9988-029A35E36707}" type="CELLRANGE">
+                    <a:fld id="{8C5B1E5B-2564-4B8E-99A4-41A3F7A69906}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2072,7 +2075,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B2D45E12-F919-4B19-B393-41F48764B218}" type="CELLRANGE">
+                    <a:fld id="{132B2611-514B-4A10-9623-A75DB545B500}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2106,7 +2109,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED43A707-4820-4536-B2E8-867E28C4F71A}" type="CELLRANGE">
+                    <a:fld id="{8C275C20-F3B1-4D82-A5D9-B07BC41DF5D9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2140,7 +2143,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EBE00B18-1DAF-4040-8E28-959C708C7B9E}" type="CELLRANGE">
+                    <a:fld id="{5890206F-27E2-4B4B-968A-0AAC0FABC952}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2174,7 +2177,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0BD78186-1B91-456E-8DEF-75D0C075A2ED}" type="CELLRANGE">
+                    <a:fld id="{B76C9F7E-2CBB-4B54-856C-5A7A6DFF4320}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2208,7 +2211,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B0C264D3-046B-4347-8508-5E8E1D3DFE28}" type="CELLRANGE">
+                    <a:fld id="{8D587E73-9787-4171-9E08-32AF2B7F6F51}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2242,7 +2245,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AC01B721-D24E-4009-BAE2-1236991BB226}" type="CELLRANGE">
+                    <a:fld id="{B4C5303E-6495-45B3-A9A6-8E18DEB36017}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2276,7 +2279,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10BB482C-996A-4861-88A3-92BED1E302F7}" type="CELLRANGE">
+                    <a:fld id="{6E0DDF21-7B20-4B5B-9295-AF176104547A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2310,7 +2313,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C6E9CB7F-C791-4516-A5AD-252A64761EF2}" type="CELLRANGE">
+                    <a:fld id="{214D57A2-7D9C-405D-BD62-59C6B7A5CD42}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2344,7 +2347,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF75B0D9-2B13-4923-A502-91202F59A874}" type="CELLRANGE">
+                    <a:fld id="{DEA5ABD2-E118-4FBD-8D0E-91BDBF6442B1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2378,7 +2381,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB9B0B5F-A1C6-4864-898F-BB99E8E20C74}" type="CELLRANGE">
+                    <a:fld id="{09AA4B0C-F6E8-4FAE-BB35-FA2B8B97A552}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2412,7 +2415,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B3A77ED0-00BD-4E11-B652-B7CC93D12C44}" type="CELLRANGE">
+                    <a:fld id="{6DFACB24-B62F-4215-BBA3-8A619627E629}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2446,7 +2449,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{905184F4-B8C7-45D5-BCB4-BDCC477E1863}" type="CELLRANGE">
+                    <a:fld id="{5BF684B8-95C7-4508-8D55-AFAFA44B4D0F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2480,7 +2483,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7121A9A4-77B1-4085-87C6-CF36B87FCEA5}" type="CELLRANGE">
+                    <a:fld id="{F768273A-7DE4-4E1C-942E-E668EFBD0A3B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2514,7 +2517,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A8023539-2402-4024-923D-7AB06EBE3170}" type="CELLRANGE">
+                    <a:fld id="{8571EC90-CD8C-48DA-9FC2-5A0BB31EC698}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2548,7 +2551,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{26FB0F57-47C6-4FBD-AD51-B37FA7CFCAED}" type="CELLRANGE">
+                    <a:fld id="{C3EC89F8-CA51-4ECC-A44E-0AB79E6CB501}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2582,7 +2585,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF85DCEC-8891-4F64-8891-CF349FE5CB7F}" type="CELLRANGE">
+                    <a:fld id="{86B5FCF4-692A-473F-99ED-95D354475EEB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2616,7 +2619,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B207B172-615D-4567-8EC6-BD10F3650FC9}" type="CELLRANGE">
+                    <a:fld id="{D0043798-A212-4DE7-9737-A50106097B72}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2650,7 +2653,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33BF6708-2498-49B0-A1B1-C9A57A35C271}" type="CELLRANGE">
+                    <a:fld id="{3C397661-921F-428C-A49C-76C26E901483}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2684,7 +2687,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7BB488D8-2EA1-43D4-8F66-621B7B0CAFFA}" type="CELLRANGE">
+                    <a:fld id="{9915D42A-3DFF-4432-86DF-FEEE29147C59}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2718,7 +2721,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9FC81DE6-A315-40A2-8028-363A8282CD49}" type="CELLRANGE">
+                    <a:fld id="{6D9E43D6-DAB8-4F2D-B0DF-70EBE7BE66B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2752,7 +2755,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B8E7D7A-D0D7-4836-BE5F-99EEE59BE552}" type="CELLRANGE">
+                    <a:fld id="{241C0F82-9DAB-47D7-B4D0-38870AF32D88}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2786,7 +2789,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{30FEBC55-55DB-40F1-A0D1-C420B940F7A2}" type="CELLRANGE">
+                    <a:fld id="{CD9CB89D-1B79-4B97-8F0B-E308E35E89F9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2820,7 +2823,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9DCB2948-569A-43B8-A521-91D52AA251CB}" type="CELLRANGE">
+                    <a:fld id="{58F67181-23E9-4217-A1E0-06CC0AC3C2B3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2854,7 +2857,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B2CB7A5-E3FD-4468-8083-5AB8E1386EEF}" type="CELLRANGE">
+                    <a:fld id="{2CA50B0F-0697-403E-A5F5-8368510A8750}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2888,7 +2891,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A564ACBD-B51B-4724-80E9-F31C70656D11}" type="CELLRANGE">
+                    <a:fld id="{78C7C6DB-9367-4F2D-B64E-8E4AEE64986B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2922,7 +2925,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C2A589C-6295-4059-B9B9-C668621A8C6E}" type="CELLRANGE">
+                    <a:fld id="{DF42453A-016B-4680-8C17-6993B85CEA72}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2946,6 +2949,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-199E-419A-8EE0-80CDE2F856E3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="75"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2018D3B7-B319-4008-BE54-AD474119E73F}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-A7A4-492C-B015-27480EA84DE4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2995,10 +3032,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$76</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="75"/>
+                <c:ptCount val="76"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -3042,7 +3079,7 @@
                   <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.1</c:v>
+                  <c:v>7.7</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>8.75</c:v>
@@ -3114,114 +3151,117 @@
                   <c:v>11.9</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>4.2</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>7.2</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>2.7</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>3.3</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>9.9</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="69">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>5.6</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="73">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="74">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="75">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -3229,10 +3269,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$76</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="75"/>
+                <c:ptCount val="76"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -3348,114 +3388,117 @@
                   <c:v>3160</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>880</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>860</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>1260</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>2600</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>3100</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>1630</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>1930</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>3180</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="69">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="73">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="74">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="75">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -3583,19 +3626,19 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="38">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="39">
+                  <c:pt idx="40">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="40">
+                  <c:pt idx="41">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="41">
+                  <c:pt idx="42">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="42">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="43">
                     <c:v>easy</c:v>
@@ -3604,19 +3647,19 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="45">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="46">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="46">
+                  <c:pt idx="47">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="47">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="48">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="49">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="50">
                     <c:v>moderate</c:v>
@@ -3625,72 +3668,75 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="52">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="53">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="53">
+                  <c:pt idx="54">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="54">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="55">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="56">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="57">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="57">
+                  <c:pt idx="58">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="58">
+                  <c:pt idx="59">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="59">
+                  <c:pt idx="60">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="60">
+                  <c:pt idx="61">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="61">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="62">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="63">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="64">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="64">
+                  <c:pt idx="65">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="65">
+                  <c:pt idx="66">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="66">
+                  <c:pt idx="67">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="67">
+                  <c:pt idx="68">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="68">
+                  <c:pt idx="69">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="69">
+                  <c:pt idx="70">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="70">
+                  <c:pt idx="71">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="71">
+                  <c:pt idx="72">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="72">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="73">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="74">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="75">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -4743,10 +4789,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D76" totalsRowShown="0">
-  <autoFilter ref="A1:D76" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D76">
-    <sortCondition ref="A1:A76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D77" totalsRowShown="0">
+  <autoFilter ref="A1:D77" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D77">
+    <sortCondition ref="A1:A77"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -5047,7 +5093,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5055,10 +5101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5285,7 +5331,7 @@
         <v>39</v>
       </c>
       <c r="B16">
-        <v>7.1</v>
+        <v>7.7</v>
       </c>
       <c r="C16">
         <v>3030</v>
@@ -5626,83 +5672,83 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="B40">
-        <v>11.4</v>
+        <v>3.2</v>
       </c>
       <c r="C40">
-        <v>2550</v>
+        <v>480</v>
       </c>
       <c r="D40" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B41">
-        <v>8.5</v>
+        <v>11.4</v>
       </c>
       <c r="C41">
-        <v>3350</v>
+        <v>2550</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B42">
-        <v>2.8</v>
+        <v>8.5</v>
       </c>
       <c r="C42">
-        <v>880</v>
+        <v>3350</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B43">
-        <v>10.4</v>
+        <v>2.8</v>
       </c>
       <c r="C43">
-        <v>1420</v>
+        <v>880</v>
       </c>
       <c r="D43" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B44">
-        <v>0.9</v>
+        <v>10.4</v>
       </c>
       <c r="C44">
-        <v>200</v>
+        <v>1420</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B45">
-        <v>4.2</v>
+        <v>0.9</v>
       </c>
       <c r="C45">
-        <v>860</v>
+        <v>200</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
@@ -5710,13 +5756,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B46">
-        <v>4.8</v>
+        <v>4.2</v>
       </c>
       <c r="C46">
-        <v>1260</v>
+        <v>860</v>
       </c>
       <c r="D46" t="s">
         <v>7</v>
@@ -5724,55 +5770,55 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>4.8</v>
       </c>
       <c r="C47">
-        <v>2600</v>
+        <v>1260</v>
       </c>
       <c r="D47" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B48">
-        <v>1.4</v>
+        <v>4</v>
       </c>
       <c r="C48">
-        <v>375</v>
+        <v>2600</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B49">
-        <v>13.6</v>
+        <v>1.4</v>
       </c>
       <c r="C49">
-        <v>3930</v>
+        <v>375</v>
       </c>
       <c r="D49" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B50">
-        <v>10.5</v>
+        <v>13.6</v>
       </c>
       <c r="C50">
-        <v>3100</v>
+        <v>3930</v>
       </c>
       <c r="D50" t="s">
         <v>10</v>
@@ -5780,27 +5826,27 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B51">
-        <v>7</v>
+        <v>10.5</v>
       </c>
       <c r="C51">
-        <v>1670</v>
+        <v>3100</v>
       </c>
       <c r="D51" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B52">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="C52">
-        <v>2400</v>
+        <v>1670</v>
       </c>
       <c r="D52" t="s">
         <v>1</v>
@@ -5808,13 +5854,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B53">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C53">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D53" t="s">
         <v>1</v>
@@ -5822,55 +5868,55 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B54">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C54">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B55">
-        <v>7.2</v>
+        <v>4.8</v>
       </c>
       <c r="C55">
-        <v>1630</v>
+        <v>1300</v>
       </c>
       <c r="D55" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B56">
-        <v>2.7</v>
+        <v>7.2</v>
       </c>
       <c r="C56">
-        <v>1090</v>
+        <v>1630</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="B57">
-        <v>4.8</v>
+        <v>2.7</v>
       </c>
       <c r="C57">
-        <v>1470</v>
+        <v>1090</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -5878,97 +5924,97 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B58">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C58">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D58" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B59">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C59">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D59" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B60">
-        <v>3.3</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C60">
-        <v>600</v>
+        <v>3490</v>
       </c>
       <c r="D60" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B61">
-        <v>8.5</v>
+        <v>3.3</v>
       </c>
       <c r="C61">
-        <v>1930</v>
+        <v>600</v>
       </c>
       <c r="D61" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B62">
-        <v>2.2000000000000002</v>
+        <v>8.5</v>
       </c>
       <c r="C62">
-        <v>750</v>
+        <v>1930</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B63">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C63">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D63" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B64">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C64">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D64" t="s">
         <v>1</v>
@@ -5976,172 +6022,186 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65">
+        <v>7.3</v>
+      </c>
+      <c r="C65">
+        <v>2250</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>25</v>
       </c>
-      <c r="B65">
+      <c r="B66">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C65">
+      <c r="C66">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D66" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>49</v>
-      </c>
-      <c r="B66">
-        <v>1.2</v>
-      </c>
-      <c r="C66">
-        <v>500</v>
-      </c>
-      <c r="D66" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B67">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C67">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D67" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B68">
-        <v>6.5</v>
+        <v>11</v>
       </c>
       <c r="C68">
-        <v>1650</v>
+        <v>3060</v>
       </c>
       <c r="D68" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B69">
-        <v>9.9</v>
+        <v>6.5</v>
       </c>
       <c r="C69">
-        <v>3180</v>
+        <v>1650</v>
       </c>
       <c r="D69" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="B70">
-        <v>6.2</v>
+        <v>9.9</v>
       </c>
       <c r="C70">
-        <v>1890</v>
+        <v>3180</v>
       </c>
       <c r="D70" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B71">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C71">
-        <v>100</v>
+        <v>1890</v>
       </c>
       <c r="D71" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B72">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C72">
-        <v>3550</v>
+        <v>100</v>
       </c>
       <c r="D72" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="B73">
-        <v>5.6</v>
+        <v>7.3</v>
       </c>
       <c r="C73">
-        <v>1680</v>
+        <v>3550</v>
       </c>
       <c r="D73" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B74">
-        <v>10.8</v>
+        <v>5.6</v>
       </c>
       <c r="C74">
-        <v>1800</v>
+        <v>1680</v>
       </c>
       <c r="D74" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
+        <v>63</v>
+      </c>
+      <c r="B75">
+        <v>10.8</v>
+      </c>
+      <c r="C75">
+        <v>1800</v>
+      </c>
+      <c r="D75" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>55</v>
       </c>
-      <c r="B75">
+      <c r="B76">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C75">
+      <c r="C76">
         <v>3800</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>29</v>
       </c>
-      <c r="B76">
+      <c r="B77">
         <v>6</v>
       </c>
-      <c r="C76">
+      <c r="C77">
         <v>2180</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D77" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Longmire Stewardship Campground entry
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065DD3DF-D716-46C6-83E7-24FDAFF8C69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99AA2D4-15E5-4BB3-9D40-9C99800C5FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -409,7 +409,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0B39BE0-ECDE-4BE9-B07F-71CB2CCB66A0}" type="CELLRANGE">
+                    <a:fld id="{574AD897-9721-4E28-BF6D-1D0B7348359E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -443,7 +443,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10AF186E-38F1-4B0B-A3D2-88ACA2327DE5}" type="CELLRANGE">
+                    <a:fld id="{9B869C78-8C33-4FDF-8FCA-1326129BD97C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -477,7 +477,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A66206BF-3CD3-485B-BA3D-03DB9C2DFE05}" type="CELLRANGE">
+                    <a:fld id="{D65AD28A-92F9-421B-BCCA-745C1E2667F0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -511,7 +511,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C8D8B6DD-A46C-4B42-A595-04870F3753FE}" type="CELLRANGE">
+                    <a:fld id="{E028DA7B-1F60-473B-B0AF-01842D349027}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -545,7 +545,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{630A8632-EA72-448F-AB47-FF39C5FB3052}" type="CELLRANGE">
+                    <a:fld id="{4A818CC4-ECC6-406F-B6FF-EC85A06386C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -579,7 +579,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0577AF11-C3F8-4BE7-A19F-E9BF09879DC4}" type="CELLRANGE">
+                    <a:fld id="{1FE68A35-B568-4B52-AECC-3C18D030EFDC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -613,7 +613,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{862D23BB-483C-479E-A063-AB5A7EF12594}" type="CELLRANGE">
+                    <a:fld id="{2477BDF3-4102-43A0-AC04-7BB631015502}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -647,7 +647,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EEEE213B-15CC-4FD1-87A8-AD23637EA1A7}" type="CELLRANGE">
+                    <a:fld id="{7EC6F5C9-4CA7-4DBB-914A-77BF16E7CDB5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -681,7 +681,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69870C59-A777-4076-9211-6CB5A7B4B4BC}" type="CELLRANGE">
+                    <a:fld id="{25FA6729-BEE3-4C8A-9FC6-C927315D8101}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -715,7 +715,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{45FE33B7-F1CE-4BEB-BCB5-61951B772A11}" type="CELLRANGE">
+                    <a:fld id="{C735A1D1-4C52-48D5-9E28-D8AA53987CDA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -749,7 +749,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E5417CB-4E6F-49ED-9D5B-CD004635E4C3}" type="CELLRANGE">
+                    <a:fld id="{D83C4F9E-76C2-4B79-B0D2-E46BF4FB09B4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -783,7 +783,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F01BD3B-4DC6-4C92-B7AF-68C9889932FA}" type="CELLRANGE">
+                    <a:fld id="{08199FDA-883F-4319-85D0-472EC95D5E32}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -817,7 +817,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D801A403-477A-4B14-9DA3-A128476F0329}" type="CELLRANGE">
+                    <a:fld id="{0881AB46-9191-44BA-97A8-29692E934F4A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -851,7 +851,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E30EB25-EA22-472D-B185-9767ABC3E82E}" type="CELLRANGE">
+                    <a:fld id="{233F6F6B-FDC1-4BEA-AA2F-46137E642A2E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -885,7 +885,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{509B6979-B58C-464C-8BC7-1BF455E7D6E9}" type="CELLRANGE">
+                    <a:fld id="{2A9365D1-B733-4A10-A1EF-377A9DDE7353}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -919,7 +919,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34703DB1-7E36-4508-BD0F-126D799B60E3}" type="CELLRANGE">
+                    <a:fld id="{341D3316-1C7E-4CC8-AC9D-751345112A83}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -953,7 +953,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{351DCD96-1828-4F59-8A54-2426DF94F025}" type="CELLRANGE">
+                    <a:fld id="{475959E0-C002-48F3-9150-0FC01677C1E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -987,7 +987,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC8BA4BE-8401-4FCB-8BA6-893F542A1A02}" type="CELLRANGE">
+                    <a:fld id="{9E9E8766-EFE4-4190-B2FC-BC2C049DDCD5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1021,7 +1021,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B70369B8-B0DA-4565-9171-869FE29B1679}" type="CELLRANGE">
+                    <a:fld id="{9DB52F8A-E7B3-4916-823D-1ACFF74CDF10}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1055,7 +1055,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B7DEE7C9-158F-4AD4-9125-BCA83F2301D4}" type="CELLRANGE">
+                    <a:fld id="{264E2ED6-15C2-4F7A-84A7-1F3E40B2CEA1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1089,7 +1089,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B197A628-7407-4A1E-B20A-67AD13672913}" type="CELLRANGE">
+                    <a:fld id="{7FF3C542-3981-42B6-833A-D8D6824259F2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1123,7 +1123,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A597A935-A679-465D-BA36-CE3C7BBCD2E5}" type="CELLRANGE">
+                    <a:fld id="{FADC7FAF-1DAD-49A3-AF05-2F9125F67776}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1157,7 +1157,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6BE2731F-DA97-4AFF-967A-18B59E071E94}" type="CELLRANGE">
+                    <a:fld id="{C9E74C95-5AE5-49A4-B4AA-09CED571916F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1191,7 +1191,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{876ACD0C-C3DC-43E9-A11F-DC1F831C88F1}" type="CELLRANGE">
+                    <a:fld id="{2EE2683B-64CC-4BD9-B4F7-2A5669367A0C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1225,7 +1225,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C6651F9F-ADA2-4D70-BAEB-5A9FB40958DB}" type="CELLRANGE">
+                    <a:fld id="{8DF4E70E-CB4C-4B4E-AE10-92EF3DE46A18}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1259,7 +1259,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63403692-3C4A-481C-84D2-E7A42566F5F8}" type="CELLRANGE">
+                    <a:fld id="{50B37D65-8A33-4718-9566-B84AEAEE649B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1293,7 +1293,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB075985-BA28-4B8E-9FDB-29F924FC975B}" type="CELLRANGE">
+                    <a:fld id="{48D68E4A-D4E7-4A78-98B2-43ECEB8E4E3D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1327,7 +1327,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6F15B6EE-8CB4-40A5-AB4A-723DAB098B8F}" type="CELLRANGE">
+                    <a:fld id="{75210513-DE6F-470C-B411-64FC96ECF989}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1361,7 +1361,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{22BD07BF-C3E9-4806-B6FB-B5810C725B2E}" type="CELLRANGE">
+                    <a:fld id="{9748852A-3226-456E-96BB-21A16A678785}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1395,7 +1395,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B43BF7C7-0CA6-4BFE-A84B-59AB3EAEC0DE}" type="CELLRANGE">
+                    <a:fld id="{89A12400-B4E2-4B61-93F2-14107F0049FA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1429,7 +1429,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8365A81-D22B-4151-A6EE-F20F6800810C}" type="CELLRANGE">
+                    <a:fld id="{CAC8493B-7E34-4555-A0A4-4395A8B426B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1463,7 +1463,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2775CB39-45D3-476B-975C-B3DEE57449B6}" type="CELLRANGE">
+                    <a:fld id="{EF6EB633-FA16-4D65-BDFF-061635B7507D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1497,7 +1497,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C9EB857B-1ABB-4B60-B7F8-4A5E45DECD2A}" type="CELLRANGE">
+                    <a:fld id="{5B0B0D14-11F5-43E9-80AB-2366195F0C21}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1531,7 +1531,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{68FE1545-E440-45CF-9158-CD86C8A04A8D}" type="CELLRANGE">
+                    <a:fld id="{4F595586-FE86-4631-955F-067ED4AE8C75}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1565,7 +1565,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B859A590-F4F6-4802-8C0D-5D581F9015B2}" type="CELLRANGE">
+                    <a:fld id="{20584335-C8FF-4904-B37F-3551AE305840}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1599,7 +1599,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3BC389D1-9591-453C-BD5A-5476A8E06F42}" type="CELLRANGE">
+                    <a:fld id="{6E731BF3-C126-456D-AD08-88A8A521657A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1633,7 +1633,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{900A479A-ED84-4A28-AC46-FBAF7ED71B37}" type="CELLRANGE">
+                    <a:fld id="{68FF4A4C-5488-43F1-AE3D-CAEE45AC27A3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1667,7 +1667,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{90D20C92-F0A6-47F5-B45F-0D8B5A29C5F9}" type="CELLRANGE">
+                    <a:fld id="{8C9B9EB5-475C-4EF5-B8CA-0503577C54DD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1701,7 +1701,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F089E5F-7A7B-494D-A451-E222727284A8}" type="CELLRANGE">
+                    <a:fld id="{48871C08-4C4F-47E5-A979-1537B246114E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1735,7 +1735,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10109EB2-7288-4E7E-9CFD-FFB621C20F8C}" type="CELLRANGE">
+                    <a:fld id="{9E9BEC51-B502-4FCC-A841-F4BEF55185A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1769,7 +1769,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D23AE8AB-0984-4268-9743-89927E663E7B}" type="CELLRANGE">
+                    <a:fld id="{BD187967-073E-4C6D-8D17-9A0368D53FF6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1803,7 +1803,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E2D2BBC-14CB-4A04-BC79-EF9E72D48EF8}" type="CELLRANGE">
+                    <a:fld id="{BF0945DC-1275-448D-A73D-E0D5A1A02E9F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1837,7 +1837,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AB03046A-A85B-4750-9271-5FDA086491CE}" type="CELLRANGE">
+                    <a:fld id="{4639F51D-960E-4904-AA05-D2F186D54684}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1871,7 +1871,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DDEE1C3A-1E1C-482E-8C98-D0F11E81C6E4}" type="CELLRANGE">
+                    <a:fld id="{BEDEBF1D-BEDE-434D-A145-1F14DEDC04A2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1905,7 +1905,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{04336D28-21F5-433E-9461-916D83E02636}" type="CELLRANGE">
+                    <a:fld id="{59FEFAD3-0565-4A54-AEC7-7EBFED369BBF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1939,7 +1939,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{874E2EA2-87F7-4905-90E2-34B4AA9DC20B}" type="CELLRANGE">
+                    <a:fld id="{D46EC7B2-C018-421D-8C75-0298486A0CAD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1973,7 +1973,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8AC5811D-471E-4686-97DA-407DF6136C27}" type="CELLRANGE">
+                    <a:fld id="{9A6A2EAE-BC20-4739-B6FD-88B553BFE812}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2007,7 +2007,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C23937F-62E7-4934-87DC-F0A70A95CAA6}" type="CELLRANGE">
+                    <a:fld id="{E92F59BF-E103-40C4-BF2D-B963712275AB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2041,7 +2041,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C5B1E5B-2564-4B8E-99A4-41A3F7A69906}" type="CELLRANGE">
+                    <a:fld id="{E71761A6-F20E-4053-96C1-33D02F745EF7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2075,7 +2075,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{132B2611-514B-4A10-9623-A75DB545B500}" type="CELLRANGE">
+                    <a:fld id="{3FABEEC9-B886-4966-BB3E-EDAC2A720D82}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2109,7 +2109,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C275C20-F3B1-4D82-A5D9-B07BC41DF5D9}" type="CELLRANGE">
+                    <a:fld id="{02953A8D-2384-4B08-A9D4-30E0FCBD9405}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2143,7 +2143,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5890206F-27E2-4B4B-968A-0AAC0FABC952}" type="CELLRANGE">
+                    <a:fld id="{0A5AE0A7-4D6B-446A-8275-E3C4798D2C8A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2177,7 +2177,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B76C9F7E-2CBB-4B54-856C-5A7A6DFF4320}" type="CELLRANGE">
+                    <a:fld id="{E6567EB1-0668-42F6-AAFB-BC4E4604AAD5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2211,7 +2211,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8D587E73-9787-4171-9E08-32AF2B7F6F51}" type="CELLRANGE">
+                    <a:fld id="{58B38892-B573-4681-AA1C-E4D018AA0481}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2245,7 +2245,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B4C5303E-6495-45B3-A9A6-8E18DEB36017}" type="CELLRANGE">
+                    <a:fld id="{321E76E3-B6C0-4FD8-95F1-E33844E78D12}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2279,7 +2279,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E0DDF21-7B20-4B5B-9295-AF176104547A}" type="CELLRANGE">
+                    <a:fld id="{67A42C59-F685-4A1F-BBBF-2A16DFA48E68}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2313,7 +2313,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{214D57A2-7D9C-405D-BD62-59C6B7A5CD42}" type="CELLRANGE">
+                    <a:fld id="{3D0B11C3-762E-4D6C-ADEA-05039567275E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2347,7 +2347,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DEA5ABD2-E118-4FBD-8D0E-91BDBF6442B1}" type="CELLRANGE">
+                    <a:fld id="{47A01107-FD58-48D2-8B1B-DAD3E693E45E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2381,7 +2381,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{09AA4B0C-F6E8-4FAE-BB35-FA2B8B97A552}" type="CELLRANGE">
+                    <a:fld id="{44667548-E4B2-464C-ACB1-0640F1D7743A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2415,7 +2415,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6DFACB24-B62F-4215-BBA3-8A619627E629}" type="CELLRANGE">
+                    <a:fld id="{3131095F-01B4-4123-835A-23D3B22943E2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2449,7 +2449,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5BF684B8-95C7-4508-8D55-AFAFA44B4D0F}" type="CELLRANGE">
+                    <a:fld id="{1C1CC1A1-C86D-4B8F-9BA3-520E8885ED9A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2483,7 +2483,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F768273A-7DE4-4E1C-942E-E668EFBD0A3B}" type="CELLRANGE">
+                    <a:fld id="{15E231F0-5746-4AC6-AA46-6232BCCA105F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2517,7 +2517,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8571EC90-CD8C-48DA-9FC2-5A0BB31EC698}" type="CELLRANGE">
+                    <a:fld id="{E6EE92CA-C4B5-419F-8A3C-29AD519B3D47}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2551,7 +2551,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3EC89F8-CA51-4ECC-A44E-0AB79E6CB501}" type="CELLRANGE">
+                    <a:fld id="{79BF7073-FC9F-4EEC-9FF4-598B94069CEE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2585,7 +2585,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{86B5FCF4-692A-473F-99ED-95D354475EEB}" type="CELLRANGE">
+                    <a:fld id="{1A4F7AF5-EFFB-4CB5-9E96-7D3B2A6CD594}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2619,7 +2619,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D0043798-A212-4DE7-9737-A50106097B72}" type="CELLRANGE">
+                    <a:fld id="{C222584B-DA7F-47A9-A1AB-417AAAA9CEF4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2653,7 +2653,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C397661-921F-428C-A49C-76C26E901483}" type="CELLRANGE">
+                    <a:fld id="{E21E6C2E-1ABA-474F-BDB7-5212B8D2C346}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2687,7 +2687,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9915D42A-3DFF-4432-86DF-FEEE29147C59}" type="CELLRANGE">
+                    <a:fld id="{10AFFF96-3A3B-4E2C-B1D6-F4842FE7EE6A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2721,7 +2721,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D9E43D6-DAB8-4F2D-B0DF-70EBE7BE66B2}" type="CELLRANGE">
+                    <a:fld id="{FFCB07D1-629A-447C-98B1-48CF57BE0D47}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2755,7 +2755,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{241C0F82-9DAB-47D7-B4D0-38870AF32D88}" type="CELLRANGE">
+                    <a:fld id="{5E04B08B-3857-4C98-ADEB-E5E585D753CC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2789,7 +2789,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD9CB89D-1B79-4B97-8F0B-E308E35E89F9}" type="CELLRANGE">
+                    <a:fld id="{F66E8082-A377-4C0E-8285-AD120FBBF9A9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2823,7 +2823,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58F67181-23E9-4217-A1E0-06CC0AC3C2B3}" type="CELLRANGE">
+                    <a:fld id="{85D6293B-419F-4AAA-84C2-55358B9BFF4C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2857,7 +2857,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2CA50B0F-0697-403E-A5F5-8368510A8750}" type="CELLRANGE">
+                    <a:fld id="{8D6CFA94-061D-4D8F-8E71-BB3901B76062}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2891,7 +2891,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{78C7C6DB-9367-4F2D-B64E-8E4AEE64986B}" type="CELLRANGE">
+                    <a:fld id="{3DFF108F-33A8-4D90-A489-9BE36E4B99B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2925,7 +2925,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF42453A-016B-4680-8C17-6993B85CEA72}" type="CELLRANGE">
+                    <a:fld id="{EDA70C8E-E114-476F-9C43-BFC51A09EC44}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2959,7 +2959,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2018D3B7-B319-4008-BE54-AD474119E73F}" type="CELLRANGE">
+                    <a:fld id="{50486487-CA9C-4BA8-88B9-A3AB01907DC2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3151,7 +3151,7 @@
                   <c:v>11.9</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>11.4</c:v>
@@ -3388,7 +3388,7 @@
                   <c:v>3160</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>480</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>2550</c:v>
@@ -5093,7 +5093,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5103,8 +5103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5675,10 +5675,10 @@
         <v>85</v>
       </c>
       <c r="B40">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C40">
-        <v>480</v>
+        <v>400</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Add Westside Road (snowshoe) entry
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99AA2D4-15E5-4BB3-9D40-9C99800C5FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87D9BF8-B490-425E-A5E8-5CBADDA5F377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hike Difficulties" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>Longmire Stewardship Campground</t>
+  </si>
+  <si>
+    <t>Westside Road (snowshoe)</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{574AD897-9721-4E28-BF6D-1D0B7348359E}" type="CELLRANGE">
+                    <a:fld id="{F60D7BA2-81C4-40C1-90B3-E599E4167F64}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -443,7 +446,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B869C78-8C33-4FDF-8FCA-1326129BD97C}" type="CELLRANGE">
+                    <a:fld id="{57FC46E7-6D73-4E60-A5EF-6ACBB76097D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -477,7 +480,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D65AD28A-92F9-421B-BCCA-745C1E2667F0}" type="CELLRANGE">
+                    <a:fld id="{B92A5064-86A4-48BB-A762-5A250AD941EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -511,7 +514,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E028DA7B-1F60-473B-B0AF-01842D349027}" type="CELLRANGE">
+                    <a:fld id="{34F1C034-8F8E-43C8-A7A4-B211898FBD86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -545,7 +548,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4A818CC4-ECC6-406F-B6FF-EC85A06386C5}" type="CELLRANGE">
+                    <a:fld id="{5DAFBE51-1CB6-42D6-BB17-722F36D2BF74}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -579,7 +582,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1FE68A35-B568-4B52-AECC-3C18D030EFDC}" type="CELLRANGE">
+                    <a:fld id="{BA7ABCB3-D9BC-400C-8900-47DAE850ECF3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -613,7 +616,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2477BDF3-4102-43A0-AC04-7BB631015502}" type="CELLRANGE">
+                    <a:fld id="{33CBF2B7-AB24-4628-84EC-1C5BFF3760FE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -647,7 +650,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7EC6F5C9-4CA7-4DBB-914A-77BF16E7CDB5}" type="CELLRANGE">
+                    <a:fld id="{2CCBDB26-EBE1-43B4-9A7A-AFFDFEADC62F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -681,7 +684,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{25FA6729-BEE3-4C8A-9FC6-C927315D8101}" type="CELLRANGE">
+                    <a:fld id="{C5739ED0-7267-4E05-95F6-436112A5AD2F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -715,7 +718,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C735A1D1-4C52-48D5-9E28-D8AA53987CDA}" type="CELLRANGE">
+                    <a:fld id="{EC13F501-89F5-4F62-93C3-84AC6D8EB006}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -749,7 +752,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D83C4F9E-76C2-4B79-B0D2-E46BF4FB09B4}" type="CELLRANGE">
+                    <a:fld id="{D579655A-49C4-43FC-8258-031CAA07BE31}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -783,7 +786,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{08199FDA-883F-4319-85D0-472EC95D5E32}" type="CELLRANGE">
+                    <a:fld id="{233E890F-7677-4B5D-8280-10AB5700D069}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -817,7 +820,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0881AB46-9191-44BA-97A8-29692E934F4A}" type="CELLRANGE">
+                    <a:fld id="{B66591E0-66CE-498D-BD83-BD8BF78C6D56}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -851,7 +854,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{233F6F6B-FDC1-4BEA-AA2F-46137E642A2E}" type="CELLRANGE">
+                    <a:fld id="{B540F2EE-98EB-42BC-8230-CD3F37B4D66E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -885,7 +888,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A9365D1-B733-4A10-A1EF-377A9DDE7353}" type="CELLRANGE">
+                    <a:fld id="{625E5596-149F-4F21-8EA6-3F5274DAFD70}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -919,7 +922,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{341D3316-1C7E-4CC8-AC9D-751345112A83}" type="CELLRANGE">
+                    <a:fld id="{FA15071E-38CC-4D99-9DC5-F83A8FB9EF51}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -953,7 +956,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{475959E0-C002-48F3-9150-0FC01677C1E4}" type="CELLRANGE">
+                    <a:fld id="{DF2BD05B-CD9D-4D22-9429-F6172CD93FCD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -987,7 +990,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E9E8766-EFE4-4190-B2FC-BC2C049DDCD5}" type="CELLRANGE">
+                    <a:fld id="{0D442E35-BAAF-4E30-946C-55B40B7E8353}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1021,7 +1024,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9DB52F8A-E7B3-4916-823D-1ACFF74CDF10}" type="CELLRANGE">
+                    <a:fld id="{0BB3CDE5-C620-4650-B583-E19484263780}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1055,7 +1058,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{264E2ED6-15C2-4F7A-84A7-1F3E40B2CEA1}" type="CELLRANGE">
+                    <a:fld id="{C03F0143-6794-476E-9817-636F4E944E79}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1089,7 +1092,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7FF3C542-3981-42B6-833A-D8D6824259F2}" type="CELLRANGE">
+                    <a:fld id="{1B604173-B7B7-4FB1-8D51-2ED8CB17DFA7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1123,7 +1126,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FADC7FAF-1DAD-49A3-AF05-2F9125F67776}" type="CELLRANGE">
+                    <a:fld id="{2939A4C3-58E4-4D68-9FAC-06C0E800255E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1157,7 +1160,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C9E74C95-5AE5-49A4-B4AA-09CED571916F}" type="CELLRANGE">
+                    <a:fld id="{A6AC2BED-0EDE-4B2F-B2D8-D4DD4C39DAF4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1191,7 +1194,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2EE2683B-64CC-4BD9-B4F7-2A5669367A0C}" type="CELLRANGE">
+                    <a:fld id="{7FF0E7F3-9FC8-4179-B60D-0E78857F54B7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1225,7 +1228,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8DF4E70E-CB4C-4B4E-AE10-92EF3DE46A18}" type="CELLRANGE">
+                    <a:fld id="{F07ADA38-D1F1-4D40-861E-D77540D07177}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1259,7 +1262,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{50B37D65-8A33-4718-9566-B84AEAEE649B}" type="CELLRANGE">
+                    <a:fld id="{FBDD9E1E-A5B4-43DB-8FE9-74AE2F3EBF74}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1293,7 +1296,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48D68E4A-D4E7-4A78-98B2-43ECEB8E4E3D}" type="CELLRANGE">
+                    <a:fld id="{F3FA4706-506C-44E1-9810-99924E9261EF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1327,7 +1330,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75210513-DE6F-470C-B411-64FC96ECF989}" type="CELLRANGE">
+                    <a:fld id="{F5C3A46D-32BC-40F4-B75D-02053F0B24C8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1361,7 +1364,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9748852A-3226-456E-96BB-21A16A678785}" type="CELLRANGE">
+                    <a:fld id="{C7CBC06C-24D0-483F-9EC0-A76593B9DCDA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1395,7 +1398,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{89A12400-B4E2-4B61-93F2-14107F0049FA}" type="CELLRANGE">
+                    <a:fld id="{F41E3614-976D-4590-9BE8-B3E7BAF56401}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1429,7 +1432,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CAC8493B-7E34-4555-A0A4-4395A8B426B2}" type="CELLRANGE">
+                    <a:fld id="{A2973834-3BA7-4784-A93B-06529E6AE679}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1463,7 +1466,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EF6EB633-FA16-4D65-BDFF-061635B7507D}" type="CELLRANGE">
+                    <a:fld id="{90D99530-F828-46BE-B722-15E5C8B0CC5D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1497,7 +1500,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B0B0D14-11F5-43E9-80AB-2366195F0C21}" type="CELLRANGE">
+                    <a:fld id="{9E2E8081-B3F4-4690-957B-B475DD27A055}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1531,7 +1534,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F595586-FE86-4631-955F-067ED4AE8C75}" type="CELLRANGE">
+                    <a:fld id="{84138DFF-04CB-4CFB-BE43-C13081BBFD85}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1565,7 +1568,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{20584335-C8FF-4904-B37F-3551AE305840}" type="CELLRANGE">
+                    <a:fld id="{4EC405B2-A99A-4EFA-8908-1C29E201EDE1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1599,7 +1602,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E731BF3-C126-456D-AD08-88A8A521657A}" type="CELLRANGE">
+                    <a:fld id="{448BF695-7383-4C87-A9FA-6E9ED4F96AEC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1633,7 +1636,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{68FF4A4C-5488-43F1-AE3D-CAEE45AC27A3}" type="CELLRANGE">
+                    <a:fld id="{CE6540EB-D422-412C-8778-54CC47B30E39}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1667,7 +1670,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C9B9EB5-475C-4EF5-B8CA-0503577C54DD}" type="CELLRANGE">
+                    <a:fld id="{ECDD77BC-B19B-419F-A9A4-AAEB254668FD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1701,7 +1704,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48871C08-4C4F-47E5-A979-1537B246114E}" type="CELLRANGE">
+                    <a:fld id="{4855E166-350F-4BED-B1D1-65BA8C15D9EA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1735,7 +1738,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E9BEC51-B502-4FCC-A841-F4BEF55185A7}" type="CELLRANGE">
+                    <a:fld id="{1E17CC4D-3026-4AAE-8737-F0ED4DBFAA67}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1769,7 +1772,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BD187967-073E-4C6D-8D17-9A0368D53FF6}" type="CELLRANGE">
+                    <a:fld id="{983764FF-60BC-4D3C-BDF1-E265F1F2EDEB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1803,7 +1806,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BF0945DC-1275-448D-A73D-E0D5A1A02E9F}" type="CELLRANGE">
+                    <a:fld id="{5018417D-801C-4ACE-AB6C-F0DDEB7D00EF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1837,7 +1840,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4639F51D-960E-4904-AA05-D2F186D54684}" type="CELLRANGE">
+                    <a:fld id="{8F8384E9-F0E9-4121-88C5-517EA29CF074}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1871,7 +1874,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BEDEBF1D-BEDE-434D-A145-1F14DEDC04A2}" type="CELLRANGE">
+                    <a:fld id="{123212AB-B021-4342-B45A-D73C9244C3EF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1905,7 +1908,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{59FEFAD3-0565-4A54-AEC7-7EBFED369BBF}" type="CELLRANGE">
+                    <a:fld id="{2F75AF93-78FE-42C0-8C83-6DA04ED7771D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1939,7 +1942,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D46EC7B2-C018-421D-8C75-0298486A0CAD}" type="CELLRANGE">
+                    <a:fld id="{C7918706-DCED-418E-A87A-2DCD32C8E196}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1973,7 +1976,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9A6A2EAE-BC20-4739-B6FD-88B553BFE812}" type="CELLRANGE">
+                    <a:fld id="{1FDD32DC-D78F-4C41-AEB9-65D009CD04F7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2007,7 +2010,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E92F59BF-E103-40C4-BF2D-B963712275AB}" type="CELLRANGE">
+                    <a:fld id="{2FF1E7A0-5447-4DC3-AC26-D14E334D81A5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2041,7 +2044,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E71761A6-F20E-4053-96C1-33D02F745EF7}" type="CELLRANGE">
+                    <a:fld id="{517E7271-7886-47A6-BE29-D9C32264331D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2075,7 +2078,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3FABEEC9-B886-4966-BB3E-EDAC2A720D82}" type="CELLRANGE">
+                    <a:fld id="{282262F3-648C-43A8-8BFB-DD32A3BF6147}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2109,7 +2112,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02953A8D-2384-4B08-A9D4-30E0FCBD9405}" type="CELLRANGE">
+                    <a:fld id="{0C378BE7-1D44-4172-95DA-31FFF58D0A08}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2143,7 +2146,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A5AE0A7-4D6B-446A-8275-E3C4798D2C8A}" type="CELLRANGE">
+                    <a:fld id="{33E7BB05-755C-4673-968E-93707DB1C2A9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2177,7 +2180,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E6567EB1-0668-42F6-AAFB-BC4E4604AAD5}" type="CELLRANGE">
+                    <a:fld id="{911FF864-8979-4510-9153-4DAE4F0802F7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2211,7 +2214,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58B38892-B573-4681-AA1C-E4D018AA0481}" type="CELLRANGE">
+                    <a:fld id="{DB51A25A-1D32-4104-ABE8-371F70A709E1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2245,7 +2248,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{321E76E3-B6C0-4FD8-95F1-E33844E78D12}" type="CELLRANGE">
+                    <a:fld id="{F3C6894C-388F-4A73-9077-B85C1EA7C92D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2279,7 +2282,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67A42C59-F685-4A1F-BBBF-2A16DFA48E68}" type="CELLRANGE">
+                    <a:fld id="{4E338512-3377-4E6A-8243-3B38DB027E73}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2313,7 +2316,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D0B11C3-762E-4D6C-ADEA-05039567275E}" type="CELLRANGE">
+                    <a:fld id="{2C8D74C6-CE08-4401-B6A4-4D7F589DF668}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2347,7 +2350,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47A01107-FD58-48D2-8B1B-DAD3E693E45E}" type="CELLRANGE">
+                    <a:fld id="{BA60A685-1F0A-4028-AEB3-54677B020053}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2381,7 +2384,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{44667548-E4B2-464C-ACB1-0640F1D7743A}" type="CELLRANGE">
+                    <a:fld id="{84DC49CF-FE56-4CA5-B8FD-5EE2BAC41A76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2415,7 +2418,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3131095F-01B4-4123-835A-23D3B22943E2}" type="CELLRANGE">
+                    <a:fld id="{40DF9DBE-979A-4EFA-9D7F-B241024662E0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2449,7 +2452,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C1CC1A1-C86D-4B8F-9BA3-520E8885ED9A}" type="CELLRANGE">
+                    <a:fld id="{9E06F182-2D1F-47E9-A23F-C3813F1E362A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2483,7 +2486,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{15E231F0-5746-4AC6-AA46-6232BCCA105F}" type="CELLRANGE">
+                    <a:fld id="{E0CA1841-5B5D-4924-8444-376D20EC2A59}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2517,7 +2520,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E6EE92CA-C4B5-419F-8A3C-29AD519B3D47}" type="CELLRANGE">
+                    <a:fld id="{C7BF25E5-6421-4DB7-B1A3-28731EE442F2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2551,7 +2554,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79BF7073-FC9F-4EEC-9FF4-598B94069CEE}" type="CELLRANGE">
+                    <a:fld id="{639D5E5D-9D60-4748-8FAC-78196D6F328F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2585,7 +2588,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A4F7AF5-EFFB-4CB5-9E96-7D3B2A6CD594}" type="CELLRANGE">
+                    <a:fld id="{FAA3DD3E-FFF7-4F43-ACA3-EDAE16E001C6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2619,7 +2622,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C222584B-DA7F-47A9-A1AB-417AAAA9CEF4}" type="CELLRANGE">
+                    <a:fld id="{334B32FE-C6E8-46CE-9DD0-FD02BE8D78C1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2653,7 +2656,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E21E6C2E-1ABA-474F-BDB7-5212B8D2C346}" type="CELLRANGE">
+                    <a:fld id="{56F0BE03-DF17-4465-896A-E295DFDFB152}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2687,7 +2690,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10AFFF96-3A3B-4E2C-B1D6-F4842FE7EE6A}" type="CELLRANGE">
+                    <a:fld id="{87CF154F-7417-4E78-96B0-164BB63EFE66}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2721,7 +2724,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FFCB07D1-629A-447C-98B1-48CF57BE0D47}" type="CELLRANGE">
+                    <a:fld id="{156AB8EB-C638-4744-BB67-0C47F256B9A5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2755,7 +2758,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5E04B08B-3857-4C98-ADEB-E5E585D753CC}" type="CELLRANGE">
+                    <a:fld id="{5DAAA7D3-A8DF-4A36-87EA-EC93675ADE3C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2789,7 +2792,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F66E8082-A377-4C0E-8285-AD120FBBF9A9}" type="CELLRANGE">
+                    <a:fld id="{5A30AF67-658D-45DA-9658-5E02978773C4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2823,7 +2826,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{85D6293B-419F-4AAA-84C2-55358B9BFF4C}" type="CELLRANGE">
+                    <a:fld id="{E61FA588-4B13-4766-87C0-8EF57CB31714}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2857,7 +2860,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8D6CFA94-061D-4D8F-8E71-BB3901B76062}" type="CELLRANGE">
+                    <a:fld id="{F6741195-A1F8-4B4E-ABEC-2A03E4D173CF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2891,7 +2894,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3DFF108F-33A8-4D90-A489-9BE36E4B99B0}" type="CELLRANGE">
+                    <a:fld id="{284AFF93-1FCD-4F97-B8AD-E22E713ADED4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2925,7 +2928,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EDA70C8E-E114-476F-9C43-BFC51A09EC44}" type="CELLRANGE">
+                    <a:fld id="{85C5DD38-68EE-42A4-B03A-682B298C023C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2959,7 +2962,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{50486487-CA9C-4BA8-88B9-A3AB01907DC2}" type="CELLRANGE">
+                    <a:fld id="{CBF91DB1-8ED1-4026-8051-35D72A132218}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2983,6 +2986,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-A7A4-492C-B015-27480EA84DE4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="76"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{12CE3FE7-169E-447E-BF3D-2FF3608AB80E}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-F6C0-43C0-8A35-4C56F2D89AFC}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3032,10 +3069,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$77</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="76"/>
+                <c:ptCount val="77"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -3259,9 +3296,12 @@
                   <c:v>10.8</c:v>
                 </c:pt>
                 <c:pt idx="74">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="75">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="76">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -3269,10 +3309,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$77</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="76"/>
+                <c:ptCount val="77"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -3496,9 +3536,12 @@
                   <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="74">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="75">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="76">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -3734,9 +3777,12 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="74">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="75">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="75">
+                  <c:pt idx="76">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -4789,10 +4835,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D77" totalsRowShown="0">
-  <autoFilter ref="A1:D77" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D77">
-    <sortCondition ref="A1:A77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D78" totalsRowShown="0">
+  <autoFilter ref="A1:D78" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D78">
+    <sortCondition ref="A1:A78"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -5101,21 +5147,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.08984375" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" customWidth="1"/>
+    <col min="1" max="1" width="28.06640625" customWidth="1"/>
+    <col min="2" max="2" width="9.53125" customWidth="1"/>
+    <col min="3" max="3" width="10.06640625" customWidth="1"/>
+    <col min="4" max="4" width="9.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -5129,7 +5175,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -5143,7 +5189,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -5157,7 +5203,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -5171,7 +5217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -5185,7 +5231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5200,7 +5246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5214,7 +5260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -5228,7 +5274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -5242,7 +5288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -5256,7 +5302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -5270,7 +5316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -5284,7 +5330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -5298,7 +5344,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -5312,7 +5358,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -5326,7 +5372,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -5340,7 +5386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -5356,7 +5402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -5370,7 +5416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -5384,7 +5430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -5398,7 +5444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -5412,7 +5458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -5426,7 +5472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -5440,7 +5486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -5454,7 +5500,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -5470,7 +5516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -5484,7 +5530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -5498,7 +5544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -5512,7 +5558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -5526,7 +5572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -5540,7 +5586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -5556,7 +5602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -5570,7 +5616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -5584,7 +5630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -5598,7 +5644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -5612,7 +5658,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -5628,7 +5674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -5642,7 +5688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -5656,7 +5702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -5670,7 +5716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -5684,7 +5730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -5698,7 +5744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -5712,7 +5758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -5726,7 +5772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -5740,7 +5786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -5754,7 +5800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -5768,7 +5814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -5782,7 +5828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>74</v>
       </c>
@@ -5796,7 +5842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -5810,7 +5856,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -5824,7 +5870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -5838,7 +5884,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>34</v>
       </c>
@@ -5852,7 +5898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>44</v>
       </c>
@@ -5866,7 +5912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -5880,7 +5926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>21</v>
       </c>
@@ -5894,7 +5940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -5908,7 +5954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -5922,7 +5968,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>22</v>
       </c>
@@ -5936,7 +5982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>23</v>
       </c>
@@ -5950,7 +5996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>45</v>
       </c>
@@ -5964,7 +6010,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -5978,7 +6024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -5992,7 +6038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>40</v>
       </c>
@@ -6006,7 +6052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>38</v>
       </c>
@@ -6020,7 +6066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -6034,7 +6080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -6050,7 +6096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>49</v>
       </c>
@@ -6064,7 +6110,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>26</v>
       </c>
@@ -6078,7 +6124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>60</v>
       </c>
@@ -6092,7 +6138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>72</v>
       </c>
@@ -6106,7 +6152,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>27</v>
       </c>
@@ -6120,7 +6166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -6134,7 +6180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>28</v>
       </c>
@@ -6148,7 +6194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>75</v>
       </c>
@@ -6162,7 +6208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>63</v>
       </c>
@@ -6176,32 +6222,46 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
+        <v>86</v>
+      </c>
+      <c r="B76">
+        <v>7</v>
+      </c>
+      <c r="C76">
+        <v>760</v>
+      </c>
+      <c r="D76" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
         <v>55</v>
       </c>
-      <c r="B76">
+      <c r="B77">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C76">
+      <c r="C77">
         <v>3800</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D77" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
         <v>29</v>
       </c>
-      <c r="B77">
+      <c r="B78">
         <v>6</v>
       </c>
-      <c r="C77">
+      <c r="C78">
         <v>2180</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D78" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Mather Memorial Parkway (snowshoe)
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawnhar\Desktop\docs\HikingTahoma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shawn\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87D9BF8-B490-425E-A5E8-5CBADDA5F377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20C8B79-458E-4A51-AEB8-FEB9D100E42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hike Difficulties" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="88">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>Westside Road (snowshoe)</t>
+  </si>
+  <si>
+    <t>Mather Memorial Parkway</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F60D7BA2-81C4-40C1-90B3-E599E4167F64}" type="CELLRANGE">
+                    <a:fld id="{AE3067FB-27A7-4246-BBFD-69400692E473}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -446,7 +449,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{57FC46E7-6D73-4E60-A5EF-6ACBB76097D8}" type="CELLRANGE">
+                    <a:fld id="{B1C4978D-F76B-46E4-A11B-ABF463A078F2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -480,7 +483,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B92A5064-86A4-48BB-A762-5A250AD941EB}" type="CELLRANGE">
+                    <a:fld id="{68076FD1-D701-4754-9C5C-4349216425AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -514,7 +517,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34F1C034-8F8E-43C8-A7A4-B211898FBD86}" type="CELLRANGE">
+                    <a:fld id="{CD5FB97C-B52A-4AD5-B43A-22EECE3A9E0B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -548,7 +551,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5DAFBE51-1CB6-42D6-BB17-722F36D2BF74}" type="CELLRANGE">
+                    <a:fld id="{D5E4B6AA-B0B1-4A3F-B275-261624601F2E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -582,7 +585,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BA7ABCB3-D9BC-400C-8900-47DAE850ECF3}" type="CELLRANGE">
+                    <a:fld id="{2A346DC8-8923-4E48-8D16-4AFCAAFCBB3B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -616,7 +619,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33CBF2B7-AB24-4628-84EC-1C5BFF3760FE}" type="CELLRANGE">
+                    <a:fld id="{056994DA-FB79-4B8E-84C0-4FFE1177B8F9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -650,7 +653,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2CCBDB26-EBE1-43B4-9A7A-AFFDFEADC62F}" type="CELLRANGE">
+                    <a:fld id="{1E7623C9-0740-47A0-B4B4-61478717544D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -684,7 +687,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5739ED0-7267-4E05-95F6-436112A5AD2F}" type="CELLRANGE">
+                    <a:fld id="{33FB575F-77DF-45FB-85E3-5AF1A992E077}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -718,7 +721,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC13F501-89F5-4F62-93C3-84AC6D8EB006}" type="CELLRANGE">
+                    <a:fld id="{1E4B1C5B-5812-4E80-A6A6-A502AFA85268}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -752,7 +755,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D579655A-49C4-43FC-8258-031CAA07BE31}" type="CELLRANGE">
+                    <a:fld id="{986D661E-859C-4993-B3E7-1A3D46FA2189}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -786,7 +789,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{233E890F-7677-4B5D-8280-10AB5700D069}" type="CELLRANGE">
+                    <a:fld id="{ABEA9EDC-6DDB-4356-91C8-6508E0EBFEAB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -820,7 +823,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B66591E0-66CE-498D-BD83-BD8BF78C6D56}" type="CELLRANGE">
+                    <a:fld id="{4CCA46D4-2C8F-4D59-8526-158679956146}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -854,7 +857,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B540F2EE-98EB-42BC-8230-CD3F37B4D66E}" type="CELLRANGE">
+                    <a:fld id="{BBF859B4-A2D0-4030-8CEF-21AE9FE566F3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -888,7 +891,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{625E5596-149F-4F21-8EA6-3F5274DAFD70}" type="CELLRANGE">
+                    <a:fld id="{B4A7E566-611E-475B-894A-49B05BB4A0E6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -922,7 +925,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA15071E-38CC-4D99-9DC5-F83A8FB9EF51}" type="CELLRANGE">
+                    <a:fld id="{3FB4BB50-2E5F-44B0-9F2E-A55A6FBFF53C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -956,7 +959,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF2BD05B-CD9D-4D22-9429-F6172CD93FCD}" type="CELLRANGE">
+                    <a:fld id="{E2A63C19-691D-410A-AEE0-5C7FBE33EE23}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -990,7 +993,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D442E35-BAAF-4E30-946C-55B40B7E8353}" type="CELLRANGE">
+                    <a:fld id="{A9C72F01-A9E3-4834-B7D2-313B4413907B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1024,7 +1027,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0BB3CDE5-C620-4650-B583-E19484263780}" type="CELLRANGE">
+                    <a:fld id="{255E4643-E384-408E-BFBC-613A1D472EEB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1058,7 +1061,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C03F0143-6794-476E-9817-636F4E944E79}" type="CELLRANGE">
+                    <a:fld id="{9D3B9630-EE42-4770-8FFD-7A2B65033049}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1092,7 +1095,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B604173-B7B7-4FB1-8D51-2ED8CB17DFA7}" type="CELLRANGE">
+                    <a:fld id="{FA354FD7-511C-444A-AA47-4ABF05E716F3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1126,7 +1129,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2939A4C3-58E4-4D68-9FAC-06C0E800255E}" type="CELLRANGE">
+                    <a:fld id="{7B6062DE-38C2-4E4F-AC82-A2FB365B002C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1160,7 +1163,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A6AC2BED-0EDE-4B2F-B2D8-D4DD4C39DAF4}" type="CELLRANGE">
+                    <a:fld id="{58D0F3F0-9A6C-4896-B97A-5CC6EAD0CA72}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1194,7 +1197,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7FF0E7F3-9FC8-4179-B60D-0E78857F54B7}" type="CELLRANGE">
+                    <a:fld id="{7C589213-2A2E-4BE9-9AED-8359359BBE53}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1228,7 +1231,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F07ADA38-D1F1-4D40-861E-D77540D07177}" type="CELLRANGE">
+                    <a:fld id="{AF65AD9D-047F-4DF7-B8F8-C9DBCBFA7F85}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1262,7 +1265,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FBDD9E1E-A5B4-43DB-8FE9-74AE2F3EBF74}" type="CELLRANGE">
+                    <a:fld id="{4D8F7E61-87DD-4F68-B4D9-2514FA0ACDA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1296,7 +1299,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3FA4706-506C-44E1-9810-99924E9261EF}" type="CELLRANGE">
+                    <a:fld id="{E7531763-0B9E-4B00-94CA-6D9711B76504}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1330,7 +1333,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5C3A46D-32BC-40F4-B75D-02053F0B24C8}" type="CELLRANGE">
+                    <a:fld id="{E02F309F-D5CB-4060-BE0A-D5DAA897AB39}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1364,7 +1367,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7CBC06C-24D0-483F-9EC0-A76593B9DCDA}" type="CELLRANGE">
+                    <a:fld id="{06E7E254-2D70-409B-B999-A70C7DD80CCB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1398,7 +1401,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F41E3614-976D-4590-9BE8-B3E7BAF56401}" type="CELLRANGE">
+                    <a:fld id="{4F3A2C62-A744-491A-9119-434F51B03E82}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1432,7 +1435,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A2973834-3BA7-4784-A93B-06529E6AE679}" type="CELLRANGE">
+                    <a:fld id="{19AA1861-B1DF-4D52-8EBF-6C5977A535A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1466,7 +1469,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{90D99530-F828-46BE-B722-15E5C8B0CC5D}" type="CELLRANGE">
+                    <a:fld id="{2649DC98-3B3E-4F67-A35A-759280D85297}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1500,7 +1503,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E2E8081-B3F4-4690-957B-B475DD27A055}" type="CELLRANGE">
+                    <a:fld id="{9F2DF003-BF38-4F80-849D-D2947D14CBBF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1534,7 +1537,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{84138DFF-04CB-4CFB-BE43-C13081BBFD85}" type="CELLRANGE">
+                    <a:fld id="{DEDB2E35-C60D-42B2-A079-250CB75923AA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1568,7 +1571,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4EC405B2-A99A-4EFA-8908-1C29E201EDE1}" type="CELLRANGE">
+                    <a:fld id="{714F15C8-55CC-4B12-947A-A9410F086C32}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1602,7 +1605,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{448BF695-7383-4C87-A9FA-6E9ED4F96AEC}" type="CELLRANGE">
+                    <a:fld id="{52C7CE72-4C07-422E-8D7C-EC7653834B36}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1636,7 +1639,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE6540EB-D422-412C-8778-54CC47B30E39}" type="CELLRANGE">
+                    <a:fld id="{3B8E41A5-FC00-4AD1-8CA0-415B4FBEB2A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1670,7 +1673,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ECDD77BC-B19B-419F-A9A4-AAEB254668FD}" type="CELLRANGE">
+                    <a:fld id="{0909186D-6120-41C8-A9DD-43571805F920}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1704,7 +1707,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4855E166-350F-4BED-B1D1-65BA8C15D9EA}" type="CELLRANGE">
+                    <a:fld id="{F7E1C5CB-2589-43FF-B139-0862746D7C68}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1738,7 +1741,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1E17CC4D-3026-4AAE-8737-F0ED4DBFAA67}" type="CELLRANGE">
+                    <a:fld id="{12795576-9DA0-4497-8BC8-E071AB4E932D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1772,7 +1775,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{983764FF-60BC-4D3C-BDF1-E265F1F2EDEB}" type="CELLRANGE">
+                    <a:fld id="{B98EEF8D-6B58-4411-A2FD-3AB5DF7F4606}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1806,7 +1809,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5018417D-801C-4ACE-AB6C-F0DDEB7D00EF}" type="CELLRANGE">
+                    <a:fld id="{6D7FA02B-B9A8-4B5F-82AA-4FE67AFEAD52}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1840,7 +1843,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8F8384E9-F0E9-4121-88C5-517EA29CF074}" type="CELLRANGE">
+                    <a:fld id="{4B5E62AE-FC3E-47F3-8ACA-3169794E0D35}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1874,7 +1877,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{123212AB-B021-4342-B45A-D73C9244C3EF}" type="CELLRANGE">
+                    <a:fld id="{21D3C1BB-3B76-44A6-A4E0-ED74354F8AFE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1908,7 +1911,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F75AF93-78FE-42C0-8C83-6DA04ED7771D}" type="CELLRANGE">
+                    <a:fld id="{CF1DA1B1-F47E-4CDA-AE4C-6BB42CCE34C6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1942,7 +1945,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7918706-DCED-418E-A87A-2DCD32C8E196}" type="CELLRANGE">
+                    <a:fld id="{7E3D5E78-92CD-440D-AF71-0D43B9C4292A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1976,7 +1979,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1FDD32DC-D78F-4C41-AEB9-65D009CD04F7}" type="CELLRANGE">
+                    <a:fld id="{8AD7A839-A0DB-49A6-BEF6-536CD842E17A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2010,7 +2013,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2FF1E7A0-5447-4DC3-AC26-D14E334D81A5}" type="CELLRANGE">
+                    <a:fld id="{1D3E07CF-8981-4D0F-9E1E-07B3E0DACDF5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2044,7 +2047,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{517E7271-7886-47A6-BE29-D9C32264331D}" type="CELLRANGE">
+                    <a:fld id="{6775B1CF-D362-4C37-80DB-179294C3A2E7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2078,7 +2081,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{282262F3-648C-43A8-8BFB-DD32A3BF6147}" type="CELLRANGE">
+                    <a:fld id="{17D5B8B3-347D-4E6E-82D5-EEEEF2C09CB4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2112,7 +2115,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C378BE7-1D44-4172-95DA-31FFF58D0A08}" type="CELLRANGE">
+                    <a:fld id="{8AADD786-9D4C-4CFE-BC86-8760793AD733}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2146,7 +2149,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33E7BB05-755C-4673-968E-93707DB1C2A9}" type="CELLRANGE">
+                    <a:fld id="{6158086A-6D1D-4016-BC4D-9702CBC791CA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2180,7 +2183,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{911FF864-8979-4510-9153-4DAE4F0802F7}" type="CELLRANGE">
+                    <a:fld id="{A400B0D0-1540-43DD-903C-7388F84CD5CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2214,7 +2217,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DB51A25A-1D32-4104-ABE8-371F70A709E1}" type="CELLRANGE">
+                    <a:fld id="{3AF03E5E-F520-4B45-AF47-EC991FA78434}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2248,7 +2251,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3C6894C-388F-4A73-9077-B85C1EA7C92D}" type="CELLRANGE">
+                    <a:fld id="{1280096C-7CFA-4F59-8AB1-3AF8479C88BD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2282,7 +2285,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E338512-3377-4E6A-8243-3B38DB027E73}" type="CELLRANGE">
+                    <a:fld id="{269336B1-5884-4052-8C53-67B177725E76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2316,7 +2319,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C8D74C6-CE08-4401-B6A4-4D7F589DF668}" type="CELLRANGE">
+                    <a:fld id="{56965B78-9E42-48F9-9E44-0D647BBDD613}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2350,7 +2353,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BA60A685-1F0A-4028-AEB3-54677B020053}" type="CELLRANGE">
+                    <a:fld id="{95E3C07A-C72E-4FB3-A338-225160C3631D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2384,7 +2387,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{84DC49CF-FE56-4CA5-B8FD-5EE2BAC41A76}" type="CELLRANGE">
+                    <a:fld id="{D4779CD2-6145-4B00-91D8-9CEBE7A3D5B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2418,7 +2421,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40DF9DBE-979A-4EFA-9D7F-B241024662E0}" type="CELLRANGE">
+                    <a:fld id="{103A760F-B618-43F0-BE7A-664B0367CE04}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2452,7 +2455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E06F182-2D1F-47E9-A23F-C3813F1E362A}" type="CELLRANGE">
+                    <a:fld id="{2D9448A6-DCAE-47BB-9A80-96C0501D9480}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2486,7 +2489,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E0CA1841-5B5D-4924-8444-376D20EC2A59}" type="CELLRANGE">
+                    <a:fld id="{2283EC3C-516F-4847-8542-64046F768A17}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2520,7 +2523,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7BF25E5-6421-4DB7-B1A3-28731EE442F2}" type="CELLRANGE">
+                    <a:fld id="{D0DE6ABF-500B-473A-9CD2-A4EE1C9BAACE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2554,7 +2557,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{639D5E5D-9D60-4748-8FAC-78196D6F328F}" type="CELLRANGE">
+                    <a:fld id="{5AC51C52-8660-4133-87E8-AD406EFABAFA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2588,7 +2591,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FAA3DD3E-FFF7-4F43-ACA3-EDAE16E001C6}" type="CELLRANGE">
+                    <a:fld id="{07DA50B0-B566-4F00-A43D-16D7A6B02138}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2622,7 +2625,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{334B32FE-C6E8-46CE-9DD0-FD02BE8D78C1}" type="CELLRANGE">
+                    <a:fld id="{28B042AE-8E90-4578-907C-0C1DCE449D02}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2656,7 +2659,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56F0BE03-DF17-4465-896A-E295DFDFB152}" type="CELLRANGE">
+                    <a:fld id="{A8D61B81-6796-4537-9141-7B9D1ECCDE12}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2690,7 +2693,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{87CF154F-7417-4E78-96B0-164BB63EFE66}" type="CELLRANGE">
+                    <a:fld id="{34B28810-917A-4DCC-AC6C-02B802A7DB9A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2724,7 +2727,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{156AB8EB-C638-4744-BB67-0C47F256B9A5}" type="CELLRANGE">
+                    <a:fld id="{29D94BA0-2F19-4594-A451-DEF5740CE573}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2758,7 +2761,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5DAAA7D3-A8DF-4A36-87EA-EC93675ADE3C}" type="CELLRANGE">
+                    <a:fld id="{D28BFC13-5D6F-4E88-AE83-D58F4516922C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2792,7 +2795,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A30AF67-658D-45DA-9658-5E02978773C4}" type="CELLRANGE">
+                    <a:fld id="{59A880C8-5EAA-4EFD-AAEF-EBA1FD6CB896}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2826,7 +2829,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E61FA588-4B13-4766-87C0-8EF57CB31714}" type="CELLRANGE">
+                    <a:fld id="{AFA7A11D-5A1A-425B-986D-5C5807217D6B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2860,7 +2863,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F6741195-A1F8-4B4E-ABEC-2A03E4D173CF}" type="CELLRANGE">
+                    <a:fld id="{D1DE3ED9-51BB-4F49-B8EC-6552DD2D15D4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2894,7 +2897,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{284AFF93-1FCD-4F97-B8AD-E22E713ADED4}" type="CELLRANGE">
+                    <a:fld id="{3122A61D-4556-49FC-B324-4181CAD92FA3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2928,7 +2931,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{85C5DD38-68EE-42A4-B03A-682B298C023C}" type="CELLRANGE">
+                    <a:fld id="{AB3F9073-4848-4356-8536-247F0733B9D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2962,7 +2965,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CBF91DB1-8ED1-4026-8051-35D72A132218}" type="CELLRANGE">
+                    <a:fld id="{5AB514ED-F2A1-424B-914D-577CA10B619D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2996,7 +2999,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12CE3FE7-169E-447E-BF3D-2FF3608AB80E}" type="CELLRANGE">
+                    <a:fld id="{34E20F04-0358-40D2-929B-2C85ABC7EDCB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3020,6 +3023,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-F6C0-43C0-8A35-4C56F2D89AFC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="77"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{41483AC7-E53A-4F93-9DFC-6EA688586E48}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-C555-4B08-8BEC-89FEEB45465B}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3069,10 +3106,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$78</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="78"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -3194,114 +3231,117 @@
                   <c:v>11.4</c:v>
                 </c:pt>
                 <c:pt idx="40">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="41">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>4.2</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>7.2</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>2.7</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>3.3</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="69">
                   <c:v>9.9</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="73">
                   <c:v>5.6</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="74">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="75">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="76">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="77">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -3309,10 +3349,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$78</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="78"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -3434,114 +3474,117 @@
                   <c:v>2550</c:v>
                 </c:pt>
                 <c:pt idx="40">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="41">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>880</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>860</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>1260</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>2600</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>3100</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>1630</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>1930</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="69">
                   <c:v>3180</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>1890</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="73">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="74">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="75">
                   <c:v>760</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="76">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="77">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -3675,16 +3718,16 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="40">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="41">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="41">
+                  <c:pt idx="42">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="42">
+                  <c:pt idx="43">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="43">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="44">
                     <c:v>easy</c:v>
@@ -3693,19 +3736,19 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="46">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="47">
+                  <c:pt idx="48">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="48">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="49">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="50">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="51">
                     <c:v>moderate</c:v>
@@ -3714,75 +3757,78 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="53">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="54">
+                  <c:pt idx="55">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="55">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="56">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="57">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="58">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="58">
+                  <c:pt idx="59">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="59">
+                  <c:pt idx="60">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="60">
+                  <c:pt idx="61">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="61">
+                  <c:pt idx="62">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="62">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="63">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="64">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="65">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="65">
+                  <c:pt idx="66">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="66">
+                  <c:pt idx="67">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="67">
+                  <c:pt idx="68">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="68">
+                  <c:pt idx="69">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="69">
+                  <c:pt idx="70">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="70">
+                  <c:pt idx="71">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="71">
+                  <c:pt idx="72">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="72">
+                  <c:pt idx="73">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="73">
+                  <c:pt idx="74">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="74">
+                  <c:pt idx="75">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="75">
+                  <c:pt idx="76">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="76">
+                  <c:pt idx="77">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -4835,10 +4881,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D78" totalsRowShown="0">
-  <autoFilter ref="A1:D78" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D78">
-    <sortCondition ref="A1:A78"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D79" totalsRowShown="0">
+  <autoFilter ref="A1:D79" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D79">
+    <sortCondition ref="A1:A79"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -5147,10 +5193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5746,69 +5792,69 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="B42">
-        <v>8.5</v>
+        <v>10.8</v>
       </c>
       <c r="C42">
-        <v>3350</v>
+        <v>1050</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B43">
-        <v>2.8</v>
+        <v>8.5</v>
       </c>
       <c r="C43">
-        <v>880</v>
+        <v>3350</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B44">
-        <v>10.4</v>
+        <v>2.8</v>
       </c>
       <c r="C44">
-        <v>1420</v>
+        <v>880</v>
       </c>
       <c r="D44" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B45">
-        <v>0.9</v>
+        <v>10.4</v>
       </c>
       <c r="C45">
-        <v>200</v>
+        <v>1420</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B46">
-        <v>4.2</v>
+        <v>0.9</v>
       </c>
       <c r="C46">
-        <v>860</v>
+        <v>200</v>
       </c>
       <c r="D46" t="s">
         <v>7</v>
@@ -5816,13 +5862,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B47">
-        <v>4.8</v>
+        <v>4.2</v>
       </c>
       <c r="C47">
-        <v>1260</v>
+        <v>860</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
@@ -5830,55 +5876,55 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B48">
-        <v>4</v>
+        <v>4.8</v>
       </c>
       <c r="C48">
-        <v>2600</v>
+        <v>1260</v>
       </c>
       <c r="D48" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B49">
-        <v>1.4</v>
+        <v>4</v>
       </c>
       <c r="C49">
-        <v>375</v>
+        <v>2600</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B50">
-        <v>13.6</v>
+        <v>1.4</v>
       </c>
       <c r="C50">
-        <v>3930</v>
+        <v>375</v>
       </c>
       <c r="D50" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B51">
-        <v>10.5</v>
+        <v>13.6</v>
       </c>
       <c r="C51">
-        <v>3100</v>
+        <v>3930</v>
       </c>
       <c r="D51" t="s">
         <v>10</v>
@@ -5886,27 +5932,27 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B52">
-        <v>7</v>
+        <v>10.5</v>
       </c>
       <c r="C52">
-        <v>1670</v>
+        <v>3100</v>
       </c>
       <c r="D52" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B53">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="C53">
-        <v>2400</v>
+        <v>1670</v>
       </c>
       <c r="D53" t="s">
         <v>1</v>
@@ -5914,13 +5960,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B54">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C54">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
@@ -5928,55 +5974,55 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B55">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C55">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B56">
-        <v>7.2</v>
+        <v>4.8</v>
       </c>
       <c r="C56">
-        <v>1630</v>
+        <v>1300</v>
       </c>
       <c r="D56" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B57">
-        <v>2.7</v>
+        <v>7.2</v>
       </c>
       <c r="C57">
-        <v>1090</v>
+        <v>1630</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="B58">
-        <v>4.8</v>
+        <v>2.7</v>
       </c>
       <c r="C58">
-        <v>1470</v>
+        <v>1090</v>
       </c>
       <c r="D58" t="s">
         <v>7</v>
@@ -5984,97 +6030,97 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B59">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C59">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D59" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B60">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C60">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D60" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B61">
-        <v>3.3</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C61">
-        <v>600</v>
+        <v>3490</v>
       </c>
       <c r="D61" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B62">
-        <v>8.5</v>
+        <v>3.3</v>
       </c>
       <c r="C62">
-        <v>1930</v>
+        <v>600</v>
       </c>
       <c r="D62" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B63">
-        <v>2.2000000000000002</v>
+        <v>8.5</v>
       </c>
       <c r="C63">
-        <v>750</v>
+        <v>1930</v>
       </c>
       <c r="D63" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B64">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C64">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D64" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B65">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C65">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D65" t="s">
         <v>1</v>
@@ -6082,186 +6128,200 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66">
+        <v>7.3</v>
+      </c>
+      <c r="C66">
+        <v>2250</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
         <v>25</v>
       </c>
-      <c r="B66">
+      <c r="B67">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C66">
+      <c r="C67">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
-        <v>49</v>
-      </c>
-      <c r="B67">
-        <v>1.2</v>
-      </c>
-      <c r="C67">
-        <v>500</v>
-      </c>
-      <c r="D67" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B68">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C68">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D68" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B69">
-        <v>6.5</v>
+        <v>11</v>
       </c>
       <c r="C69">
-        <v>1650</v>
+        <v>3060</v>
       </c>
       <c r="D69" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B70">
-        <v>9.9</v>
+        <v>6.5</v>
       </c>
       <c r="C70">
-        <v>3180</v>
+        <v>1650</v>
       </c>
       <c r="D70" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="B71">
-        <v>6.2</v>
+        <v>9.9</v>
       </c>
       <c r="C71">
-        <v>1890</v>
+        <v>3180</v>
       </c>
       <c r="D71" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B72">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
       <c r="C72">
-        <v>100</v>
+        <v>1890</v>
       </c>
       <c r="D72" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B73">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C73">
-        <v>3550</v>
+        <v>100</v>
       </c>
       <c r="D73" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="B74">
-        <v>5.6</v>
+        <v>7.3</v>
       </c>
       <c r="C74">
-        <v>1680</v>
+        <v>3550</v>
       </c>
       <c r="D74" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B75">
-        <v>10.8</v>
+        <v>5.6</v>
       </c>
       <c r="C75">
-        <v>1800</v>
+        <v>1680</v>
       </c>
       <c r="D75" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B76">
-        <v>7</v>
+        <v>10.8</v>
       </c>
       <c r="C76">
-        <v>760</v>
+        <v>1800</v>
       </c>
       <c r="D76" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
+        <v>86</v>
+      </c>
+      <c r="B77">
+        <v>7</v>
+      </c>
+      <c r="C77">
+        <v>760</v>
+      </c>
+      <c r="D77" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
         <v>55</v>
       </c>
-      <c r="B77">
+      <c r="B78">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C77">
+      <c r="C78">
         <v>3800</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D78" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
         <v>29</v>
       </c>
-      <c r="B78">
+      <c r="B79">
         <v>6</v>
       </c>
-      <c r="C78">
+      <c r="C79">
         <v>2180</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D79" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Emmons Moraine entry
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shawn\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20C8B79-458E-4A51-AEB8-FEB9D100E42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585DE341-8709-4485-BE2E-735EE0B59DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -415,7 +415,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE3067FB-27A7-4246-BBFD-69400692E473}" type="CELLRANGE">
+                    <a:fld id="{59E2A27D-EE3F-4C22-8429-9AC59E2ED1CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -449,7 +449,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B1C4978D-F76B-46E4-A11B-ABF463A078F2}" type="CELLRANGE">
+                    <a:fld id="{4BC0F5B2-8C95-428C-9224-6C48E3AF9F81}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -483,7 +483,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{68076FD1-D701-4754-9C5C-4349216425AC}" type="CELLRANGE">
+                    <a:fld id="{11207B2E-85C6-4D73-AB23-D17B57761668}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -517,7 +517,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD5FB97C-B52A-4AD5-B43A-22EECE3A9E0B}" type="CELLRANGE">
+                    <a:fld id="{A0BA0030-2316-4645-BECE-3A6ED7DBDC34}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -551,7 +551,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D5E4B6AA-B0B1-4A3F-B275-261624601F2E}" type="CELLRANGE">
+                    <a:fld id="{3180C816-5A1D-44ED-9E29-0F01811C5C90}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -585,7 +585,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A346DC8-8923-4E48-8D16-4AFCAAFCBB3B}" type="CELLRANGE">
+                    <a:fld id="{7F9DCBBA-DBC9-4AB1-BAB6-FBAC0B5C50BF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -619,7 +619,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{056994DA-FB79-4B8E-84C0-4FFE1177B8F9}" type="CELLRANGE">
+                    <a:fld id="{1D019A4E-CC17-471E-8734-C4BC7AAB5FB0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -653,7 +653,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1E7623C9-0740-47A0-B4B4-61478717544D}" type="CELLRANGE">
+                    <a:fld id="{96E2C5C3-680D-48AD-88B0-9B22A11EABD2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -687,7 +687,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33FB575F-77DF-45FB-85E3-5AF1A992E077}" type="CELLRANGE">
+                    <a:fld id="{85DCF0C5-7383-4FE1-991A-2D5305415525}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -721,7 +721,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1E4B1C5B-5812-4E80-A6A6-A502AFA85268}" type="CELLRANGE">
+                    <a:fld id="{2901BCA3-C081-4B8E-8D91-057D9B290B00}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -755,7 +755,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{986D661E-859C-4993-B3E7-1A3D46FA2189}" type="CELLRANGE">
+                    <a:fld id="{9ABB3EE7-BCD1-4D5B-8BB3-05CFFEE9C3E3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -789,7 +789,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ABEA9EDC-6DDB-4356-91C8-6508E0EBFEAB}" type="CELLRANGE">
+                    <a:fld id="{DB8E33D7-C9E4-436F-8324-19CFC9F54AF7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -823,7 +823,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4CCA46D4-2C8F-4D59-8526-158679956146}" type="CELLRANGE">
+                    <a:fld id="{EA389902-73BB-4D2C-BFDD-9992F153490F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -857,7 +857,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BBF859B4-A2D0-4030-8CEF-21AE9FE566F3}" type="CELLRANGE">
+                    <a:fld id="{3333CEAD-CFA8-4AD9-8951-A18F5C66E7A3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -891,7 +891,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B4A7E566-611E-475B-894A-49B05BB4A0E6}" type="CELLRANGE">
+                    <a:fld id="{8FDFE6E1-1ACB-49EF-9B4C-17E5A2788001}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -925,7 +925,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3FB4BB50-2E5F-44B0-9F2E-A55A6FBFF53C}" type="CELLRANGE">
+                    <a:fld id="{44947F32-E90F-41D3-ACD0-09BE6B3F3FF0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -959,7 +959,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E2A63C19-691D-410A-AEE0-5C7FBE33EE23}" type="CELLRANGE">
+                    <a:fld id="{81A592D6-42C6-4112-B1C4-7F7B36270675}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -993,7 +993,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9C72F01-A9E3-4834-B7D2-313B4413907B}" type="CELLRANGE">
+                    <a:fld id="{437639AF-9B7C-4FB3-985D-26FF9D21309D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1027,7 +1027,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{255E4643-E384-408E-BFBC-613A1D472EEB}" type="CELLRANGE">
+                    <a:fld id="{8E6001DE-68F1-45A0-AACF-9E9F4DA500DF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1061,7 +1061,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D3B9630-EE42-4770-8FFD-7A2B65033049}" type="CELLRANGE">
+                    <a:fld id="{D254E612-EB62-4359-8195-6E945322DE13}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1095,7 +1095,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA354FD7-511C-444A-AA47-4ABF05E716F3}" type="CELLRANGE">
+                    <a:fld id="{B08EFD20-3E6C-4A22-AE05-A5731C1F7B46}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1129,7 +1129,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7B6062DE-38C2-4E4F-AC82-A2FB365B002C}" type="CELLRANGE">
+                    <a:fld id="{A64D5871-BC92-43AC-8E3A-1CA6A973DA10}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1163,7 +1163,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58D0F3F0-9A6C-4896-B97A-5CC6EAD0CA72}" type="CELLRANGE">
+                    <a:fld id="{F66D14FB-6414-44FA-9ED1-A1443442C092}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1197,7 +1197,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7C589213-2A2E-4BE9-9AED-8359359BBE53}" type="CELLRANGE">
+                    <a:fld id="{89A6BB89-C086-4DA1-94DE-D3E2B33DE1BD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1231,7 +1231,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AF65AD9D-047F-4DF7-B8F8-C9DBCBFA7F85}" type="CELLRANGE">
+                    <a:fld id="{572247A2-667A-4BA9-9E1B-03C50FCC50B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1265,7 +1265,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D8F7E61-87DD-4F68-B4D9-2514FA0ACDA5}" type="CELLRANGE">
+                    <a:fld id="{C1F1F7B2-45DC-4CC4-9720-774DED9E8C6B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1299,7 +1299,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7531763-0B9E-4B00-94CA-6D9711B76504}" type="CELLRANGE">
+                    <a:fld id="{344C9F89-C0E2-4103-9315-EB90E3A03DF0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1333,7 +1333,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E02F309F-D5CB-4060-BE0A-D5DAA897AB39}" type="CELLRANGE">
+                    <a:fld id="{B2A24224-8A2D-4D0E-A33E-AD74EFBC6F0B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1367,7 +1367,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06E7E254-2D70-409B-B999-A70C7DD80CCB}" type="CELLRANGE">
+                    <a:fld id="{8E733CFA-D6EA-4E92-8E3F-3DD8A1DADAE8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1401,7 +1401,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F3A2C62-A744-491A-9119-434F51B03E82}" type="CELLRANGE">
+                    <a:fld id="{01CA5FEC-B4F6-43A7-9CC7-F70063508F2B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1435,7 +1435,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19AA1861-B1DF-4D52-8EBF-6C5977A535A8}" type="CELLRANGE">
+                    <a:fld id="{3E15ACD2-C4D3-494C-BF39-B1F0F5F2A04D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1469,7 +1469,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2649DC98-3B3E-4F67-A35A-759280D85297}" type="CELLRANGE">
+                    <a:fld id="{6248D773-3238-4F6C-8DB4-2527F05C6979}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1503,7 +1503,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F2DF003-BF38-4F80-849D-D2947D14CBBF}" type="CELLRANGE">
+                    <a:fld id="{88E25FE9-2AAC-4749-AE7A-A7AFC41D3BF8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1537,7 +1537,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DEDB2E35-C60D-42B2-A079-250CB75923AA}" type="CELLRANGE">
+                    <a:fld id="{76EA1E22-C2D7-423F-9A60-AF9CB0719872}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1571,7 +1571,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{714F15C8-55CC-4B12-947A-A9410F086C32}" type="CELLRANGE">
+                    <a:fld id="{C72903D0-2E6B-4257-A1EA-2F0A35553D1E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1605,7 +1605,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{52C7CE72-4C07-422E-8D7C-EC7653834B36}" type="CELLRANGE">
+                    <a:fld id="{A684E87C-AC62-4A8E-A1B1-0EC6F8972C36}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1639,7 +1639,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B8E41A5-FC00-4AD1-8CA0-415B4FBEB2A1}" type="CELLRANGE">
+                    <a:fld id="{6B15CA5A-B5CC-4D71-B7A4-D7F5C019A169}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1673,7 +1673,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0909186D-6120-41C8-A9DD-43571805F920}" type="CELLRANGE">
+                    <a:fld id="{6B0AF3DC-18A9-4D7B-87A8-692A084B2949}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1707,7 +1707,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F7E1C5CB-2589-43FF-B139-0862746D7C68}" type="CELLRANGE">
+                    <a:fld id="{4AEF81E0-9F28-474B-ACDE-06719475FF83}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1741,7 +1741,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12795576-9DA0-4497-8BC8-E071AB4E932D}" type="CELLRANGE">
+                    <a:fld id="{92BE76A3-AC57-4CB7-B8B8-98EDB777A898}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1775,7 +1775,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B98EEF8D-6B58-4411-A2FD-3AB5DF7F4606}" type="CELLRANGE">
+                    <a:fld id="{98EECB2C-8196-4869-911E-728E5C95181C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1809,7 +1809,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D7FA02B-B9A8-4B5F-82AA-4FE67AFEAD52}" type="CELLRANGE">
+                    <a:fld id="{92E32E58-887D-4225-AF2C-24002C75FC0B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1843,7 +1843,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4B5E62AE-FC3E-47F3-8ACA-3169794E0D35}" type="CELLRANGE">
+                    <a:fld id="{6966ACDA-93A1-43F3-9122-B27B9D14A43A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1877,7 +1877,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{21D3C1BB-3B76-44A6-A4E0-ED74354F8AFE}" type="CELLRANGE">
+                    <a:fld id="{80D4A6FF-18EF-44D4-97E2-87567C424F56}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1911,7 +1911,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CF1DA1B1-F47E-4CDA-AE4C-6BB42CCE34C6}" type="CELLRANGE">
+                    <a:fld id="{2654F0DD-FCF6-4245-8A3B-053D48EB0E9A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1945,7 +1945,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E3D5E78-92CD-440D-AF71-0D43B9C4292A}" type="CELLRANGE">
+                    <a:fld id="{63320659-FF90-4ED9-94BD-8EF2991A2A3A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1979,7 +1979,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8AD7A839-A0DB-49A6-BEF6-536CD842E17A}" type="CELLRANGE">
+                    <a:fld id="{EB0C7CBC-7D34-437F-9DB9-C6B0A4E0559B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2013,7 +2013,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1D3E07CF-8981-4D0F-9E1E-07B3E0DACDF5}" type="CELLRANGE">
+                    <a:fld id="{67AC21D1-7C54-4C76-9A1C-0C3EF67CC1EC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2047,7 +2047,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6775B1CF-D362-4C37-80DB-179294C3A2E7}" type="CELLRANGE">
+                    <a:fld id="{B4FA2CED-A781-4FA1-8FB2-E68E251737A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2081,7 +2081,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17D5B8B3-347D-4E6E-82D5-EEEEF2C09CB4}" type="CELLRANGE">
+                    <a:fld id="{D11A4780-B5F5-4D3C-824F-00548292F137}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2115,7 +2115,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8AADD786-9D4C-4CFE-BC86-8760793AD733}" type="CELLRANGE">
+                    <a:fld id="{53580E5A-392B-4D53-B019-F68B42BA844D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2149,7 +2149,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6158086A-6D1D-4016-BC4D-9702CBC791CA}" type="CELLRANGE">
+                    <a:fld id="{3DB003CC-80C7-4692-926D-2F0C05F41840}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2183,7 +2183,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A400B0D0-1540-43DD-903C-7388F84CD5CB}" type="CELLRANGE">
+                    <a:fld id="{B5F3ABA8-CA6B-41D1-B15A-CCF6492A9D5F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2217,7 +2217,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3AF03E5E-F520-4B45-AF47-EC991FA78434}" type="CELLRANGE">
+                    <a:fld id="{809D5F75-3680-443A-8536-36DFD2BB5B8D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2251,7 +2251,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1280096C-7CFA-4F59-8AB1-3AF8479C88BD}" type="CELLRANGE">
+                    <a:fld id="{9217C3B5-15CA-42D6-B59A-C9B8408426C4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2285,7 +2285,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{269336B1-5884-4052-8C53-67B177725E76}" type="CELLRANGE">
+                    <a:fld id="{50403B91-B247-4747-BC29-A51C0B062356}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2319,7 +2319,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56965B78-9E42-48F9-9E44-0D647BBDD613}" type="CELLRANGE">
+                    <a:fld id="{C30A5327-28EC-4B00-8721-6F61824C6ED9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2353,7 +2353,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95E3C07A-C72E-4FB3-A338-225160C3631D}" type="CELLRANGE">
+                    <a:fld id="{CA985E20-95DE-4442-A506-97C7DC55DA3D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2387,7 +2387,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4779CD2-6145-4B00-91D8-9CEBE7A3D5B2}" type="CELLRANGE">
+                    <a:fld id="{AA92EBCF-C5F3-43AF-91CA-C85EAC71811D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2421,7 +2421,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{103A760F-B618-43F0-BE7A-664B0367CE04}" type="CELLRANGE">
+                    <a:fld id="{E001FDE8-2E79-4821-86AD-7AA830792BA1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2455,7 +2455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D9448A6-DCAE-47BB-9A80-96C0501D9480}" type="CELLRANGE">
+                    <a:fld id="{78EBA1C1-63D0-49B1-BB64-FE82DBBF024D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2489,7 +2489,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2283EC3C-516F-4847-8542-64046F768A17}" type="CELLRANGE">
+                    <a:fld id="{4BF383B0-5DA4-4750-B826-932BBC9EC0B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2523,7 +2523,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D0DE6ABF-500B-473A-9CD2-A4EE1C9BAACE}" type="CELLRANGE">
+                    <a:fld id="{B7BFB006-C01E-4803-A0E4-4D9F0B752B12}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2557,7 +2557,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5AC51C52-8660-4133-87E8-AD406EFABAFA}" type="CELLRANGE">
+                    <a:fld id="{2B63DC7C-62DB-4B0F-BFF2-BC136F4A6BB4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2591,7 +2591,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{07DA50B0-B566-4F00-A43D-16D7A6B02138}" type="CELLRANGE">
+                    <a:fld id="{F9D85862-0D64-42B6-B6DA-544C0D927278}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2625,7 +2625,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{28B042AE-8E90-4578-907C-0C1DCE449D02}" type="CELLRANGE">
+                    <a:fld id="{5E75BB38-62D8-4031-8944-447B7FEC3B26}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2659,7 +2659,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A8D61B81-6796-4537-9141-7B9D1ECCDE12}" type="CELLRANGE">
+                    <a:fld id="{58EFEDDA-ED85-481A-A64A-1203D6223E10}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2693,7 +2693,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34B28810-917A-4DCC-AC6C-02B802A7DB9A}" type="CELLRANGE">
+                    <a:fld id="{55BAC808-C543-49A8-A4FA-16450CFE032E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2727,7 +2727,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29D94BA0-2F19-4594-A451-DEF5740CE573}" type="CELLRANGE">
+                    <a:fld id="{59782F78-533B-42A3-A98B-DA3D6334879B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2761,7 +2761,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D28BFC13-5D6F-4E88-AE83-D58F4516922C}" type="CELLRANGE">
+                    <a:fld id="{B4E04B28-ACDC-4D67-ACA6-2949185584FB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2795,7 +2795,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{59A880C8-5EAA-4EFD-AAEF-EBA1FD6CB896}" type="CELLRANGE">
+                    <a:fld id="{153B3B3E-09CF-4144-9F1D-6F4ACDAE4889}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2829,7 +2829,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AFA7A11D-5A1A-425B-986D-5C5807217D6B}" type="CELLRANGE">
+                    <a:fld id="{C95E2DE1-F672-475D-A4E1-D395D0101FD9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2863,7 +2863,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1DE3ED9-51BB-4F49-B8EC-6552DD2D15D4}" type="CELLRANGE">
+                    <a:fld id="{51B75103-6850-4B17-A952-0FFC220DFD50}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2897,7 +2897,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3122A61D-4556-49FC-B324-4181CAD92FA3}" type="CELLRANGE">
+                    <a:fld id="{02B3B418-8979-4C77-859C-E967E426E05E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2931,7 +2931,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AB3F9073-4848-4356-8536-247F0733B9D7}" type="CELLRANGE">
+                    <a:fld id="{45F63F0E-9D20-4FA7-88D6-42D1A53EAF9B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2965,7 +2965,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5AB514ED-F2A1-424B-914D-577CA10B619D}" type="CELLRANGE">
+                    <a:fld id="{C053D4F9-CA7B-470D-A7FF-3C6DD128BCE8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2999,7 +2999,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34E20F04-0358-40D2-929B-2C85ABC7EDCB}" type="CELLRANGE">
+                    <a:fld id="{B6E41F90-2A68-4CBC-8BCA-52227EE92DA1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3033,7 +3033,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{41483AC7-E53A-4F93-9DFC-6EA688586E48}" type="CELLRANGE">
+                    <a:fld id="{C5FF5A2C-2417-4368-B14E-3F0EBD51CAC7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3168,7 +3168,7 @@
                   <c:v>6.8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.4000000000000004</c:v>
+                  <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>6.5</c:v>
@@ -3411,7 +3411,7 @@
                   <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>960</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>1540</c:v>
@@ -5196,7 +5196,7 @@
   <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5495,10 +5495,10 @@
         <v>84</v>
       </c>
       <c r="B21">
-        <v>4.4000000000000004</v>
+        <v>3.4</v>
       </c>
       <c r="C21">
-        <v>960</v>
+        <v>750</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Add entry for Bald Rock
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shawn\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCAC450-AC1B-4B85-BB1D-1443A16F60A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D3C185-BDCB-4620-B7E9-57A2314C7A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4628" yWindow="225" windowWidth="21142" windowHeight="14333" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hike Difficulties" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="89">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>Mather Memorial Parkway</t>
+  </si>
+  <si>
+    <t>Bald Rock</t>
   </si>
 </sst>
 </file>
@@ -415,7 +418,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{275156AB-E614-4B42-A614-EB59DD5969AF}" type="CELLRANGE">
+                    <a:fld id="{A5CDBBBA-4430-48F6-AC4E-4DE385DD90B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -449,7 +452,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0299DA39-6C9B-450D-8AF2-FB4609D6DACA}" type="CELLRANGE">
+                    <a:fld id="{7E8E33AA-E5EE-4160-85BA-F5EBEF0C23D6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -483,7 +486,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1D9B40E8-AAAE-4FF5-BE6B-58F38C60FE92}" type="CELLRANGE">
+                    <a:fld id="{B14F112D-998F-4241-9B8B-4012E146634E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -517,7 +520,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D273D6E-34CF-48E1-801C-EF0C0691A773}" type="CELLRANGE">
+                    <a:fld id="{82A23430-02F8-442A-9696-60CF25B36F01}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -551,7 +554,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D335CA27-6BC6-4004-A80C-0FC28637AF49}" type="CELLRANGE">
+                    <a:fld id="{EC61D4E5-F253-417C-90E4-995A836AFFF6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -585,7 +588,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7A463740-EA8F-447C-AF28-AF4CD4416FD1}" type="CELLRANGE">
+                    <a:fld id="{2BBDE2C0-87A6-4F92-82DF-6301528C3D36}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -619,7 +622,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE56329A-49C6-4EB9-B6DA-7633BD34F0C8}" type="CELLRANGE">
+                    <a:fld id="{D4A6536B-BD85-4822-916C-094F07ECC6F7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -653,7 +656,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0CD7E503-553A-442B-918C-FDD7273EC68E}" type="CELLRANGE">
+                    <a:fld id="{587D1EE3-2D54-48F3-99CD-D879858224F2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -687,7 +690,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4839E1EE-76F3-4B94-91BA-660173DFCD6B}" type="CELLRANGE">
+                    <a:fld id="{6808FBE0-316B-4126-8DDD-A564108F7011}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -721,7 +724,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{113D20C6-7CBF-44F5-89E3-C21C3129B690}" type="CELLRANGE">
+                    <a:fld id="{6CC79359-87EC-4723-A078-F48D28A39157}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -755,7 +758,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{812A8418-C96A-468D-8C77-E7D47CE8E28A}" type="CELLRANGE">
+                    <a:fld id="{759140C8-8C76-4CB1-842B-A96CA477B5B6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -789,7 +792,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{27FBC4C7-E6EB-4221-B116-0476B9F83B74}" type="CELLRANGE">
+                    <a:fld id="{04E42AE5-8AB1-4CE2-81BD-E3E6BBA832BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -823,7 +826,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC387B76-0086-4922-A2AE-32A334B0C57E}" type="CELLRANGE">
+                    <a:fld id="{6D363D65-F77F-49C1-9160-0D62ACCE69DA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -857,7 +860,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{09AFEE3E-25FF-4185-B7F3-9824F17BC5C9}" type="CELLRANGE">
+                    <a:fld id="{7939D106-9EFD-4DE2-828E-CF2BCFC385F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -891,7 +894,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{204DAB1E-DF0F-4285-8CFD-C7D27FB06529}" type="CELLRANGE">
+                    <a:fld id="{58977053-5997-4A59-9EDF-0A2DC7705A36}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -925,7 +928,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{923E856C-1D87-4F7F-97A9-555887E77698}" type="CELLRANGE">
+                    <a:fld id="{288C2758-8E32-4265-9D67-FE548560CBD6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -959,7 +962,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F3F568D-BE00-48E7-A345-6C544BC4B652}" type="CELLRANGE">
+                    <a:fld id="{5AA128B5-7D51-4012-919E-0DC62FF44AFE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -993,7 +996,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B1A939B-DCD6-454A-8FA3-D996F674F799}" type="CELLRANGE">
+                    <a:fld id="{D10061C3-F1ED-4DB5-A9A9-783E87F25BBE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1027,7 +1030,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5166451-793A-48CB-BAE4-EB671EA1A948}" type="CELLRANGE">
+                    <a:fld id="{5CC6DBC7-8E68-442F-8E03-5AE4059F9DA1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1061,7 +1064,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2ED2E40D-94A0-41F4-B370-2AF69FB90912}" type="CELLRANGE">
+                    <a:fld id="{5CE6C167-404F-48F8-B12E-5FDEFD42DF4C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1095,7 +1098,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC154D96-E05A-4336-9638-904D58FC7654}" type="CELLRANGE">
+                    <a:fld id="{25FE0E30-335F-4561-934F-3E55D3646BF7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1129,7 +1132,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D08D387F-10AD-4746-9A29-CCA2CE1C6454}" type="CELLRANGE">
+                    <a:fld id="{6238388E-CC0E-4B3D-B8FC-E0CBF9F78137}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1163,7 +1166,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E7C0923-80B8-4B9A-892F-FCC0BCD5037C}" type="CELLRANGE">
+                    <a:fld id="{52A64685-C45A-43DA-9761-6DDDAFC10368}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1197,7 +1200,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CDB1F024-9A08-467D-AC29-BC2F2E5BF99B}" type="CELLRANGE">
+                    <a:fld id="{A1245F00-E963-4E7E-8C42-17036CD1E936}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1231,7 +1234,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB6A1D53-69B3-4A1C-A857-FF251E30778A}" type="CELLRANGE">
+                    <a:fld id="{CB9B6553-4043-4281-84D0-227ED86BEAC5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1265,7 +1268,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5690EDF0-D2BB-4EF6-90C1-E38DFD19F632}" type="CELLRANGE">
+                    <a:fld id="{B073E70C-2F1B-4295-849F-B1101025A95E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1299,7 +1302,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{22B53D79-3573-4039-963A-B27A50DF01E2}" type="CELLRANGE">
+                    <a:fld id="{D991024B-2A2F-4AA1-90D0-74E5C92E27A9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1333,7 +1336,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD56E305-7544-40D5-A646-25B0DEDD59BC}" type="CELLRANGE">
+                    <a:fld id="{3EE1DE25-7C34-43D8-A792-9C3B01DC14D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1367,7 +1370,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{25CFBD8C-D105-40C5-8842-27585BB5AEC2}" type="CELLRANGE">
+                    <a:fld id="{96F17CE9-43DB-4BFA-BAB1-003A34288E1F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1401,7 +1404,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{77565DDD-3B51-41BD-90E9-79A247F7BF19}" type="CELLRANGE">
+                    <a:fld id="{64C2DA87-B52F-4F25-AF4F-8DACD043C6E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1435,7 +1438,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4094102-8B69-4D20-BCED-47D371EECFED}" type="CELLRANGE">
+                    <a:fld id="{2B976423-378E-4241-A613-561C25EEB454}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1469,7 +1472,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5E14899-7CC8-4A4C-A505-625792036513}" type="CELLRANGE">
+                    <a:fld id="{B9230B4F-58F1-416A-9EFE-5558762CBDA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1503,7 +1506,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5427C8E8-B4EC-407D-8BA6-954C217CB63E}" type="CELLRANGE">
+                    <a:fld id="{DAE8A3EA-BBED-4716-95D7-FB506F7A9F91}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1537,7 +1540,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C621F095-4755-4BCE-A306-DE753F6CEF25}" type="CELLRANGE">
+                    <a:fld id="{B98511AA-1E80-4EBF-A6E4-B1448A664A69}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1571,7 +1574,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF1D5221-AEBD-4FE5-BEF2-2BBE666C1C1A}" type="CELLRANGE">
+                    <a:fld id="{CA1443C4-1AAE-439C-955D-950615643A83}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1605,7 +1608,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{55AD617D-DA26-4A84-A68C-5B7F47E55360}" type="CELLRANGE">
+                    <a:fld id="{7518CFDA-A62A-48C7-9083-08729B035157}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1639,7 +1642,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8F5758CD-89FD-4D81-939A-190F213D2A94}" type="CELLRANGE">
+                    <a:fld id="{D3DA633A-F6DE-4BBB-BB2B-C090181A844A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1673,7 +1676,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42DE0031-E484-4F49-BBC6-79C9AE54BE76}" type="CELLRANGE">
+                    <a:fld id="{48065AAF-D3E2-4FF6-B984-EFB8D06CCB13}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1707,7 +1710,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BD2EE8A2-F73F-4733-AF38-F9EFE6C56FAE}" type="CELLRANGE">
+                    <a:fld id="{DD1F90DC-6BC9-49FE-B57A-F7DD179347A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1741,7 +1744,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2FD4E411-5940-4CAF-87F1-9EED0DF4D918}" type="CELLRANGE">
+                    <a:fld id="{52C5A9CF-50BA-4BC2-A59E-7055BB026806}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1775,7 +1778,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A7DEA7C-E0BA-4053-8C01-2B928DFBD10C}" type="CELLRANGE">
+                    <a:fld id="{5584AAA7-D3F0-4FA0-A9C2-BBF696D27687}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1809,7 +1812,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C746257-E888-47CB-9070-FBDB79E53D5C}" type="CELLRANGE">
+                    <a:fld id="{189854D7-F3AF-478F-80B7-A377D5AB58C8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1843,7 +1846,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{971A2CC3-28A3-4453-A18C-6F3B924BBF0F}" type="CELLRANGE">
+                    <a:fld id="{6081FA79-7257-41E7-A608-DB7A6EDDBF01}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1877,7 +1880,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{174BE77C-F591-4ADB-A771-2021DE97FBEC}" type="CELLRANGE">
+                    <a:fld id="{82E4C480-F0DB-496D-8FC3-F646E1559002}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1911,7 +1914,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7B35A000-9D66-40E3-ACFC-26BA66E217A0}" type="CELLRANGE">
+                    <a:fld id="{1F86F05A-AD70-4F63-9D40-EB94AE6ADAA9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1945,7 +1948,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E2448D51-1ABA-497F-9D00-6E3883592FA4}" type="CELLRANGE">
+                    <a:fld id="{CA191BBB-3850-49B1-9968-E60E5F10393D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1979,7 +1982,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4FE973C-0D3A-4822-9025-09415565B6D0}" type="CELLRANGE">
+                    <a:fld id="{1C20F73A-33B0-4796-A7D8-CF6B3C629344}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2013,7 +2016,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14C0EFE3-F16F-4EB9-A477-952C5273F462}" type="CELLRANGE">
+                    <a:fld id="{B80A10DA-5A0F-4BAE-8FEF-E4213D6C33E0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2047,7 +2050,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{890D614F-F5FE-4EBE-B23E-964AC9ED9AF8}" type="CELLRANGE">
+                    <a:fld id="{03FB9139-1DB0-4E28-952F-A94000D132D5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2081,7 +2084,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7021101D-BD75-424C-BB43-9793CE1857C0}" type="CELLRANGE">
+                    <a:fld id="{25408FBC-D507-4EB9-9DC7-EF1B22DBF068}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2115,7 +2118,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{169BB4D5-60C4-4E06-95FE-8260736F2BAF}" type="CELLRANGE">
+                    <a:fld id="{E06FD4BA-3FBA-4854-B9FC-25D0A4F4A8D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2149,7 +2152,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3AEBB82E-2715-4F8C-8C76-F0870901FFDA}" type="CELLRANGE">
+                    <a:fld id="{E554BD4E-870D-4EA7-8B10-319904AD3D33}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2183,7 +2186,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{00BB2E75-A8B3-40B1-A1AE-0B7E670E079A}" type="CELLRANGE">
+                    <a:fld id="{0D3D3558-1E1D-4E53-8AA3-EAC12589B103}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2217,7 +2220,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9A5E7E59-E8FB-41F2-B0EE-B35DAE2AB226}" type="CELLRANGE">
+                    <a:fld id="{1EC459AF-A951-4ED3-BA06-E6CF07CF9B26}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2251,7 +2254,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8618AA79-A800-4670-8A5B-481AD3AC8BE5}" type="CELLRANGE">
+                    <a:fld id="{4D02617F-29B8-4362-B082-4E5B73E26C12}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2285,7 +2288,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5CEBFBEB-9EA8-4568-8808-3FB7B0A7ABEC}" type="CELLRANGE">
+                    <a:fld id="{167803CF-CAA2-41F7-B066-486568DEF7F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2319,7 +2322,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CCC81A3E-549A-4E2C-896A-47BD6E941B47}" type="CELLRANGE">
+                    <a:fld id="{C35A8238-91B3-4679-802F-17B06D1F05DF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2353,7 +2356,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FCBABF70-760C-4C02-80E5-B61958E07BF5}" type="CELLRANGE">
+                    <a:fld id="{73A008CB-96AE-488D-90EB-9D86B2469D5E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2387,7 +2390,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0CAEA6D5-3234-4EDB-9FFA-AA9434E4A1A2}" type="CELLRANGE">
+                    <a:fld id="{68030A63-684D-4B52-9F4E-BACA5082E282}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2421,7 +2424,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{215A3B14-EB65-4918-BC8D-A031CEF6360E}" type="CELLRANGE">
+                    <a:fld id="{B6B9EA44-F9A6-4315-BA59-8343E8417940}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2455,7 +2458,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AA8C36C7-BCBD-40FA-BBD1-8A35806C8D83}" type="CELLRANGE">
+                    <a:fld id="{3CEFFB75-E0B4-4FBA-AFB0-821D8A039A3C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2489,7 +2492,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{055EE37D-5EC8-4AF8-A485-728E81F84F30}" type="CELLRANGE">
+                    <a:fld id="{0B2714DF-B834-4D91-9CAA-D43102702576}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2523,7 +2526,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C9B41283-CF31-4417-9542-B350E18F307C}" type="CELLRANGE">
+                    <a:fld id="{10C20FDB-F0CD-49B6-A6AC-82F15EC234D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2557,7 +2560,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40AA0154-A9C0-469A-8D85-72935972839B}" type="CELLRANGE">
+                    <a:fld id="{B61D510E-90FF-463B-84B6-29EABADA0CE2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2591,7 +2594,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C36A5846-C7D5-4DF3-BFE3-DE728F2E2FEE}" type="CELLRANGE">
+                    <a:fld id="{F7E1F03E-0AB3-4328-A293-E2D998132C01}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2625,7 +2628,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E29046E-7FB1-4C07-A156-6C6D36B80409}" type="CELLRANGE">
+                    <a:fld id="{BDB90B86-FC7B-4B1D-870F-B1DFCBCDA74E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2659,7 +2662,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F4E73DA3-A842-457E-867A-D98AA8617631}" type="CELLRANGE">
+                    <a:fld id="{F8860CC9-B272-403A-946A-28FD1AD11BDF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2693,7 +2696,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1F97AD5F-8DC3-4524-9E74-DBE2B0FB4D2B}" type="CELLRANGE">
+                    <a:fld id="{291EB2BF-AAE1-467E-9EEE-2DAC226F21E5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2727,7 +2730,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02934CEF-51F6-4FAF-8F74-7EA98E992D52}" type="CELLRANGE">
+                    <a:fld id="{794C815C-3088-494E-BAA9-57CE70471C1E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2761,7 +2764,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9919A0C-906A-42FA-A041-D3B61E8416A3}" type="CELLRANGE">
+                    <a:fld id="{93E9E27C-10DB-4F6D-8660-25BE29CED5E9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2795,7 +2798,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC502EA2-6C3D-4C5B-A20C-747D094913FE}" type="CELLRANGE">
+                    <a:fld id="{520C617F-8B54-43B5-9EB8-64350FE00203}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2829,7 +2832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC03EA03-48BB-4E51-AA85-388ACDAEDEAC}" type="CELLRANGE">
+                    <a:fld id="{60690370-C7F5-4946-80EC-4997A4ADFE76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2863,7 +2866,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD8A4D50-EDA4-4FFF-9938-C39AD0B242E5}" type="CELLRANGE">
+                    <a:fld id="{4212481D-2E64-42ED-B0EA-B76494F174F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2897,7 +2900,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12C7EC12-0E71-47CB-B677-FFB7FE1E6EE2}" type="CELLRANGE">
+                    <a:fld id="{128E593B-CA7B-4DD8-8E80-862DC887BD86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2931,7 +2934,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8CB5A86-F5E6-4C29-A626-F564C6FC3560}" type="CELLRANGE">
+                    <a:fld id="{36DD4985-4553-43F2-AB7B-C40759A7F082}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2965,7 +2968,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{108295C4-0F4B-41EF-A16C-3ECE4617F3BA}" type="CELLRANGE">
+                    <a:fld id="{131EC869-F585-4B0C-BFFC-DB29BEBD1C31}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2999,7 +3002,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C7B912C-9548-4A97-BCFB-729643D1DE2F}" type="CELLRANGE">
+                    <a:fld id="{C82AEE16-7920-4645-A12B-BA77785C149E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3033,7 +3036,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8A29B16D-BFF3-403B-9943-6ED756C12F87}" type="CELLRANGE">
+                    <a:fld id="{2DC1F393-D2C4-4834-B6FD-D648C155A6E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3057,6 +3060,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-C555-4B08-8BEC-89FEEB45465B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="78"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{CCF2A0CE-1DF1-44C0-B71F-59C5087699F7}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-363E-4205-A432-E7DFA9A91746}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3106,242 +3143,245 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$79</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="78"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>7.6</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>11.866666666666667</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>10.3</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>6.3</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>7.5</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>3.4</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>2.9</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>7.7</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>8.75</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>7.9</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>11.3</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>6.8</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>3.4</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>9.6</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>11.6</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>12.5</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>9.1</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>9.5500000000000007</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>12.2</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>9.75</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>5.4</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>11.9</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>4.2</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>7.2</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>2.7</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>3.3</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="69">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>9.9</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>5.8</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="73">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="74">
                   <c:v>5.6</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="75">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="76">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="77">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="78">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -3349,242 +3389,245 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$79</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="78"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>3950</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2840</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4700</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2010</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>690</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1270</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1920</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>2970</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>3110</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>940</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>3030</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>3200</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>1200</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>1540</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>2380</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>3290</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>2660</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>2780</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>2425</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>4100</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>4800</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>4120</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>3420</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>2050</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>1450</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>3160</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>1050</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>880</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>860</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>1260</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>2600</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>3100</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>1630</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>1930</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="69">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>3180</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>1540</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="73">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="74">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="75">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="76">
                   <c:v>760</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="77">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="78">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -3604,19 +3647,19 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="2">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>omg yikes wtf</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>easy (but long)</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>moderate</c:v>
@@ -3628,67 +3671,67 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="10">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="12">
                     <c:v>moderate (because rough)</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="13">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="15">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>strenuous</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="17">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>easy</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="19">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="21">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="22">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="24">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="25">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="27">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="28">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="29">
+                  <c:pt idx="30">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="30">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="31">
                     <c:v>strenuous</c:v>
@@ -3703,34 +3746,34 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="35">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="36">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="36">
+                  <c:pt idx="37">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="37">
+                  <c:pt idx="38">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="38">
+                  <c:pt idx="39">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="39">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="40">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="41">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="42">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="42">
+                  <c:pt idx="43">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="43">
+                  <c:pt idx="44">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="44">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="45">
                     <c:v>easy</c:v>
@@ -3739,19 +3782,19 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="47">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="48">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="48">
+                  <c:pt idx="49">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="49">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="50">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="51">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="52">
                     <c:v>moderate</c:v>
@@ -3760,75 +3803,78 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="54">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="55">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="55">
+                  <c:pt idx="56">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="56">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="57">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="58">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="59">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="59">
+                  <c:pt idx="60">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="60">
+                  <c:pt idx="61">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="61">
+                  <c:pt idx="62">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="62">
+                  <c:pt idx="63">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="63">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="64">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="65">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="66">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="66">
+                  <c:pt idx="67">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="67">
+                  <c:pt idx="68">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="68">
+                  <c:pt idx="69">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="69">
+                  <c:pt idx="70">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="70">
+                  <c:pt idx="71">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="71">
+                  <c:pt idx="72">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="72">
+                  <c:pt idx="73">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="73">
+                  <c:pt idx="74">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="74">
+                  <c:pt idx="75">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="75">
+                  <c:pt idx="76">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="76">
+                  <c:pt idx="77">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="77">
+                  <c:pt idx="78">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -4881,10 +4927,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D79" totalsRowShown="0">
-  <autoFilter ref="A1:D79" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D79">
-    <sortCondition ref="A1:A79"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D80" totalsRowShown="0">
+  <autoFilter ref="A1:D80" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D80">
+    <sortCondition ref="A1:A80"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -5193,10 +5239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5237,13 +5283,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="B3">
-        <v>7.6</v>
+        <v>9.1</v>
       </c>
       <c r="C3">
-        <v>3950</v>
+        <v>3100</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -5251,84 +5297,84 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="B4">
-        <v>9.1999999999999993</v>
+        <v>7.6</v>
       </c>
       <c r="C4">
-        <v>2840</v>
+        <v>3950</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>8.5</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C5">
-        <v>4700</v>
+        <v>2840</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>8.5</v>
+      </c>
+      <c r="C6">
+        <v>4700</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <f>17.8*2/3</f>
         <v>11.866666666666667</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>2010</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>10.3</v>
-      </c>
-      <c r="C7">
-        <v>690</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>10.3</v>
       </c>
       <c r="C8">
-        <v>1270</v>
+        <v>690</v>
       </c>
       <c r="D8" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>2400</v>
+        <v>1270</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
@@ -5336,13 +5382,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B10">
-        <v>6.3</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>1920</v>
+        <v>2400</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
@@ -5350,13 +5396,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="B11">
-        <v>7.5</v>
+        <v>6.3</v>
       </c>
       <c r="C11">
-        <v>2970</v>
+        <v>1920</v>
       </c>
       <c r="D11" t="s">
         <v>1</v>
@@ -5364,55 +5410,55 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B12">
-        <v>8.1999999999999993</v>
+        <v>7.5</v>
       </c>
       <c r="C12">
-        <v>3110</v>
+        <v>2970</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B13">
-        <v>3.4</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C13">
-        <v>940</v>
+        <v>3110</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="C14">
-        <v>1000</v>
+        <v>940</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15">
-        <v>2.9</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>1090</v>
+        <v>1000</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -5420,57 +5466,57 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>7.7</v>
+        <v>2.9</v>
       </c>
       <c r="C16">
-        <v>3030</v>
+        <v>1090</v>
       </c>
       <c r="D16" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17">
+        <v>7.7</v>
+      </c>
+      <c r="C17">
+        <v>3030</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>81</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <f>35/4</f>
         <v>8.75</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <f>9000/4</f>
         <v>2250</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18">
-        <v>7.9</v>
-      </c>
-      <c r="C18">
-        <v>3200</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19">
-        <v>11.3</v>
+        <v>7.9</v>
       </c>
       <c r="C19">
-        <v>3850</v>
+        <v>3200</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -5478,27 +5524,27 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20">
-        <v>6.8</v>
+        <v>11.3</v>
       </c>
       <c r="C20">
-        <v>1200</v>
+        <v>3850</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B21">
-        <v>3.4</v>
+        <v>6.8</v>
       </c>
       <c r="C21">
-        <v>750</v>
+        <v>1200</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -5506,27 +5552,27 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="B22">
-        <v>6.5</v>
+        <v>3.4</v>
       </c>
       <c r="C22">
-        <v>1540</v>
+        <v>750</v>
       </c>
       <c r="D22" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B23">
-        <v>8.5</v>
+        <v>6.5</v>
       </c>
       <c r="C23">
-        <v>2380</v>
+        <v>1540</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
@@ -5534,85 +5580,85 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24">
-        <v>9.6</v>
+        <v>8.5</v>
       </c>
       <c r="C24">
-        <v>3290</v>
+        <v>2380</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>9.6</v>
+      </c>
+      <c r="C25">
+        <v>3290</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>82</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <f>14.6/2</f>
         <v>7.3</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <f>3160/2</f>
         <v>1580</v>
       </c>
-      <c r="D25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26">
-        <v>11.6</v>
-      </c>
-      <c r="C26">
-        <v>2660</v>
-      </c>
       <c r="D26" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B27">
-        <v>12.5</v>
+        <v>11.6</v>
       </c>
       <c r="C27">
-        <v>2780</v>
+        <v>2660</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="B28">
-        <v>9</v>
+        <v>12.5</v>
       </c>
       <c r="C28">
-        <v>1680</v>
+        <v>2780</v>
       </c>
       <c r="D28" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B29">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="C29">
-        <v>1580</v>
+        <v>1680</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
@@ -5620,57 +5666,57 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B30">
-        <v>5.2</v>
+        <v>9.1</v>
       </c>
       <c r="C30">
-        <v>1000</v>
+        <v>1580</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31">
+        <v>5.2</v>
+      </c>
+      <c r="C31">
+        <v>1000</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>79</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <f>19.1/2</f>
         <v>9.5500000000000007</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <f>4850/2</f>
         <v>2425</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32">
-        <v>9.5</v>
-      </c>
-      <c r="C32">
-        <v>4100</v>
-      </c>
-      <c r="D32" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="B33">
-        <v>14</v>
+        <v>9.5</v>
       </c>
       <c r="C33">
-        <v>4800</v>
+        <v>4100</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
@@ -5678,13 +5724,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34">
         <v>14</v>
       </c>
-      <c r="B34">
-        <v>12.2</v>
-      </c>
       <c r="C34">
-        <v>4120</v>
+        <v>4800</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
@@ -5692,13 +5738,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B35">
-        <v>12</v>
+        <v>12.2</v>
       </c>
       <c r="C35">
-        <v>3420</v>
+        <v>4120</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
@@ -5706,99 +5752,99 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>3420</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>37</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <f>19.5/2</f>
         <v>9.75</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <f>4400*7/8</f>
         <v>3850</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37">
-        <v>6.9</v>
-      </c>
-      <c r="C37">
-        <v>2050</v>
-      </c>
-      <c r="D37" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="B38">
-        <v>5.4</v>
+        <v>6.9</v>
       </c>
       <c r="C38">
-        <v>1450</v>
+        <v>2050</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B39">
-        <v>11.9</v>
+        <v>5.4</v>
       </c>
       <c r="C39">
-        <v>3160</v>
+        <v>1450</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>11.9</v>
       </c>
       <c r="C40">
-        <v>400</v>
+        <v>3160</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="B41">
-        <v>11.4</v>
+        <v>3</v>
       </c>
       <c r="C41">
-        <v>2550</v>
+        <v>400</v>
       </c>
       <c r="D41" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="B42">
-        <v>10.8</v>
+        <v>11.4</v>
       </c>
       <c r="C42">
-        <v>1050</v>
+        <v>2550</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
@@ -5806,69 +5852,69 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="B43">
-        <v>8.5</v>
+        <v>10.8</v>
       </c>
       <c r="C43">
-        <v>3350</v>
+        <v>1050</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B44">
-        <v>2.8</v>
+        <v>8.5</v>
       </c>
       <c r="C44">
-        <v>880</v>
+        <v>3350</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B45">
-        <v>10.4</v>
+        <v>2.8</v>
       </c>
       <c r="C45">
-        <v>1420</v>
+        <v>880</v>
       </c>
       <c r="D45" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B46">
-        <v>0.9</v>
+        <v>10.4</v>
       </c>
       <c r="C46">
-        <v>200</v>
+        <v>1420</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B47">
-        <v>4.2</v>
+        <v>0.9</v>
       </c>
       <c r="C47">
-        <v>860</v>
+        <v>200</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
@@ -5876,13 +5922,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B48">
-        <v>4.8</v>
+        <v>4.2</v>
       </c>
       <c r="C48">
-        <v>1260</v>
+        <v>860</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
@@ -5890,55 +5936,55 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B49">
-        <v>4</v>
+        <v>4.8</v>
       </c>
       <c r="C49">
-        <v>2600</v>
+        <v>1260</v>
       </c>
       <c r="D49" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B50">
-        <v>1.4</v>
+        <v>4</v>
       </c>
       <c r="C50">
-        <v>375</v>
+        <v>2600</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B51">
-        <v>13.6</v>
+        <v>1.4</v>
       </c>
       <c r="C51">
-        <v>3930</v>
+        <v>375</v>
       </c>
       <c r="D51" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B52">
-        <v>10.5</v>
+        <v>13.6</v>
       </c>
       <c r="C52">
-        <v>3100</v>
+        <v>3930</v>
       </c>
       <c r="D52" t="s">
         <v>10</v>
@@ -5946,27 +5992,27 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B53">
-        <v>7</v>
+        <v>10.5</v>
       </c>
       <c r="C53">
-        <v>1670</v>
+        <v>3100</v>
       </c>
       <c r="D53" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B54">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="C54">
-        <v>2400</v>
+        <v>1670</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
@@ -5974,13 +6020,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B55">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C55">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D55" t="s">
         <v>1</v>
@@ -5988,55 +6034,55 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B56">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C56">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B57">
-        <v>7.2</v>
+        <v>4.8</v>
       </c>
       <c r="C57">
-        <v>1630</v>
+        <v>1300</v>
       </c>
       <c r="D57" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B58">
-        <v>2.7</v>
+        <v>7.2</v>
       </c>
       <c r="C58">
-        <v>1090</v>
+        <v>1630</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="B59">
-        <v>4.8</v>
+        <v>2.7</v>
       </c>
       <c r="C59">
-        <v>1470</v>
+        <v>1090</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
@@ -6044,97 +6090,97 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B60">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C60">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D60" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B61">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C61">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D61" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B62">
-        <v>3.3</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C62">
-        <v>600</v>
+        <v>3490</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B63">
-        <v>8.5</v>
+        <v>3.3</v>
       </c>
       <c r="C63">
-        <v>1930</v>
+        <v>600</v>
       </c>
       <c r="D63" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B64">
-        <v>2.2000000000000002</v>
+        <v>8.5</v>
       </c>
       <c r="C64">
-        <v>750</v>
+        <v>1930</v>
       </c>
       <c r="D64" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B65">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C65">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D65" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B66">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C66">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D66" t="s">
         <v>1</v>
@@ -6142,186 +6188,200 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67">
+        <v>7.3</v>
+      </c>
+      <c r="C67">
+        <v>2250</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
         <v>25</v>
       </c>
-      <c r="B67">
+      <c r="B68">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C67">
+      <c r="C68">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
-        <v>49</v>
-      </c>
-      <c r="B68">
-        <v>1.2</v>
-      </c>
-      <c r="C68">
-        <v>500</v>
-      </c>
-      <c r="D68" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B69">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C69">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D69" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B70">
-        <v>6.5</v>
+        <v>11</v>
       </c>
       <c r="C70">
-        <v>1650</v>
+        <v>3060</v>
       </c>
       <c r="D70" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B71">
-        <v>9.9</v>
+        <v>6.5</v>
       </c>
       <c r="C71">
-        <v>3180</v>
+        <v>1650</v>
       </c>
       <c r="D71" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="B72">
-        <v>5.8</v>
+        <v>9.9</v>
       </c>
       <c r="C72">
-        <v>1540</v>
+        <v>3180</v>
       </c>
       <c r="D72" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B73">
-        <v>0.4</v>
+        <v>5.8</v>
       </c>
       <c r="C73">
-        <v>100</v>
+        <v>1540</v>
       </c>
       <c r="D73" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B74">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C74">
-        <v>3550</v>
+        <v>100</v>
       </c>
       <c r="D74" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="B75">
-        <v>5.6</v>
+        <v>7.3</v>
       </c>
       <c r="C75">
-        <v>1680</v>
+        <v>3550</v>
       </c>
       <c r="D75" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B76">
-        <v>10.8</v>
+        <v>5.6</v>
       </c>
       <c r="C76">
-        <v>1800</v>
+        <v>1680</v>
       </c>
       <c r="D76" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B77">
-        <v>7</v>
+        <v>10.8</v>
       </c>
       <c r="C77">
-        <v>760</v>
+        <v>1800</v>
       </c>
       <c r="D77" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78">
+        <v>7</v>
+      </c>
+      <c r="C78">
+        <v>760</v>
+      </c>
+      <c r="D78" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
         <v>55</v>
       </c>
-      <c r="B78">
+      <c r="B79">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C78">
+      <c r="C79">
         <v>3800</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D79" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
         <v>29</v>
       </c>
-      <c r="B79">
+      <c r="B80">
         <v>6</v>
       </c>
-      <c r="C79">
+      <c r="C80">
         <v>2180</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D80" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Brown Peak and Green Park
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shawn\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D3C185-BDCB-4620-B7E9-57A2314C7A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A2F0EC-1C25-4647-ACF5-78B1F9D0B746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>Bald Rock</t>
+  </si>
+  <si>
+    <t>Brown Peak</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5CDBBBA-4430-48F6-AC4E-4DE385DD90B2}" type="CELLRANGE">
+                    <a:fld id="{8D3DA45D-E5BC-47E7-BE96-E4D182FA5246}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -452,7 +455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E8E33AA-E5EE-4160-85BA-F5EBEF0C23D6}" type="CELLRANGE">
+                    <a:fld id="{AE1B2FD0-A260-40C4-808E-F8EFE514A693}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -486,7 +489,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B14F112D-998F-4241-9B8B-4012E146634E}" type="CELLRANGE">
+                    <a:fld id="{0C8522D9-8027-4376-9C6D-2C0558B4EBB5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -520,7 +523,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{82A23430-02F8-442A-9696-60CF25B36F01}" type="CELLRANGE">
+                    <a:fld id="{FC89BAD4-6D49-4142-BA0E-5BB2F9742489}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -554,7 +557,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC61D4E5-F253-417C-90E4-995A836AFFF6}" type="CELLRANGE">
+                    <a:fld id="{0AB9FE5D-1F18-4364-AABD-98DD9CADF1D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -588,7 +591,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2BBDE2C0-87A6-4F92-82DF-6301528C3D36}" type="CELLRANGE">
+                    <a:fld id="{2F489AB8-97A5-4736-9E1B-EC59D29138D1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -622,7 +625,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4A6536B-BD85-4822-916C-094F07ECC6F7}" type="CELLRANGE">
+                    <a:fld id="{3A02411F-78CF-485F-BD38-B18C47131B11}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -656,7 +659,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{587D1EE3-2D54-48F3-99CD-D879858224F2}" type="CELLRANGE">
+                    <a:fld id="{DF384655-7EF2-4DB0-8BAD-B2D6A222B8D9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -690,7 +693,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6808FBE0-316B-4126-8DDD-A564108F7011}" type="CELLRANGE">
+                    <a:fld id="{3E60A3E5-4087-4C9C-B24F-3F780046C356}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -724,7 +727,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CC79359-87EC-4723-A078-F48D28A39157}" type="CELLRANGE">
+                    <a:fld id="{1A1018E1-BB87-4114-BFF0-FF7150A93DD7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -758,7 +761,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{759140C8-8C76-4CB1-842B-A96CA477B5B6}" type="CELLRANGE">
+                    <a:fld id="{EFA89423-58D7-4D28-90E6-8AE70E03EA4C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -792,7 +795,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{04E42AE5-8AB1-4CE2-81BD-E3E6BBA832BA}" type="CELLRANGE">
+                    <a:fld id="{34089EC4-0F52-4735-BF92-730371234ACA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -826,7 +829,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D363D65-F77F-49C1-9160-0D62ACCE69DA}" type="CELLRANGE">
+                    <a:fld id="{0E951527-35F1-4127-BD83-2FC28841BE15}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -860,7 +863,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7939D106-9EFD-4DE2-828E-CF2BCFC385F5}" type="CELLRANGE">
+                    <a:fld id="{E8A380D2-BC28-4D02-AA70-02721961FCA3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -894,7 +897,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58977053-5997-4A59-9EDF-0A2DC7705A36}" type="CELLRANGE">
+                    <a:fld id="{01846907-7331-4DE5-81BA-C50765BA716A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -928,7 +931,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{288C2758-8E32-4265-9D67-FE548560CBD6}" type="CELLRANGE">
+                    <a:fld id="{5BF7342D-B9BE-4D74-B4C1-9598D5161CED}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -962,7 +965,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5AA128B5-7D51-4012-919E-0DC62FF44AFE}" type="CELLRANGE">
+                    <a:fld id="{F81993E3-8F00-414E-BB04-09CD4EC28CD1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -996,7 +999,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D10061C3-F1ED-4DB5-A9A9-783E87F25BBE}" type="CELLRANGE">
+                    <a:fld id="{2C222C73-093A-4713-BC55-3EBD8369C2B6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1030,7 +1033,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5CC6DBC7-8E68-442F-8E03-5AE4059F9DA1}" type="CELLRANGE">
+                    <a:fld id="{8D9C6600-2913-47F5-9972-28CAC85CCEE8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1064,7 +1067,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5CE6C167-404F-48F8-B12E-5FDEFD42DF4C}" type="CELLRANGE">
+                    <a:fld id="{0918DDFA-F0A6-4FE5-8B77-868341165AD0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1098,7 +1101,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{25FE0E30-335F-4561-934F-3E55D3646BF7}" type="CELLRANGE">
+                    <a:fld id="{34CE7A06-8622-41D2-9EAB-99FC25837849}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1132,7 +1135,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6238388E-CC0E-4B3D-B8FC-E0CBF9F78137}" type="CELLRANGE">
+                    <a:fld id="{30F643A9-CB5F-4437-9844-9AA18ECDBB04}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1166,7 +1169,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{52A64685-C45A-43DA-9761-6DDDAFC10368}" type="CELLRANGE">
+                    <a:fld id="{3197FC1B-9FC9-4B3A-B467-EDC364BC9ACF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1200,7 +1203,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A1245F00-E963-4E7E-8C42-17036CD1E936}" type="CELLRANGE">
+                    <a:fld id="{A040B548-24FE-4AD1-9B4F-561DD99A22BD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1234,7 +1237,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB9B6553-4043-4281-84D0-227ED86BEAC5}" type="CELLRANGE">
+                    <a:fld id="{3E0C7868-9098-4F26-9698-823A8FCEF58B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1268,7 +1271,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B073E70C-2F1B-4295-849F-B1101025A95E}" type="CELLRANGE">
+                    <a:fld id="{BEB6A28F-2C8F-44F1-9B04-5F5947FB2530}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1302,7 +1305,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D991024B-2A2F-4AA1-90D0-74E5C92E27A9}" type="CELLRANGE">
+                    <a:fld id="{F6957CFD-333D-4214-9CE3-0DAE2FCC2A06}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1336,7 +1339,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3EE1DE25-7C34-43D8-A792-9C3B01DC14D7}" type="CELLRANGE">
+                    <a:fld id="{1033C60C-895C-4CC5-A9C8-A9BFC01F13CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1370,7 +1373,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96F17CE9-43DB-4BFA-BAB1-003A34288E1F}" type="CELLRANGE">
+                    <a:fld id="{E0A0008C-25C6-4E85-B133-F2B6436D621B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1404,7 +1407,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{64C2DA87-B52F-4F25-AF4F-8DACD043C6E8}" type="CELLRANGE">
+                    <a:fld id="{70A97B06-D370-4615-BFBF-F47CD659DD7D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1438,7 +1441,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2B976423-378E-4241-A613-561C25EEB454}" type="CELLRANGE">
+                    <a:fld id="{6E20B31B-B40B-4AE3-B57E-A487464E3854}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1472,7 +1475,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B9230B4F-58F1-416A-9EFE-5558762CBDA5}" type="CELLRANGE">
+                    <a:fld id="{4350CA50-D1C3-49A8-8B3E-3FA1DCDC2D53}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1506,7 +1509,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DAE8A3EA-BBED-4716-95D7-FB506F7A9F91}" type="CELLRANGE">
+                    <a:fld id="{8F1C54CC-BEE6-4B32-97F0-F4F2936C13CE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1540,7 +1543,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B98511AA-1E80-4EBF-A6E4-B1448A664A69}" type="CELLRANGE">
+                    <a:fld id="{96DDB6BA-1BD5-4694-98E7-6AAE370096E7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1574,7 +1577,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA1443C4-1AAE-439C-955D-950615643A83}" type="CELLRANGE">
+                    <a:fld id="{6397FC7D-9376-462C-BDE5-E37834E0026D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1608,7 +1611,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7518CFDA-A62A-48C7-9083-08729B035157}" type="CELLRANGE">
+                    <a:fld id="{609B31FB-E1F9-4C40-A5D2-26A8D672BFBE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1642,7 +1645,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3DA633A-F6DE-4BBB-BB2B-C090181A844A}" type="CELLRANGE">
+                    <a:fld id="{9E216560-4E83-449C-8D14-C8DA0B523BDA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1676,7 +1679,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48065AAF-D3E2-4FF6-B984-EFB8D06CCB13}" type="CELLRANGE">
+                    <a:fld id="{86510544-89B6-4F46-ADFD-42B661294C93}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1710,7 +1713,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD1F90DC-6BC9-49FE-B57A-F7DD179347A8}" type="CELLRANGE">
+                    <a:fld id="{48835EDD-827D-4BEC-B6A2-AE8520DF9CC5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1744,7 +1747,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{52C5A9CF-50BA-4BC2-A59E-7055BB026806}" type="CELLRANGE">
+                    <a:fld id="{71BF2F21-4D6E-4C18-8B03-565F520DF325}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1778,7 +1781,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5584AAA7-D3F0-4FA0-A9C2-BBF696D27687}" type="CELLRANGE">
+                    <a:fld id="{75DF7B77-E8C8-4D3E-BCF3-226BFA0CB65C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1812,7 +1815,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{189854D7-F3AF-478F-80B7-A377D5AB58C8}" type="CELLRANGE">
+                    <a:fld id="{032E124D-E5B9-48B6-BF64-2594C670529F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1846,7 +1849,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6081FA79-7257-41E7-A608-DB7A6EDDBF01}" type="CELLRANGE">
+                    <a:fld id="{9ECC5AB6-33A5-4C7B-BE11-EE44402152BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1880,7 +1883,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{82E4C480-F0DB-496D-8FC3-F646E1559002}" type="CELLRANGE">
+                    <a:fld id="{75750379-D9DC-404E-B417-C029210F24D2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1914,7 +1917,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1F86F05A-AD70-4F63-9D40-EB94AE6ADAA9}" type="CELLRANGE">
+                    <a:fld id="{2A945DEB-4155-45FC-9626-1B58CC07882E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1948,7 +1951,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA191BBB-3850-49B1-9968-E60E5F10393D}" type="CELLRANGE">
+                    <a:fld id="{FD3178ED-C5A5-48AC-AA0C-6B8C6F0856BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1982,7 +1985,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C20F73A-33B0-4796-A7D8-CF6B3C629344}" type="CELLRANGE">
+                    <a:fld id="{3E827851-57F8-49A0-AB2F-CEE3C0B0BDF6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2016,7 +2019,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B80A10DA-5A0F-4BAE-8FEF-E4213D6C33E0}" type="CELLRANGE">
+                    <a:fld id="{B833E133-5932-41F8-9D30-0669F079BAC3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2050,7 +2053,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{03FB9139-1DB0-4E28-952F-A94000D132D5}" type="CELLRANGE">
+                    <a:fld id="{69CF8BDA-ABF5-4BDD-9C2A-482C513850D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2084,7 +2087,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{25408FBC-D507-4EB9-9DC7-EF1B22DBF068}" type="CELLRANGE">
+                    <a:fld id="{28BE8B34-1303-4B58-BE40-2E199D636985}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2118,7 +2121,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E06FD4BA-3FBA-4854-B9FC-25D0A4F4A8D7}" type="CELLRANGE">
+                    <a:fld id="{A827DA03-3018-4659-B308-D4F7C20EB00B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2152,7 +2155,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E554BD4E-870D-4EA7-8B10-319904AD3D33}" type="CELLRANGE">
+                    <a:fld id="{5D2632D3-E856-4CC9-A0CA-AE9DAC2643B7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2186,7 +2189,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D3D3558-1E1D-4E53-8AA3-EAC12589B103}" type="CELLRANGE">
+                    <a:fld id="{45B6F1F4-1CE3-4B4F-BA02-F255D851102A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2220,7 +2223,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1EC459AF-A951-4ED3-BA06-E6CF07CF9B26}" type="CELLRANGE">
+                    <a:fld id="{59206E79-7B37-4982-B36C-BAC5E9D990A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2254,7 +2257,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D02617F-29B8-4362-B082-4E5B73E26C12}" type="CELLRANGE">
+                    <a:fld id="{9C346184-B4A7-4FAA-8656-1508BFE06F17}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2288,7 +2291,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{167803CF-CAA2-41F7-B066-486568DEF7F5}" type="CELLRANGE">
+                    <a:fld id="{5F0A7653-403F-440D-9309-E4F2D19C722C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2322,7 +2325,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C35A8238-91B3-4679-802F-17B06D1F05DF}" type="CELLRANGE">
+                    <a:fld id="{C38B8ED4-9260-44C2-9CA0-E0C0FAC15DD0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2356,7 +2359,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73A008CB-96AE-488D-90EB-9D86B2469D5E}" type="CELLRANGE">
+                    <a:fld id="{8BFC5DAB-4E3B-4A12-BFFD-C0909024FB01}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2390,7 +2393,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{68030A63-684D-4B52-9F4E-BACA5082E282}" type="CELLRANGE">
+                    <a:fld id="{A6DAD473-1CC4-451C-B409-E591736F78CC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2424,7 +2427,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6B9EA44-F9A6-4315-BA59-8343E8417940}" type="CELLRANGE">
+                    <a:fld id="{8F9A0B36-2F6D-4309-8C89-E3559EB4A75B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2458,7 +2461,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3CEFFB75-E0B4-4FBA-AFB0-821D8A039A3C}" type="CELLRANGE">
+                    <a:fld id="{43472CA3-29A2-44D1-970F-A157324E21FF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2492,7 +2495,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0B2714DF-B834-4D91-9CAA-D43102702576}" type="CELLRANGE">
+                    <a:fld id="{06C737CD-FAF0-481D-9ECD-F4B7AD4F7625}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2526,7 +2529,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10C20FDB-F0CD-49B6-A6AC-82F15EC234D7}" type="CELLRANGE">
+                    <a:fld id="{58BD1B6A-23CD-4C31-A744-292B5B28FEC7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2560,7 +2563,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B61D510E-90FF-463B-84B6-29EABADA0CE2}" type="CELLRANGE">
+                    <a:fld id="{6DEFD8B6-0DAA-4358-B19D-C2FB44ECCC66}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2594,7 +2597,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F7E1F03E-0AB3-4328-A293-E2D998132C01}" type="CELLRANGE">
+                    <a:fld id="{0328FD50-4291-47C6-B558-963BF1E57BD4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2628,7 +2631,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BDB90B86-FC7B-4B1D-870F-B1DFCBCDA74E}" type="CELLRANGE">
+                    <a:fld id="{27646545-DBD1-4CA8-9D3D-EB0F8C1AA995}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2662,7 +2665,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8860CC9-B272-403A-946A-28FD1AD11BDF}" type="CELLRANGE">
+                    <a:fld id="{EE5D4FCD-9027-4225-AD26-31C82B6F2365}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2696,7 +2699,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{291EB2BF-AAE1-467E-9EEE-2DAC226F21E5}" type="CELLRANGE">
+                    <a:fld id="{EB9C29F9-627D-4B95-9214-889229811A23}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2730,7 +2733,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{794C815C-3088-494E-BAA9-57CE70471C1E}" type="CELLRANGE">
+                    <a:fld id="{3C65748A-56FB-4497-AD77-539F31B47E0E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2764,7 +2767,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{93E9E27C-10DB-4F6D-8660-25BE29CED5E9}" type="CELLRANGE">
+                    <a:fld id="{FCB234D6-87C5-4D76-90A9-B15737D6E76B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2798,7 +2801,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{520C617F-8B54-43B5-9EB8-64350FE00203}" type="CELLRANGE">
+                    <a:fld id="{3A392567-F3C2-4904-AF4D-EBA3AA23CB87}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2832,7 +2835,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60690370-C7F5-4946-80EC-4997A4ADFE76}" type="CELLRANGE">
+                    <a:fld id="{F8BC65CA-85A1-4485-BB94-08BCC0179DF3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2866,7 +2869,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4212481D-2E64-42ED-B0EA-B76494F174F5}" type="CELLRANGE">
+                    <a:fld id="{61EFB5ED-C5CF-4FD2-BAF4-E48A12BAD4FE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2900,7 +2903,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{128E593B-CA7B-4DD8-8E80-862DC887BD86}" type="CELLRANGE">
+                    <a:fld id="{33DABA36-600B-43B7-9BA0-7F5B07DB4FBC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2934,7 +2937,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36DD4985-4553-43F2-AB7B-C40759A7F082}" type="CELLRANGE">
+                    <a:fld id="{88F7871C-5576-4959-9954-FBCE15A38C65}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2968,7 +2971,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{131EC869-F585-4B0C-BFFC-DB29BEBD1C31}" type="CELLRANGE">
+                    <a:fld id="{34C1057E-FE0C-4E30-8ABD-C994F4AF3F87}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3002,7 +3005,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C82AEE16-7920-4645-A12B-BA77785C149E}" type="CELLRANGE">
+                    <a:fld id="{CA7B64A7-48AD-4832-BFB5-4E8A7CBAD449}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3036,7 +3039,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2DC1F393-D2C4-4834-B6FD-D648C155A6E8}" type="CELLRANGE">
+                    <a:fld id="{2F076E60-86AD-4FCC-A437-3D661F0F77EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3070,7 +3073,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CCF2A0CE-1DF1-44C0-B71F-59C5087699F7}" type="CELLRANGE">
+                    <a:fld id="{0D71493A-C19A-4662-81BC-AB715D2E92EA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3094,6 +3097,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-363E-4205-A432-E7DFA9A91746}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="79"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{D56D22F5-0CEE-4F70-89CD-CAF7E73E36CE}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-1FA8-4CA8-94B9-2F0FBDFCBC20}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3143,10 +3180,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$80</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="79"/>
+                <c:ptCount val="80"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -3157,231 +3194,234 @@
                   <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>11.866666666666667</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>10.3</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>6.3</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>7.5</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>3.4</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>2.9</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>7.7</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>8.75</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>7.9</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>11.3</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>6.8</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>3.4</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>9.6</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>11.6</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>12.5</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>9.1</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>9.5500000000000007</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>12.2</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>9.75</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>5.4</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>11.9</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>11.4</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>10.4</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>4.2</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>13.6</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>7.2</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>2.7</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>6.9</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>3.3</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="69">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>9.9</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>5.8</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="73">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="74">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="75">
                   <c:v>5.6</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="76">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="77">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="78">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="78">
+                <c:pt idx="79">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -3389,10 +3429,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$80</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="79"/>
+                <c:ptCount val="80"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -3403,231 +3443,234 @@
                   <c:v>3950</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>2590</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2840</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>4700</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2010</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>690</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>1270</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>1920</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>2970</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>3110</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>940</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>3030</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>3200</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>1200</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>1540</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>2380</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>3290</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>2660</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>2780</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>2425</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>4100</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>4800</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>4120</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>3420</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>3850</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>2050</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>1450</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>3160</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>2550</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>1050</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>3350</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>880</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>1420</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>860</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>1260</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>2600</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>3930</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>3100</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>1670</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>1850</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>1630</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>1090</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>1470</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>3490</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>1930</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>2170</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>2250</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="69">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>3180</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>1540</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="73">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="74">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="75">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="76">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="77">
                   <c:v>760</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="78">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="78">
+                <c:pt idx="79">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -3653,16 +3696,16 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="4">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>omg yikes wtf</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>easy (but long)</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="8">
                     <c:v>moderate</c:v>
@@ -3674,67 +3717,67 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="11">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="13">
                     <c:v>moderate (because rough)</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="14">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="16">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>strenuous</c:v>
+                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="18">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>easy</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="20">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="21">
-                    <c:v>moderate</c:v>
+                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="22">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="23">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="25">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="26">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
                     <c:v>strenuous</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="28">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="29">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="30">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="30">
+                  <c:pt idx="31">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="31">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="32">
                     <c:v>strenuous</c:v>
@@ -3749,34 +3792,34 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="36">
+                    <c:v>strenuous</c:v>
+                  </c:pt>
+                  <c:pt idx="37">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="37">
+                  <c:pt idx="38">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="38">
+                  <c:pt idx="39">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="39">
+                  <c:pt idx="40">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="40">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="41">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="42">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="43">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="43">
+                  <c:pt idx="44">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="44">
+                  <c:pt idx="45">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="45">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="46">
                     <c:v>easy</c:v>
@@ -3785,19 +3828,19 @@
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="48">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="49">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="49">
+                  <c:pt idx="50">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="50">
-                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="51">
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="52">
-                    <c:v>moderate</c:v>
+                    <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="53">
                     <c:v>moderate</c:v>
@@ -3806,75 +3849,78 @@
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="55">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="56">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="56">
+                  <c:pt idx="57">
                     <c:v>moderate</c:v>
-                  </c:pt>
-                  <c:pt idx="57">
-                    <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="58">
                     <c:v>easy</c:v>
                   </c:pt>
                   <c:pt idx="59">
+                    <c:v>easy</c:v>
+                  </c:pt>
+                  <c:pt idx="60">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="60">
+                  <c:pt idx="61">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="61">
+                  <c:pt idx="62">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="62">
+                  <c:pt idx="63">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="63">
+                  <c:pt idx="64">
                     <c:v>easy</c:v>
-                  </c:pt>
-                  <c:pt idx="64">
-                    <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="65">
                     <c:v>moderate</c:v>
                   </c:pt>
                   <c:pt idx="66">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="67">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="67">
+                  <c:pt idx="68">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="68">
+                  <c:pt idx="69">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="69">
+                  <c:pt idx="70">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="70">
+                  <c:pt idx="71">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="71">
+                  <c:pt idx="72">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="72">
+                  <c:pt idx="73">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="73">
+                  <c:pt idx="74">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="74">
+                  <c:pt idx="75">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="75">
+                  <c:pt idx="76">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="76">
+                  <c:pt idx="77">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="77">
+                  <c:pt idx="78">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="78">
+                  <c:pt idx="79">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -4927,10 +4973,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D80" totalsRowShown="0">
-  <autoFilter ref="A1:D80" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D80">
-    <sortCondition ref="A1:A80"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D81" totalsRowShown="0">
+  <autoFilter ref="A1:D81" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D81">
+    <sortCondition ref="A1:A81"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -5239,10 +5285,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5311,13 +5357,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="B5">
-        <v>9.1999999999999993</v>
+        <v>9.5</v>
       </c>
       <c r="C5">
-        <v>2840</v>
+        <v>2590</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -5325,70 +5371,70 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>8.5</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C6">
-        <v>4700</v>
+        <v>2840</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>8.5</v>
+      </c>
+      <c r="C7">
+        <v>4700</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <f>17.8*2/3</f>
         <v>11.866666666666667</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>2010</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>10.3</v>
-      </c>
-      <c r="C8">
-        <v>690</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>10.3</v>
       </c>
       <c r="C9">
-        <v>1270</v>
+        <v>690</v>
       </c>
       <c r="D9" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>2400</v>
+        <v>1270</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
@@ -5396,13 +5442,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B11">
-        <v>6.3</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>1920</v>
+        <v>2400</v>
       </c>
       <c r="D11" t="s">
         <v>1</v>
@@ -5410,13 +5456,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="B12">
-        <v>7.5</v>
+        <v>6.3</v>
       </c>
       <c r="C12">
-        <v>2970</v>
+        <v>1920</v>
       </c>
       <c r="D12" t="s">
         <v>1</v>
@@ -5424,55 +5470,55 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B13">
-        <v>8.1999999999999993</v>
+        <v>7.5</v>
       </c>
       <c r="C13">
-        <v>3110</v>
+        <v>2970</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14">
-        <v>3.4</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C14">
-        <v>940</v>
+        <v>3110</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="C15">
-        <v>1000</v>
+        <v>940</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16">
-        <v>2.9</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>1090</v>
+        <v>1000</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -5480,57 +5526,57 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B17">
-        <v>7.7</v>
+        <v>2.9</v>
       </c>
       <c r="C17">
-        <v>3030</v>
+        <v>1090</v>
       </c>
       <c r="D17" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <v>7.7</v>
+      </c>
+      <c r="C18">
+        <v>3030</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>81</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <f>35/4</f>
         <v>8.75</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <f>9000/4</f>
         <v>2250</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19">
-        <v>7.9</v>
-      </c>
-      <c r="C19">
-        <v>3200</v>
-      </c>
-      <c r="D19" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20">
-        <v>11.3</v>
+        <v>7.9</v>
       </c>
       <c r="C20">
-        <v>3850</v>
+        <v>3200</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
@@ -5538,27 +5584,27 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21">
-        <v>6.8</v>
+        <v>11.3</v>
       </c>
       <c r="C21">
-        <v>1200</v>
+        <v>3850</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B22">
-        <v>3.4</v>
+        <v>6.8</v>
       </c>
       <c r="C22">
-        <v>750</v>
+        <v>1200</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
@@ -5566,27 +5612,27 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="B23">
-        <v>6.5</v>
+        <v>3.4</v>
       </c>
       <c r="C23">
-        <v>1540</v>
+        <v>750</v>
       </c>
       <c r="D23" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B24">
-        <v>8.5</v>
+        <v>6.5</v>
       </c>
       <c r="C24">
-        <v>2380</v>
+        <v>1540</v>
       </c>
       <c r="D24" t="s">
         <v>1</v>
@@ -5594,85 +5640,85 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25">
-        <v>9.6</v>
+        <v>8.5</v>
       </c>
       <c r="C25">
-        <v>3290</v>
+        <v>2380</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>9.6</v>
+      </c>
+      <c r="C26">
+        <v>3290</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>82</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <f>14.6/2</f>
         <v>7.3</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <f>3160/2</f>
         <v>1580</v>
       </c>
-      <c r="D26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27">
-        <v>11.6</v>
-      </c>
-      <c r="C27">
-        <v>2660</v>
-      </c>
       <c r="D27" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B28">
-        <v>12.5</v>
+        <v>11.6</v>
       </c>
       <c r="C28">
-        <v>2780</v>
+        <v>2660</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="B29">
-        <v>9</v>
+        <v>12.5</v>
       </c>
       <c r="C29">
-        <v>1680</v>
+        <v>2780</v>
       </c>
       <c r="D29" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B30">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="C30">
-        <v>1580</v>
+        <v>1680</v>
       </c>
       <c r="D30" t="s">
         <v>1</v>
@@ -5680,57 +5726,57 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B31">
-        <v>5.2</v>
+        <v>9.1</v>
       </c>
       <c r="C31">
-        <v>1000</v>
+        <v>1580</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>5.2</v>
+      </c>
+      <c r="C32">
+        <v>1000</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
         <v>79</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <f>19.1/2</f>
         <v>9.5500000000000007</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <f>4850/2</f>
         <v>2425</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>78</v>
-      </c>
-      <c r="B33">
-        <v>9.5</v>
-      </c>
-      <c r="C33">
-        <v>4100</v>
-      </c>
-      <c r="D33" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="B34">
-        <v>14</v>
+        <v>9.5</v>
       </c>
       <c r="C34">
-        <v>4800</v>
+        <v>4100</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
@@ -5738,13 +5784,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35">
         <v>14</v>
       </c>
-      <c r="B35">
-        <v>12.2</v>
-      </c>
       <c r="C35">
-        <v>4120</v>
+        <v>4800</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
@@ -5752,13 +5798,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B36">
-        <v>12</v>
+        <v>12.2</v>
       </c>
       <c r="C36">
-        <v>3420</v>
+        <v>4120</v>
       </c>
       <c r="D36" t="s">
         <v>10</v>
@@ -5766,99 +5812,99 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>12</v>
+      </c>
+      <c r="C37">
+        <v>3420</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <f>19.5/2</f>
         <v>9.75</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <f>4400*7/8</f>
         <v>3850</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38">
-        <v>6.9</v>
-      </c>
-      <c r="C38">
-        <v>2050</v>
-      </c>
-      <c r="D38" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="B39">
-        <v>5.4</v>
+        <v>6.9</v>
       </c>
       <c r="C39">
-        <v>1450</v>
+        <v>2050</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B40">
-        <v>11.9</v>
+        <v>5.4</v>
       </c>
       <c r="C40">
-        <v>3160</v>
+        <v>1450</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>11.9</v>
       </c>
       <c r="C41">
-        <v>400</v>
+        <v>3160</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="B42">
-        <v>11.4</v>
+        <v>3</v>
       </c>
       <c r="C42">
-        <v>2550</v>
+        <v>400</v>
       </c>
       <c r="D42" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="B43">
-        <v>10.8</v>
+        <v>11.4</v>
       </c>
       <c r="C43">
-        <v>1050</v>
+        <v>2550</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
@@ -5866,69 +5912,69 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="B44">
-        <v>8.5</v>
+        <v>10.8</v>
       </c>
       <c r="C44">
-        <v>3350</v>
+        <v>1050</v>
       </c>
       <c r="D44" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B45">
-        <v>2.8</v>
+        <v>8.5</v>
       </c>
       <c r="C45">
-        <v>880</v>
+        <v>3350</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B46">
-        <v>10.4</v>
+        <v>2.8</v>
       </c>
       <c r="C46">
-        <v>1420</v>
+        <v>880</v>
       </c>
       <c r="D46" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B47">
-        <v>0.9</v>
+        <v>10.4</v>
       </c>
       <c r="C47">
-        <v>200</v>
+        <v>1420</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B48">
-        <v>4.2</v>
+        <v>0.9</v>
       </c>
       <c r="C48">
-        <v>860</v>
+        <v>200</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
@@ -5936,13 +5982,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B49">
-        <v>4.8</v>
+        <v>4.2</v>
       </c>
       <c r="C49">
-        <v>1260</v>
+        <v>860</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
@@ -5950,55 +5996,55 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B50">
-        <v>4</v>
+        <v>4.8</v>
       </c>
       <c r="C50">
-        <v>2600</v>
+        <v>1260</v>
       </c>
       <c r="D50" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B51">
-        <v>1.4</v>
+        <v>4</v>
       </c>
       <c r="C51">
-        <v>375</v>
+        <v>2600</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B52">
-        <v>13.6</v>
+        <v>1.4</v>
       </c>
       <c r="C52">
-        <v>3930</v>
+        <v>375</v>
       </c>
       <c r="D52" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B53">
-        <v>10.5</v>
+        <v>13.6</v>
       </c>
       <c r="C53">
-        <v>3100</v>
+        <v>3930</v>
       </c>
       <c r="D53" t="s">
         <v>10</v>
@@ -6006,27 +6052,27 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B54">
-        <v>7</v>
+        <v>10.5</v>
       </c>
       <c r="C54">
-        <v>1670</v>
+        <v>3100</v>
       </c>
       <c r="D54" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B55">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="C55">
-        <v>2400</v>
+        <v>1670</v>
       </c>
       <c r="D55" t="s">
         <v>1</v>
@@ -6034,13 +6080,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B56">
-        <v>5.5</v>
+        <v>8.1</v>
       </c>
       <c r="C56">
-        <v>1850</v>
+        <v>2400</v>
       </c>
       <c r="D56" t="s">
         <v>1</v>
@@ -6048,55 +6094,55 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B57">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C57">
-        <v>1300</v>
+        <v>1850</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B58">
-        <v>7.2</v>
+        <v>4.8</v>
       </c>
       <c r="C58">
-        <v>1630</v>
+        <v>1300</v>
       </c>
       <c r="D58" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B59">
-        <v>2.7</v>
+        <v>7.2</v>
       </c>
       <c r="C59">
-        <v>1090</v>
+        <v>1630</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="B60">
-        <v>4.8</v>
+        <v>2.7</v>
       </c>
       <c r="C60">
-        <v>1470</v>
+        <v>1090</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
@@ -6104,97 +6150,97 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B61">
-        <v>6.9</v>
+        <v>4.8</v>
       </c>
       <c r="C61">
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="D61" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B62">
-        <v>8.1999999999999993</v>
+        <v>6.9</v>
       </c>
       <c r="C62">
-        <v>3490</v>
+        <v>2000</v>
       </c>
       <c r="D62" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B63">
-        <v>3.3</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C63">
-        <v>600</v>
+        <v>3490</v>
       </c>
       <c r="D63" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B64">
-        <v>8.5</v>
+        <v>3.3</v>
       </c>
       <c r="C64">
-        <v>1930</v>
+        <v>600</v>
       </c>
       <c r="D64" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B65">
-        <v>2.2000000000000002</v>
+        <v>8.5</v>
       </c>
       <c r="C65">
-        <v>750</v>
+        <v>1930</v>
       </c>
       <c r="D65" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B66">
-        <v>11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C66">
-        <v>2170</v>
+        <v>750</v>
       </c>
       <c r="D66" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B67">
-        <v>7.3</v>
+        <v>11</v>
       </c>
       <c r="C67">
-        <v>2250</v>
+        <v>2170</v>
       </c>
       <c r="D67" t="s">
         <v>1</v>
@@ -6202,186 +6248,200 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
+        <v>24</v>
+      </c>
+      <c r="B68">
+        <v>7.3</v>
+      </c>
+      <c r="C68">
+        <v>2250</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
         <v>25</v>
       </c>
-      <c r="B68">
+      <c r="B69">
         <f>16*2/3</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="C68">
+      <c r="C69">
         <f>4910*2/3</f>
         <v>3273.3333333333335</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D69" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>49</v>
-      </c>
-      <c r="B69">
-        <v>1.2</v>
-      </c>
-      <c r="C69">
-        <v>500</v>
-      </c>
-      <c r="D69" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B70">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C70">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D70" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B71">
-        <v>6.5</v>
+        <v>11</v>
       </c>
       <c r="C71">
-        <v>1650</v>
+        <v>3060</v>
       </c>
       <c r="D71" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B72">
-        <v>9.9</v>
+        <v>6.5</v>
       </c>
       <c r="C72">
-        <v>3180</v>
+        <v>1650</v>
       </c>
       <c r="D72" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="B73">
-        <v>5.8</v>
+        <v>9.9</v>
       </c>
       <c r="C73">
-        <v>1540</v>
+        <v>3180</v>
       </c>
       <c r="D73" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B74">
-        <v>0.4</v>
+        <v>5.8</v>
       </c>
       <c r="C74">
-        <v>100</v>
+        <v>1540</v>
       </c>
       <c r="D74" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B75">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C75">
-        <v>3550</v>
+        <v>100</v>
       </c>
       <c r="D75" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="B76">
-        <v>5.6</v>
+        <v>7.3</v>
       </c>
       <c r="C76">
-        <v>1680</v>
+        <v>3550</v>
       </c>
       <c r="D76" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B77">
-        <v>10.8</v>
+        <v>5.6</v>
       </c>
       <c r="C77">
-        <v>1800</v>
+        <v>1680</v>
       </c>
       <c r="D77" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B78">
-        <v>7</v>
+        <v>10.8</v>
       </c>
       <c r="C78">
-        <v>760</v>
+        <v>1800</v>
       </c>
       <c r="D78" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79">
+        <v>7</v>
+      </c>
+      <c r="C79">
+        <v>760</v>
+      </c>
+      <c r="D79" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
         <v>55</v>
       </c>
-      <c r="B79">
+      <c r="B80">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C79">
+      <c r="C80">
         <v>3800</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D80" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
         <v>29</v>
       </c>
-      <c r="B80">
+      <c r="B81">
         <v>6</v>
       </c>
-      <c r="C80">
+      <c r="C81">
         <v>2180</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D81" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Stevens Canyon entry
</commit_message>
<xml_diff>
--- a/DifficultyAnalysis.xlsx
+++ b/DifficultyAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shawn\Desktop\docs\HikingTahoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A2F0EC-1C25-4647-ACF5-78B1F9D0B746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89A9A9C-D7FC-4C02-B036-917E93F4DB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" xr2:uid="{A6EDCF44-0070-4784-B0C7-EC99C3A4E4FD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="91">
   <si>
     <t>Burroughs Mountain</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>Brown Peak</t>
+  </si>
+  <si>
+    <t>Stevens Canyon</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8D3DA45D-E5BC-47E7-BE96-E4D182FA5246}" type="CELLRANGE">
+                    <a:fld id="{61BE8B35-C201-4F16-8741-D7812DAD5195}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -455,7 +458,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE1B2FD0-A260-40C4-808E-F8EFE514A693}" type="CELLRANGE">
+                    <a:fld id="{328177C6-0B06-40DA-AE12-3B37A0054DF1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -489,7 +492,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C8522D9-8027-4376-9C6D-2C0558B4EBB5}" type="CELLRANGE">
+                    <a:fld id="{BE09CCD0-8480-4A2E-99E0-6C0747324570}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -523,7 +526,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC89BAD4-6D49-4142-BA0E-5BB2F9742489}" type="CELLRANGE">
+                    <a:fld id="{4E2A8653-022E-4CD5-8004-8EE159393011}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -557,7 +560,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0AB9FE5D-1F18-4364-AABD-98DD9CADF1D3}" type="CELLRANGE">
+                    <a:fld id="{3B46E71B-4746-46DE-83AC-CE663F72E97D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -591,7 +594,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F489AB8-97A5-4736-9E1B-EC59D29138D1}" type="CELLRANGE">
+                    <a:fld id="{4514DEB8-523A-4A25-A563-D41D4C7BCDDE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -625,7 +628,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3A02411F-78CF-485F-BD38-B18C47131B11}" type="CELLRANGE">
+                    <a:fld id="{40185A61-15F0-43F2-BEC6-38A2CB094503}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -659,7 +662,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF384655-7EF2-4DB0-8BAD-B2D6A222B8D9}" type="CELLRANGE">
+                    <a:fld id="{6DD862FD-DF42-42B3-B864-0AD7F583BBF6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -693,7 +696,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E60A3E5-4087-4C9C-B24F-3F780046C356}" type="CELLRANGE">
+                    <a:fld id="{B5F6CCEE-6DA8-4172-923D-5360AB4D5432}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -727,7 +730,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A1018E1-BB87-4114-BFF0-FF7150A93DD7}" type="CELLRANGE">
+                    <a:fld id="{3E07533D-1E7F-4C84-94EC-87F5DDDF39A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -761,7 +764,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EFA89423-58D7-4D28-90E6-8AE70E03EA4C}" type="CELLRANGE">
+                    <a:fld id="{318171B2-E432-4CF4-A157-C1E0B5C30939}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -795,7 +798,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34089EC4-0F52-4735-BF92-730371234ACA}" type="CELLRANGE">
+                    <a:fld id="{3699DABC-FC77-4815-B35B-B3322C4F6EA3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -829,7 +832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E951527-35F1-4127-BD83-2FC28841BE15}" type="CELLRANGE">
+                    <a:fld id="{16EFC40E-1E21-447A-99B7-53319D2748C6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -863,7 +866,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E8A380D2-BC28-4D02-AA70-02721961FCA3}" type="CELLRANGE">
+                    <a:fld id="{8C8F4F9C-FF3C-465A-8DFD-CFDEBBE7AC01}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -897,7 +900,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{01846907-7331-4DE5-81BA-C50765BA716A}" type="CELLRANGE">
+                    <a:fld id="{D2D0E318-566A-4DDA-B1B4-31845930F1B6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -931,7 +934,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5BF7342D-B9BE-4D74-B4C1-9598D5161CED}" type="CELLRANGE">
+                    <a:fld id="{67A7C2FF-2E3C-4C1B-B156-314E03F0F772}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -965,7 +968,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F81993E3-8F00-414E-BB04-09CD4EC28CD1}" type="CELLRANGE">
+                    <a:fld id="{7E890389-C368-4CD2-AA99-495DEDEEE8F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -999,7 +1002,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C222C73-093A-4713-BC55-3EBD8369C2B6}" type="CELLRANGE">
+                    <a:fld id="{F28622F2-1D4D-479D-82B3-004AA6D813D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1033,7 +1036,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8D9C6600-2913-47F5-9972-28CAC85CCEE8}" type="CELLRANGE">
+                    <a:fld id="{8488FAAF-C550-4E5D-8457-E4452274A4D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1067,7 +1070,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0918DDFA-F0A6-4FE5-8B77-868341165AD0}" type="CELLRANGE">
+                    <a:fld id="{AC2E2448-7053-47D1-80FF-D699E2B40AA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1101,7 +1104,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34CE7A06-8622-41D2-9EAB-99FC25837849}" type="CELLRANGE">
+                    <a:fld id="{EDB3BE9B-AAFC-43E0-854D-99B4DFBDBDAD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1135,7 +1138,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{30F643A9-CB5F-4437-9844-9AA18ECDBB04}" type="CELLRANGE">
+                    <a:fld id="{D9C10AAC-40AC-4480-ABEC-9FA02522158E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1169,7 +1172,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3197FC1B-9FC9-4B3A-B467-EDC364BC9ACF}" type="CELLRANGE">
+                    <a:fld id="{5B539420-2CB9-45D8-8B67-E4C8202F6EC0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1203,7 +1206,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A040B548-24FE-4AD1-9B4F-561DD99A22BD}" type="CELLRANGE">
+                    <a:fld id="{1EA683E7-9B74-47AE-8AFF-2760096E57EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1237,7 +1240,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E0C7868-9098-4F26-9698-823A8FCEF58B}" type="CELLRANGE">
+                    <a:fld id="{3F5FBC0B-C317-42F0-B8CD-D572EBD81445}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1271,7 +1274,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BEB6A28F-2C8F-44F1-9B04-5F5947FB2530}" type="CELLRANGE">
+                    <a:fld id="{C45D1623-FA6E-43F4-8B2C-FAC292B99310}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1305,7 +1308,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F6957CFD-333D-4214-9CE3-0DAE2FCC2A06}" type="CELLRANGE">
+                    <a:fld id="{F127CAA9-4A1C-4A2B-A6F7-1DB651FAD330}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1339,7 +1342,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1033C60C-895C-4CC5-A9C8-A9BFC01F13CB}" type="CELLRANGE">
+                    <a:fld id="{DA2478CB-F28B-4406-8F26-50C28B9A4F17}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1373,7 +1376,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E0A0008C-25C6-4E85-B133-F2B6436D621B}" type="CELLRANGE">
+                    <a:fld id="{DDB37193-624D-42E1-8FB3-041D8F9E4253}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1407,7 +1410,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70A97B06-D370-4615-BFBF-F47CD659DD7D}" type="CELLRANGE">
+                    <a:fld id="{B89205BF-0362-4A2D-A70F-F9F58A4B4F4A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1441,7 +1444,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E20B31B-B40B-4AE3-B57E-A487464E3854}" type="CELLRANGE">
+                    <a:fld id="{C67A14AB-1AE3-4116-826C-3CD496D10107}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1475,7 +1478,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4350CA50-D1C3-49A8-8B3E-3FA1DCDC2D53}" type="CELLRANGE">
+                    <a:fld id="{489BA886-3546-47DC-A542-D3914098FF43}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1509,7 +1512,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8F1C54CC-BEE6-4B32-97F0-F4F2936C13CE}" type="CELLRANGE">
+                    <a:fld id="{28610D62-A5D6-418E-B5DF-CB63CDF25E9A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1543,7 +1546,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96DDB6BA-1BD5-4694-98E7-6AAE370096E7}" type="CELLRANGE">
+                    <a:fld id="{91264AA6-D3D1-40B9-88A9-B016DC225377}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1577,7 +1580,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6397FC7D-9376-462C-BDE5-E37834E0026D}" type="CELLRANGE">
+                    <a:fld id="{33C304DA-ABA6-4A9E-9A4D-CCD3751B8D76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1611,7 +1614,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{609B31FB-E1F9-4C40-A5D2-26A8D672BFBE}" type="CELLRANGE">
+                    <a:fld id="{92C262BB-57A6-4439-AF1D-85CD524BF878}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1645,7 +1648,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E216560-4E83-449C-8D14-C8DA0B523BDA}" type="CELLRANGE">
+                    <a:fld id="{7EF6A52F-2DAF-4D8B-BA88-4D4E29E80BB8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1679,7 +1682,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{86510544-89B6-4F46-ADFD-42B661294C93}" type="CELLRANGE">
+                    <a:fld id="{ABD716A1-3A1C-45E4-B5D6-EB44683B01C0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1713,7 +1716,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48835EDD-827D-4BEC-B6A2-AE8520DF9CC5}" type="CELLRANGE">
+                    <a:fld id="{448AC6E8-63AE-4F56-8271-4AC08CF131A0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1747,7 +1750,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{71BF2F21-4D6E-4C18-8B03-565F520DF325}" type="CELLRANGE">
+                    <a:fld id="{88F6E92C-B761-45D6-8EF9-760CEACEEC40}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1781,7 +1784,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75DF7B77-E8C8-4D3E-BCF3-226BFA0CB65C}" type="CELLRANGE">
+                    <a:fld id="{9B1E1A19-FA04-4E81-A629-F1A5CD9A3ABD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1815,7 +1818,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{032E124D-E5B9-48B6-BF64-2594C670529F}" type="CELLRANGE">
+                    <a:fld id="{838D061F-9FB7-4E86-89F2-FFB03F6EF87C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1849,7 +1852,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9ECC5AB6-33A5-4C7B-BE11-EE44402152BE}" type="CELLRANGE">
+                    <a:fld id="{5C431686-0151-43B0-A2D2-1331E352C848}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1883,7 +1886,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75750379-D9DC-404E-B417-C029210F24D2}" type="CELLRANGE">
+                    <a:fld id="{B664BE9F-3FD3-4AF6-A0E3-F919B1BE056D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1917,7 +1920,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A945DEB-4155-45FC-9626-1B58CC07882E}" type="CELLRANGE">
+                    <a:fld id="{5398B8F1-41BB-48E3-86BB-2CD1526D851D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1951,7 +1954,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD3178ED-C5A5-48AC-AA0C-6B8C6F0856BE}" type="CELLRANGE">
+                    <a:fld id="{E95B6E8F-1490-4C52-811B-134950765CC0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1985,7 +1988,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E827851-57F8-49A0-AB2F-CEE3C0B0BDF6}" type="CELLRANGE">
+                    <a:fld id="{6D9CD01A-95A2-430A-8827-25CCAF9ED9C3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2019,7 +2022,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B833E133-5932-41F8-9D30-0669F079BAC3}" type="CELLRANGE">
+                    <a:fld id="{CE6D2864-472F-45A9-936E-62C7DF5C8C4D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2053,7 +2056,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69CF8BDA-ABF5-4BDD-9C2A-482C513850D3}" type="CELLRANGE">
+                    <a:fld id="{F8A28B45-08E0-42FB-9A21-51405B15ADA2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2087,7 +2090,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{28BE8B34-1303-4B58-BE40-2E199D636985}" type="CELLRANGE">
+                    <a:fld id="{D733F19F-0CA1-4289-8150-D997FE3FC5DA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2121,7 +2124,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A827DA03-3018-4659-B308-D4F7C20EB00B}" type="CELLRANGE">
+                    <a:fld id="{9ADA6069-AC5C-4C7D-A79F-FAD4CB9F84DC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2155,7 +2158,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D2632D3-E856-4CC9-A0CA-AE9DAC2643B7}" type="CELLRANGE">
+                    <a:fld id="{195B77EB-A0F2-4210-B763-84B8486596FB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2189,7 +2192,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{45B6F1F4-1CE3-4B4F-BA02-F255D851102A}" type="CELLRANGE">
+                    <a:fld id="{7A7888D5-0E85-4048-8C16-7F217E33D44A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2223,7 +2226,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{59206E79-7B37-4982-B36C-BAC5E9D990A1}" type="CELLRANGE">
+                    <a:fld id="{282DCF6C-7DA6-492C-B0A7-387DACE4AA49}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2257,7 +2260,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C346184-B4A7-4FAA-8656-1508BFE06F17}" type="CELLRANGE">
+                    <a:fld id="{C71C6FDB-A0E0-49FB-BF2C-29EC791109A0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2291,7 +2294,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F0A7653-403F-440D-9309-E4F2D19C722C}" type="CELLRANGE">
+                    <a:fld id="{D7E8C91B-AE20-4F09-A506-8CF2283C8FA1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2325,7 +2328,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C38B8ED4-9260-44C2-9CA0-E0C0FAC15DD0}" type="CELLRANGE">
+                    <a:fld id="{D8EDB275-834E-4D36-B656-6A1A447184CD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2359,7 +2362,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8BFC5DAB-4E3B-4A12-BFFD-C0909024FB01}" type="CELLRANGE">
+                    <a:fld id="{DB55E97B-E0E0-47BD-B695-298C25641300}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2393,7 +2396,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A6DAD473-1CC4-451C-B409-E591736F78CC}" type="CELLRANGE">
+                    <a:fld id="{FD9F5A67-D86C-4C27-B422-4EA16A930E1E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2427,7 +2430,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8F9A0B36-2F6D-4309-8C89-E3559EB4A75B}" type="CELLRANGE">
+                    <a:fld id="{73AD750D-E3BA-4ED9-830E-69D3EA3A3B5B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2461,7 +2464,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{43472CA3-29A2-44D1-970F-A157324E21FF}" type="CELLRANGE">
+                    <a:fld id="{6E3F2689-90E5-477C-A8DA-D883C91D8AD6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2495,7 +2498,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06C737CD-FAF0-481D-9ECD-F4B7AD4F7625}" type="CELLRANGE">
+                    <a:fld id="{035CA9C2-B333-4151-B548-3D0CB3E4C077}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2529,7 +2532,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58BD1B6A-23CD-4C31-A744-292B5B28FEC7}" type="CELLRANGE">
+                    <a:fld id="{65567DBC-5154-439B-965F-D83686ED5032}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2563,7 +2566,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6DEFD8B6-0DAA-4358-B19D-C2FB44ECCC66}" type="CELLRANGE">
+                    <a:fld id="{99AD98ED-7285-48D0-9410-BC061061268A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2597,7 +2600,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0328FD50-4291-47C6-B558-963BF1E57BD4}" type="CELLRANGE">
+                    <a:fld id="{22158A4E-BE1C-4ABB-85F4-6136E97DB5F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2631,7 +2634,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{27646545-DBD1-4CA8-9D3D-EB0F8C1AA995}" type="CELLRANGE">
+                    <a:fld id="{FF3F8A31-ACC6-4F0D-91B6-8EC3DB7353D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2665,7 +2668,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EE5D4FCD-9027-4225-AD26-31C82B6F2365}" type="CELLRANGE">
+                    <a:fld id="{F0CB03B4-ECC0-4820-8A1F-AB4DBFD6F579}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2699,7 +2702,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB9C29F9-627D-4B95-9214-889229811A23}" type="CELLRANGE">
+                    <a:fld id="{62BBF1D1-4147-41BD-97A6-EF7DC140D5F0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2733,7 +2736,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C65748A-56FB-4497-AD77-539F31B47E0E}" type="CELLRANGE">
+                    <a:fld id="{B45239C8-E49A-4BCE-A030-86FA7FCA2B6A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2767,7 +2770,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FCB234D6-87C5-4D76-90A9-B15737D6E76B}" type="CELLRANGE">
+                    <a:fld id="{7C67E8BA-D04B-47FE-B41A-B938B46B8623}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2801,7 +2804,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3A392567-F3C2-4904-AF4D-EBA3AA23CB87}" type="CELLRANGE">
+                    <a:fld id="{DC9CCF6F-DA41-4840-99A5-E8A745548C62}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2835,7 +2838,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8BC65CA-85A1-4485-BB94-08BCC0179DF3}" type="CELLRANGE">
+                    <a:fld id="{99262B79-1D21-41CB-82F0-B8483C2EA85A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2869,7 +2872,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{61EFB5ED-C5CF-4FD2-BAF4-E48A12BAD4FE}" type="CELLRANGE">
+                    <a:fld id="{C6635DBA-38C5-40C8-B6E6-24355C7E735E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2903,7 +2906,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33DABA36-600B-43B7-9BA0-7F5B07DB4FBC}" type="CELLRANGE">
+                    <a:fld id="{3CD05772-08D3-4CA4-A1F9-26F828BA2D3F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2937,7 +2940,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88F7871C-5576-4959-9954-FBCE15A38C65}" type="CELLRANGE">
+                    <a:fld id="{DB875052-B625-4D9B-9753-0C4D79E7F2B5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2971,7 +2974,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34C1057E-FE0C-4E30-8ABD-C994F4AF3F87}" type="CELLRANGE">
+                    <a:fld id="{38684799-E80A-4528-97E7-9F034F980887}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3005,7 +3008,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA7B64A7-48AD-4832-BFB5-4E8A7CBAD449}" type="CELLRANGE">
+                    <a:fld id="{3D0C2A9B-542A-4D3C-BCEE-6DA292358356}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3039,7 +3042,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F076E60-86AD-4FCC-A437-3D661F0F77EB}" type="CELLRANGE">
+                    <a:fld id="{387894AB-4862-47CE-9E28-1BCC4D714854}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3073,7 +3076,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D71493A-C19A-4662-81BC-AB715D2E92EA}" type="CELLRANGE">
+                    <a:fld id="{4947E8BC-8360-4F58-9171-C4F0333F11CA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3107,7 +3110,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D56D22F5-0CEE-4F70-89CD-CAF7E73E36CE}" type="CELLRANGE">
+                    <a:fld id="{EC0A742A-838C-4532-AF23-B259CCC80E2E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3131,6 +3134,40 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-1FA8-4CA8-94B9-2F0FBDFCBC20}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="80"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{93239A47-5A24-4FAC-A5CE-E2D17D54DB60}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-126C-4408-BC43-B58F790EF8DD}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3180,10 +3217,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$B$2:$B$81</c:f>
+              <c:f>'Hike Difficulties'!$B$2:$B$82</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="80"/>
+                <c:ptCount val="81"/>
                 <c:pt idx="0">
                   <c:v>10.8</c:v>
                 </c:pt>
@@ -3389,39 +3426,42 @@
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="68">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="69">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>9.9</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="73">
                   <c:v>5.8</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="74">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="75">
                   <c:v>7.3</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="76">
                   <c:v>5.6</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="77">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="78">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="78">
+                <c:pt idx="79">
                   <c:v>11.25</c:v>
                 </c:pt>
-                <c:pt idx="79">
+                <c:pt idx="80">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -3429,10 +3469,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hike Difficulties'!$C$2:$C$81</c:f>
+              <c:f>'Hike Difficulties'!$C$2:$C$82</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="80"/>
+                <c:ptCount val="81"/>
                 <c:pt idx="0">
                   <c:v>2990</c:v>
                 </c:pt>
@@ -3638,39 +3678,42 @@
                   <c:v>3273.3333333333335</c:v>
                 </c:pt>
                 <c:pt idx="68">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="69">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>3060</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>3180</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="73">
                   <c:v>1540</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="74">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="75">
                   <c:v>3550</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="76">
                   <c:v>1680</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="77">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="78">
                   <c:v>760</c:v>
                 </c:pt>
-                <c:pt idx="78">
+                <c:pt idx="79">
                   <c:v>3800</c:v>
                 </c:pt>
-                <c:pt idx="79">
+                <c:pt idx="80">
                   <c:v>2180</c:v>
                 </c:pt>
               </c:numCache>
@@ -3888,39 +3931,42 @@
                     <c:v>strenuous</c:v>
                   </c:pt>
                   <c:pt idx="68">
+                    <c:v>moderate</c:v>
+                  </c:pt>
+                  <c:pt idx="69">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="69">
+                  <c:pt idx="70">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="70">
+                  <c:pt idx="71">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="71">
+                  <c:pt idx="72">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="72">
+                  <c:pt idx="73">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="73">
+                  <c:pt idx="74">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="74">
+                  <c:pt idx="75">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="75">
+                  <c:pt idx="76">
                     <c:v>moderate</c:v>
                   </c:pt>
-                  <c:pt idx="76">
+                  <c:pt idx="77">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="77">
+                  <c:pt idx="78">
                     <c:v>easy</c:v>
                   </c:pt>
-                  <c:pt idx="78">
+                  <c:pt idx="79">
                     <c:v>strenuous</c:v>
                   </c:pt>
-                  <c:pt idx="79">
+                  <c:pt idx="80">
                     <c:v>moderate</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -4973,10 +5019,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D81" totalsRowShown="0">
-  <autoFilter ref="A1:D81" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D81">
-    <sortCondition ref="A1:A81"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84E5C422-267E-4EC2-B7F6-C6296A30534C}" name="Table1" displayName="Table1" ref="A1:D82" totalsRowShown="0">
+  <autoFilter ref="A1:D82" xr:uid="{F6E6D1D2-BEAF-41EC-8549-7BFCED1FD786}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D82">
+    <sortCondition ref="A1:A82"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{78FA270C-AB01-49C8-9535-1CF6BB2765CA}" name="Name"/>
@@ -5285,10 +5331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2FDABD-EE36-403A-85EC-C27298216BB6}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6278,170 +6324,184 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="B70">
-        <v>1.2</v>
+        <v>7.4</v>
       </c>
       <c r="C70">
-        <v>500</v>
+        <v>2800</v>
       </c>
       <c r="D70" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B71">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="C71">
-        <v>3060</v>
+        <v>500</v>
       </c>
       <c r="D71" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B72">
-        <v>6.5</v>
+        <v>11</v>
       </c>
       <c r="C72">
-        <v>1650</v>
+        <v>3060</v>
       </c>
       <c r="D72" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B73">
-        <v>9.9</v>
+        <v>6.5</v>
       </c>
       <c r="C73">
-        <v>3180</v>
+        <v>1650</v>
       </c>
       <c r="D73" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="B74">
-        <v>5.8</v>
+        <v>9.9</v>
       </c>
       <c r="C74">
-        <v>1540</v>
+        <v>3180</v>
       </c>
       <c r="D74" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B75">
-        <v>0.4</v>
+        <v>5.8</v>
       </c>
       <c r="C75">
-        <v>100</v>
+        <v>1540</v>
       </c>
       <c r="D75" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B76">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="C76">
-        <v>3550</v>
+        <v>100</v>
       </c>
       <c r="D76" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="B77">
-        <v>5.6</v>
+        <v>7.3</v>
       </c>
       <c r="C77">
-        <v>1680</v>
+        <v>3550</v>
       </c>
       <c r="D77" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B78">
-        <v>10.8</v>
+        <v>5.6</v>
       </c>
       <c r="C78">
-        <v>1800</v>
+        <v>1680</v>
       </c>
       <c r="D78" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B79">
-        <v>7</v>
+        <v>10.8</v>
       </c>
       <c r="C79">
-        <v>760</v>
+        <v>1800</v>
       </c>
       <c r="D79" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
+        <v>86</v>
+      </c>
+      <c r="B80">
+        <v>7</v>
+      </c>
+      <c r="C80">
+        <v>760</v>
+      </c>
+      <c r="D80" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
         <v>55</v>
       </c>
-      <c r="B80">
+      <c r="B81">
         <f>22.5/2</f>
         <v>11.25</v>
       </c>
-      <c r="C80">
+      <c r="C81">
         <v>3800</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D81" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
         <v>29</v>
       </c>
-      <c r="B81">
+      <c r="B82">
         <v>6</v>
       </c>
-      <c r="C81">
+      <c r="C82">
         <v>2180</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D82" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>